<commit_message>
Added Support for switching between Bidding Systems, but TODO Bug in navigation "back"
</commit_message>
<xml_diff>
--- a/bridgeIn.xlsx
+++ b/bridgeIn.xlsx
@@ -8,7 +8,8 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Bridge Bids" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="W-J 2017" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="W-J 2013" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="57">
   <si>
     <t xml:space="preserve">bidId</t>
   </si>
@@ -658,6 +659,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">6+ PC 4+ kier</t>
     </r>
@@ -829,6 +831,181 @@
   </si>
   <si>
     <t xml:space="preserve">16PC+ na  5+ karo</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">→ 2013!!! (12)</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="7"/>
+        <color rgb="FFFF3333"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">15</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="7"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">-17</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> PC, 5+ trefl </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="7"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">(naturalne, słaba piątka może też pasować na  1BA – patrz dalej)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="7"/>
+        <color rgb="FFFF0066"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">&lt;br&gt;&lt;font color=red&gt;w wersji pro od 15 a nawet 16 PC!!! - słaby trefl wtedy do BA albo 1 karo (o ile jest 4 karo)&lt;/font&gt;
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">&lt;br&gt;→ 12-17 PC, układ 4414  tzw </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="7"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">TRÓJKOLORÓWKA
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">(singiel karo)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">&lt;br&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">→ 12-14 PC, skład bez atutowy  tzw. </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="7"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">PRZYGOTOWAWCZE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> 
+(</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="7"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">słabe NT) 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">&lt;br&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">→ 18+ PC,  skład dowolny
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="7"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">(silne dowolne)
+uwaga: może też być licytowane przy zał że partner ma skład zrównoważony i jak powiem coś innego na co on spasuje (bez punktów) i ucieknie nam końcówka (np. na układzie 5-4 lub 6-4 – układy na dwóch piątkach raczej </t>
+    </r>
   </si>
 </sst>
 </file>
@@ -840,7 +1017,7 @@
     <numFmt numFmtId="165" formatCode="0"/>
     <numFmt numFmtId="166" formatCode="@"/>
   </numFmts>
-  <fonts count="16">
+  <fonts count="15">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -926,6 +1103,7 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="7"/>
@@ -935,13 +1113,6 @@
     </font>
     <font>
       <sz val="7"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="7"/>
-      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
@@ -1022,7 +1193,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1113,17 +1284,16 @@
   </sheetPr>
   <dimension ref="A1:M18"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J16" activeCellId="0" sqref="J16"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C21" activeCellId="0" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.1224489795918"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="10" min="3" style="0" width="10.1224489795918"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="43.7397959183673"/>
-    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="10.1224489795918"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="10" min="3" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="42.6581632653061"/>
+    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1837,4 +2007,193 @@
     <oddFooter/>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:M6"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="10" min="3" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="42.6581632653061"/>
+    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="8.50510204081633"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="102" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C2" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D2" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="G2" s="0" t="n">
+        <v>37</v>
+      </c>
+      <c r="H2" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="I2" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J2" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="L2" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="M2" s="3"/>
+    </row>
+    <row r="3" customFormat="false" ht="53.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C3" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="G3" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="H3" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="I3" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J3" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="L3" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="M3" s="3"/>
+    </row>
+    <row r="4" customFormat="false" ht="78.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C4" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D4" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E4" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G4" s="0" t="n">
+        <v>37</v>
+      </c>
+      <c r="H4" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="I4" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J4" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="L4" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="M4" s="3"/>
+    </row>
+    <row r="6" customFormat="false" ht="55.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Fixed bug (in data), added some comments
</commit_message>
<xml_diff>
--- a/bridgeIn.xlsx
+++ b/bridgeIn.xlsx
@@ -5,11 +5,11 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="W-J 2017" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="W-J 2013" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Other W-J" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="56">
   <si>
     <t xml:space="preserve">bidId</t>
   </si>
@@ -831,181 +831,6 @@
   </si>
   <si>
     <t xml:space="preserve">16PC+ na  5+ karo</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="7"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">→ 2013!!! (12)</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="7"/>
-        <color rgb="FFFF3333"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">15</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="7"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">-17</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="7"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve"> PC, 5+ trefl </t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="7"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">(naturalne, słaba piątka może też pasować na  1BA – patrz dalej)
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="7"/>
-        <color rgb="FFFF0066"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">&lt;br&gt;&lt;font color=red&gt;w wersji pro od 15 a nawet 16 PC!!! - słaby trefl wtedy do BA albo 1 karo (o ile jest 4 karo)&lt;/font&gt;
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="7"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">&lt;br&gt;→ 12-17 PC, układ 4414  tzw </t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="7"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">TRÓJKOLORÓWKA
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="7"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">(singiel karo)
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="7"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">&lt;br&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="7"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">→ 12-14 PC, skład bez atutowy  tzw. </t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="7"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">PRZYGOTOWAWCZE</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="7"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve"> 
-(</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="7"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">słabe NT) 
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="7"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">&lt;br&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="7"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">→ 18+ PC,  skład dowolny
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="7"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">(silne dowolne)
-uwaga: może też być licytowane przy zał że partner ma skład zrównoważony i jak powiem coś innego na co on spasuje (bez punktów) i ucieknie nam końcówka (np. na układzie 5-4 lub 6-4 – układy na dwóch piątkach raczej </t>
-    </r>
   </si>
 </sst>
 </file>
@@ -1284,8 +1109,8 @@
   </sheetPr>
   <dimension ref="A1:M18"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C21" activeCellId="0" sqref="C21"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -2016,16 +1841,13 @@
   </sheetPr>
   <dimension ref="A1:M6"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="10" min="3" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="42.6581632653061"/>
-    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2069,7 +1891,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="102" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="323" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
         <v>1</v>
       </c>
@@ -2101,14 +1923,14 @@
         <v>15</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>56</v>
+        <v>16</v>
       </c>
       <c r="L2" s="0" t="s">
         <v>17</v>
       </c>
       <c r="M2" s="3"/>
     </row>
-    <row r="3" customFormat="false" ht="53.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="170.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="n">
         <v>2</v>
       </c>
@@ -2147,7 +1969,7 @@
       </c>
       <c r="M3" s="3"/>
     </row>
-    <row r="4" customFormat="false" ht="78.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="282.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="n">
         <v>3</v>
       </c>
@@ -2186,14 +2008,91 @@
       </c>
       <c r="M4" s="3"/>
     </row>
-    <row r="6" customFormat="false" ht="55.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="5" customFormat="false" ht="129.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D5" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E5" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="F5" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="G5" s="0" t="n">
+        <v>37</v>
+      </c>
+      <c r="H5" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="I5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J5" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="L5" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="M5" s="3"/>
+    </row>
+    <row r="6" customFormat="false" ht="129.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C6" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D6" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E6" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="F6" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="G6" s="0" t="n">
+        <v>37</v>
+      </c>
+      <c r="H6" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="I6" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J6" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="L6" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="M6" s="3"/>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
+    <oddHeader>&amp;C&amp;"Times New Roman,Normalny"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normalny"&amp;12Strona &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
all possible opening - zero bid level
</commit_message>
<xml_diff>
--- a/bridgeIn.xlsx
+++ b/bridgeIn.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="781" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="33" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="W-J 2017" sheetId="1" state="visible" r:id="rId2"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="102">
   <si>
     <t>bidId</t>
   </si>
@@ -235,7 +235,7 @@
     </r>
   </si>
   <si>
-    <t>F</t>
+    <t>F1</t>
   </si>
   <si>
     <t>D</t>
@@ -305,6 +305,9 @@
   </si>
   <si>
     <t>S</t>
+  </si>
+  <si>
+    <t>Naturalna</t>
   </si>
   <si>
     <t>0+</t>
@@ -595,6 +598,9 @@
 dalej z innymi układami.</t>
   </si>
   <si>
+    <t>F</t>
+  </si>
+  <si>
     <t>7-10 na (5)6+ treflach</t>
   </si>
   <si>
@@ -772,7 +778,7 @@
     <t>(w wersji pro przed partią nawet 10-17) (wyklucza piątkę pików chyba że kierów jest więcej :), może być też dowolna młodsza piątka)</t>
   </si>
   <si>
-    <t>Open</t>
+    <t>NF</t>
   </si>
   <si>
     <r>
@@ -817,6 +823,9 @@
     </r>
   </si>
   <si>
+    <t>słaba</t>
+  </si>
+  <si>
     <t>6+</t>
   </si>
   <si>
@@ -829,13 +838,91 @@
     <t>x-5-X-X</t>
   </si>
   <si>
-    <t>DWUKOLORÓWKA</t>
-  </si>
-  <si>
-    <t>(6)7-10(11) PC, (przed partią nawet 4-9) dwie piątki: kierowa i dowolna /pikowa i młodsza Licytacja po interwencji przeciwnika Po interwencji przeciwnika kontry są karne, a nowy kolor pełni rolę „pa­suj lub popraw".  </t>
+    <t>DWUKOLORÓWKA na kierach i dowolny</t>
+  </si>
+  <si>
+    <t>(6)7-10(11) PC, (przed partią nawet 4-9) dwie piątki: kierowa i dowolna  Licytacja po interwencji przeciwnika Po interwencji przeciwnika kontry są karne, a nowy kolor pełni rolę „pa­suj lub popraw".  </t>
   </si>
   <si>
     <t>5-x-X-X</t>
+  </si>
+  <si>
+    <t>DWUKOLORÓWKA na pikach i ?</t>
+  </si>
+  <si>
+    <t>(6)7-10(11) PC, (przed partią nawet 4-9) dwie piątki: pikowa i młodsza Licytacja po interwencji przeciwnika Po interwencji przeciwnika kontry są karne, a nowy kolor pełni rolę „pa­suj lub popraw".  </t>
+  </si>
+  <si>
+    <t>'x-x-5-5</t>
+  </si>
+  <si>
+    <t>DWUKOLORÓWKA na Młodszych</t>
+  </si>
+  <si>
+    <t>2BA DWUKOLORÓWNA NA MŁODSZYCH  7-10(11) PC,  dwie młodsze piątki</t>
+  </si>
+  <si>
+    <t>7+</t>
+  </si>
+  <si>
+    <t>BLOK</t>
+  </si>
+  <si>
+    <t>(blokujące) (5)6-10 PC,  dobry licytowany kolor   7+ (przed partią może być dobre 6); w młodszym chętnie 8+ (lub dobry)</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>GAMBLINGg</t>
+  </si>
+  <si>
+    <t> Pełny 7-kartowy kolor młodszy  (AKDWxxx,AKDxxxxx)  bez dojścia w bocznym kolorze typu As lub Król</t>
+  </si>
+  <si>
+    <t>8-x-x-x</t>
+  </si>
+  <si>
+    <t>TEKSAS PDAF</t>
+  </si>
+  <si>
+    <t> lepiej naturalne (blok?)  ale jest dawna opcja TEKSAS POŁUDNIOWO AFRYKANSKI) mało PC 8+ w kolorze STARSZYM   pełny kolor MOCNE- (około 9 lew) </t>
+  </si>
+  <si>
+    <t>x-8-x-x</t>
+  </si>
+  <si>
+    <t>x-7-x-x</t>
+  </si>
+  <si>
+    <t>do 10 PC 7+ w kolorze licytowanym co najmniej dwie figury – dobry kolor!  (około 8 lew) Siła otwarcia i długość koloru atutowego zależy od stylu gracza i ustaleń w parze. Powinno się stosować metodę 4-3-2-2 (patrz **).</t>
+  </si>
+  <si>
+    <t>7-x-x-x</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>AS</t>
+  </si>
+  <si>
+    <t>pytanie o kolor Asa</t>
+  </si>
+  <si>
+    <t>8+</t>
+  </si>
+  <si>
+    <t> (6) do 10 PC 8+ w kolorze licytowanym co najmniej dwie figury  – dobry kolor!  (około 9 lew)</t>
+  </si>
+  <si>
+    <t>kompletna ręka w kolorze licytowanym BEZ Asa i Króla &lt;font color=red&gt; [chyba to znaczy wszystkie zatrzymania i 7+ kartowy kolor (11 lew) </t>
+  </si>
+  <si>
+    <t>inne</t>
+  </si>
+  <si>
+    <t>pełen kolor</t>
   </si>
 </sst>
 </file>
@@ -1121,12 +1208,12 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M25"/>
+  <dimension ref="A1:M51"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="525" topLeftCell="A10" activePane="bottomLeft" state="split"/>
+      <pane xSplit="0" ySplit="525" topLeftCell="B18" activePane="bottomLeft" state="split"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="H22" activeCellId="0" sqref="H22"/>
+      <selection pane="bottomLeft" activeCell="K41" activeCellId="0" sqref="K41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1255,7 +1342,9 @@
       <c r="L3" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="M3" s="3"/>
+      <c r="M3" s="3" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="56.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="n">
@@ -1280,21 +1369,23 @@
         <v>37</v>
       </c>
       <c r="H4" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="I4" s="0" t="n">
         <v>0</v>
       </c>
       <c r="J4" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="L4" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="M4" s="3"/>
+      <c r="M4" s="3" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="39.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="n">
@@ -1310,7 +1401,7 @@
         <v>1</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F5" s="0" t="n">
         <v>7</v>
@@ -1319,21 +1410,23 @@
         <v>37</v>
       </c>
       <c r="H5" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="I5" s="0" t="n">
         <v>0</v>
       </c>
       <c r="J5" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="L5" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="M5" s="3"/>
+      <c r="M5" s="3" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="44.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="n">
@@ -1358,16 +1451,16 @@
         <v>37</v>
       </c>
       <c r="H6" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="I6" s="0" t="n">
         <v>0</v>
       </c>
       <c r="J6" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="L6" s="0" t="s">
         <v>22</v>
@@ -1388,7 +1481,7 @@
         <v>1</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F7" s="0" t="n">
         <v>12</v>
@@ -1397,16 +1490,16 @@
         <v>17</v>
       </c>
       <c r="H7" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="I7" s="0" t="n">
         <v>0</v>
       </c>
       <c r="J7" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="K7" s="4" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="L7" s="0" t="s">
         <v>22</v>
@@ -1436,16 +1529,16 @@
         <v>18</v>
       </c>
       <c r="H8" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="I8" s="0" t="n">
         <v>0</v>
       </c>
       <c r="J8" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="K8" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="L8" s="0" t="s">
         <v>22</v>
@@ -1466,7 +1559,7 @@
         <v>1</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="F9" s="0" t="n">
         <v>18</v>
@@ -1475,16 +1568,16 @@
         <v>20</v>
       </c>
       <c r="H9" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="I9" s="0" t="n">
         <v>0</v>
       </c>
       <c r="J9" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="K9" s="5" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="L9" s="0" t="s">
         <v>22</v>
@@ -1505,7 +1598,7 @@
         <v>1</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F10" s="0" t="n">
         <v>0</v>
@@ -1514,16 +1607,16 @@
         <v>4</v>
       </c>
       <c r="H10" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="I10" s="0" t="n">
         <v>0</v>
       </c>
       <c r="J10" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="K10" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="L10" s="0" t="s">
         <v>22</v>
@@ -1544,7 +1637,7 @@
         <v>1</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="F11" s="0" t="n">
         <v>5</v>
@@ -1553,19 +1646,19 @@
         <v>8</v>
       </c>
       <c r="H11" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="I11" s="0" t="n">
         <v>0</v>
       </c>
       <c r="J11" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="K11" s="2" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="L11" s="0" t="s">
-        <v>17</v>
+        <v>46</v>
       </c>
       <c r="M11" s="3"/>
     </row>
@@ -1598,10 +1691,10 @@
         <v>0</v>
       </c>
       <c r="J12" s="5" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="K12" s="5" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="L12" s="0" t="s">
         <v>22</v>
@@ -1637,13 +1730,13 @@
         <v>0</v>
       </c>
       <c r="J13" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="K13" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="L13" s="0" t="s">
         <v>46</v>
-      </c>
-      <c r="K13" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="L13" s="0" t="s">
-        <v>17</v>
       </c>
       <c r="M13" s="3"/>
     </row>
@@ -1661,7 +1754,7 @@
         <v>2</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F14" s="0" t="n">
         <v>16</v>
@@ -1670,22 +1763,22 @@
         <v>37</v>
       </c>
       <c r="H14" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="I14" s="0" t="n">
         <v>0</v>
       </c>
       <c r="J14" s="6" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="K14" s="7" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="L14" s="0" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="M14" s="0" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="26.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1711,16 +1804,16 @@
         <v>37</v>
       </c>
       <c r="H15" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="I15" s="0" t="n">
         <v>0</v>
       </c>
       <c r="J15" s="8" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="K15" s="9" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="L15" s="0" t="s">
         <v>22</v>
@@ -1740,7 +1833,7 @@
         <v>2</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="F16" s="0" t="n">
         <v>16</v>
@@ -1749,16 +1842,16 @@
         <v>37</v>
       </c>
       <c r="H16" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="I16" s="0" t="n">
         <v>0</v>
       </c>
       <c r="J16" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="K16" s="2" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="L16" s="0" t="s">
         <v>22</v>
@@ -1793,10 +1886,10 @@
         <v>0</v>
       </c>
       <c r="J17" s="10" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="K17" s="10" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="L17" s="0" t="s">
         <v>22</v>
@@ -1831,13 +1924,13 @@
         <v>0</v>
       </c>
       <c r="J18" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="K18" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="L18" s="0" t="s">
-        <v>17</v>
+        <v>46</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1854,7 +1947,7 @@
         <v>1</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F19" s="0" t="n">
         <v>12</v>
@@ -1869,13 +1962,13 @@
         <v>0</v>
       </c>
       <c r="J19" s="0" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="K19" s="11" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="L19" s="0" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1907,10 +2000,13 @@
         <v>0</v>
       </c>
       <c r="J20" s="0" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="K20" s="11" t="s">
-        <v>59</v>
+        <v>61</v>
+      </c>
+      <c r="L20" s="0" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1927,7 +2023,7 @@
         <v>1</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="F21" s="0" t="n">
         <v>15</v>
@@ -1936,16 +2032,19 @@
         <v>17</v>
       </c>
       <c r="H21" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="I21" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J21" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="K21" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="L21" s="0" t="s">
         <v>60</v>
-      </c>
-      <c r="I21" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="J21" s="0" t="s">
-        <v>61</v>
-      </c>
-      <c r="K21" s="10" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1971,16 +2070,22 @@
         <v>16</v>
       </c>
       <c r="H22" s="0" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="I22" s="0" t="n">
         <v>0</v>
       </c>
       <c r="J22" s="0" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="K22" s="9" t="s">
-        <v>65</v>
+        <v>67</v>
+      </c>
+      <c r="L22" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="M22" s="0" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2006,15 +2111,21 @@
         <v>11</v>
       </c>
       <c r="H23" s="0" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="I23" s="0" t="n">
         <v>0</v>
       </c>
       <c r="J23" s="0" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="K23" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="L23" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="M23" s="0" t="s">
         <v>68</v>
       </c>
     </row>
@@ -2032,7 +2143,7 @@
         <v>2</v>
       </c>
       <c r="E24" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F24" s="0" t="n">
         <v>7</v>
@@ -2041,16 +2152,22 @@
         <v>11</v>
       </c>
       <c r="H24" s="0" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="I24" s="0" t="n">
         <v>0</v>
       </c>
       <c r="J24" s="0" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="K24" s="0" t="s">
-        <v>71</v>
+        <v>74</v>
+      </c>
+      <c r="L24" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="M24" s="0" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2076,13 +2193,936 @@
         <v>11</v>
       </c>
       <c r="H25" s="0" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="I25" s="0" t="n">
         <v>0</v>
       </c>
       <c r="J25" s="0" t="s">
-        <v>70</v>
+        <v>76</v>
+      </c>
+      <c r="K25" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="L25" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="M25" s="0" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="B26" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C26" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D26" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="E26" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="F26" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="G26" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="H26" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="I26" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J26" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="K26" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="L26" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="M26" s="0" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="n">
+        <v>26</v>
+      </c>
+      <c r="B27" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C27" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D27" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="E27" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="F27" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="G27" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="H27" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="I27" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J27" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="K27" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="L27" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="M27" s="0" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="n">
+        <v>27</v>
+      </c>
+      <c r="B28" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C28" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D28" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="E28" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="F28" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="G28" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="H28" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="I28" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J28" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="K28" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="L28" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="M28" s="0" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="B29" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C29" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D29" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="E29" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="F29" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="G29" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="H29" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="I29" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J29" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="K29" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="L29" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="M29" s="0" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0" t="n">
+        <v>29</v>
+      </c>
+      <c r="B30" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C30" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D30" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="E30" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="F30" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="G30" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="H30" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="I30" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J30" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="K30" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="L30" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="M30" s="0" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="B31" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C31" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D31" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="E31" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="F31" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="G31" s="0" t="n">
+        <f aca="false">F31+13</f>
+        <v>22</v>
+      </c>
+      <c r="H31" s="0" t="s">
+        <v>84</v>
+      </c>
+      <c r="I31" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J31" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="K31" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="L31" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="M31" s="0" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="0" t="n">
+        <v>31</v>
+      </c>
+      <c r="B32" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C32" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D32" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="E32" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="F32" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G32" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H32" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="I32" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J32" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="K32" s="0" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="0" t="n">
+        <v>32</v>
+      </c>
+      <c r="B33" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C33" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D33" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="E33" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="F33" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G33" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H33" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="I33" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J33" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="K33" s="0" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="0" t="n">
+        <v>33</v>
+      </c>
+      <c r="B34" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C34" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D34" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="E34" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="F34" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G34" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="H34" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="I34" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J34" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="K34" s="0" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="0" t="n">
+        <v>34</v>
+      </c>
+      <c r="B35" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C35" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D35" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="E35" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="F35" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G35" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="H35" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="I35" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J35" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="K35" s="0" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="0" t="n">
+        <v>35</v>
+      </c>
+      <c r="B36" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C36" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D36" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="E36" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="F36" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="G36" s="0" t="n">
+        <v>32</v>
+      </c>
+      <c r="H36" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="I36" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J36" s="0" t="s">
+        <v>95</v>
+      </c>
+      <c r="K36" s="0" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="0" t="n">
+        <v>36</v>
+      </c>
+      <c r="B37" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C37" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D37" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="E37" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="F37" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="G37" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="H37" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="I37" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J37" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="K37" s="0" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="0" t="n">
+        <v>37</v>
+      </c>
+      <c r="B38" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C38" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D38" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="E38" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="F38" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="G38" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="H38" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="I38" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J38" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="K38" s="0" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="0" t="n">
+        <v>38</v>
+      </c>
+      <c r="B39" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C39" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D39" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="E39" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="F39" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G39" s="0" t="n">
+        <v>37</v>
+      </c>
+      <c r="H39" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="I39" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J39" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="K39" s="0" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="0" t="n">
+        <v>39</v>
+      </c>
+      <c r="B40" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C40" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D40" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="E40" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="F40" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G40" s="0" t="n">
+        <v>37</v>
+      </c>
+      <c r="H40" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="I40" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J40" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="K40" s="0" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="0" t="n">
+        <v>40</v>
+      </c>
+      <c r="B41" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C41" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D41" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="E41" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="F41" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G41" s="0" t="n">
+        <v>37</v>
+      </c>
+      <c r="H41" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="I41" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J41" s="0" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="0" t="n">
+        <v>41</v>
+      </c>
+      <c r="B42" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C42" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D42" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="E42" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="F42" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G42" s="0" t="n">
+        <v>37</v>
+      </c>
+      <c r="H42" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="I42" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J42" s="0" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="0" t="n">
+        <v>42</v>
+      </c>
+      <c r="B43" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C43" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D43" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="E43" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="F43" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G43" s="0" t="n">
+        <v>37</v>
+      </c>
+      <c r="H43" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="I43" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J43" s="0" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="0" t="n">
+        <v>43</v>
+      </c>
+      <c r="B44" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C44" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D44" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="E44" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="F44" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G44" s="0" t="n">
+        <v>37</v>
+      </c>
+      <c r="H44" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="I44" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J44" s="0" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="0" t="n">
+        <v>44</v>
+      </c>
+      <c r="B45" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C45" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D45" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="E45" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="F45" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G45" s="0" t="n">
+        <v>37</v>
+      </c>
+      <c r="H45" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="I45" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J45" s="0" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="0" t="n">
+        <v>45</v>
+      </c>
+      <c r="B46" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C46" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D46" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="E46" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="F46" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G46" s="0" t="n">
+        <v>37</v>
+      </c>
+      <c r="H46" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="I46" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J46" s="0" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="0" t="n">
+        <v>46</v>
+      </c>
+      <c r="B47" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C47" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D47" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="E47" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="F47" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="G47" s="0" t="n">
+        <v>37</v>
+      </c>
+      <c r="H47" s="0" t="s">
+        <v>101</v>
+      </c>
+      <c r="I47" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J47" s="0" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="0" t="n">
+        <v>47</v>
+      </c>
+      <c r="B48" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C48" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D48" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="E48" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="F48" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="G48" s="0" t="n">
+        <v>37</v>
+      </c>
+      <c r="H48" s="0" t="s">
+        <v>101</v>
+      </c>
+      <c r="I48" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J48" s="0" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="0" t="n">
+        <v>48</v>
+      </c>
+      <c r="B49" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C49" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D49" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="E49" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="F49" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="G49" s="0" t="n">
+        <v>37</v>
+      </c>
+      <c r="H49" s="0" t="s">
+        <v>101</v>
+      </c>
+      <c r="I49" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J49" s="0" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="0" t="n">
+        <v>49</v>
+      </c>
+      <c r="B50" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C50" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D50" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="E50" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="F50" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="G50" s="0" t="n">
+        <v>37</v>
+      </c>
+      <c r="H50" s="0" t="s">
+        <v>101</v>
+      </c>
+      <c r="I50" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J50" s="0" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="B51" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C51" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D51" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="E51" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="F51" s="0" t="n">
+        <v>22</v>
+      </c>
+      <c r="G51" s="0" t="n">
+        <v>37</v>
+      </c>
+      <c r="H51" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="I51" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J51" s="0" t="s">
+        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -2190,7 +3230,7 @@
         <v>16</v>
       </c>
       <c r="L2" s="0" t="s">
-        <v>17</v>
+        <v>46</v>
       </c>
       <c r="M2" s="3"/>
     </row>
@@ -2256,16 +3296,16 @@
         <v>37</v>
       </c>
       <c r="H4" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="I4" s="0" t="n">
         <v>0</v>
       </c>
       <c r="J4" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="L4" s="0" t="s">
         <v>22</v>
@@ -2286,7 +3326,7 @@
         <v>1</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F5" s="0" t="n">
         <v>7</v>
@@ -2295,16 +3335,16 @@
         <v>37</v>
       </c>
       <c r="H5" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="I5" s="0" t="n">
         <v>0</v>
       </c>
       <c r="J5" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="L5" s="0" t="s">
         <v>22</v>
@@ -2334,16 +3374,16 @@
         <v>37</v>
       </c>
       <c r="H6" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="I6" s="0" t="n">
         <v>0</v>
       </c>
       <c r="J6" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="L6" s="0" t="s">
         <v>22</v>

</xml_diff>

<commit_message>
descirbe which person is bidding (not good name (gracz N and gracz S) and it will be better above table but how?
 some other small corection
</commit_message>
<xml_diff>
--- a/bridgeIn.xlsx
+++ b/bridgeIn.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2067" uniqueCount="365">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2067" uniqueCount="367">
   <si>
     <t>bidId</t>
   </si>
@@ -1592,7 +1592,7 @@
     <t>5-3-3-2 lub 4-4-3-2</t>
   </si>
   <si>
-    <t>Naturalne bez Atu</t>
+    <t>Naturalne BA</t>
   </si>
   <si>
     <t>skład zrównoważony bez krótkości, bez starszej piątki, otwarcie może zawierać piątkę młodszą (wyjątkowo również bardzo słabą starszą) układy 5-3-3-2 4-4-3-2 itp. Po interwencji opozycji obowiązują dalej Stayman i transfery z wykorzystaniem odzywek opozycji.</t>
@@ -1601,7 +1601,7 @@
     <t>xxx6 lub XXx5</t>
   </si>
   <si>
-    <t>PRESSIOSION</t>
+    <t>PRESSISION</t>
   </si>
   <si>
     <r>
@@ -1628,7 +1628,7 @@
     <t>x-5-X-X</t>
   </si>
   <si>
-    <t>DWUKOLORÓWKA na kierach i dowolny</t>
+    <t>DWUKOLORÓWKA  5+ kier i 5+ młodszy</t>
   </si>
   <si>
     <t>(6)7-10(11) PC, (przed partią nawet 4-9) dwie piątki: kierowa i dowolna  Licytacja po interwencji przeciwnika Po interwencji przeciwnika kontry są karne, a nowy kolor pełni rolę „pa­suj lub popraw".</t>
@@ -1637,7 +1637,7 @@
     <t>5-x-X-X</t>
   </si>
   <si>
-    <t>DWUKOLORÓWKA na pikach i ?</t>
+    <t>DWUKOLORÓWKA 5+ pik i 5+ dowolny</t>
   </si>
   <si>
     <t>(6)7-10(11) PC, (przed partią nawet 4-9) dwie piątki: pikowa i młodsza Licytacja po interwencji przeciwnika Po interwencji przeciwnika kontry są karne, a nowy kolor pełni rolę „pa­suj lub popraw".</t>
@@ -1655,34 +1655,37 @@
     <t>7+</t>
   </si>
   <si>
+    <t>BLOK słaby</t>
+  </si>
+  <si>
+    <t>(blokujące) (5)6-10 PC,  dobry licytowany kolor   7+ (przed partią może być dobre 6); w młodszym chętnie 8+ (lub dobry)</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>GAMBLING</t>
+  </si>
+  <si>
+    <t>Pełny 7-kartowy kolor młodszy  (AKDWxxx,AKDxxxxx)  bez dojścia w bocznym kolorze typu As lub Król</t>
+  </si>
+  <si>
+    <t>8-x-x-x</t>
+  </si>
+  <si>
+    <t>TEKSAS PDAF</t>
+  </si>
+  <si>
+    <t>lepiej naturalne (blok?)  ale jest dawna opcja TEKSAS POŁUDNIOWO AFRYKANSKI) mało PC 8+ w kolorze STARSZYM   pełny kolor MOCNE- (około 9 lew)</t>
+  </si>
+  <si>
+    <t>x-8-x-x</t>
+  </si>
+  <si>
+    <t>x-7-x-x</t>
+  </si>
+  <si>
     <t>BLOK</t>
-  </si>
-  <si>
-    <t>(blokujące) (5)6-10 PC,  dobry licytowany kolor   7+ (przed partią może być dobre 6); w młodszym chętnie 8+ (lub dobry)</t>
-  </si>
-  <si>
-    <t>7</t>
-  </si>
-  <si>
-    <t>GAMBLINGg</t>
-  </si>
-  <si>
-    <t>Pełny 7-kartowy kolor młodszy  (AKDWxxx,AKDxxxxx)  bez dojścia w bocznym kolorze typu As lub Król</t>
-  </si>
-  <si>
-    <t>8-x-x-x</t>
-  </si>
-  <si>
-    <t>TEKSAS PDAF</t>
-  </si>
-  <si>
-    <t>lepiej naturalne (blok?)  ale jest dawna opcja TEKSAS POŁUDNIOWO AFRYKANSKI) mało PC 8+ w kolorze STARSZYM   pełny kolor MOCNE- (około 9 lew)</t>
-  </si>
-  <si>
-    <t>x-8-x-x</t>
-  </si>
-  <si>
-    <t>x-7-x-x</t>
   </si>
   <si>
     <t>do 10 PC 7+ w kolorze licytowanym co najmniej dwie figury – dobry kolor!  (około 8 lew) Siła otwarcia i długość koloru atutowego zależy od stylu gracza i ustaleń w parze. Powinno się stosować metodę 4-3-2-2 (patrz **).</t>
@@ -1817,6 +1820,9 @@
   </si>
   <si>
     <t>6+ PC, 5+ trefli, wyklucza 4 kara, 4 kiery, 4 piki;</t>
+  </si>
+  <si>
+    <t>Naturalne bez Atu</t>
   </si>
 </sst>
 </file>
@@ -2427,9 +2433,9 @@
   <dimension ref="A1:M306"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="525" topLeftCell="A10" activePane="bottomLeft" state="split"/>
+      <pane xSplit="0" ySplit="525" topLeftCell="A280" activePane="bottomLeft" state="split"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="K22" activeCellId="0" sqref="K22"/>
+      <selection pane="bottomLeft" activeCell="J292" activeCellId="0" sqref="J292"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -14489,7 +14495,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="288" customFormat="false" ht="23.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="288" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A288" s="0" t="n">
         <v>287</v>
       </c>
@@ -14917,10 +14923,10 @@
         <v>13</v>
       </c>
       <c r="F298" s="3" t="n">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="G298" s="3" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="H298" s="3" t="s">
         <v>331</v>
@@ -14958,10 +14964,10 @@
         <v>19</v>
       </c>
       <c r="F299" s="3" t="n">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="G299" s="3" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="H299" s="3" t="s">
         <v>334</v>
@@ -14999,7 +15005,7 @@
         <v>22</v>
       </c>
       <c r="F300" s="3" t="n">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="G300" s="3" t="n">
         <v>10</v>
@@ -15011,10 +15017,10 @@
         <v>0</v>
       </c>
       <c r="J300" s="5" t="s">
-        <v>326</v>
+        <v>336</v>
       </c>
       <c r="K300" s="6" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="L300" s="3" t="s">
         <v>108</v>
@@ -15040,22 +15046,22 @@
         <v>31</v>
       </c>
       <c r="F301" s="3" t="n">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="G301" s="3" t="n">
         <v>10</v>
       </c>
       <c r="H301" s="3" t="s">
+        <v>338</v>
+      </c>
+      <c r="I301" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="J301" s="5" t="s">
+        <v>336</v>
+      </c>
+      <c r="K301" s="6" t="s">
         <v>337</v>
-      </c>
-      <c r="I301" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="J301" s="5" t="s">
-        <v>326</v>
-      </c>
-      <c r="K301" s="6" t="s">
-        <v>336</v>
       </c>
       <c r="L301" s="3" t="s">
         <v>108</v>
@@ -15093,10 +15099,10 @@
         <v>0</v>
       </c>
       <c r="J302" s="5" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="K302" s="6" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="L302" s="3" t="s">
         <v>108</v>
@@ -15128,16 +15134,16 @@
         <v>10</v>
       </c>
       <c r="H303" s="3" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="I303" s="4" t="n">
         <v>0</v>
       </c>
       <c r="J303" s="5" t="s">
-        <v>326</v>
+        <v>336</v>
       </c>
       <c r="K303" s="6" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="L303" s="3" t="s">
         <v>108</v>
@@ -15169,16 +15175,16 @@
         <v>10</v>
       </c>
       <c r="H304" s="3" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="I304" s="4" t="n">
         <v>0</v>
       </c>
       <c r="J304" s="5" t="s">
-        <v>326</v>
+        <v>336</v>
       </c>
       <c r="K304" s="6" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="L304" s="3" t="s">
         <v>108</v>
@@ -15216,10 +15222,10 @@
         <v>0</v>
       </c>
       <c r="J305" s="5" t="s">
-        <v>326</v>
+        <v>336</v>
       </c>
       <c r="K305" s="6" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="L305" s="3" t="s">
         <v>108</v>
@@ -15257,10 +15263,10 @@
         <v>0</v>
       </c>
       <c r="J306" s="5" t="s">
-        <v>326</v>
+        <v>336</v>
       </c>
       <c r="K306" s="6" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="L306" s="3" t="s">
         <v>108</v>
@@ -15366,10 +15372,10 @@
         <v>0</v>
       </c>
       <c r="J2" s="0" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="K2" s="77" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="L2" s="0" t="s">
         <v>31</v>
@@ -15408,10 +15414,10 @@
         <v>1</v>
       </c>
       <c r="J3" s="0" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="K3" s="77" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="L3" s="0" t="s">
         <v>31</v>
@@ -15449,10 +15455,10 @@
         <v>1</v>
       </c>
       <c r="J4" s="0" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="K4" s="77" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="L4" s="0" t="s">
         <v>31</v>
@@ -15490,10 +15496,10 @@
         <v>1</v>
       </c>
       <c r="J5" s="0" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="K5" s="77" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="L5" s="0" t="s">
         <v>31</v>
@@ -15601,10 +15607,10 @@
         <v>0</v>
       </c>
       <c r="J2" s="0" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="K2" s="77" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="L2" s="0" t="s">
         <v>80</v>
@@ -15679,10 +15685,10 @@
         <v>0</v>
       </c>
       <c r="J4" s="0" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="K4" s="77" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="L4" s="0" t="s">
         <v>31</v>
@@ -15718,10 +15724,10 @@
         <v>0</v>
       </c>
       <c r="J5" s="0" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="K5" s="77" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="L5" s="0" t="s">
         <v>31</v>
@@ -15760,7 +15766,7 @@
         <v>253</v>
       </c>
       <c r="K6" s="77" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="L6" s="0" t="s">
         <v>31</v>
@@ -15868,16 +15874,16 @@
         <v>21</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="I2" s="4" t="n">
         <v>0</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="K2" s="6" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="L2" s="3" t="s">
         <v>17</v>
@@ -15916,10 +15922,10 @@
         <v>0</v>
       </c>
       <c r="J3" s="12" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="K3" s="13" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="L3" s="10" t="s">
         <v>108</v>
@@ -15958,10 +15964,10 @@
         <v>0</v>
       </c>
       <c r="J4" s="12" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="K4" s="13" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="L4" s="10" t="s">
         <v>108</v>
@@ -16000,10 +16006,10 @@
         <v>0</v>
       </c>
       <c r="J5" s="12" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="K5" s="13" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="L5" s="10" t="s">
         <v>108</v>
@@ -16044,7 +16050,7 @@
         <v>101</v>
       </c>
       <c r="K6" s="12" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="L6" s="10" t="s">
         <v>108</v>
@@ -16085,7 +16091,7 @@
         <v>263</v>
       </c>
       <c r="K7" s="12" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="L7" s="10" t="s">
         <v>108</v>
@@ -16195,13 +16201,13 @@
         <v>21</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="I10" s="4" t="n">
         <v>0</v>
       </c>
       <c r="J10" s="5" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="K10" s="6"/>
       <c r="L10" s="3" t="s">
@@ -16318,7 +16324,7 @@
         <v>0</v>
       </c>
       <c r="J13" s="5" t="s">
-        <v>309</v>
+        <v>366</v>
       </c>
       <c r="K13" s="6"/>
       <c r="L13" s="3" t="s">
@@ -16394,7 +16400,7 @@
         <v>0</v>
       </c>
       <c r="J15" s="5" t="s">
-        <v>326</v>
+        <v>336</v>
       </c>
       <c r="K15" s="5"/>
       <c r="L15" s="3" t="s">
@@ -16433,7 +16439,7 @@
         <v>0</v>
       </c>
       <c r="J16" s="5" t="s">
-        <v>326</v>
+        <v>336</v>
       </c>
       <c r="K16" s="5"/>
       <c r="L16" s="3" t="s">
@@ -16472,7 +16478,7 @@
         <v>0</v>
       </c>
       <c r="J17" s="5" t="s">
-        <v>326</v>
+        <v>336</v>
       </c>
       <c r="K17" s="5"/>
       <c r="L17" s="3" t="s">
@@ -16550,7 +16556,7 @@
         <v>0</v>
       </c>
       <c r="J19" s="5" t="s">
-        <v>326</v>
+        <v>336</v>
       </c>
       <c r="K19" s="6"/>
       <c r="L19" s="3" t="s">
@@ -16589,7 +16595,7 @@
         <v>0</v>
       </c>
       <c r="J20" s="5" t="s">
-        <v>326</v>
+        <v>336</v>
       </c>
       <c r="K20" s="6"/>
       <c r="L20" s="3" t="s">
@@ -16628,7 +16634,7 @@
         <v>0</v>
       </c>
       <c r="J21" s="5" t="s">
-        <v>326</v>
+        <v>336</v>
       </c>
       <c r="K21" s="6"/>
       <c r="L21" s="3" t="s">
@@ -16667,7 +16673,7 @@
         <v>0</v>
       </c>
       <c r="J22" s="5" t="s">
-        <v>326</v>
+        <v>336</v>
       </c>
       <c r="K22" s="6"/>
       <c r="L22" s="3" t="s">
@@ -16739,13 +16745,13 @@
         <v>12</v>
       </c>
       <c r="H24" s="3" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="I24" s="4" t="n">
         <v>0</v>
       </c>
       <c r="J24" s="5" t="s">
-        <v>326</v>
+        <v>336</v>
       </c>
       <c r="K24" s="6"/>
       <c r="L24" s="3" t="s">
@@ -16778,13 +16784,13 @@
         <v>12</v>
       </c>
       <c r="H25" s="3" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="I25" s="4" t="n">
         <v>0</v>
       </c>
       <c r="J25" s="5" t="s">
-        <v>326</v>
+        <v>336</v>
       </c>
       <c r="K25" s="6"/>
       <c r="L25" s="3" t="s">
@@ -16817,13 +16823,13 @@
         <v>12</v>
       </c>
       <c r="H26" s="3" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="I26" s="4" t="n">
         <v>0</v>
       </c>
       <c r="J26" s="5" t="s">
-        <v>326</v>
+        <v>336</v>
       </c>
       <c r="K26" s="6"/>
       <c r="L26" s="3" t="s">
@@ -16856,13 +16862,13 @@
         <v>12</v>
       </c>
       <c r="H27" s="3" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="I27" s="4" t="n">
         <v>0</v>
       </c>
       <c r="J27" s="5" t="s">
-        <v>326</v>
+        <v>336</v>
       </c>
       <c r="K27" s="6"/>
       <c r="L27" s="3" t="s">

</xml_diff>

<commit_message>
opening 1 diamonds (lower part) withou 1H/1S
</commit_message>
<xml_diff>
--- a/bridgeIn.xlsx
+++ b/bridgeIn.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="781" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="544" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="W-J 2017" sheetId="1" state="visible" r:id="rId2"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2067" uniqueCount="368">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2247" uniqueCount="421">
   <si>
     <t>bidId</t>
   </si>
@@ -1561,9 +1561,171 @@
       <t xml:space="preserve"> 1BA – patrz dalej)
 &lt;br&gt;12-17PC układ na czwórkach w tym karowa  
 TRÓJKOLORÓWKA (czyli to co drugie znaczenie trefla tylko z singlem innym niż karo)
-&lt;br&gt;&lt;br&gt;&lt;font color=red&gt;opcjonalnie układ na piątce trefl i czwórce karo? 
+&lt;br&gt;&lt;br&gt;&lt;font color=green&gt;opcjonalnie układ na piątce trefl i czwórce karo? 
 12-14 PC (inaczej to wchodzi do trefla)&lt;/font&gt;</t>
     </r>
+  </si>
+  <si>
+    <t>Brak 4 kar</t>
+  </si>
+  <si>
+    <t>pas</t>
+  </si>
+  <si>
+    <t>nic ciekawego – patrz 3 kara...</t>
+  </si>
+  <si>
+    <t>7+ PC,  4 +  kierów/pików ; przy dwóch czwórkach kierowa, przy dwóch piątkach pikowa;  forsuje na jedno okrążenie</t>
+  </si>
+  <si>
+    <t>czwórka w pikach</t>
+  </si>
+  <si>
+    <t>brak 4s</t>
+  </si>
+  <si>
+    <t> 7-9(10) PC, bez starszej czwórki, nie forsuje</t>
+  </si>
+  <si>
+    <t>5+ kar i 4+ trefl</t>
+  </si>
+  <si>
+    <t>kara i trefle</t>
+  </si>
+  <si>
+    <t>12-14 PC   5+ kar i  4+  trefl .(w wersji opcjonalnej też z 5 trefli i czwórką karo przy 12-17 PC oraz na dwóch piątkach młodszych 12-14PC)</t>
+  </si>
+  <si>
+    <t>6+, brak 4s</t>
+  </si>
+  <si>
+    <t>kara bez starszej</t>
+  </si>
+  <si>
+    <t> 12-14 PC, 6+ kar, możliwe trefle, starsza czwórka wykluczona </t>
+  </si>
+  <si>
+    <t>4 kiery 5+kar</t>
+  </si>
+  <si>
+    <t>kara i kiery</t>
+  </si>
+  <si>
+    <t>15-17 PC  4 w kolor, 5+ kar</t>
+  </si>
+  <si>
+    <t>4 piki 5+kar</t>
+  </si>
+  <si>
+    <t>kara i piki</t>
+  </si>
+  <si>
+    <t>5+, 5+ na młodszych</t>
+  </si>
+  <si>
+    <t>15-17 PC, układ 5+-5+ na kolorach młodszych</t>
+  </si>
+  <si>
+    <t>6 kar</t>
+  </si>
+  <si>
+    <t>sześć kar</t>
+  </si>
+  <si>
+    <t>15-17 PC, 6 kar z dwiema starszymi figurami, forsing</t>
+  </si>
+  <si>
+    <t>10 (12)+ PC, 5+-trefli,nie wyklucza starszej czwórki, forsuje na jedno okrążenie</t>
+  </si>
+  <si>
+    <t>kara</t>
+  </si>
+  <si>
+    <t>12-14 PC – 5+ kar</t>
+  </si>
+  <si>
+    <t>5+kar i 4 kiery</t>
+  </si>
+  <si>
+    <t>15-17  PC –5+kar 4 w kolor</t>
+  </si>
+  <si>
+    <t>5+ kar i 4 piki</t>
+  </si>
+  <si>
+    <t>4-4-4-1</t>
+  </si>
+  <si>
+    <t>układ na czwórkach</t>
+  </si>
+  <si>
+    <t>(RELAY) 15-17  PC 4-4-4-1 (singiel trefl)</t>
+  </si>
+  <si>
+    <t>5+ kar i 4 trefle</t>
+  </si>
+  <si>
+    <t>15-17 PC – 5+ kar oraz  4+trefl</t>
+  </si>
+  <si>
+    <t>15-17 PC –6+kar</t>
+  </si>
+  <si>
+    <t>5+ kar, 4 trefle i krótkość</t>
+  </si>
+  <si>
+    <t>15-17  PC –5+ kar,  4trefle oraz krótkość w kolor  SPLINTER</t>
+  </si>
+  <si>
+    <t>(RELAY) –12-14 PC  4-4-4-1 </t>
+  </si>
+  <si>
+    <t>3+ kara brak 4s</t>
+  </si>
+  <si>
+    <t>12+  PC, fit (3+), brak starszej czwórki, ze względu na krótkość nie nadająca się do zalicytowania 1BA</t>
+  </si>
+  <si>
+    <t>12+  PC,  5+-kierów/pików, forsing do końcówki</t>
+  </si>
+  <si>
+    <t>11-12 PC, bez starszej czwórki, nie forsuje (jest to inwit do 3BA)</t>
+  </si>
+  <si>
+    <t>4+ kar bez 4s</t>
+  </si>
+  <si>
+    <t>9-11 PC, fit (4+ kar), brak starszej czwórki, inwit do 3BA</t>
+  </si>
+  <si>
+    <t>4+ kara</t>
+  </si>
+  <si>
+    <t>BLOK</t>
+  </si>
+  <si>
+    <t>7-9 PC (wersja pro 0-6PC), fit (4+ kar), blok</t>
+  </si>
+  <si>
+    <t>BL</t>
+  </si>
+  <si>
+    <t>4+ kara i krótkość w kolorze</t>
+  </si>
+  <si>
+    <t>12-15  PC,  4+KARA i krótkość w kierach/ pikach SPLINTER forsing do końcówki</t>
+  </si>
+  <si>
+    <t>bez 4s i 5m</t>
+  </si>
+  <si>
+    <t> (12)13-16 PC, bez starszej czwórki i młodszej piątki – do gry</t>
+  </si>
+  <si>
+    <t>4+ kara i singiel terfl</t>
+  </si>
+  <si>
+    <t>12-15  PC,  4+KARA i krótkość w   SPLINTER forsing do końcówki</t>
   </si>
   <si>
     <t>Naturalne 1 kier</t>
@@ -1658,9 +1820,6 @@
     <t>(blokujące) (5)6-10 PC,  dobry licytowany kolor   7+ (przed partią może być dobre 6); w młodszym chętnie 8+ (lub dobry)</t>
   </si>
   <si>
-    <t>BL</t>
-  </si>
-  <si>
     <t>7</t>
   </si>
   <si>
@@ -1683,9 +1842,6 @@
   </si>
   <si>
     <t>x-7-x-x</t>
-  </si>
-  <si>
-    <t>BLOK</t>
   </si>
   <si>
     <t>do 10 PC 7+ w kolorze licytowanym co najmniej dwie figury – dobry kolor!  (około 8 lew) Siła otwarcia i długość koloru atutowego zależy od stylu gracza i ustaleń w parze. Powinno się stosować metodę 4-3-2-2 (patrz **).</t>
@@ -1747,6 +1903,24 @@
   </si>
   <si>
     <t>F</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">12-17 PC, 5+ kar (naturalne ale  uwaga na </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> 1BA – patrz dalej)
+&lt;br&gt;12-17PC układ na czwórkach w tym karowa  
+TRÓJKOLORÓWKA (czyli to co drugie znaczenie trefla tylko z singlem innym niż karo)
+&lt;br&gt;&lt;br&gt;&lt;font color=red&gt;opcjonalnie układ na piątce trefl i czwórce karo? 
+12-14 PC (inaczej to wchodzi do trefla)&lt;/font&gt;</t>
+    </r>
   </si>
   <si>
     <t>Trójznaczne forsuje na 1 okrążenie</t>
@@ -2433,12 +2607,12 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M306"/>
+  <dimension ref="A1:M336"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="525" topLeftCell="A282" activePane="bottomLeft" state="split"/>
-      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
-      <selection pane="bottomLeft" activeCell="J299" activeCellId="0" sqref="J299"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="525" topLeftCell="A278" activePane="bottomLeft" state="split"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="L291" activeCellId="0" sqref="L291"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -14334,7 +14508,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="284" customFormat="false" ht="55.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="284" customFormat="false" ht="82.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A284" s="0" t="n">
         <v>283</v>
       </c>
@@ -14379,40 +14553,41 @@
       <c r="A285" s="0" t="n">
         <v>284</v>
       </c>
-      <c r="B285" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="C285" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="D285" s="1" t="n">
+      <c r="B285" s="8" t="n">
+        <f aca="false">A$284</f>
+        <v>283</v>
+      </c>
+      <c r="C285" s="8" t="n">
         <v>1</v>
       </c>
-      <c r="E285" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F285" s="3" t="n">
-        <v>12</v>
-      </c>
-      <c r="G285" s="3" t="n">
-        <v>17</v>
-      </c>
-      <c r="H285" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="I285" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="J285" s="5" t="s">
+      <c r="D285" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="E285" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="F285" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="G285" s="10" t="n">
+        <v>6</v>
+      </c>
+      <c r="H285" s="10" t="s">
         <v>304</v>
       </c>
-      <c r="K285" s="6" t="s">
+      <c r="I285" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="J285" s="12" t="s">
         <v>305</v>
       </c>
-      <c r="L285" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="M285" s="3" t="s">
+      <c r="K285" s="13" t="s">
+        <v>306</v>
+      </c>
+      <c r="L285" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="M285" s="14" t="s">
         <v>62</v>
       </c>
     </row>
@@ -14420,656 +14595,671 @@
       <c r="A286" s="0" t="n">
         <v>285</v>
       </c>
-      <c r="B286" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="C286" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="D286" s="1" t="n">
+      <c r="B286" s="8" t="n">
+        <f aca="false">A$284</f>
+        <v>283</v>
+      </c>
+      <c r="C286" s="8" t="n">
         <v>1</v>
       </c>
-      <c r="E286" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="F286" s="3" t="n">
-        <v>12</v>
-      </c>
-      <c r="G286" s="3" t="n">
+      <c r="D286" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="E286" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="F286" s="10" t="n">
+        <v>7</v>
+      </c>
+      <c r="G286" s="10" t="n">
+        <v>37</v>
+      </c>
+      <c r="H286" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="I286" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="J286" s="12" t="s">
+        <v>235</v>
+      </c>
+      <c r="K286" s="13" t="s">
+        <v>307</v>
+      </c>
+      <c r="L286" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="H286" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="I286" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="J286" s="5" t="s">
-        <v>304</v>
-      </c>
-      <c r="K286" s="6" t="s">
-        <v>306</v>
-      </c>
-      <c r="L286" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="M286" s="3" t="s">
+      <c r="M286" s="14" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="287" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="287" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A287" s="0" t="n">
         <v>286</v>
       </c>
-      <c r="B287" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="C287" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="D287" s="1" t="n">
+      <c r="B287" s="8" t="n">
+        <f aca="false">A$284</f>
+        <v>283</v>
+      </c>
+      <c r="C287" s="8" t="n">
         <v>1</v>
       </c>
-      <c r="E287" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="F287" s="3" t="n">
-        <v>15</v>
-      </c>
-      <c r="G287" s="3" t="n">
+      <c r="D287" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="E287" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="F287" s="10" t="n">
+        <v>7</v>
+      </c>
+      <c r="G287" s="10" t="n">
+        <v>37</v>
+      </c>
+      <c r="H287" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="I287" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="J287" s="12" t="s">
+        <v>308</v>
+      </c>
+      <c r="K287" s="13" t="s">
+        <v>307</v>
+      </c>
+      <c r="L287" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="H287" s="3" t="s">
-        <v>307</v>
-      </c>
-      <c r="I287" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="J287" s="5" t="s">
-        <v>308</v>
-      </c>
-      <c r="K287" s="6" t="s">
-        <v>309</v>
-      </c>
-      <c r="L287" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="M287" s="3" t="s">
+      <c r="M287" s="14" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="288" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="288" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A288" s="0" t="n">
         <v>287</v>
       </c>
-      <c r="B288" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="C288" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="D288" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="E288" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F288" s="3" t="n">
-        <v>11</v>
-      </c>
-      <c r="G288" s="3" t="n">
-        <v>15</v>
-      </c>
-      <c r="H288" s="3" t="s">
+      <c r="B288" s="8" t="n">
+        <f aca="false">A$284</f>
+        <v>283</v>
+      </c>
+      <c r="C288" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="D288" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="E288" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="F288" s="10" t="n">
+        <v>7</v>
+      </c>
+      <c r="G288" s="10" t="n">
+        <v>9</v>
+      </c>
+      <c r="H288" s="10" t="s">
+        <v>309</v>
+      </c>
+      <c r="I288" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="J288" s="12" t="s">
+        <v>100</v>
+      </c>
+      <c r="K288" s="13" t="s">
         <v>310</v>
       </c>
-      <c r="I288" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="J288" s="5" t="s">
-        <v>311</v>
-      </c>
-      <c r="K288" s="6" t="s">
-        <v>312</v>
-      </c>
-      <c r="L288" s="3" t="s">
+      <c r="L288" s="10" t="s">
         <v>107</v>
       </c>
-      <c r="M288" s="3" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="289" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M288" s="14" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="289" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A289" s="0" t="n">
         <v>288</v>
       </c>
-      <c r="B289" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="C289" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="D289" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="E289" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F289" s="3" t="n">
-        <v>7</v>
-      </c>
-      <c r="G289" s="3" t="n">
-        <v>11</v>
-      </c>
-      <c r="H289" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="I289" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="J289" s="5" t="s">
+      <c r="B289" s="15" t="n">
+        <f aca="false">A288</f>
+        <v>287</v>
+      </c>
+      <c r="C289" s="15" t="n">
+        <v>2</v>
+      </c>
+      <c r="D289" s="16" t="n">
+        <v>2</v>
+      </c>
+      <c r="E289" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="F289" s="17" t="n">
+        <v>12</v>
+      </c>
+      <c r="G289" s="17" t="n">
+        <v>14</v>
+      </c>
+      <c r="H289" s="17" t="s">
+        <v>311</v>
+      </c>
+      <c r="I289" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="J289" s="19" t="s">
+        <v>312</v>
+      </c>
+      <c r="K289" s="30" t="s">
         <v>313</v>
       </c>
-      <c r="K289" s="6" t="s">
-        <v>314</v>
-      </c>
-      <c r="L289" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="M289" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="290" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L289" s="17" t="s">
+        <v>107</v>
+      </c>
+      <c r="M289" s="21" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="290" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A290" s="0" t="n">
         <v>289</v>
       </c>
-      <c r="B290" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="C290" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="D290" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="E290" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F290" s="3" t="n">
-        <v>7</v>
-      </c>
-      <c r="G290" s="3" t="n">
-        <v>11</v>
-      </c>
-      <c r="H290" s="3" t="s">
+      <c r="B290" s="15" t="n">
+        <f aca="false">A288</f>
+        <v>287</v>
+      </c>
+      <c r="C290" s="15" t="n">
+        <v>2</v>
+      </c>
+      <c r="D290" s="16" t="n">
+        <v>2</v>
+      </c>
+      <c r="E290" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="F290" s="17" t="n">
+        <v>12</v>
+      </c>
+      <c r="G290" s="17" t="n">
+        <v>14</v>
+      </c>
+      <c r="H290" s="17" t="s">
+        <v>314</v>
+      </c>
+      <c r="I290" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="J290" s="19" t="s">
         <v>315</v>
       </c>
-      <c r="I290" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="J290" s="5" t="s">
+      <c r="K290" s="30" t="s">
         <v>316</v>
       </c>
-      <c r="K290" s="6" t="s">
-        <v>317</v>
-      </c>
-      <c r="L290" s="3" t="s">
+      <c r="L290" s="17" t="s">
         <v>107</v>
       </c>
-      <c r="M290" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="291" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M290" s="21" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="291" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A291" s="0" t="n">
         <v>290</v>
       </c>
-      <c r="B291" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="C291" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="D291" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="E291" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="F291" s="3" t="n">
-        <v>7</v>
-      </c>
-      <c r="G291" s="3" t="n">
-        <v>11</v>
-      </c>
-      <c r="H291" s="3" t="s">
+      <c r="B291" s="15" t="n">
+        <f aca="false">A288</f>
+        <v>287</v>
+      </c>
+      <c r="C291" s="15" t="n">
+        <v>2</v>
+      </c>
+      <c r="D291" s="16" t="n">
+        <v>2</v>
+      </c>
+      <c r="E291" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="F291" s="17" t="n">
+        <v>15</v>
+      </c>
+      <c r="G291" s="17" t="n">
+        <v>17</v>
+      </c>
+      <c r="H291" s="17" t="s">
+        <v>317</v>
+      </c>
+      <c r="I291" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="J291" s="19" t="s">
         <v>318</v>
       </c>
-      <c r="I291" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="J291" s="5" t="s">
+      <c r="K291" s="30" t="s">
         <v>319</v>
       </c>
-      <c r="K291" s="6" t="s">
-        <v>320</v>
-      </c>
-      <c r="L291" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="M291" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="292" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L291" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="M291" s="21" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="292" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A292" s="0" t="n">
         <v>291</v>
       </c>
-      <c r="B292" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="C292" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="D292" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="E292" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="F292" s="3" t="n">
-        <v>7</v>
-      </c>
-      <c r="G292" s="3" t="n">
-        <v>11</v>
-      </c>
-      <c r="H292" s="3" t="s">
+      <c r="B292" s="15" t="n">
+        <f aca="false">A288</f>
+        <v>287</v>
+      </c>
+      <c r="C292" s="15" t="n">
+        <v>2</v>
+      </c>
+      <c r="D292" s="16" t="n">
+        <v>2</v>
+      </c>
+      <c r="E292" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="F292" s="17" t="n">
+        <v>15</v>
+      </c>
+      <c r="G292" s="17" t="n">
+        <v>17</v>
+      </c>
+      <c r="H292" s="17" t="s">
+        <v>320</v>
+      </c>
+      <c r="I292" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="J292" s="19" t="s">
         <v>321</v>
       </c>
-      <c r="I292" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="J292" s="5" t="s">
-        <v>322</v>
-      </c>
-      <c r="K292" s="6" t="s">
-        <v>323</v>
-      </c>
-      <c r="L292" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="M292" s="3" t="s">
-        <v>18</v>
+      <c r="K292" s="30" t="s">
+        <v>319</v>
+      </c>
+      <c r="L292" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="M292" s="21" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="293" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A293" s="0" t="n">
         <v>292</v>
       </c>
-      <c r="B293" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="C293" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="D293" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="E293" s="1" t="s">
+      <c r="B293" s="15" t="n">
+        <f aca="false">A288</f>
+        <v>287</v>
+      </c>
+      <c r="C293" s="15" t="n">
+        <v>2</v>
+      </c>
+      <c r="D293" s="16" t="n">
+        <v>3</v>
+      </c>
+      <c r="E293" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="F293" s="3" t="n">
-        <v>6</v>
-      </c>
-      <c r="G293" s="3" t="n">
-        <v>10</v>
-      </c>
-      <c r="H293" s="3" t="s">
-        <v>324</v>
-      </c>
-      <c r="I293" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="J293" s="5" t="s">
-        <v>325</v>
-      </c>
-      <c r="K293" s="6" t="s">
-        <v>326</v>
-      </c>
-      <c r="L293" s="3" t="s">
-        <v>327</v>
-      </c>
-      <c r="M293" s="3" t="s">
-        <v>55</v>
+      <c r="F293" s="17" t="n">
+        <v>15</v>
+      </c>
+      <c r="G293" s="17" t="n">
+        <v>17</v>
+      </c>
+      <c r="H293" s="17" t="s">
+        <v>322</v>
+      </c>
+      <c r="I293" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="J293" s="19" t="s">
+        <v>312</v>
+      </c>
+      <c r="K293" s="30" t="s">
+        <v>323</v>
+      </c>
+      <c r="L293" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="M293" s="21" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="294" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A294" s="0" t="n">
         <v>293</v>
       </c>
-      <c r="B294" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="C294" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="D294" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="E294" s="1" t="s">
+      <c r="B294" s="15" t="n">
+        <f aca="false">A288</f>
+        <v>287</v>
+      </c>
+      <c r="C294" s="15" t="n">
+        <v>2</v>
+      </c>
+      <c r="D294" s="16" t="n">
+        <v>3</v>
+      </c>
+      <c r="E294" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="F294" s="3" t="n">
-        <v>6</v>
-      </c>
-      <c r="G294" s="3" t="n">
-        <v>10</v>
-      </c>
-      <c r="H294" s="3" t="s">
+      <c r="F294" s="17" t="n">
+        <v>15</v>
+      </c>
+      <c r="G294" s="17" t="n">
+        <v>17</v>
+      </c>
+      <c r="H294" s="17" t="s">
         <v>324</v>
       </c>
-      <c r="I294" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="J294" s="5" t="s">
+      <c r="I294" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="J294" s="19" t="s">
         <v>325</v>
       </c>
-      <c r="K294" s="6" t="s">
+      <c r="K294" s="30" t="s">
         <v>326</v>
       </c>
-      <c r="L294" s="3" t="s">
-        <v>327</v>
-      </c>
-      <c r="M294" s="3" t="s">
-        <v>55</v>
+      <c r="L294" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="M294" s="21" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="295" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A295" s="0" t="n">
         <v>294</v>
       </c>
-      <c r="B295" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="C295" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="D295" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="E295" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F295" s="3" t="n">
-        <v>6</v>
-      </c>
-      <c r="G295" s="3" t="n">
+      <c r="B295" s="8" t="n">
+        <f aca="false">A$284</f>
+        <v>283</v>
+      </c>
+      <c r="C295" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="D295" s="9" t="n">
+        <v>2</v>
+      </c>
+      <c r="E295" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="F295" s="10" t="n">
         <v>10</v>
       </c>
-      <c r="H295" s="3" t="s">
-        <v>324</v>
-      </c>
-      <c r="I295" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="J295" s="5" t="s">
-        <v>325</v>
-      </c>
-      <c r="K295" s="6" t="s">
-        <v>326</v>
-      </c>
-      <c r="L295" s="3" t="s">
+      <c r="G295" s="10" t="n">
+        <v>37</v>
+      </c>
+      <c r="H295" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="I295" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="J295" s="12" t="s">
+        <v>262</v>
+      </c>
+      <c r="K295" s="13" t="s">
         <v>327</v>
       </c>
-      <c r="M295" s="3" t="s">
-        <v>55</v>
+      <c r="L295" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="M295" s="14" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="296" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A296" s="0" t="n">
         <v>295</v>
       </c>
-      <c r="B296" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="C296" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="D296" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="E296" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="F296" s="3" t="n">
-        <v>6</v>
-      </c>
-      <c r="G296" s="3" t="n">
-        <v>10</v>
-      </c>
-      <c r="H296" s="3" t="s">
-        <v>324</v>
-      </c>
-      <c r="I296" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="J296" s="5" t="s">
-        <v>325</v>
-      </c>
-      <c r="K296" s="6" t="s">
-        <v>326</v>
-      </c>
-      <c r="L296" s="3" t="s">
-        <v>327</v>
-      </c>
-      <c r="M296" s="3" t="s">
-        <v>55</v>
+      <c r="B296" s="15" t="n">
+        <f aca="false">A295</f>
+        <v>294</v>
+      </c>
+      <c r="C296" s="15" t="n">
+        <v>2</v>
+      </c>
+      <c r="D296" s="16" t="n">
+        <v>2</v>
+      </c>
+      <c r="E296" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="F296" s="17" t="n">
+        <v>12</v>
+      </c>
+      <c r="G296" s="17" t="n">
+        <v>14</v>
+      </c>
+      <c r="H296" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="I296" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="J296" s="19" t="s">
+        <v>328</v>
+      </c>
+      <c r="K296" s="30" t="s">
+        <v>329</v>
+      </c>
+      <c r="L296" s="17" t="s">
+        <v>107</v>
+      </c>
+      <c r="M296" s="21" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="297" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A297" s="0" t="n">
         <v>296</v>
       </c>
-      <c r="B297" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="C297" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="D297" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="E297" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="F297" s="3" t="n">
-        <v>9</v>
-      </c>
-      <c r="G297" s="3" t="n">
-        <f aca="false">F297+13</f>
+      <c r="B297" s="15" t="n">
+        <f aca="false">A295</f>
+        <v>294</v>
+      </c>
+      <c r="C297" s="15" t="n">
+        <v>2</v>
+      </c>
+      <c r="D297" s="16" t="n">
+        <v>2</v>
+      </c>
+      <c r="E297" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="H297" s="3" t="s">
-        <v>328</v>
-      </c>
-      <c r="I297" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="J297" s="5" t="s">
-        <v>329</v>
-      </c>
-      <c r="K297" s="6" t="s">
+      <c r="F297" s="17" t="n">
+        <v>15</v>
+      </c>
+      <c r="G297" s="17" t="n">
+        <v>17</v>
+      </c>
+      <c r="H297" s="17" t="s">
         <v>330</v>
       </c>
-      <c r="L297" s="3" t="s">
-        <v>327</v>
-      </c>
-      <c r="M297" s="3" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="298" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I297" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="J297" s="19" t="s">
+        <v>318</v>
+      </c>
+      <c r="K297" s="30" t="s">
+        <v>331</v>
+      </c>
+      <c r="L297" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="M297" s="21" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="298" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A298" s="0" t="n">
         <v>297</v>
       </c>
-      <c r="B298" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="C298" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="D298" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="E298" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F298" s="3" t="n">
-        <v>8</v>
-      </c>
-      <c r="G298" s="3" t="n">
-        <v>10</v>
-      </c>
-      <c r="H298" s="3" t="s">
+      <c r="B298" s="15" t="n">
+        <f aca="false">A295</f>
+        <v>294</v>
+      </c>
+      <c r="C298" s="15" t="n">
+        <v>2</v>
+      </c>
+      <c r="D298" s="16" t="n">
+        <v>2</v>
+      </c>
+      <c r="E298" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="F298" s="17" t="n">
+        <v>15</v>
+      </c>
+      <c r="G298" s="17" t="n">
+        <v>17</v>
+      </c>
+      <c r="H298" s="17" t="s">
+        <v>332</v>
+      </c>
+      <c r="I298" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="J298" s="19" t="s">
+        <v>321</v>
+      </c>
+      <c r="K298" s="30" t="s">
         <v>331</v>
       </c>
-      <c r="I298" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="J298" s="5" t="s">
-        <v>332</v>
-      </c>
-      <c r="K298" s="6" t="s">
-        <v>333</v>
-      </c>
-      <c r="L298" s="3" t="s">
-        <v>327</v>
-      </c>
-      <c r="M298" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="299" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L298" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="M298" s="21" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="299" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A299" s="0" t="n">
         <v>298</v>
       </c>
-      <c r="B299" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="C299" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="D299" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="E299" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F299" s="3" t="n">
-        <v>8</v>
-      </c>
-      <c r="G299" s="3" t="n">
-        <v>10</v>
-      </c>
-      <c r="H299" s="3" t="s">
+      <c r="B299" s="15" t="n">
+        <f aca="false">A295</f>
+        <v>294</v>
+      </c>
+      <c r="C299" s="15" t="n">
+        <v>2</v>
+      </c>
+      <c r="D299" s="16" t="n">
+        <v>2</v>
+      </c>
+      <c r="E299" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="F299" s="17" t="n">
+        <v>15</v>
+      </c>
+      <c r="G299" s="17" t="n">
+        <v>17</v>
+      </c>
+      <c r="H299" s="17" t="s">
+        <v>333</v>
+      </c>
+      <c r="I299" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="J299" s="19" t="s">
         <v>334</v>
       </c>
-      <c r="I299" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="J299" s="5" t="s">
-        <v>332</v>
-      </c>
-      <c r="K299" s="6" t="s">
-        <v>333</v>
-      </c>
-      <c r="L299" s="3" t="s">
-        <v>327</v>
-      </c>
-      <c r="M299" s="3" t="s">
+      <c r="K299" s="30" t="s">
+        <v>335</v>
+      </c>
+      <c r="L299" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="M299" s="21" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="300" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="300" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A300" s="0" t="n">
         <v>299</v>
       </c>
-      <c r="B300" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="C300" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="D300" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="E300" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F300" s="3" t="n">
-        <v>8</v>
-      </c>
-      <c r="G300" s="3" t="n">
-        <v>10</v>
-      </c>
-      <c r="H300" s="3" t="s">
-        <v>335</v>
-      </c>
-      <c r="I300" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="J300" s="5" t="s">
+      <c r="B300" s="15" t="n">
+        <f aca="false">A295</f>
+        <v>294</v>
+      </c>
+      <c r="C300" s="15" t="n">
+        <v>2</v>
+      </c>
+      <c r="D300" s="16" t="n">
+        <v>3</v>
+      </c>
+      <c r="E300" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="F300" s="17" t="n">
+        <v>15</v>
+      </c>
+      <c r="G300" s="17" t="n">
+        <v>17</v>
+      </c>
+      <c r="H300" s="17" t="s">
         <v>336</v>
       </c>
-      <c r="K300" s="6" t="s">
+      <c r="I300" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="J300" s="19" t="s">
+        <v>312</v>
+      </c>
+      <c r="K300" s="30" t="s">
         <v>337</v>
       </c>
-      <c r="L300" s="3" t="s">
-        <v>327</v>
-      </c>
-      <c r="M300" s="3" t="s">
+      <c r="L300" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="M300" s="21" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="301" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="301" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A301" s="0" t="n">
         <v>300</v>
       </c>
-      <c r="B301" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="C301" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="D301" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="E301" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="F301" s="3" t="n">
-        <v>8</v>
-      </c>
-      <c r="G301" s="3" t="n">
-        <v>10</v>
-      </c>
-      <c r="H301" s="3" t="s">
+      <c r="B301" s="15" t="n">
+        <f aca="false">A295</f>
+        <v>294</v>
+      </c>
+      <c r="C301" s="15" t="n">
+        <v>2</v>
+      </c>
+      <c r="D301" s="16" t="n">
+        <v>3</v>
+      </c>
+      <c r="E301" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="F301" s="17" t="n">
+        <v>15</v>
+      </c>
+      <c r="G301" s="17" t="n">
+        <v>17</v>
+      </c>
+      <c r="H301" s="17" t="s">
+        <v>95</v>
+      </c>
+      <c r="I301" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="J301" s="19" t="s">
+        <v>112</v>
+      </c>
+      <c r="K301" s="30" t="s">
         <v>338</v>
       </c>
-      <c r="I301" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="J301" s="5" t="s">
-        <v>336</v>
-      </c>
-      <c r="K301" s="6" t="s">
-        <v>337</v>
-      </c>
-      <c r="L301" s="3" t="s">
-        <v>327</v>
-      </c>
-      <c r="M301" s="3" t="s">
+      <c r="L301" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="M301" s="21" t="s">
         <v>62</v>
       </c>
     </row>
@@ -15077,40 +15267,41 @@
       <c r="A302" s="0" t="n">
         <v>301</v>
       </c>
-      <c r="B302" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="C302" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="D302" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="E302" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="F302" s="3" t="n">
-        <v>16</v>
-      </c>
-      <c r="G302" s="3" t="n">
-        <v>32</v>
-      </c>
-      <c r="H302" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="I302" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="J302" s="5" t="s">
+      <c r="B302" s="15" t="n">
+        <f aca="false">A295</f>
+        <v>294</v>
+      </c>
+      <c r="C302" s="15" t="n">
+        <v>2</v>
+      </c>
+      <c r="D302" s="16" t="n">
+        <v>3</v>
+      </c>
+      <c r="E302" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="F302" s="17" t="n">
+        <v>15</v>
+      </c>
+      <c r="G302" s="17" t="n">
+        <v>17</v>
+      </c>
+      <c r="H302" s="17" t="s">
         <v>339</v>
       </c>
-      <c r="K302" s="6" t="s">
+      <c r="I302" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="J302" s="19" t="s">
+        <v>280</v>
+      </c>
+      <c r="K302" s="30" t="s">
         <v>340</v>
       </c>
-      <c r="L302" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="M302" s="3" t="s">
+      <c r="L302" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="M302" s="21" t="s">
         <v>18</v>
       </c>
     </row>
@@ -15118,122 +15309,125 @@
       <c r="A303" s="0" t="n">
         <v>302</v>
       </c>
-      <c r="B303" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="C303" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="D303" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="E303" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F303" s="3" t="n">
-        <v>6</v>
-      </c>
-      <c r="G303" s="3" t="n">
-        <v>10</v>
-      </c>
-      <c r="H303" s="3" t="s">
-        <v>341</v>
-      </c>
-      <c r="I303" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="J303" s="5" t="s">
-        <v>336</v>
-      </c>
-      <c r="K303" s="6" t="s">
-        <v>342</v>
-      </c>
-      <c r="L303" s="3" t="s">
-        <v>327</v>
-      </c>
-      <c r="M303" s="3" t="s">
-        <v>62</v>
+      <c r="B303" s="15" t="n">
+        <f aca="false">A295</f>
+        <v>294</v>
+      </c>
+      <c r="C303" s="15" t="n">
+        <v>2</v>
+      </c>
+      <c r="D303" s="16" t="n">
+        <v>3</v>
+      </c>
+      <c r="E303" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="F303" s="17" t="n">
+        <v>15</v>
+      </c>
+      <c r="G303" s="17" t="n">
+        <v>17</v>
+      </c>
+      <c r="H303" s="17" t="s">
+        <v>339</v>
+      </c>
+      <c r="I303" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="J303" s="19" t="s">
+        <v>280</v>
+      </c>
+      <c r="K303" s="30" t="s">
+        <v>340</v>
+      </c>
+      <c r="L303" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="M303" s="21" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="304" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A304" s="0" t="n">
         <v>303</v>
       </c>
-      <c r="B304" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="C304" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="D304" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="E304" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F304" s="3" t="n">
-        <v>6</v>
-      </c>
-      <c r="G304" s="3" t="n">
-        <v>10</v>
-      </c>
-      <c r="H304" s="3" t="s">
+      <c r="B304" s="15" t="n">
+        <f aca="false">A295</f>
+        <v>294</v>
+      </c>
+      <c r="C304" s="15" t="n">
+        <v>2</v>
+      </c>
+      <c r="D304" s="16" t="n">
+        <v>3</v>
+      </c>
+      <c r="E304" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="F304" s="17" t="n">
+        <v>12</v>
+      </c>
+      <c r="G304" s="17" t="n">
+        <v>14</v>
+      </c>
+      <c r="H304" s="17" t="s">
+        <v>333</v>
+      </c>
+      <c r="I304" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="J304" s="19" t="s">
+        <v>167</v>
+      </c>
+      <c r="K304" s="30" t="s">
         <v>341</v>
       </c>
-      <c r="I304" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="J304" s="5" t="s">
-        <v>336</v>
-      </c>
-      <c r="K304" s="6" t="s">
-        <v>342</v>
-      </c>
-      <c r="L304" s="3" t="s">
-        <v>327</v>
-      </c>
-      <c r="M304" s="3" t="s">
-        <v>62</v>
+      <c r="L304" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="M304" s="21" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="305" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A305" s="0" t="n">
         <v>304</v>
       </c>
-      <c r="B305" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="C305" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="D305" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="E305" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F305" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="G305" s="3" t="n">
+      <c r="B305" s="8" t="n">
+        <f aca="false">A$284</f>
+        <v>283</v>
+      </c>
+      <c r="C305" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="D305" s="9" t="n">
+        <v>2</v>
+      </c>
+      <c r="E305" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="F305" s="10" t="n">
+        <v>12</v>
+      </c>
+      <c r="G305" s="10" t="n">
         <v>37</v>
       </c>
-      <c r="H305" s="3" t="s">
-        <v>324</v>
-      </c>
-      <c r="I305" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="J305" s="5" t="s">
-        <v>336</v>
-      </c>
-      <c r="K305" s="6" t="s">
+      <c r="H305" s="10" t="s">
+        <v>342</v>
+      </c>
+      <c r="I305" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="J305" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="K305" s="13" t="s">
         <v>343</v>
       </c>
-      <c r="L305" s="3" t="s">
-        <v>327</v>
-      </c>
-      <c r="M305" s="3" t="s">
+      <c r="L305" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="M305" s="14" t="s">
         <v>62</v>
       </c>
     </row>
@@ -15241,40 +15435,1280 @@
       <c r="A306" s="0" t="n">
         <v>305</v>
       </c>
-      <c r="B306" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="C306" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="D306" s="1" t="n">
+      <c r="B306" s="8" t="n">
+        <f aca="false">A$284</f>
+        <v>283</v>
+      </c>
+      <c r="C306" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="D306" s="9" t="n">
+        <v>2</v>
+      </c>
+      <c r="E306" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="F306" s="10" t="n">
+        <v>12</v>
+      </c>
+      <c r="G306" s="10" t="n">
+        <v>37</v>
+      </c>
+      <c r="H306" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="I306" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="J306" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="K306" s="13" t="s">
+        <v>344</v>
+      </c>
+      <c r="L306" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="M306" s="14" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="307" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A307" s="0" t="n">
+        <v>306</v>
+      </c>
+      <c r="B307" s="8" t="n">
+        <f aca="false">A$284</f>
+        <v>283</v>
+      </c>
+      <c r="C307" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="D307" s="9" t="n">
+        <v>2</v>
+      </c>
+      <c r="E307" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="F307" s="10" t="n">
+        <v>12</v>
+      </c>
+      <c r="G307" s="10" t="n">
+        <v>37</v>
+      </c>
+      <c r="H307" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="I307" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="J307" s="12" t="s">
+        <v>274</v>
+      </c>
+      <c r="K307" s="13" t="s">
+        <v>344</v>
+      </c>
+      <c r="L307" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="M307" s="14" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="308" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A308" s="0" t="n">
+        <v>307</v>
+      </c>
+      <c r="B308" s="8" t="n">
+        <f aca="false">A$284</f>
+        <v>283</v>
+      </c>
+      <c r="C308" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="D308" s="9" t="n">
+        <v>2</v>
+      </c>
+      <c r="E308" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="F308" s="10" t="n">
+        <v>11</v>
+      </c>
+      <c r="G308" s="10" t="n">
+        <v>12</v>
+      </c>
+      <c r="H308" s="10" t="s">
+        <v>309</v>
+      </c>
+      <c r="I308" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="J308" s="12" t="s">
+        <v>119</v>
+      </c>
+      <c r="K308" s="13" t="s">
+        <v>345</v>
+      </c>
+      <c r="L308" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="M308" s="14" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="309" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A309" s="0" t="n">
+        <v>308</v>
+      </c>
+      <c r="B309" s="8" t="n">
+        <f aca="false">A$284</f>
+        <v>283</v>
+      </c>
+      <c r="C309" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="D309" s="9" t="n">
+        <v>3</v>
+      </c>
+      <c r="E309" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="F309" s="10" t="n">
+        <v>9</v>
+      </c>
+      <c r="G309" s="10" t="n">
+        <v>11</v>
+      </c>
+      <c r="H309" s="10" t="s">
+        <v>346</v>
+      </c>
+      <c r="I309" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="J309" s="12" t="s">
+        <v>119</v>
+      </c>
+      <c r="K309" s="13" t="s">
+        <v>347</v>
+      </c>
+      <c r="L309" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="M309" s="14" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="310" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A310" s="0" t="n">
+        <v>309</v>
+      </c>
+      <c r="B310" s="8" t="n">
+        <f aca="false">A$284</f>
+        <v>283</v>
+      </c>
+      <c r="C310" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="D310" s="9" t="n">
+        <v>3</v>
+      </c>
+      <c r="E310" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="F310" s="10" t="n">
+        <v>7</v>
+      </c>
+      <c r="G310" s="10" t="n">
+        <v>9</v>
+      </c>
+      <c r="H310" s="10" t="s">
+        <v>348</v>
+      </c>
+      <c r="I310" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="J310" s="12" t="s">
+        <v>349</v>
+      </c>
+      <c r="K310" s="13" t="s">
+        <v>350</v>
+      </c>
+      <c r="L310" s="10" t="s">
+        <v>351</v>
+      </c>
+      <c r="M310" s="14" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="311" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A311" s="0" t="n">
+        <v>310</v>
+      </c>
+      <c r="B311" s="8" t="n">
+        <f aca="false">A$284</f>
+        <v>283</v>
+      </c>
+      <c r="C311" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="D311" s="9" t="n">
+        <v>3</v>
+      </c>
+      <c r="E311" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="F311" s="10" t="n">
+        <v>12</v>
+      </c>
+      <c r="G311" s="10" t="n">
+        <v>15</v>
+      </c>
+      <c r="H311" s="10" t="s">
+        <v>352</v>
+      </c>
+      <c r="I311" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="J311" s="12" t="s">
+        <v>280</v>
+      </c>
+      <c r="K311" s="13" t="s">
+        <v>353</v>
+      </c>
+      <c r="L311" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="M311" s="14" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="312" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A312" s="0" t="n">
+        <v>311</v>
+      </c>
+      <c r="B312" s="8" t="n">
+        <f aca="false">A$284</f>
+        <v>283</v>
+      </c>
+      <c r="C312" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="D312" s="9" t="n">
+        <v>3</v>
+      </c>
+      <c r="E312" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="F312" s="10" t="n">
+        <v>12</v>
+      </c>
+      <c r="G312" s="10" t="n">
+        <v>15</v>
+      </c>
+      <c r="H312" s="10" t="s">
+        <v>352</v>
+      </c>
+      <c r="I312" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="J312" s="12" t="s">
+        <v>280</v>
+      </c>
+      <c r="K312" s="13" t="s">
+        <v>353</v>
+      </c>
+      <c r="L312" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="M312" s="14" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="313" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A313" s="0" t="n">
+        <v>312</v>
+      </c>
+      <c r="B313" s="8" t="n">
+        <f aca="false">A$284</f>
+        <v>283</v>
+      </c>
+      <c r="C313" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="D313" s="9" t="n">
+        <v>3</v>
+      </c>
+      <c r="E313" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="F313" s="10" t="n">
+        <v>13</v>
+      </c>
+      <c r="G313" s="10" t="n">
+        <v>16</v>
+      </c>
+      <c r="H313" s="10" t="s">
+        <v>354</v>
+      </c>
+      <c r="I313" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="J313" s="12" t="s">
+        <v>128</v>
+      </c>
+      <c r="K313" s="13" t="s">
+        <v>355</v>
+      </c>
+      <c r="L313" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="M313" s="14" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="314" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A314" s="0" t="n">
+        <v>313</v>
+      </c>
+      <c r="B314" s="8" t="n">
+        <f aca="false">A$284</f>
+        <v>283</v>
+      </c>
+      <c r="C314" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="D314" s="9" t="n">
+        <v>4</v>
+      </c>
+      <c r="E314" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="F314" s="10" t="n">
+        <v>12</v>
+      </c>
+      <c r="G314" s="10" t="n">
+        <v>15</v>
+      </c>
+      <c r="H314" s="10" t="s">
+        <v>356</v>
+      </c>
+      <c r="I314" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="J314" s="12" t="s">
+        <v>280</v>
+      </c>
+      <c r="K314" s="13" t="s">
+        <v>357</v>
+      </c>
+      <c r="L314" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="M314" s="14" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="315" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A315" s="0" t="n">
+        <v>314</v>
+      </c>
+      <c r="B315" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C315" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D315" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E315" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F315" s="3" t="n">
+        <v>12</v>
+      </c>
+      <c r="G315" s="3" t="n">
+        <v>17</v>
+      </c>
+      <c r="H315" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="I315" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="J315" s="5" t="s">
+        <v>358</v>
+      </c>
+      <c r="K315" s="6" t="s">
+        <v>359</v>
+      </c>
+      <c r="L315" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="M315" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="316" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A316" s="0" t="n">
+        <v>315</v>
+      </c>
+      <c r="B316" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C316" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D316" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E316" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F316" s="3" t="n">
+        <v>12</v>
+      </c>
+      <c r="G316" s="3" t="n">
+        <v>17</v>
+      </c>
+      <c r="H316" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="I316" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="J316" s="5" t="s">
+        <v>358</v>
+      </c>
+      <c r="K316" s="6" t="s">
+        <v>360</v>
+      </c>
+      <c r="L316" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="M316" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="317" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A317" s="0" t="n">
+        <v>316</v>
+      </c>
+      <c r="B317" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C317" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D317" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E317" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F317" s="3" t="n">
+        <v>15</v>
+      </c>
+      <c r="G317" s="3" t="n">
+        <v>17</v>
+      </c>
+      <c r="H317" s="3" t="s">
+        <v>361</v>
+      </c>
+      <c r="I317" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="J317" s="5" t="s">
+        <v>362</v>
+      </c>
+      <c r="K317" s="6" t="s">
+        <v>363</v>
+      </c>
+      <c r="L317" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="M317" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="318" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A318" s="0" t="n">
+        <v>317</v>
+      </c>
+      <c r="B318" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C318" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D318" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="E318" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F318" s="3" t="n">
+        <v>11</v>
+      </c>
+      <c r="G318" s="3" t="n">
+        <v>15</v>
+      </c>
+      <c r="H318" s="3" t="s">
+        <v>364</v>
+      </c>
+      <c r="I318" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="J318" s="5" t="s">
+        <v>365</v>
+      </c>
+      <c r="K318" s="6" t="s">
+        <v>366</v>
+      </c>
+      <c r="L318" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="M318" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="319" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A319" s="0" t="n">
+        <v>318</v>
+      </c>
+      <c r="B319" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C319" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D319" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="E319" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F319" s="3" t="n">
+        <v>7</v>
+      </c>
+      <c r="G319" s="3" t="n">
+        <v>11</v>
+      </c>
+      <c r="H319" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="I319" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="J319" s="5" t="s">
+        <v>367</v>
+      </c>
+      <c r="K319" s="6" t="s">
+        <v>368</v>
+      </c>
+      <c r="L319" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="M319" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="320" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A320" s="0" t="n">
+        <v>319</v>
+      </c>
+      <c r="B320" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C320" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D320" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="E320" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F320" s="3" t="n">
+        <v>7</v>
+      </c>
+      <c r="G320" s="3" t="n">
+        <v>11</v>
+      </c>
+      <c r="H320" s="3" t="s">
+        <v>369</v>
+      </c>
+      <c r="I320" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="J320" s="5" t="s">
+        <v>370</v>
+      </c>
+      <c r="K320" s="6" t="s">
+        <v>371</v>
+      </c>
+      <c r="L320" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="M320" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="321" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A321" s="0" t="n">
+        <v>320</v>
+      </c>
+      <c r="B321" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C321" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D321" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="E321" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F321" s="3" t="n">
+        <v>7</v>
+      </c>
+      <c r="G321" s="3" t="n">
+        <v>11</v>
+      </c>
+      <c r="H321" s="3" t="s">
+        <v>372</v>
+      </c>
+      <c r="I321" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="J321" s="5" t="s">
+        <v>373</v>
+      </c>
+      <c r="K321" s="6" t="s">
+        <v>374</v>
+      </c>
+      <c r="L321" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="M321" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="322" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A322" s="0" t="n">
+        <v>321</v>
+      </c>
+      <c r="B322" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C322" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D322" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="E322" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F322" s="3" t="n">
+        <v>7</v>
+      </c>
+      <c r="G322" s="3" t="n">
+        <v>11</v>
+      </c>
+      <c r="H322" s="3" t="s">
+        <v>375</v>
+      </c>
+      <c r="I322" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="J322" s="5" t="s">
+        <v>376</v>
+      </c>
+      <c r="K322" s="6" t="s">
+        <v>377</v>
+      </c>
+      <c r="L322" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="M322" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="323" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A323" s="0" t="n">
+        <v>322</v>
+      </c>
+      <c r="B323" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C323" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D323" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="E323" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F323" s="3" t="n">
+        <v>6</v>
+      </c>
+      <c r="G323" s="3" t="n">
+        <v>10</v>
+      </c>
+      <c r="H323" s="3" t="s">
+        <v>378</v>
+      </c>
+      <c r="I323" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="J323" s="5" t="s">
+        <v>379</v>
+      </c>
+      <c r="K323" s="6" t="s">
+        <v>380</v>
+      </c>
+      <c r="L323" s="3" t="s">
+        <v>351</v>
+      </c>
+      <c r="M323" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="324" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A324" s="0" t="n">
+        <v>323</v>
+      </c>
+      <c r="B324" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C324" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D324" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="E324" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F324" s="3" t="n">
+        <v>6</v>
+      </c>
+      <c r="G324" s="3" t="n">
+        <v>10</v>
+      </c>
+      <c r="H324" s="3" t="s">
+        <v>378</v>
+      </c>
+      <c r="I324" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="J324" s="5" t="s">
+        <v>379</v>
+      </c>
+      <c r="K324" s="6" t="s">
+        <v>380</v>
+      </c>
+      <c r="L324" s="3" t="s">
+        <v>351</v>
+      </c>
+      <c r="M324" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="325" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A325" s="0" t="n">
+        <v>324</v>
+      </c>
+      <c r="B325" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C325" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D325" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="E325" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F325" s="3" t="n">
+        <v>6</v>
+      </c>
+      <c r="G325" s="3" t="n">
+        <v>10</v>
+      </c>
+      <c r="H325" s="3" t="s">
+        <v>378</v>
+      </c>
+      <c r="I325" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="J325" s="5" t="s">
+        <v>379</v>
+      </c>
+      <c r="K325" s="6" t="s">
+        <v>380</v>
+      </c>
+      <c r="L325" s="3" t="s">
+        <v>351</v>
+      </c>
+      <c r="M325" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="326" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A326" s="0" t="n">
+        <v>325</v>
+      </c>
+      <c r="B326" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C326" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D326" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="E326" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F326" s="3" t="n">
+        <v>6</v>
+      </c>
+      <c r="G326" s="3" t="n">
+        <v>10</v>
+      </c>
+      <c r="H326" s="3" t="s">
+        <v>378</v>
+      </c>
+      <c r="I326" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="J326" s="5" t="s">
+        <v>379</v>
+      </c>
+      <c r="K326" s="6" t="s">
+        <v>380</v>
+      </c>
+      <c r="L326" s="3" t="s">
+        <v>351</v>
+      </c>
+      <c r="M326" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="327" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A327" s="0" t="n">
+        <v>326</v>
+      </c>
+      <c r="B327" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C327" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D327" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="E327" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F327" s="3" t="n">
+        <v>9</v>
+      </c>
+      <c r="G327" s="3" t="n">
+        <f aca="false">F327+13</f>
+        <v>22</v>
+      </c>
+      <c r="H327" s="3" t="s">
+        <v>381</v>
+      </c>
+      <c r="I327" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="J327" s="5" t="s">
+        <v>382</v>
+      </c>
+      <c r="K327" s="6" t="s">
+        <v>383</v>
+      </c>
+      <c r="L327" s="3" t="s">
+        <v>351</v>
+      </c>
+      <c r="M327" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="328" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A328" s="0" t="n">
+        <v>327</v>
+      </c>
+      <c r="B328" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C328" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D328" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="E328" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F328" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="G328" s="3" t="n">
+        <v>10</v>
+      </c>
+      <c r="H328" s="3" t="s">
+        <v>384</v>
+      </c>
+      <c r="I328" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="J328" s="5" t="s">
+        <v>385</v>
+      </c>
+      <c r="K328" s="6" t="s">
+        <v>386</v>
+      </c>
+      <c r="L328" s="3" t="s">
+        <v>351</v>
+      </c>
+      <c r="M328" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="329" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A329" s="0" t="n">
+        <v>328</v>
+      </c>
+      <c r="B329" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C329" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D329" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="E329" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F329" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="G329" s="3" t="n">
+        <v>10</v>
+      </c>
+      <c r="H329" s="3" t="s">
+        <v>387</v>
+      </c>
+      <c r="I329" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="J329" s="5" t="s">
+        <v>385</v>
+      </c>
+      <c r="K329" s="6" t="s">
+        <v>386</v>
+      </c>
+      <c r="L329" s="3" t="s">
+        <v>351</v>
+      </c>
+      <c r="M329" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="330" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A330" s="0" t="n">
+        <v>329</v>
+      </c>
+      <c r="B330" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C330" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D330" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="E330" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F330" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="G330" s="3" t="n">
+        <v>10</v>
+      </c>
+      <c r="H330" s="3" t="s">
+        <v>388</v>
+      </c>
+      <c r="I330" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="J330" s="5" t="s">
+        <v>349</v>
+      </c>
+      <c r="K330" s="6" t="s">
+        <v>389</v>
+      </c>
+      <c r="L330" s="3" t="s">
+        <v>351</v>
+      </c>
+      <c r="M330" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="331" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A331" s="0" t="n">
+        <v>330</v>
+      </c>
+      <c r="B331" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C331" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D331" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="E331" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F331" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="G331" s="3" t="n">
+        <v>10</v>
+      </c>
+      <c r="H331" s="3" t="s">
+        <v>390</v>
+      </c>
+      <c r="I331" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="J331" s="5" t="s">
+        <v>349</v>
+      </c>
+      <c r="K331" s="6" t="s">
+        <v>389</v>
+      </c>
+      <c r="L331" s="3" t="s">
+        <v>351</v>
+      </c>
+      <c r="M331" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="332" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A332" s="0" t="n">
+        <v>331</v>
+      </c>
+      <c r="B332" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C332" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D332" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="E332" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F332" s="3" t="n">
+        <v>16</v>
+      </c>
+      <c r="G332" s="3" t="n">
+        <v>32</v>
+      </c>
+      <c r="H332" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="I332" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="J332" s="5" t="s">
+        <v>391</v>
+      </c>
+      <c r="K332" s="6" t="s">
+        <v>392</v>
+      </c>
+      <c r="L332" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="M332" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="333" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A333" s="0" t="n">
+        <v>332</v>
+      </c>
+      <c r="B333" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C333" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D333" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="E306" s="1" t="s">
+      <c r="E333" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F333" s="3" t="n">
+        <v>6</v>
+      </c>
+      <c r="G333" s="3" t="n">
+        <v>10</v>
+      </c>
+      <c r="H333" s="3" t="s">
+        <v>393</v>
+      </c>
+      <c r="I333" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="J333" s="5" t="s">
+        <v>349</v>
+      </c>
+      <c r="K333" s="6" t="s">
+        <v>394</v>
+      </c>
+      <c r="L333" s="3" t="s">
+        <v>351</v>
+      </c>
+      <c r="M333" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="334" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A334" s="0" t="n">
+        <v>333</v>
+      </c>
+      <c r="B334" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C334" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D334" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="E334" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F334" s="3" t="n">
+        <v>6</v>
+      </c>
+      <c r="G334" s="3" t="n">
+        <v>10</v>
+      </c>
+      <c r="H334" s="3" t="s">
+        <v>393</v>
+      </c>
+      <c r="I334" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="J334" s="5" t="s">
+        <v>349</v>
+      </c>
+      <c r="K334" s="6" t="s">
+        <v>394</v>
+      </c>
+      <c r="L334" s="3" t="s">
+        <v>351</v>
+      </c>
+      <c r="M334" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="335" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A335" s="0" t="n">
+        <v>334</v>
+      </c>
+      <c r="B335" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C335" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D335" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="E335" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F335" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G335" s="3" t="n">
+        <v>37</v>
+      </c>
+      <c r="H335" s="3" t="s">
+        <v>378</v>
+      </c>
+      <c r="I335" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="J335" s="5" t="s">
+        <v>349</v>
+      </c>
+      <c r="K335" s="6" t="s">
+        <v>395</v>
+      </c>
+      <c r="L335" s="3" t="s">
+        <v>351</v>
+      </c>
+      <c r="M335" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="336" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A336" s="0" t="n">
+        <v>335</v>
+      </c>
+      <c r="B336" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C336" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D336" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="E336" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="F306" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="G306" s="3" t="n">
+      <c r="F336" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G336" s="3" t="n">
         <v>37</v>
       </c>
-      <c r="H306" s="3" t="s">
-        <v>324</v>
-      </c>
-      <c r="I306" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="J306" s="5" t="s">
-        <v>336</v>
-      </c>
-      <c r="K306" s="6" t="s">
-        <v>343</v>
-      </c>
-      <c r="L306" s="3" t="s">
-        <v>327</v>
-      </c>
-      <c r="M306" s="3" t="s">
+      <c r="H336" s="3" t="s">
+        <v>378</v>
+      </c>
+      <c r="I336" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="J336" s="5" t="s">
+        <v>349</v>
+      </c>
+      <c r="K336" s="6" t="s">
+        <v>395</v>
+      </c>
+      <c r="L336" s="3" t="s">
+        <v>351</v>
+      </c>
+      <c r="M336" s="3" t="s">
         <v>62</v>
       </c>
     </row>
@@ -15297,7 +16731,7 @@
   <dimension ref="A1:M5"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="J299 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -15375,10 +16809,10 @@
         <v>0</v>
       </c>
       <c r="J2" s="0" t="s">
-        <v>344</v>
+        <v>396</v>
       </c>
       <c r="K2" s="77" t="s">
-        <v>345</v>
+        <v>397</v>
       </c>
       <c r="L2" s="0" t="s">
         <v>31</v>
@@ -15417,10 +16851,10 @@
         <v>1</v>
       </c>
       <c r="J3" s="0" t="s">
-        <v>344</v>
+        <v>396</v>
       </c>
       <c r="K3" s="77" t="s">
-        <v>346</v>
+        <v>398</v>
       </c>
       <c r="L3" s="0" t="s">
         <v>31</v>
@@ -15458,10 +16892,10 @@
         <v>1</v>
       </c>
       <c r="J4" s="0" t="s">
-        <v>344</v>
+        <v>396</v>
       </c>
       <c r="K4" s="77" t="s">
-        <v>347</v>
+        <v>399</v>
       </c>
       <c r="L4" s="0" t="s">
         <v>31</v>
@@ -15499,10 +16933,10 @@
         <v>1</v>
       </c>
       <c r="J5" s="0" t="s">
-        <v>344</v>
+        <v>396</v>
       </c>
       <c r="K5" s="77" t="s">
-        <v>347</v>
+        <v>399</v>
       </c>
       <c r="L5" s="0" t="s">
         <v>31</v>
@@ -15530,7 +16964,7 @@
   <dimension ref="A1:M6"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J2" activeCellId="1" sqref="J299 J2"/>
+      <selection pane="topLeft" activeCell="J2" activeCellId="0" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -15610,13 +17044,13 @@
         <v>0</v>
       </c>
       <c r="J2" s="0" t="s">
-        <v>348</v>
+        <v>400</v>
       </c>
       <c r="K2" s="77" t="s">
-        <v>349</v>
+        <v>401</v>
       </c>
       <c r="L2" s="0" t="s">
-        <v>350</v>
+        <v>402</v>
       </c>
       <c r="M2" s="79"/>
     </row>
@@ -15652,7 +17086,7 @@
         <v>302</v>
       </c>
       <c r="K3" s="77" t="s">
-        <v>303</v>
+        <v>403</v>
       </c>
       <c r="L3" s="0" t="s">
         <v>31</v>
@@ -15688,10 +17122,10 @@
         <v>0</v>
       </c>
       <c r="J4" s="0" t="s">
-        <v>351</v>
+        <v>404</v>
       </c>
       <c r="K4" s="77" t="s">
-        <v>352</v>
+        <v>405</v>
       </c>
       <c r="L4" s="0" t="s">
         <v>31</v>
@@ -15727,10 +17161,10 @@
         <v>0</v>
       </c>
       <c r="J5" s="0" t="s">
-        <v>353</v>
+        <v>406</v>
       </c>
       <c r="K5" s="77" t="s">
-        <v>354</v>
+        <v>407</v>
       </c>
       <c r="L5" s="0" t="s">
         <v>31</v>
@@ -15769,7 +17203,7 @@
         <v>252</v>
       </c>
       <c r="K6" s="77" t="s">
-        <v>355</v>
+        <v>408</v>
       </c>
       <c r="L6" s="0" t="s">
         <v>31</v>
@@ -15797,7 +17231,7 @@
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="525" topLeftCell="A1" activePane="bottomLeft" state="split"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="K14" activeCellId="1" sqref="J299 K14"/>
+      <selection pane="bottomLeft" activeCell="K14" activeCellId="0" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -15877,16 +17311,16 @@
         <v>21</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>356</v>
+        <v>409</v>
       </c>
       <c r="I2" s="4" t="n">
         <v>0</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>357</v>
+        <v>410</v>
       </c>
       <c r="K2" s="6" t="s">
-        <v>358</v>
+        <v>411</v>
       </c>
       <c r="L2" s="3" t="s">
         <v>17</v>
@@ -15925,10 +17359,10 @@
         <v>0</v>
       </c>
       <c r="J3" s="12" t="s">
-        <v>359</v>
+        <v>412</v>
       </c>
       <c r="K3" s="13" t="s">
-        <v>360</v>
+        <v>413</v>
       </c>
       <c r="L3" s="10" t="s">
         <v>107</v>
@@ -15967,10 +17401,10 @@
         <v>0</v>
       </c>
       <c r="J4" s="12" t="s">
-        <v>361</v>
+        <v>414</v>
       </c>
       <c r="K4" s="13" t="s">
-        <v>362</v>
+        <v>415</v>
       </c>
       <c r="L4" s="10" t="s">
         <v>107</v>
@@ -16009,10 +17443,10 @@
         <v>0</v>
       </c>
       <c r="J5" s="12" t="s">
-        <v>363</v>
+        <v>416</v>
       </c>
       <c r="K5" s="13" t="s">
-        <v>364</v>
+        <v>417</v>
       </c>
       <c r="L5" s="10" t="s">
         <v>107</v>
@@ -16053,7 +17487,7 @@
         <v>100</v>
       </c>
       <c r="K6" s="12" t="s">
-        <v>365</v>
+        <v>418</v>
       </c>
       <c r="L6" s="10" t="s">
         <v>107</v>
@@ -16094,7 +17528,7 @@
         <v>262</v>
       </c>
       <c r="K7" s="12" t="s">
-        <v>366</v>
+        <v>419</v>
       </c>
       <c r="L7" s="10" t="s">
         <v>107</v>
@@ -16204,13 +17638,13 @@
         <v>21</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>356</v>
+        <v>409</v>
       </c>
       <c r="I10" s="4" t="n">
         <v>0</v>
       </c>
       <c r="J10" s="5" t="s">
-        <v>357</v>
+        <v>410</v>
       </c>
       <c r="K10" s="6"/>
       <c r="L10" s="3" t="s">
@@ -16249,7 +17683,7 @@
         <v>0</v>
       </c>
       <c r="J11" s="5" t="s">
-        <v>304</v>
+        <v>358</v>
       </c>
       <c r="K11" s="6"/>
       <c r="L11" s="3" t="s">
@@ -16288,7 +17722,7 @@
         <v>0</v>
       </c>
       <c r="J12" s="5" t="s">
-        <v>304</v>
+        <v>358</v>
       </c>
       <c r="K12" s="6"/>
       <c r="L12" s="3" t="s">
@@ -16327,7 +17761,7 @@
         <v>0</v>
       </c>
       <c r="J13" s="5" t="s">
-        <v>367</v>
+        <v>420</v>
       </c>
       <c r="K13" s="6"/>
       <c r="L13" s="3" t="s">
@@ -16368,7 +17802,7 @@
       </c>
       <c r="K14" s="6"/>
       <c r="L14" s="3" t="s">
-        <v>350</v>
+        <v>402</v>
       </c>
       <c r="M14" s="3" t="s">
         <v>45</v>
@@ -16403,7 +17837,7 @@
         <v>0</v>
       </c>
       <c r="J15" s="5" t="s">
-        <v>336</v>
+        <v>349</v>
       </c>
       <c r="K15" s="5"/>
       <c r="L15" s="3" t="s">
@@ -16442,7 +17876,7 @@
         <v>0</v>
       </c>
       <c r="J16" s="5" t="s">
-        <v>336</v>
+        <v>349</v>
       </c>
       <c r="K16" s="5"/>
       <c r="L16" s="3" t="s">
@@ -16481,7 +17915,7 @@
         <v>0</v>
       </c>
       <c r="J17" s="5" t="s">
-        <v>336</v>
+        <v>349</v>
       </c>
       <c r="K17" s="5"/>
       <c r="L17" s="3" t="s">
@@ -16553,13 +17987,13 @@
         <v>12</v>
       </c>
       <c r="H19" s="3" t="s">
-        <v>324</v>
+        <v>378</v>
       </c>
       <c r="I19" s="4" t="n">
         <v>0</v>
       </c>
       <c r="J19" s="5" t="s">
-        <v>336</v>
+        <v>349</v>
       </c>
       <c r="K19" s="6"/>
       <c r="L19" s="3" t="s">
@@ -16592,13 +18026,13 @@
         <v>12</v>
       </c>
       <c r="H20" s="3" t="s">
-        <v>324</v>
+        <v>378</v>
       </c>
       <c r="I20" s="4" t="n">
         <v>0</v>
       </c>
       <c r="J20" s="5" t="s">
-        <v>336</v>
+        <v>349</v>
       </c>
       <c r="K20" s="6"/>
       <c r="L20" s="3" t="s">
@@ -16631,13 +18065,13 @@
         <v>12</v>
       </c>
       <c r="H21" s="3" t="s">
-        <v>324</v>
+        <v>378</v>
       </c>
       <c r="I21" s="4" t="n">
         <v>0</v>
       </c>
       <c r="J21" s="5" t="s">
-        <v>336</v>
+        <v>349</v>
       </c>
       <c r="K21" s="6"/>
       <c r="L21" s="3" t="s">
@@ -16670,13 +18104,13 @@
         <v>12</v>
       </c>
       <c r="H22" s="3" t="s">
-        <v>324</v>
+        <v>378</v>
       </c>
       <c r="I22" s="4" t="n">
         <v>0</v>
       </c>
       <c r="J22" s="5" t="s">
-        <v>336</v>
+        <v>349</v>
       </c>
       <c r="K22" s="6"/>
       <c r="L22" s="3" t="s">
@@ -16748,13 +18182,13 @@
         <v>12</v>
       </c>
       <c r="H24" s="3" t="s">
-        <v>341</v>
+        <v>393</v>
       </c>
       <c r="I24" s="4" t="n">
         <v>0</v>
       </c>
       <c r="J24" s="5" t="s">
-        <v>336</v>
+        <v>349</v>
       </c>
       <c r="K24" s="6"/>
       <c r="L24" s="3" t="s">
@@ -16787,13 +18221,13 @@
         <v>12</v>
       </c>
       <c r="H25" s="3" t="s">
-        <v>341</v>
+        <v>393</v>
       </c>
       <c r="I25" s="4" t="n">
         <v>0</v>
       </c>
       <c r="J25" s="5" t="s">
-        <v>336</v>
+        <v>349</v>
       </c>
       <c r="K25" s="6"/>
       <c r="L25" s="3" t="s">
@@ -16826,13 +18260,13 @@
         <v>12</v>
       </c>
       <c r="H26" s="3" t="s">
-        <v>341</v>
+        <v>393</v>
       </c>
       <c r="I26" s="4" t="n">
         <v>0</v>
       </c>
       <c r="J26" s="5" t="s">
-        <v>336</v>
+        <v>349</v>
       </c>
       <c r="K26" s="6"/>
       <c r="L26" s="3" t="s">
@@ -16865,13 +18299,13 @@
         <v>12</v>
       </c>
       <c r="H27" s="3" t="s">
-        <v>341</v>
+        <v>393</v>
       </c>
       <c r="I27" s="4" t="n">
         <v>0</v>
       </c>
       <c r="J27" s="5" t="s">
-        <v>336</v>
+        <v>349</v>
       </c>
       <c r="K27" s="6"/>
       <c r="L27" s="3" t="s">

</xml_diff>

<commit_message>
Trying to automatically create sub bids for HS bids but that's too complex...
</commit_message>
<xml_diff>
--- a/bridgeIn.xlsx
+++ b/bridgeIn.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="544" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="W-J 2017" sheetId="1" state="visible" r:id="rId2"/>
@@ -14,61 +14,66 @@
     <sheet name="SA_z_piatek" sheetId="4" state="visible" r:id="rId5"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <extLst>
+    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
+      <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2247" uniqueCount="421">
-  <si>
-    <t>bidId</t>
-  </si>
-  <si>
-    <t>parentBid</t>
-  </si>
-  <si>
-    <t>bidLevel</t>
-  </si>
-  <si>
-    <t>level</t>
-  </si>
-  <si>
-    <t>suit</t>
-  </si>
-  <si>
-    <t>pointsMin</t>
-  </si>
-  <si>
-    <t>pointsMax</t>
-  </si>
-  <si>
-    <t>suitLength</t>
-  </si>
-  <si>
-    <t>afterInterven</t>
-  </si>
-  <si>
-    <t>shortDesc</t>
-  </si>
-  <si>
-    <t>description</t>
-  </si>
-  <si>
-    <t>bidType</t>
-  </si>
-  <si>
-    <t>bidClass</t>
-  </si>
-  <si>
-    <t>C</t>
-  </si>
-  <si>
-    <t>dowolny</t>
-  </si>
-  <si>
-    <t>Czteroznaczne trefl</t>
-  </si>
-  <si>
-    <t>&lt;br&gt; → (12)15-17 PC, 5+ trefl (naturalne, słaba piątka może też pasować na  1BA – patrz dalej)
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2246" uniqueCount="424">
+  <si>
+    <t xml:space="preserve">bidId</t>
+  </si>
+  <si>
+    <t xml:space="preserve">parentBid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bidLevel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">level</t>
+  </si>
+  <si>
+    <t xml:space="preserve">suit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pointsMin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pointsMax</t>
+  </si>
+  <si>
+    <t xml:space="preserve">suitLength</t>
+  </si>
+  <si>
+    <t xml:space="preserve">afterInterven</t>
+  </si>
+  <si>
+    <t xml:space="preserve">shortDesc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">description</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bidType</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bidClass</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dowolny</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Czteroznaczne trefl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;br&gt; → (12)15-17 PC, 5+ trefl (naturalne, słaba piątka może też pasować na  1BA – patrz dalej)
 &lt;br&gt;&lt;font color=green&gt;w wersji pro od 15 a nawet 16 PC!!! - słaby trefl wtedy do BA albo 1 karo (o ile jest 4 karo )&lt;/font&gt;
 &lt;br&gt;→ 12-17 PC, układ 4414  tzw TRÓJKOLORÓWKA (singiel karo )
 &lt;br&gt;→ 12-14 PC, skład bez atutowy  tzw. PRZYGOTOWAWCZE  (słabe NT) 
@@ -76,101 +81,107 @@
 uwaga: może też być licytowane przy założeniu że partner ma skład zrównoważony i jak powiem coś innego na co on spasuje (bez punktów) i ucieknie nam końcówka (np. na układzie 5-4 lub 6-4 – układy na dwóch piątkach raczej wykluczone)</t>
   </si>
   <si>
-    <t>F1</t>
-  </si>
-  <si>
-    <t>Relay</t>
-  </si>
-  <si>
-    <t>D</t>
-  </si>
-  <si>
-    <t>Trójznaczne karo</t>
-  </si>
-  <si>
-    <t>Trójznaczne słaby  forsing na 1 okrążenie &lt;br&gt; → tzw. negat , 0-6(8) PC, skład dowolny  (w kolejnym okrążeniu możliwy pas jeżeli jest 0-4 PC) 
+    <t xml:space="preserve">F1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Relay</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Trójznaczne karo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Trójznaczne słaby  forsing na 1 okrążenie &lt;br&gt; → tzw. negat , 0-6(8) PC, skład dowolny  (w kolejnym okrążeniu możliwy pas jeżeli jest 0-4 PC) 
 &lt;br&gt;→ 16+ PC, skład dowolny *  (w kolejnym okrążeniu przeskok) &lt;font color=red&gt;[skład bez starszych czwórek- patrz niżej i młodszych piątek – skład zrównoważony– chyba sensownie, ale karta niedobra do zajęcia BA i na 12-16PC!!!!] &lt;/font&gt;
 &lt;br&gt;→ 7-10(11)  PC, 5+ karo  (w kolejny okrążeniu powtarza kolor karowy)
 (inna opcja to 7(9)-11 PC, SKŁAD NIEZRÓWNOWAŻONY – chyba fajne - młodsza szóstka, bez czwórki starsze lub układ 5/4 na młodszych! Ale jak to dalej zgłaszać?? )</t>
   </si>
   <si>
-    <t>H</t>
-  </si>
-  <si>
-    <t>czwórka</t>
-  </si>
-  <si>
-    <t>Kolor kierowy (4) lub trójkolorówka z singlem karo</t>
-  </si>
-  <si>
-    <t>→ 12-14 PC   4 kier (kier nie wykluczają pik), forsuje do 1BA &lt;br&gt;&lt;font color=red&gt;[uwaga – układ raczej zrównoważony – ew propozycja nawet od 3 kart??- bez sensu wg mnie ale konieczne jeżeli poniżej silne BA]&lt;/font&gt;
+    <t xml:space="preserve">H</t>
+  </si>
+  <si>
+    <t xml:space="preserve">czwórka</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kolor kierowy (4) lub trójkolorówka z singlem karo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">→ 12-14 PC   4 kier (kier nie wykluczają pik), forsuje do 1BA &lt;br&gt;&lt;font color=red&gt;[uwaga – układ raczej zrównoważony – ew propozycja nawet od 3 kart??- bez sensu wg mnie ale konieczne jeżeli poniżej silne BA]&lt;/font&gt;
  &lt;br&gt;→ TRÓJKOLORÓWKA  cała → 12-17PC 4414, nie forsuje</t>
   </si>
   <si>
-    <t>Słaba</t>
-  </si>
-  <si>
-    <t>P</t>
-  </si>
-  <si>
-    <t>???</t>
-  </si>
-  <si>
-    <t>Bardzo słabe</t>
-  </si>
-  <si>
-    <t>Pas (ale co z układem ???)</t>
-  </si>
-  <si>
-    <t>S</t>
-  </si>
-  <si>
-    <t>NT</t>
-  </si>
-  <si>
-    <t>Negat</t>
-  </si>
-  <si>
-    <t>(dawnej nawet 5-6(7)PC na co otwierający pasuje ze słabym NT a licytuje  dalej z innymi układami.</t>
-  </si>
-  <si>
-    <t>I</t>
-  </si>
-  <si>
-    <t>5+</t>
-  </si>
-  <si>
-    <t>Słabe poparcie na 5 treflach</t>
-  </si>
-  <si>
-    <t>7-10 na (5)6+ trefl</t>
-  </si>
-  <si>
-    <t>Słabe poparcie na 5 karach</t>
-  </si>
-  <si>
-    <t>7-10  na 5+ karo</t>
-  </si>
-  <si>
-    <t>4+</t>
-  </si>
-  <si>
-    <t>Silne poparcie na 4 kierach</t>
-  </si>
-  <si>
-    <t>16+ PC 4+ kier</t>
-  </si>
-  <si>
-    <t>FD</t>
-  </si>
-  <si>
-    <t>Silne</t>
-  </si>
-  <si>
-    <t>REWERS</t>
+    <t xml:space="preserve">Słaba</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P</t>
+  </si>
+  <si>
+    <t xml:space="preserve">???</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bardzo słabe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pas (ale co z układem ???)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Negat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(dawnej nawet 5-6(7)PC na co otwierający pasuje ze słabym NT a licytuje  dalej z innymi układami.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Słabe poparcie na 5 treflach</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7-10 na (5)6+ trefl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Słabe poparcie na 5 karach</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7-10  na 5+ karo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Silne poparcie na 4 kierach</t>
+  </si>
+  <si>
+    <t xml:space="preserve">16+ PC 4+ kier</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Silne</t>
+  </si>
+  <si>
+    <t xml:space="preserve">REWERS</t>
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
       <t xml:space="preserve">16</t>
     </r>
     <r>
@@ -184,13 +195,19 @@
     </r>
   </si>
   <si>
-    <t>0+</t>
-  </si>
-  <si>
-    <t>Mocne BA</t>
+    <t xml:space="preserve">0+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mocne BA</t>
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
       <t xml:space="preserve">dalej 3</t>
     </r>
     <r>
@@ -205,28 +222,34 @@
     </r>
   </si>
   <si>
-    <t>16PC+ na  5+ trefl</t>
-  </si>
-  <si>
-    <t>16PC+ na  5+ karo</t>
-  </si>
-  <si>
-    <t>Kolor pikowy (4)</t>
-  </si>
-  <si>
-    <t>→ 12-14 PC  dokładnie 4 pik (kier wykluczone ), forsuje do 1BA &lt;br&gt;&lt;font color=red&gt;[uwaga – układ raczej zrównoważony – ew propozycja nawet od 3 kart??- bez sensu wg mnie ale konieczne jeżeli poniżej silne BA]&lt;/font&gt;</t>
-  </si>
-  <si>
-    <t>słaba</t>
-  </si>
-  <si>
-    <t>16+ PC 6+ kier   (REWERS) odzywka skacząca w drugi starszy wymusza zgłoszenie 3BA przez odpowiadającego o ile ma słabe otwarcie, a jeżeli nie to coś sobie dalej powie..</t>
-  </si>
-  <si>
-    <t>Silne poparcie</t>
+    <t xml:space="preserve">16PC+ na  5+ trefl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">16PC+ na  5+ karo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kolor pikowy (4)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">→ 12-14 PC  dokładnie 4 pik (kier wykluczone ), forsuje do 1BA &lt;br&gt;&lt;font color=red&gt;[uwaga – układ raczej zrównoważony – ew propozycja nawet od 3 kart??- bez sensu wg mnie ale konieczne jeżeli poniżej silne BA]&lt;/font&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">słaba</t>
+  </si>
+  <si>
+    <t xml:space="preserve">16+ PC 6+ kier   (REWERS) odzywka skacząca w drugi starszy wymusza zgłoszenie 3BA przez odpowiadającego o ile ma słabe otwarcie, a jeżeli nie to coś sobie dalej powie..</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Silne poparcie</t>
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
       <t xml:space="preserve">16</t>
     </r>
     <r>
@@ -241,6 +264,12 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
       <t xml:space="preserve">dalej 3</t>
     </r>
     <r>
@@ -255,91 +284,97 @@
     </r>
   </si>
   <si>
-    <t>zrównoważony</t>
-  </si>
-  <si>
-    <t>1BA 18-20 PC  [dawniej 12-14 PC] skład zrównoważony bez starszej czwórki, nie wyklucza piątki trefl, nie forsuje [ ale jak wtedy zgłosić słabe BA? - chyba jednen w starszy – może być mylące?] &lt;b&gt; &lt;strong&gt; Dalej Stayman i teksasy tylko z punktami jak wcześniej (patrz licytacja po 1BA) &lt;font color = red&gt; POWINNO MOŻE PRZESKAKIWIAĆ DO NT? Albo tu przepisać wszystkie odzywki do NT? &lt;strong&gt; &lt;b&gt;</t>
-  </si>
-  <si>
-    <t>Naturalna</t>
-  </si>
-  <si>
-    <t>bez starszej czwórki nie wyklucza 5 trefl</t>
-  </si>
-  <si>
-    <t>Słabsze BA</t>
-  </si>
-  <si>
-    <t>15-17  PC,  5+ trefli (nie forsuje) -  bez ztarszej czwórki!!! słabsze trefle traktujemy 1 BA (patrz wyżej)</t>
-  </si>
-  <si>
-    <t>Nic</t>
-  </si>
-  <si>
-    <t>Pas – 0-6 PC</t>
-  </si>
-  <si>
-    <t>2 10+PC – układ  dowolny – forsing do dogranej (GF) – dalsza licytacja ???</t>
-  </si>
-  <si>
-    <t>GF</t>
-  </si>
-  <si>
-    <t>STOP</t>
-  </si>
-  <si>
-    <t>(przeskok) – 16+PC czwórka w starszym (?)  - lepszy kolor?</t>
-  </si>
-  <si>
-    <t>nie wiem</t>
-  </si>
-  <si>
-    <t>?</t>
-  </si>
-  <si>
-    <t>3+ - fit!</t>
-  </si>
-  <si>
-    <t>fit</t>
-  </si>
-  <si>
-    <t>7-9 PC, 3+trefl -  (fit)</t>
-  </si>
-  <si>
-    <t>niezrównoważony</t>
-  </si>
-  <si>
-    <t>ACOL</t>
-  </si>
-  <si>
-    <t>forsujące do dogranej  wg WJ2005 wyklucza dwukolorówkę → (dawniej 19)23+  PC skład niezrównoważony (może być 5 starsza)  → 25+ PC  skład zrównoważony  Dalej licytacja w zasadzie naturalna poza negatem 2 kier</t>
-  </si>
-  <si>
-    <t>wtórny negat</t>
-  </si>
-  <si>
-    <t>wtórny negat 0-3 PC   (nie mam koloru i nie mogę zająć bez atu, ewentualnie mam słabe kiery ale na to nie licz, dalej pas (po BA) albo ewentualnie kiery? )</t>
-  </si>
-  <si>
-    <t>4s 5m</t>
-  </si>
-  <si>
-    <t>odpowiedź</t>
-  </si>
-  <si>
-    <t>(2) 4-6 PC na  4+ kart  w starszy (lub 4s-5m), 5+ młodszy (wyklucza starszą)</t>
-  </si>
-  <si>
-    <t>bez atu</t>
-  </si>
-  <si>
-    <t>4-6 PC zrównoważony (nie wyklucza czwórki) – dalej 3 jest Staymanem</t>
-  </si>
-  <si>
-    <t>Splinter</t>
+    <t xml:space="preserve">zrównoważony</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1BA 18-20 PC  [dawniej 12-14 PC] skład zrównoważony bez starszej czwórki, nie wyklucza piątki trefl, nie forsuje [ ale jak wtedy zgłosić słabe BA? - chyba jednen w starszy – może być mylące?] &lt;b&gt; &lt;strong&gt; Dalej Stayman i teksasy tylko z punktami jak wcześniej (patrz licytacja po 1BA) &lt;font color = red&gt; POWINNO MOŻE PRZESKAKIWIAĆ DO NT? Albo tu przepisać wszystkie odzywki do NT? &lt;strong&gt; &lt;b&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Naturalna</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bez starszej czwórki nie wyklucza 5 trefl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Słabsze BA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15-17  PC,  5+ trefli (nie forsuje) -  bez ztarszej czwórki!!! słabsze trefle traktujemy 1 BA (patrz wyżej)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pas – 0-6 PC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 10+PC – układ  dowolny – forsing do dogranej (GF) – dalsza licytacja ???</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">STOP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(przeskok) – 16+PC czwórka w starszym (?)  - lepszy kolor?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nie wiem</t>
+  </si>
+  <si>
+    <t xml:space="preserve">?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3+ - fit!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7-9 PC, 3+trefl -  (fit)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">niezrównoważony</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ACOL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">forsujące do dogranej  wg WJ2005 wyklucza dwukolorówkę → (dawniej 19)23+  PC skład niezrównoważony (może być 5 starsza)  → 25+ PC  skład zrównoważony  Dalej licytacja w zasadzie naturalna poza negatem 2 kier</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wtórny negat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wtórny negat 0-3 PC   (nie mam koloru i nie mogę zająć bez atu, ewentualnie mam słabe kiery ale na to nie licz, dalej pas (po BA) albo ewentualnie kiery? )</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4s 5m</t>
+  </si>
+  <si>
+    <t xml:space="preserve">odpowiedź</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(2) 4-6 PC na  4+ kart  w starszy (lub 4s-5m), 5+ młodszy (wyklucza starszą)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bez atu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4-6 PC zrównoważony (nie wyklucza czwórki) – dalej 3 jest Staymanem</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Splinter</t>
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
       <t xml:space="preserve">7-10(11)</t>
     </r>
     <r>
@@ -353,22 +388,28 @@
     </r>
   </si>
   <si>
-    <t>5 dokładnie</t>
-  </si>
-  <si>
-    <t>silny kolor starszy</t>
-  </si>
-  <si>
-    <t>18+ PC, dokładnie 5 kart w kierach  kolorze starszym (mniejsza siła bez przeskoku! - silny naturalny inwit)</t>
-  </si>
-  <si>
-    <t>18+ PC, dokładnie 5 kart w pikach kolorze starszym (mniejsza siła bez przeskoku! - silny naturalny inwit)</t>
-  </si>
-  <si>
-    <t>Srednie Bez Atu</t>
+    <t xml:space="preserve">5 dokładnie</t>
+  </si>
+  <si>
+    <t xml:space="preserve">silny kolor starszy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">18+ PC, dokładnie 5 kart w kierach  kolorze starszym (mniejsza siła bez przeskoku! - silny naturalny inwit)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">18+ PC, dokładnie 5 kart w pikach kolorze starszym (mniejsza siła bez przeskoku! - silny naturalny inwit)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Srednie Bez Atu</t>
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
       <t xml:space="preserve">   2BA  22-24 PC skład zrównoważony) - inwit  dalej </t>
     </r>
     <r>
@@ -382,19 +423,25 @@
     </r>
   </si>
   <si>
-    <t>6+</t>
-  </si>
-  <si>
-    <t>silny młodszy</t>
-  </si>
-  <si>
-    <t>18+ PC, 6+kart w młodszym bez starszej czwórki -naturalny silny inwit</t>
-  </si>
-  <si>
-    <t>długi starszy</t>
+    <t xml:space="preserve">6+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">silny młodszy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">18+ PC, 6+kart w młodszym bez starszej czwórki -naturalny silny inwit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">długi starszy</t>
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
       <t xml:space="preserve">3 </t>
     </r>
     <r>
@@ -408,26 +455,32 @@
     </r>
   </si>
   <si>
-    <t>słabe BA</t>
-  </si>
-  <si>
-    <t>3BA     18-21 PC i skład bezatutowy  - kontrakt jeżeli negat  końcówka jeżeli kara (choć często próba wzięcia 9 lew na karach)</t>
-  </si>
-  <si>
-    <t>4+ kier, nie limitowane</t>
-  </si>
-  <si>
-    <t>4+ kier,  forsuje na jedno okrążenie
+    <t xml:space="preserve">słabe BA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3BA     18-21 PC i skład bezatutowy  - kontrakt jeżeli negat  końcówka jeżeli kara (choć często próba wzięcia 9 lew na karach)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4+ kier, nie limitowane</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4+ kier,  forsuje na jedno okrążenie
 &lt;br&gt;  →  kiery nie wykluczają pików przy 4 kartach &lt;br&gt; → nie wyklucza młodszej piątki przy sile poniżej 11PC &lt;br&gt; przy dwóch starszych zgłaszam  dłuższy - przy dwóch czwórkach kierową, przy dwóch piątkach pikową :)</t>
   </si>
   <si>
-    <t>4+ pik, nie limitowane</t>
-  </si>
-  <si>
-    <t>forsuje na jedno okrążenie  : &lt;br&gt; → 12-14(17) PC, 4pików (dokładnie), brak 4 kierów (słabe BA), &lt;br&gt; → 15+ PC 5+ trefli i 4 pik (w kolejnym okrążeniu trefl – dalej forsuje),  &lt;br&gt; → 18+ (4)5+ pik! (w kolejnym okrążeniu  piki = 18+PC i 5+pik i to forsuje do końcówki)</t>
+    <t xml:space="preserve">4+ pik, nie limitowane</t>
+  </si>
+  <si>
+    <t xml:space="preserve">forsuje na jedno okrążenie  : &lt;br&gt; → 12-14(17) PC, 4pików (dokładnie), brak 4 kierów (słabe BA), &lt;br&gt; → 15+ PC 5+ trefli i 4 pik (w kolejnym okrążeniu trefl – dalej forsuje),  &lt;br&gt; → 18+ (4)5+ pik! (w kolejnym okrążeniu  piki = 18+PC i 5+pik i to forsuje do końcówki)</t>
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
       <t xml:space="preserve">1BA  7-10PC skład zrównoważony brak 4</t>
     </r>
     <r>
@@ -441,16 +494,22 @@
     </r>
   </si>
   <si>
-    <t>NF</t>
-  </si>
-  <si>
-    <t>4(5)+ kierów</t>
-  </si>
-  <si>
-    <t>Magister</t>
+    <t xml:space="preserve">NF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4(5)+ kierów</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Magister</t>
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="7"/>
+        <rFont val="Symbol"/>
+        <family val="1"/>
+        <charset val="2"/>
+      </rPr>
       <t xml:space="preserve">2 </t>
     </r>
     <r>
@@ -465,13 +524,19 @@
     </r>
   </si>
   <si>
-    <t>4 kiery i 5+ kar</t>
-  </si>
-  <si>
-    <t>kolor karowy</t>
+    <t xml:space="preserve">4 kiery i 5+ kar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kolor karowy</t>
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
       <t xml:space="preserve">2 ♦   7-10 PC, 4</t>
     </r>
     <r>
@@ -485,10 +550,16 @@
     </r>
   </si>
   <si>
-    <t>kolor kierowy</t>
+    <t xml:space="preserve">kolor kierowy</t>
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
       <t xml:space="preserve">2</t>
     </r>
     <r>
@@ -502,13 +573,19 @@
     </r>
   </si>
   <si>
-    <t>na starszych 4-4 lub 5-4</t>
-  </si>
-  <si>
-    <t>sprzedaż układu</t>
+    <t xml:space="preserve">na starszych 4-4 lub 5-4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sprzedaż układu</t>
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Symbol"/>
+        <family val="1"/>
+        <charset val="2"/>
+      </rPr>
       <t xml:space="preserve">2   </t>
     </r>
     <r>
@@ -522,10 +599,16 @@
     </r>
   </si>
   <si>
-    <t>inwit do 3 NT</t>
+    <t xml:space="preserve">inwit do 3 NT</t>
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="7"/>
+        <rFont val="Symbol"/>
+        <family val="1"/>
+        <charset val="2"/>
+      </rPr>
       <t xml:space="preserve">2BA </t>
     </r>
     <r>
@@ -539,13 +622,19 @@
     </r>
   </si>
   <si>
-    <t>5 kierów i młodsza piątka</t>
-  </si>
-  <si>
-    <t>forsing do końcówki kolorowej</t>
+    <t xml:space="preserve">5 kierów i młodsza piątka</t>
+  </si>
+  <si>
+    <t xml:space="preserve">forsing do końcówki kolorowej</t>
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Symbol"/>
+        <family val="1"/>
+        <charset val="2"/>
+      </rPr>
       <t xml:space="preserve">3/3</t>
     </r>
     <r>
@@ -559,13 +648,19 @@
     </r>
   </si>
   <si>
-    <t>6 kierów / lub 4- 4</t>
-  </si>
-  <si>
-    <t>inwit do 4 kier</t>
+    <t xml:space="preserve">6 kierów / lub 4- 4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">inwit do 4 kier</t>
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
       <t xml:space="preserve">3</t>
     </r>
     <r>
@@ -579,13 +674,19 @@
     </r>
   </si>
   <si>
-    <t>inwit do 4 pik</t>
-  </si>
-  <si>
-    <t>kontakt 3NT</t>
+    <t xml:space="preserve">inwit do 4 pik</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kontakt 3NT</t>
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
       <t xml:space="preserve">3BA 13-16PC  skład zrównoważony, brak 4</t>
     </r>
     <r>
@@ -599,10 +700,16 @@
     </r>
   </si>
   <si>
-    <t>Kontrakt 4 kier</t>
+    <t xml:space="preserve">Kontrakt 4 kier</t>
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
       <t xml:space="preserve">4</t>
     </r>
     <r>
@@ -616,62 +723,68 @@
     </r>
   </si>
   <si>
-    <t>Kontrakt 4 pik</t>
-  </si>
-  <si>
-    <t>bez starszej czwórki</t>
-  </si>
-  <si>
-    <t>Brak koloru</t>
-  </si>
-  <si>
-    <t>1BA  12-14 PC, bez starszej czwórki (po pikach nie wyklucza 4 kierów)</t>
-  </si>
-  <si>
-    <t>Relay Magister</t>
-  </si>
-  <si>
-    <t>RELAY -  MAGISTER – pytanie o PC i kiery  &lt;br&gt;  → 10+ PC, 5+kiery     &lt;br&gt;  → ewentualnie  16+PC, 4+kiery     &lt;br&gt; [ → ew. 7-10PC 4kiery  i 5+trefli (odpowiedzi patrz niżej)  &lt;br&gt; &lt;strong&gt; gadżet  MAGISTER(zwany też PRO pytający rebid odpowiadającego:
+    <t xml:space="preserve">Kontrakt 4 pik</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bez starszej czwórki</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Brak koloru</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1BA  12-14 PC, bez starszej czwórki (po pikach nie wyklucza 4 kierów)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Relay Magister</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RELAY -  MAGISTER – pytanie o PC i kiery  &lt;br&gt;  → 10+ PC, 5+kiery     &lt;br&gt;  → ewentualnie  16+PC, 4+kiery     &lt;br&gt; [ → ew. 7-10PC 4kiery  i 5+trefli (odpowiedzi patrz niżej)  &lt;br&gt; &lt;strong&gt; gadżet  MAGISTER(zwany też PRO pytający rebid odpowiadającego:
 (pytanie o liczbę kart w kolorze, czyli ma sens chyba jeżeli sam ma więcej w starszy i trefle???) &lt;strong&gt;</t>
   </si>
   <si>
-    <t>2kiery</t>
-  </si>
-  <si>
-    <t>Odpowiedź Magister</t>
-  </si>
-  <si>
-    <t>2♦ - 12-13 PC, dubel w kolor (fit 2 kartowy)</t>
-  </si>
-  <si>
-    <t>4 (5) pik – brak fitu, dużo terfli</t>
-  </si>
-  <si>
-    <t>Rebid Magister</t>
-  </si>
-  <si>
-    <t>Sing off – do gry – też na innej wysokości</t>
-  </si>
-  <si>
-    <t>5 pików</t>
-  </si>
-  <si>
-    <t>→ 2 kiery / piki jest 10-12PC i kierach (można przenieść na 2BA)</t>
-  </si>
-  <si>
-    <t>'4+pików</t>
-  </si>
-  <si>
-    <t>→  2BA jest forsująca !</t>
-  </si>
-  <si>
-    <t>3 kiery</t>
-  </si>
-  <si>
-    <t>2♥ (kolor partnera) - 12-13 PC - 3 karty w kolor (fit 3 kartowy)</t>
+    <t xml:space="preserve">2kiery</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Odpowiedź Magister</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2♦ - 12-13 PC, dubel w kolor (fit 2 kartowy)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4 (5) pik – brak fitu, dużo terfli</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rebid Magister</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sing off – do gry – też na innej wysokości</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5 pików</t>
+  </si>
+  <si>
+    <t xml:space="preserve">→ 2 kiery / piki jest 10-12PC i kierach (można przenieść na 2BA)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">'4+pików</t>
+  </si>
+  <si>
+    <t xml:space="preserve">→  2BA jest forsująca !</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3 kiery</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2♥ (kolor partnera) - 12-13 PC - 3 karty w kolor (fit 3 kartowy)</t>
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
       <t xml:space="preserve">2</t>
     </r>
     <r>
@@ -685,16 +798,22 @@
     </r>
   </si>
   <si>
-    <t>2kiery brak 4 trefli</t>
-  </si>
-  <si>
-    <t>2BA - 14-15, dubel w kolor, brak 4 trefli (fit 2 kartowy)</t>
-  </si>
-  <si>
-    <t>2kiery i 4 trefli</t>
+    <t xml:space="preserve">2kiery brak 4 trefli</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2BA - 14-15, dubel w kolor, brak 4 trefli (fit 2 kartowy)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2kiery i 4 trefli</t>
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
       <t xml:space="preserve">3</t>
     </r>
     <r>
@@ -708,32 +827,38 @@
     </r>
   </si>
   <si>
-    <t>5+ (ew 4)</t>
-  </si>
-  <si>
-    <t>RELAY -  MAGISTER – pytanie o PC i piki  &lt;br&gt;  → 10+ PC, 5+pik     &lt;br&gt;  → ewentualnie  16+PC, 4+pik     &lt;br&gt; [ → ew. 7-10PC 4pik  i 5+trefli (odpowiedzi patrz niżej)  &lt;br&gt; &lt;strong&gt; gadżet  MAGISTER(zwany też PRO pytający rebid odpowiadającego:
+    <t xml:space="preserve">5+ (ew 4)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RELAY -  MAGISTER – pytanie o PC i piki  &lt;br&gt;  → 10+ PC, 5+pik     &lt;br&gt;  → ewentualnie  16+PC, 4+pik     &lt;br&gt; [ → ew. 7-10PC 4pik  i 5+trefli (odpowiedzi patrz niżej)  &lt;br&gt; &lt;strong&gt; gadżet  MAGISTER(zwany też PRO pytający rebid odpowiadającego:
 (pytanie o liczbę kart w kolorze, czyli ma sens chyba jeżeli sam ma więcej w starszy i trefle???) &lt;strong&gt;</t>
   </si>
   <si>
-    <t>2 pik</t>
-  </si>
-  <si>
-    <t>3 piki</t>
-  </si>
-  <si>
-    <t>→ jest 10-12PC i (4)5+ kier (można przenieść na 2BA)</t>
-  </si>
-  <si>
-    <t>2 pik brak 4 trefli</t>
-  </si>
-  <si>
-    <t>→ jest 10-12PC i (4)5+ pik (można przenieść na 2BA)</t>
-  </si>
-  <si>
-    <t>2 piki i 4 trefli</t>
+    <t xml:space="preserve">2 pik</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3 piki</t>
+  </si>
+  <si>
+    <t xml:space="preserve">→ jest 10-12PC i (4)5+ kier (można przenieść na 2BA)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 pik brak 4 trefli</t>
+  </si>
+  <si>
+    <t xml:space="preserve">→ jest 10-12PC i (4)5+ pik (można przenieść na 2BA)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 piki i 4 trefli</t>
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
       <t xml:space="preserve">3</t>
     </r>
     <r>
@@ -747,10 +872,16 @@
     </r>
   </si>
   <si>
-    <t>4 s + 5 karo</t>
+    <t xml:space="preserve">4 s + 5 karo</t>
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
       <t xml:space="preserve"> 7-10 PC, 4</t>
     </r>
     <r>
@@ -764,19 +895,25 @@
     </r>
   </si>
   <si>
-    <t>5+ kierów</t>
-  </si>
-  <si>
-    <t>Do gry</t>
-  </si>
-  <si>
-    <t>(kolor zgłoszony w pierwszym okrążeniu) 7-10 PC, 5+ kier  (sing off)</t>
-  </si>
-  <si>
-    <t>5 kierów i 4 piki</t>
+    <t xml:space="preserve">5+ kierów</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Do gry</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(kolor zgłoszony w pierwszym okrążeniu) 7-10 PC, 5+ kier  (sing off)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5 kierów i 4 piki</t>
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
       <t xml:space="preserve">REWERS  12+ PC  5+ </t>
     </r>
     <r>
@@ -790,58 +927,64 @@
     </r>
   </si>
   <si>
-    <t>5+ trefli</t>
-  </si>
-  <si>
-    <t>inwit do 3 NT/ Magister INŻYNIER</t>
-  </si>
-  <si>
-    <t>2BA 11-12 PC skład zrównoważony inwit do 3BA – ??????? albo  (AUTORELAY) - gadżet  MAGISTER INŻYNIER (jak MAGISTER.  oraz 5+ trefli!)</t>
-  </si>
-  <si>
-    <t>AUTOMAT</t>
-  </si>
-  <si>
-    <t>automat (tego co zaczął) i potem warianty (ten co zgłosił kolor i inżyniera):</t>
-  </si>
-  <si>
-    <t>6 trefli i 4 w kolor</t>
-  </si>
-  <si>
-    <t>odpowiedź na Inzyniera</t>
-  </si>
-  <si>
-    <t>pas - 6-9 PC, 6 trefli, 4 w kolor</t>
-  </si>
-  <si>
-    <t>6 trefli, 4 3 kolor i krótkość w karo</t>
-  </si>
-  <si>
-    <t>2♦ - 10-11 PC, 6 trefli, 4  w kolor, krótkość karo</t>
-  </si>
-  <si>
-    <t>6 trefli 4 w kolor (piki) i krótkość kier</t>
-  </si>
-  <si>
-    <t>2♥ - (po pikach) - 10-11 PC, 6 trefli, 4  w kolor(piki), krótkość kier</t>
-  </si>
-  <si>
-    <t>5 + w kolor, 5 trefli</t>
-  </si>
-  <si>
-    <t>3 w kolor odpowiedzi  - 5+ w kolor, 5+ trefli, forsing do końcówki</t>
-  </si>
-  <si>
-    <t>5 trefli 4 kiery</t>
-  </si>
-  <si>
-    <t>3BA - maksimum siły, 5+ trefli, 4 kiery</t>
-  </si>
-  <si>
-    <t>5 kierów i 5 trefli</t>
+    <t xml:space="preserve">5+ trefli</t>
+  </si>
+  <si>
+    <t xml:space="preserve">inwit do 3 NT/ Magister INŻYNIER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2BA 11-12 PC skład zrównoważony inwit do 3BA – ??????? albo  (AUTORELAY) - gadżet  MAGISTER INŻYNIER (jak MAGISTER.  oraz 5+ trefli!)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AUTOMAT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">automat (tego co zaczął) i potem warianty (ten co zgłosił kolor i inżyniera):</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6 trefli i 4 w kolor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">odpowiedź na Inzyniera</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pas - 6-9 PC, 6 trefli, 4 w kolor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6 trefli, 4 3 kolor i krótkość w karo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2♦ - 10-11 PC, 6 trefli, 4  w kolor, krótkość karo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6 trefli 4 w kolor (piki) i krótkość kier</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2♥ - (po pikach) - 10-11 PC, 6 trefli, 4  w kolor(piki), krótkość kier</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5 + w kolor, 5 trefli</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3 w kolor odpowiedzi  - 5+ w kolor, 5+ trefli, forsing do końcówki</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5 trefli 4 kiery</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3BA - maksimum siły, 5+ trefli, 4 kiery</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5 kierów i 5 trefli</t>
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Symbol"/>
+        <family val="1"/>
+        <charset val="2"/>
+      </rPr>
       <t xml:space="preserve">3/3</t>
     </r>
     <r>
@@ -855,13 +998,19 @@
     </r>
   </si>
   <si>
-    <t>5 kierów i 5 kar</t>
-  </si>
-  <si>
-    <t>Inwit do końcówki</t>
+    <t xml:space="preserve">5 kierów i 5 kar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Inwit do końcówki</t>
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
       <t xml:space="preserve">3</t>
     </r>
     <r>
@@ -875,13 +1024,19 @@
     </r>
   </si>
   <si>
-    <t>6 kierów  krótkość w pikach</t>
-  </si>
-  <si>
-    <t>AUTOSPLINTER</t>
+    <t xml:space="preserve">6 kierów  krótkość w pikach</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AUTOSPLINTER</t>
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="7"/>
+        <rFont val="Symbol"/>
+        <family val="1"/>
+        <charset val="2"/>
+      </rPr>
       <t xml:space="preserve">3  [</t>
     </r>
     <r>
@@ -895,13 +1050,19 @@
     </r>
   </si>
   <si>
-    <t>3BA 13-16 PC, skład zrównoważony (sing off) do gry</t>
-  </si>
-  <si>
-    <t>6+ krótkość trefl</t>
+    <t xml:space="preserve">3BA 13-16 PC, skład zrównoważony (sing off) do gry</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6+ krótkość trefl</t>
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="7"/>
+        <rFont val="Symbol"/>
+        <family val="1"/>
+        <charset val="2"/>
+      </rPr>
       <t xml:space="preserve">4/4</t>
     </r>
     <r>
@@ -915,10 +1076,16 @@
     </r>
   </si>
   <si>
-    <t>6+ krótkośc karo</t>
+    <t xml:space="preserve">6+ krótkośc karo</t>
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
       <t xml:space="preserve">4</t>
     </r>
     <r>
@@ -932,13 +1099,19 @@
     </r>
   </si>
   <si>
-    <t>5+ trefl, brak starszej czwórki</t>
-  </si>
-  <si>
-    <t>Naturalne silny 1 trefl</t>
+    <t xml:space="preserve">5+ trefl, brak starszej czwórki</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Naturalne silny 1 trefl</t>
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
       <t xml:space="preserve">2</t>
     </r>
     <r>
@@ -952,10 +1125,16 @@
     </r>
   </si>
   <si>
-    <t>prawie dowolny</t>
+    <t xml:space="preserve">prawie dowolny</t>
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
       <t xml:space="preserve">2</t>
     </r>
     <r>
@@ -969,10 +1148,16 @@
     </r>
   </si>
   <si>
-    <t>5+ w kolor</t>
+    <t xml:space="preserve">5+ w kolor</t>
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
       <t xml:space="preserve">2</t>
     </r>
     <r>
@@ -986,10 +1171,16 @@
     </r>
   </si>
   <si>
-    <t>4+ kierów i 4 piki</t>
+    <t xml:space="preserve">4+ kierów i 4 piki</t>
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
       <t xml:space="preserve">2 </t>
     </r>
     <r>
@@ -1003,10 +1194,16 @@
     </r>
   </si>
   <si>
-    <t>Dokładnie 4 kiery, brak drugiej czwórki</t>
+    <t xml:space="preserve">Dokładnie 4 kiery, brak drugiej czwórki</t>
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
       <t xml:space="preserve">2BA   7-9(10) PC, dokładnie 4 </t>
     </r>
     <r>
@@ -1020,10 +1217,16 @@
     </r>
   </si>
   <si>
-    <t>3 + fit pikowy</t>
+    <t xml:space="preserve">3 + fit pikowy</t>
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
       <t xml:space="preserve">3</t>
     </r>
     <r>
@@ -1037,10 +1240,16 @@
     </r>
   </si>
   <si>
-    <t>5 + w kolor, 5 kar</t>
+    <t xml:space="preserve">5 + w kolor, 5 kar</t>
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
       <t xml:space="preserve">3</t>
     </r>
     <r>
@@ -1054,10 +1263,16 @@
     </r>
   </si>
   <si>
-    <t>6+ w kolor</t>
+    <t xml:space="preserve">6+ w kolor</t>
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
       <t xml:space="preserve">3</t>
     </r>
     <r>
@@ -1071,10 +1286,16 @@
     </r>
   </si>
   <si>
-    <t>5 kierów i 5+ pików</t>
+    <t xml:space="preserve">5 kierów i 5+ pików</t>
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
       <t xml:space="preserve">REWERS [ tylko po piku] 10+PC,  5+ </t>
     </r>
     <r>
@@ -1088,13 +1309,19 @@
     </r>
   </si>
   <si>
-    <t>3 fit</t>
-  </si>
-  <si>
-    <t>ODWROTKA</t>
+    <t xml:space="preserve">3 fit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ODWROTKA</t>
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="7"/>
+        <rFont val="Symbol"/>
+        <family val="1"/>
+        <charset val="2"/>
+      </rPr>
       <t xml:space="preserve">2</t>
     </r>
     <r>
@@ -1108,13 +1335,19 @@
     </r>
   </si>
   <si>
-    <t>4 kiery</t>
-  </si>
-  <si>
-    <t>odpowiedź na odwrotkę</t>
+    <t xml:space="preserve">4 kiery</t>
+  </si>
+  <si>
+    <t xml:space="preserve">odpowiedź na odwrotkę</t>
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
       <t xml:space="preserve">2</t>
     </r>
     <r>
@@ -1129,6 +1362,12 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
       <t xml:space="preserve">2</t>
     </r>
     <r>
@@ -1142,13 +1381,19 @@
     </r>
   </si>
   <si>
-    <t>5 kierów</t>
-  </si>
-  <si>
-    <t>2BA   7-9(10) PC, 5 kierów(pików)             (Bubrotka – 11+ PC 5+ w starszym)</t>
+    <t xml:space="preserve">5 kierów</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2BA   7-9(10) PC, 5 kierów(pików)             (Bubrotka – 11+ PC 5+ w starszym)</t>
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
       <t xml:space="preserve">3</t>
     </r>
     <r>
@@ -1162,10 +1407,16 @@
     </r>
   </si>
   <si>
-    <t>6 kierów</t>
+    <t xml:space="preserve">6 kierów</t>
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
       <t xml:space="preserve">3</t>
     </r>
     <r>
@@ -1180,10 +1431,16 @@
     </r>
   </si>
   <si>
-    <t>Na 5 (układ 5332)</t>
+    <t xml:space="preserve">Na 5 (układ 5332)</t>
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
       <t xml:space="preserve">3</t>
     </r>
     <r>
@@ -1198,6 +1455,12 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="7"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
       <t xml:space="preserve">3</t>
     </r>
     <r>
@@ -1211,13 +1474,19 @@
     </r>
   </si>
   <si>
-    <t>4 karty</t>
-  </si>
-  <si>
-    <t>czwórka w kierach</t>
+    <t xml:space="preserve">4 karty</t>
+  </si>
+  <si>
+    <t xml:space="preserve">czwórka w kierach</t>
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
       <t xml:space="preserve">2</t>
     </r>
     <r>
@@ -1235,13 +1504,19 @@
     </r>
   </si>
   <si>
-    <t>5(6) kart</t>
-  </si>
-  <si>
-    <t>własny kolor silny</t>
+    <t xml:space="preserve">5(6) kart</t>
+  </si>
+  <si>
+    <t xml:space="preserve">własny kolor silny</t>
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
       <t xml:space="preserve">REWERS 18+ PC,  5(6) kart drugi starszy, forsing dalej jak po otwarciu jeden w starszy i podniesieniu do 2 </t>
     </r>
     <r>
@@ -1259,10 +1534,16 @@
     </r>
   </si>
   <si>
-    <t>aspiracje szlemikowe</t>
+    <t xml:space="preserve">aspiracje szlemikowe</t>
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="7"/>
+        <rFont val="Symbol"/>
+        <family val="1"/>
+        <charset val="2"/>
+      </rPr>
       <t xml:space="preserve"> 3/</t>
     </r>
     <r>
@@ -1276,13 +1557,19 @@
     </r>
   </si>
   <si>
-    <t>4-4-4-1 lub 4s i 5 trefl</t>
-  </si>
-  <si>
-    <t>inwit do końćówki</t>
+    <t xml:space="preserve">4-4-4-1 lub 4s i 5 trefl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">inwit do końćówki</t>
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="7"/>
+        <rFont val="Symbol"/>
+        <family val="1"/>
+        <charset val="2"/>
+      </rPr>
       <t xml:space="preserve">3 </t>
     </r>
     <r>
@@ -1296,25 +1583,31 @@
     </r>
   </si>
   <si>
-    <t>6+ pików</t>
-  </si>
-  <si>
-    <t>REWERS: 18+ PC, 6+ kart w licytowanym kolorze – aspiracje szlemikowe albo SPLINTER 17-18PC</t>
-  </si>
-  <si>
-    <t>szukanie koloru</t>
-  </si>
-  <si>
-    <t>2BA  18+ PC, brak fitu (po kierze nie wyklucza 4 pik), forsing</t>
-  </si>
-  <si>
-    <t>3BA  14-17PC ?  kontrakt</t>
-  </si>
-  <si>
-    <t>układ</t>
+    <t xml:space="preserve">6+ pików</t>
+  </si>
+  <si>
+    <t xml:space="preserve">REWERS: 18+ PC, 6+ kart w licytowanym kolorze – aspiracje szlemikowe albo SPLINTER 17-18PC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">szukanie koloru</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2BA  18+ PC, brak fitu (po kierze nie wyklucza 4 pik), forsing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3BA  14-17PC ?  kontrakt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">układ</t>
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
       <t xml:space="preserve">4</t>
     </r>
     <r>
@@ -1328,71 +1621,77 @@
     </r>
   </si>
   <si>
-    <t>4ka pik</t>
-  </si>
-  <si>
-    <t>4+ pik,  forsuje na jedno okrążenie 
+    <t xml:space="preserve">4ka pik</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4+ pik,  forsuje na jedno okrążenie 
 &lt;br&gt;  → 4 kiery wykluczone  (5 możliwe) -  nie wyklucza młodszej piątki przy sile poniżej 11PC - przy dwóch starszych zgłaszam dłuższy - przy dwóch czwórkach kierową,  przy dwóch piątkach pikową :)</t>
   </si>
   <si>
-    <t>18+ PC, 5(6)+kart w kolorze - b.dobry kolor -aspiracje szlemikowe</t>
-  </si>
-  <si>
-    <t>18+ PC, 5(6)+ kart w kolorze - b.dobry kolor -aspiracje szlemikowe</t>
-  </si>
-  <si>
-    <t>15-16PC – 4-4-4-1 lub 4 starsza i 5  - inwit do koncówki</t>
-  </si>
-  <si>
-    <t>kontrakt</t>
-  </si>
-  <si>
-    <t>1BA (7)8-10 PC, bez starszej czwórki, może zawierać młodszą piątkę, nie forsuje (przy słabych 7PC lepiej negat)</t>
-  </si>
-  <si>
-    <t>4414 albo zrównoważony</t>
-  </si>
-  <si>
-    <t>negat</t>
-  </si>
-  <si>
-    <t>Pas  12-14 PC układ zrównoważony albo 4414</t>
-  </si>
-  <si>
-    <t>kolor treflowy</t>
-  </si>
-  <si>
-    <t>15+ PC   5+ trefli</t>
-  </si>
-  <si>
-    <t>PYTANIE O SKŁAD</t>
-  </si>
-  <si>
-    <t>18+  PC,RELAY karta układowa (pytanie o skład ) → patrz obok</t>
-  </si>
-  <si>
-    <t>silny kolor kierowy</t>
-  </si>
-  <si>
-    <t>18+  PC, 5 kart  kolor licytowany (bo odpowiadający wykluczył czwórki, gdyby było mniej punktów to otwarcie było by w piki!!!)</t>
-  </si>
-  <si>
-    <t>silny kolor pikowy</t>
-  </si>
-  <si>
-    <t>inwit do szlemika</t>
-  </si>
-  <si>
-    <t>2BA  22-24 PC, układ zrównoważony inwit do szlemika ??? coś było inaczej ale bez sensu</t>
-  </si>
-  <si>
-    <t>3BA  18-21 PC  układ zrównoważony - kontrakt</t>
-  </si>
-  <si>
-    <t>12+  PC, 5+ trefli/kar, forsuje do końcówki  (nie wyklucza starszej czwórki? ) Nie ma sensu przeskakiwać bo i tak licytacja jest sforsowana, otwierający zgłasza starsze czwórki, podniesienie jest fitem bez nadwyżek</t>
+    <t xml:space="preserve">18+ PC, 5(6)+kart w kolorze - b.dobry kolor -aspiracje szlemikowe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">18+ PC, 5(6)+ kart w kolorze - b.dobry kolor -aspiracje szlemikowe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15-16PC – 4-4-4-1 lub 4 starsza i 5  - inwit do koncówki</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kontrakt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1BA (7)8-10 PC, bez starszej czwórki, może zawierać młodszą piątkę, nie forsuje (przy słabych 7PC lepiej negat)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4414 albo zrównoważony</t>
+  </si>
+  <si>
+    <t xml:space="preserve">negat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pas  12-14 PC układ zrównoważony albo 4414</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kolor treflowy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15+ PC   5+ trefli</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PYTANIE O SKŁAD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">18+  PC,RELAY karta układowa (pytanie o skład ) → patrz obok</t>
+  </si>
+  <si>
+    <t xml:space="preserve">silny kolor kierowy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">18+  PC, 5 kart  kolor licytowany (bo odpowiadający wykluczył czwórki, gdyby było mniej punktów to otwarcie było by w piki!!!)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">silny kolor pikowy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">inwit do szlemika</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2BA  22-24 PC, układ zrównoważony inwit do szlemika ??? coś było inaczej ale bez sensu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3BA  18-21 PC  układ zrównoważony - kontrakt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12+  PC, 5+ trefli/kar, forsuje do końcówki  (nie wyklucza starszej czwórki? ) Nie ma sensu przeskakiwać bo i tak licytacja jest sforsowana, otwierający zgłasza starsze czwórki, podniesienie jest fitem bez nadwyżek</t>
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
       <t xml:space="preserve">2w kolor </t>
     </r>
     <r>
@@ -1406,46 +1705,52 @@
     </r>
   </si>
   <si>
-    <t>kolor pikowy</t>
-  </si>
-  <si>
-    <t>2BA  12-14 PC, układ zrównoważony bez starszej czówórki</t>
-  </si>
-  <si>
-    <t>4 kara</t>
-  </si>
-  <si>
-    <t>silne uzgodnienie koloru</t>
-  </si>
-  <si>
-    <t>12-14  PC, 4 kar- silne uzgodnienie koloru</t>
-  </si>
-  <si>
-    <t>4 kara + splinter</t>
-  </si>
-  <si>
-    <t>SPLINTER</t>
-  </si>
-  <si>
-    <t>15+  PC, 4 kart w kolorze partnera – SPLINTER wskazanie krótkości</t>
-  </si>
-  <si>
-    <t>16+  PC, 4 kart w kolorze partnera – SPLINTER wskazanie krótkości</t>
-  </si>
-  <si>
-    <t>17+  PC, 4 kart w kolorze partnera – SPLINTER wskazanie krótkości</t>
-  </si>
-  <si>
-    <t>18+  PC, 4 kart w kolorze partnera – SPLINTER wskazanie krótkości</t>
-  </si>
-  <si>
-    <t>Dobra 5 lub 6+</t>
-  </si>
-  <si>
-    <t>12+  PC,  dobra 5 lub 6+, forsing do  końcówki Nie ma sensu przeskakiwać bo i tak licytacja jest sforsowana – szanse na szlemika...</t>
+    <t xml:space="preserve">kolor pikowy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2BA  12-14 PC, układ zrównoważony bez starszej czówórki</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4 kara</t>
+  </si>
+  <si>
+    <t xml:space="preserve">silne uzgodnienie koloru</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12-14  PC, 4 kar- silne uzgodnienie koloru</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4 kara + splinter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SPLINTER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15+  PC, 4 kart w kolorze partnera – SPLINTER wskazanie krótkości</t>
+  </si>
+  <si>
+    <t xml:space="preserve">16+  PC, 4 kart w kolorze partnera – SPLINTER wskazanie krótkości</t>
+  </si>
+  <si>
+    <t xml:space="preserve">17+  PC, 4 kart w kolorze partnera – SPLINTER wskazanie krótkości</t>
+  </si>
+  <si>
+    <t xml:space="preserve">18+  PC, 4 kart w kolorze partnera – SPLINTER wskazanie krótkości</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dobra 5 lub 6+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12+  PC,  dobra 5 lub 6+, forsing do  końcówki Nie ma sensu przeskakiwać bo i tak licytacja jest sforsowana – szanse na szlemika...</t>
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Symbol"/>
+        <family val="1"/>
+        <charset val="2"/>
+      </rPr>
       <t xml:space="preserve">  </t>
     </r>
     <r>
@@ -1459,28 +1764,34 @@
     </r>
   </si>
   <si>
-    <t>11-12 PC, bez starszej czwórki, inwit do 3BA</t>
-  </si>
-  <si>
-    <t>do gry</t>
-  </si>
-  <si>
-    <t>15-17 PC piątka trefli – kolor treflowy</t>
-  </si>
-  <si>
-    <t>18+PC piątka kar …</t>
-  </si>
-  <si>
-    <t>18+ PC piątka kierów</t>
-  </si>
-  <si>
-    <t>18+ PC piątka pików</t>
-  </si>
-  <si>
-    <t>(6?) 7+</t>
+    <t xml:space="preserve">11-12 PC, bez starszej czwórki, inwit do 3BA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">do gry</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15-17 PC piątka trefli – kolor treflowy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">18+PC piątka kar …</t>
+  </si>
+  <si>
+    <t xml:space="preserve">18+ PC piątka kierów</t>
+  </si>
+  <si>
+    <t xml:space="preserve">18+ PC piątka pików</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(6?) 7+</t>
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Symbol"/>
+        <family val="1"/>
+        <charset val="2"/>
+      </rPr>
       <t xml:space="preserve"> 9-11</t>
     </r>
     <r>
@@ -1495,6 +1806,12 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Symbol"/>
+        <family val="1"/>
+        <charset val="2"/>
+      </rPr>
       <t xml:space="preserve">9-11</t>
     </r>
     <r>
@@ -1508,10 +1825,16 @@
     </r>
   </si>
   <si>
-    <t>Blok albo autosplintere</t>
+    <t xml:space="preserve">Blok albo autosplintere</t>
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Symbol"/>
+        <family val="1"/>
+        <charset val="2"/>
+      </rPr>
       <t xml:space="preserve"> 4-7</t>
     </r>
     <r>
@@ -1526,6 +1849,12 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Symbol"/>
+        <family val="1"/>
+        <charset val="2"/>
+      </rPr>
       <t xml:space="preserve">4-7</t>
     </r>
     <r>
@@ -1539,16 +1868,22 @@
     </r>
   </si>
   <si>
-    <t>Nie ma takiej odzywki</t>
-  </si>
-  <si>
-    <t>3BA 13-16 PC, bez starszej czwórki i młodszej piątki, nie forsuje – kontrakt (kiepski pomysł bo może blokować)</t>
-  </si>
-  <si>
-    <t>Naturalne 1 karo</t>
+    <t xml:space="preserve">Nie ma takiej odzywki</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3BA 13-16 PC, bez starszej czwórki i młodszej piątki, nie forsuje – kontrakt (kiepski pomysł bo może blokować)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Naturalne 1 karo</t>
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
       <t xml:space="preserve">12-17 PC, 5+ kar (naturalne ale  uwaga na </t>
     </r>
     <r>
@@ -1566,175 +1901,190 @@
     </r>
   </si>
   <si>
-    <t>Brak 4 kar</t>
-  </si>
-  <si>
-    <t>pas</t>
-  </si>
-  <si>
-    <t>nic ciekawego – patrz 3 kara...</t>
-  </si>
-  <si>
-    <t>7+ PC,  4 +  kierów/pików ; przy dwóch czwórkach kierowa, przy dwóch piątkach pikowa;  forsuje na jedno okrążenie</t>
-  </si>
-  <si>
-    <t>czwórka w pikach</t>
-  </si>
-  <si>
-    <t>brak 4s</t>
-  </si>
-  <si>
-    <t> 7-9(10) PC, bez starszej czwórki, nie forsuje</t>
-  </si>
-  <si>
-    <t>5+ kar i 4+ trefl</t>
-  </si>
-  <si>
-    <t>kara i trefle</t>
-  </si>
-  <si>
-    <t>12-14 PC   5+ kar i  4+  trefl .(w wersji opcjonalnej też z 5 trefli i czwórką karo przy 12-17 PC oraz na dwóch piątkach młodszych 12-14PC)</t>
-  </si>
-  <si>
-    <t>6+, brak 4s</t>
-  </si>
-  <si>
-    <t>kara bez starszej</t>
-  </si>
-  <si>
-    <t> 12-14 PC, 6+ kar, możliwe trefle, starsza czwórka wykluczona </t>
-  </si>
-  <si>
-    <t>4 kiery 5+kar</t>
-  </si>
-  <si>
-    <t>kara i kiery</t>
-  </si>
-  <si>
-    <t>15-17 PC  4 w kolor, 5+ kar</t>
-  </si>
-  <si>
-    <t>4 piki 5+kar</t>
-  </si>
-  <si>
-    <t>kara i piki</t>
-  </si>
-  <si>
-    <t>5+, 5+ na młodszych</t>
-  </si>
-  <si>
-    <t>15-17 PC, układ 5+-5+ na kolorach młodszych</t>
-  </si>
-  <si>
-    <t>6 kar</t>
-  </si>
-  <si>
-    <t>sześć kar</t>
-  </si>
-  <si>
-    <t>15-17 PC, 6 kar z dwiema starszymi figurami, forsing</t>
-  </si>
-  <si>
-    <t>10 (12)+ PC, 5+-trefli,nie wyklucza starszej czwórki, forsuje na jedno okrążenie</t>
-  </si>
-  <si>
-    <t>kara</t>
-  </si>
-  <si>
-    <t>12-14 PC – 5+ kar</t>
-  </si>
-  <si>
-    <t>5+kar i 4 kiery</t>
-  </si>
-  <si>
-    <t>15-17  PC –5+kar 4 w kolor</t>
-  </si>
-  <si>
-    <t>5+ kar i 4 piki</t>
-  </si>
-  <si>
-    <t>4-4-4-1</t>
-  </si>
-  <si>
-    <t>układ na czwórkach</t>
-  </si>
-  <si>
-    <t>(RELAY) 15-17  PC 4-4-4-1 (singiel trefl)</t>
-  </si>
-  <si>
-    <t>5+ kar i 4 trefle</t>
-  </si>
-  <si>
-    <t>15-17 PC – 5+ kar oraz  4+trefl</t>
-  </si>
-  <si>
-    <t>15-17 PC –6+kar</t>
-  </si>
-  <si>
-    <t>5+ kar, 4 trefle i krótkość</t>
-  </si>
-  <si>
-    <t>15-17  PC –5+ kar,  4trefle oraz krótkość w kolor  SPLINTER</t>
-  </si>
-  <si>
-    <t>(RELAY) –12-14 PC  4-4-4-1 </t>
-  </si>
-  <si>
-    <t>3+ kara brak 4s</t>
-  </si>
-  <si>
-    <t>12+  PC, fit (3+), brak starszej czwórki, ze względu na krótkość nie nadająca się do zalicytowania 1BA</t>
-  </si>
-  <si>
-    <t>12+  PC,  5+-kierów/pików, forsing do końcówki</t>
-  </si>
-  <si>
-    <t>11-12 PC, bez starszej czwórki, nie forsuje (jest to inwit do 3BA)</t>
-  </si>
-  <si>
-    <t>4+ kar bez 4s</t>
-  </si>
-  <si>
-    <t>9-11 PC, fit (4+ kar), brak starszej czwórki, inwit do 3BA</t>
-  </si>
-  <si>
-    <t>4+ kara</t>
-  </si>
-  <si>
-    <t>BLOK</t>
-  </si>
-  <si>
-    <t>7-9 PC (wersja pro 0-6PC), fit (4+ kar), blok</t>
-  </si>
-  <si>
-    <t>BL</t>
-  </si>
-  <si>
-    <t>4+ kara i krótkość w kolorze</t>
-  </si>
-  <si>
-    <t>12-15  PC,  4+KARA i krótkość w kierach/ pikach SPLINTER forsing do końcówki</t>
-  </si>
-  <si>
-    <t>bez 4s i 5m</t>
-  </si>
-  <si>
-    <t> (12)13-16 PC, bez starszej czwórki i młodszej piątki – do gry</t>
-  </si>
-  <si>
-    <t>4+ kara i singiel terfl</t>
-  </si>
-  <si>
-    <t>12-15  PC,  4+KARA i krótkość w   SPLINTER forsing do końcówki</t>
-  </si>
-  <si>
-    <t>Naturalne 1 kier</t>
-  </si>
-  <si>
-    <t>(w wersji pro przed partią nawet 10-17) (wyklucza piątkę pików chyba że kierów jest więcej :), może być też dowolna młodsza piątka)</t>
+    <t xml:space="preserve">Brak 4 kar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nic ciekawego – patrz 3 kara...</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">czwórka w KOLOR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7+ PC,  4 +  KOLORów ; przy dwóch czwórkach kierowa, przy dwóch piątkach pikowa;  forsuje na jedno okrążenie</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5-3-3-2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bez starszej czwórki - układ -5-3-3-2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">brak 4s</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ', / ( ) 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5+ kar i 4+ trefl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kara i trefle</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 4 ! , !.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6+, brak 4s</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kara bez starszej</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ,*,&lt;,&lt;,'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4 kiery 5+kar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kara i kiery</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15-17 PC  4 w kolor, 5+ kar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4 piki 5+kar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kara i piki</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5+, 5+ na młodszych</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15-17 PC, układ 5+-5+ na kolorach młodszych</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6 kar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sześć kar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15-17 PC, 6 kar z dwiema starszymi figurami, forsing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10 (12)+ PC, 5+-trefli,nie wyklucza starszej czwórki, forsuje na jedno okrążenie</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kara</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12-14 PC – 5+ kar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5+kar i 4 kiery</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15-17  PC –5+kar 4 w kolor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5+ kar i 4 piki</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4-4-4-1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">układ na czwórkach</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(RELAY) 15-17  PC 4-4-4-1 (singiel trefl)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5+ kar i 4 trefle</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15-17 PC – 5+ kar oraz  4+trefl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15-17 PC –6+kar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5+ kar, 4 trefle i krótkość</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15-17  PC –5+ kar,  4trefle oraz krótkość w kolor  SPLINTER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(RELAY) –12-14 PC  4-4-4-1 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">3+ kara brak 4s</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12+  PC, fit (3+), brak starszej czwórki, ze względu na krótkość nie nadająca się do zalicytowania 1BA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12+  PC,  5+-kierów/pików, forsing do końcówki</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11-12 PC, bez starszej czwórki, nie forsuje (jest to inwit do 3BA)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4+ kar bez 4s</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9-11 PC, fit (4+ kar), brak starszej czwórki, inwit do 3BA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4+ kara</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BLOK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7-9 PC (wersja pro 0-6PC), fit (4+ kar), blok</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4+ kara i krótkość w kolorze</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12-15  PC,  4+KARA i krótkość w kierach/ pikach SPLINTER forsing do końcówki</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bez 4s i 5m</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> (12)13-16 PC, bez starszej czwórki i młodszej piątki – do gry</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4+ kara i singiel terfl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12-15  PC,  4+KARA i krótkość w   SPLINTER forsing do końcówki</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Naturalne 1 kier</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(w wersji pro przed partią nawet 10-17) (wyklucza piątkę pików chyba że kierów jest więcej :), może być też dowolna młodsza piątka)</t>
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
       <t xml:space="preserve">(w wersji pro przed partią nawet 10-17) </t>
     </r>
     <r>
@@ -1748,22 +2098,28 @@
     </r>
   </si>
   <si>
-    <t>5-3-3-2 lub 4-4-3-2</t>
-  </si>
-  <si>
-    <t>Naturalne BA</t>
-  </si>
-  <si>
-    <t>skład zrównoważony bez krótkości, bez starszej piątki, otwarcie może zawierać piątkę młodszą (wyjątkowo również bardzo słabą starszą) układy 5-3-3-2 4-4-3-2 itp. Po interwencji opozycji obowiązują dalej Stayman i transfery z wykorzystaniem odzywek opozycji.</t>
-  </si>
-  <si>
-    <t>xxx6 lub XXx5</t>
-  </si>
-  <si>
-    <t>PRESSISION</t>
+    <t xml:space="preserve">5-3-3-2 lub 4-4-3-2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Naturalne BA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">skład zrównoważony bez krótkości, bez starszej piątki, otwarcie może zawierać piątkę młodszą (wyjątkowo również bardzo słabą starszą) układy 5-3-3-2 4-4-3-2 itp. Po interwencji opozycji obowiązują dalej Stayman i transfery z wykorzystaniem odzywek opozycji.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">xxx6 lub XXx5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PRESSISION</t>
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
       <t xml:space="preserve"> (10)11-16 PC (w wersji pro12-15), 5+ trefli + starsza czwórka lub 6 + trefli  </t>
     </r>
     <r>
@@ -1778,109 +2134,115 @@
     </r>
   </si>
   <si>
-    <t>MULTI</t>
-  </si>
-  <si>
-    <t>MULTI dawne słabe dwa na starszym (blokujące) 7-10(11) PC, starszy kolor sześciokartowy 5 – przed partią (chyba że b dobry) inaczej 6+,  Licytacja po interwencji przeciwnika  Po interwencji przeciwnika kontry są karne, a nowy kolor pełni rolę „pa­suj lub popraw".</t>
-  </si>
-  <si>
-    <t>x-5-X-X</t>
-  </si>
-  <si>
-    <t>DWUKOLORÓWKA  5+ kier i 5+ młodszy</t>
-  </si>
-  <si>
-    <t>(6)7-10(11) PC, (przed partią nawet 4-9) dwie piątki: kierowa i dowolna  Licytacja po interwencji przeciwnika Po interwencji przeciwnika kontry są karne, a nowy kolor pełni rolę „pa­suj lub popraw".</t>
-  </si>
-  <si>
-    <t>5-x-X-X</t>
-  </si>
-  <si>
-    <t>DWUKOLORÓWKA 5+ pik i 5+ dowolny</t>
-  </si>
-  <si>
-    <t>(6)7-10(11) PC, (przed partią nawet 4-9) dwie piątki: pikowa i młodsza Licytacja po interwencji przeciwnika Po interwencji przeciwnika kontry są karne, a nowy kolor pełni rolę „pa­suj lub popraw".</t>
-  </si>
-  <si>
-    <t>'x-x-5-5</t>
-  </si>
-  <si>
-    <t>DWUKOLORÓWKA na Młodszych</t>
-  </si>
-  <si>
-    <t>2BA DWUKOLORÓWNA NA MŁODSZYCH  7-10(11) PC,  dwie młodsze piątki</t>
-  </si>
-  <si>
-    <t>7+</t>
-  </si>
-  <si>
-    <t>BLOK słaby</t>
-  </si>
-  <si>
-    <t>(blokujące) (5)6-10 PC,  dobry licytowany kolor   7+ (przed partią może być dobre 6); w młodszym chętnie 8+ (lub dobry)</t>
-  </si>
-  <si>
-    <t>7</t>
-  </si>
-  <si>
-    <t>GAMBLING</t>
-  </si>
-  <si>
-    <t>Pełny 7-kartowy kolor młodszy  (AKDWxxx,AKDxxxxx)  bez dojścia w bocznym kolorze typu As lub Król</t>
-  </si>
-  <si>
-    <t>8-x-x-x</t>
-  </si>
-  <si>
-    <t>BLOK (dawny Teksas pdaf)</t>
-  </si>
-  <si>
-    <t>lepiej naturalne (blok?)  ale jest dawna opcja TEKSAS POŁUDNIOWO AFRYKANSKI) mało PC 8+ w kolorze STARSZYM   pełny kolor MOCNE- (około 9 lew)</t>
-  </si>
-  <si>
-    <t>x-8-x-x</t>
-  </si>
-  <si>
-    <t>x-7-x-x</t>
-  </si>
-  <si>
-    <t>do 10 PC 7+ w kolorze licytowanym co najmniej dwie figury – dobry kolor!  (około 8 lew) Siła otwarcia i długość koloru atutowego zależy od stylu gracza i ustaleń w parze. Powinno się stosować metodę 4-3-2-2 (patrz **).</t>
-  </si>
-  <si>
-    <t>7-x-x-x</t>
-  </si>
-  <si>
-    <t>AS</t>
-  </si>
-  <si>
-    <t>pytanie o kolor Asa</t>
-  </si>
-  <si>
-    <t>8+</t>
-  </si>
-  <si>
-    <t>(6) do 10 PC 8+ w kolorze licytowanym co najmniej dwie figury  – dobry kolor!  (około 9 lew)</t>
-  </si>
-  <si>
-    <t>kompletna ręka w kolorze licytowanym BEZ Asa i Króla &lt;font color=red&gt; [chyba to znaczy wszystkie zatrzymania i 7+ kartowy kolor (11 lew)</t>
-  </si>
-  <si>
-    <t>Pas</t>
-  </si>
-  <si>
-    <t>brak odzywki na otwarcie na pierwszym ręku na poziomie 1 (0-11PC) lub 2 (0-5 PC i długi kolor (6+) lub układ na dwóch piątkach) lub 3 itp. ...</t>
-  </si>
-  <si>
-    <t>brak odzywki na otwarcie na drugim ręku  na poziomie 1 (0-11PC) lub 2 (0-5 PC i długi kolor (6+) lub układ na dwóch piątkach) lub 3 itp. ...</t>
-  </si>
-  <si>
-    <t>brak odzywki na otwarcie po pasie partnera  na poziomie 1 (0-11PC) lub 2 (0-5 PC i długi kolor (6+) lub układ na dwóch piątkach) lub 3 itp. ...</t>
-  </si>
-  <si>
-    <t>Wieloznaczny trefl</t>
+    <t xml:space="preserve">MULTI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MULTI dawne słabe dwa na starszym (blokujące) 7-10(11) PC, starszy kolor sześciokartowy 5 – przed partią (chyba że b dobry) inaczej 6+,  Licytacja po interwencji przeciwnika  Po interwencji przeciwnika kontry są karne, a nowy kolor pełni rolę „pa­suj lub popraw".</t>
+  </si>
+  <si>
+    <t xml:space="preserve">x-5-X-X</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DWUKOLORÓWKA  5+ kier i 5+ młodszy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(6)7-10(11) PC, (przed partią nawet 4-9) dwie piątki: kierowa i dowolna  Licytacja po interwencji przeciwnika Po interwencji przeciwnika kontry są karne, a nowy kolor pełni rolę „pa­suj lub popraw".</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5-x-X-X</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DWUKOLORÓWKA 5+ pik i 5+ dowolny</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(6)7-10(11) PC, (przed partią nawet 4-9) dwie piątki: pikowa i młodsza Licytacja po interwencji przeciwnika Po interwencji przeciwnika kontry są karne, a nowy kolor pełni rolę „pa­suj lub popraw".</t>
+  </si>
+  <si>
+    <t xml:space="preserve">'x-x-5-5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DWUKOLORÓWKA na Młodszych</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2BA DWUKOLORÓWNA NA MŁODSZYCH  7-10(11) PC,  dwie młodsze piątki</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BLOK słaby</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(blokujące) (5)6-10 PC,  dobry licytowany kolor   7+ (przed partią może być dobre 6); w młodszym chętnie 8+ (lub dobry)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GAMBLING</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pełny 7-kartowy kolor młodszy  (AKDWxxx,AKDxxxxx)  bez dojścia w bocznym kolorze typu As lub Król</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8-x-x-x</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BLOK (dawny Teksas pdaf)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lepiej naturalne (blok?)  ale jest dawna opcja TEKSAS POŁUDNIOWO AFRYKANSKI) mało PC 8+ w kolorze STARSZYM   pełny kolor MOCNE- (około 9 lew)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">x-8-x-x</t>
+  </si>
+  <si>
+    <t xml:space="preserve">x-7-x-x</t>
+  </si>
+  <si>
+    <t xml:space="preserve">do 10 PC 7+ w kolorze licytowanym co najmniej dwie figury – dobry kolor!  (około 8 lew) Siła otwarcia i długość koloru atutowego zależy od stylu gracza i ustaleń w parze. Powinno się stosować metodę 4-3-2-2 (patrz **).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7-x-x-x</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pytanie o kolor Asa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(6) do 10 PC 8+ w kolorze licytowanym co najmniej dwie figury  – dobry kolor!  (około 9 lew)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kompletna ręka w kolorze licytowanym BEZ Asa i Króla &lt;font color=red&gt; [chyba to znaczy wszystkie zatrzymania i 7+ kartowy kolor (11 lew)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">brak odzywki na otwarcie na pierwszym ręku na poziomie 1 (0-11PC) lub 2 (0-5 PC i długi kolor (6+) lub układ na dwóch piątkach) lub 3 itp. ...</t>
+  </si>
+  <si>
+    <t xml:space="preserve">brak odzywki na otwarcie na drugim ręku  na poziomie 1 (0-11PC) lub 2 (0-5 PC i długi kolor (6+) lub układ na dwóch piątkach) lub 3 itp. ...</t>
+  </si>
+  <si>
+    <t xml:space="preserve">brak odzywki na otwarcie po pasie partnera  na poziomie 1 (0-11PC) lub 2 (0-5 PC i długi kolor (6+) lub układ na dwóch piątkach) lub 3 itp. ...</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wieloznaczny trefl</t>
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="7"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
       <t xml:space="preserve">→ (12)</t>
     </r>
     <r>
@@ -1902,10 +2264,16 @@
     </r>
   </si>
   <si>
-    <t>F</t>
+    <t xml:space="preserve">F</t>
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="7"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
       <t xml:space="preserve">12-17 PC, 5+ kar (naturalne ale  uwaga na </t>
     </r>
     <r>
@@ -1923,10 +2291,16 @@
     </r>
   </si>
   <si>
-    <t>Trójznaczne forsuje na 1 okrążenie</t>
+    <t xml:space="preserve">Trójznaczne forsuje na 1 okrążenie</t>
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="7"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
       <t xml:space="preserve">→ tzw. negat , 0-6(8) PC, skład dowolny  
 (w kolejnym okrążeniu możliwy pas jeżeli jest 0-4 PC) 
 &lt;br&gt;→ 16+ PC, skład dowolny *  (w kolejnym okrążeniu przeskok)
@@ -1945,10 +2319,10 @@
     </r>
   </si>
   <si>
-    <t>4ka kier</t>
-  </si>
-  <si>
-    <t>4+ kier,  forsuje na jedno okrążenie
+    <t xml:space="preserve">4ka kier</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4+ kier,  forsuje na jedno okrążenie
 uwagi:
 – kiery nie wykluczają pików przy 4 kartach
 nie wyklucza młodszej piątki przy sile poniżej 11PC
@@ -1957,7 +2331,7 @@
 przy dwóch piątkach pikową :)</t>
   </si>
   <si>
-    <t>4+ pik,  forsuje na jedno okrążenie
+    <t xml:space="preserve">4+ pik,  forsuje na jedno okrążenie
 uwagi:
 &lt;br&gt;– kiery nie wykluczają pików przy 4 kartach
 nie wyklucza młodszej piątki przy sile poniżej 11PC
@@ -1966,40 +2340,40 @@
 przy dwóch piątkach pikową :)</t>
   </si>
   <si>
-    <t>3+</t>
-  </si>
-  <si>
-    <t>Otwarcie 1 młodszy</t>
-  </si>
-  <si>
-    <t>otwarcie bez starszej piątki – w dłuższy młodszy oraz 3-3 na karach i treflach</t>
-  </si>
-  <si>
-    <t>poparcie na 4 karo</t>
-  </si>
-  <si>
-    <t>czwórka karowa nie wyklucza fitu trefl ani starszej czwórki...</t>
-  </si>
-  <si>
-    <t>poparcie na 4 kier</t>
-  </si>
-  <si>
-    <t>czwórka kierowa, wyklucza czwórkę karo, nie wyklucza pikowej, ani fitu trefl</t>
-  </si>
-  <si>
-    <t>poparcie na 4 pik</t>
-  </si>
-  <si>
-    <t>czwórka pikowa, wyklucza czwórki karo i kier, nie wyklucza fitu trefl</t>
-  </si>
-  <si>
-    <t>6-10 PC, wyklucza 4 kara, 4 kiery, 4 piki i 5 trefli;</t>
-  </si>
-  <si>
-    <t>6+ PC, 5+ trefli, wyklucza 4 kara, 4 kiery, 4 piki;</t>
-  </si>
-  <si>
-    <t>Naturalne bez Atu</t>
+    <t xml:space="preserve">3+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Otwarcie 1 młodszy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">otwarcie bez starszej piątki – w dłuższy młodszy oraz 3-3 na karach i treflach</t>
+  </si>
+  <si>
+    <t xml:space="preserve">poparcie na 4 karo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">czwórka karowa nie wyklucza fitu trefl ani starszej czwórki...</t>
+  </si>
+  <si>
+    <t xml:space="preserve">poparcie na 4 kier</t>
+  </si>
+  <si>
+    <t xml:space="preserve">czwórka kierowa, wyklucza czwórkę karo, nie wyklucza pikowej, ani fitu trefl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">poparcie na 4 pik</t>
+  </si>
+  <si>
+    <t xml:space="preserve">czwórka pikowa, wyklucza czwórki karo i kier, nie wyklucza fitu trefl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6-10 PC, wyklucza 4 kara, 4 kiery, 4 piki i 5 trefli;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6+ PC, 5+ trefli, wyklucza 4 kara, 4 kiery, 4 piki;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Naturalne bez Atu</t>
   </si>
 </sst>
 </file>
@@ -2007,11 +2381,11 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="3">
-    <numFmt numFmtId="164" formatCode="GENERAL"/>
+    <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="0"/>
     <numFmt numFmtId="166" formatCode="@"/>
   </numFmts>
-  <fonts count="15">
+  <fonts count="16">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -2101,6 +2475,11 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="7"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="8">
@@ -2209,7 +2588,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="80">
+  <cellXfs count="81">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2514,6 +2893,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="15" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2610,22 +2993,22 @@
   <dimension ref="A1:M336"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="525" topLeftCell="A278" activePane="bottomLeft" state="split"/>
+      <pane xSplit="0" ySplit="735" topLeftCell="A279" activePane="bottomLeft" state="split"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="L291" activeCellId="0" sqref="L291"/>
+      <selection pane="bottomLeft" activeCell="C287" activeCellId="0" sqref="C287"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.72959183673469"/>
-    <col collapsed="false" hidden="false" max="7" min="3" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="14.8673469387755"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="16.6683673469388"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="138.107142857143"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="6.11224489795918"/>
-    <col collapsed="false" hidden="false" max="1025" min="13" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="7" min="3" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="14.5816326530612"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="16.469387755102"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="136.612244897959"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="6.0765306122449"/>
+    <col collapsed="false" hidden="false" max="1025" min="13" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14591,7 +14974,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="286" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="286" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A286" s="0" t="n">
         <v>285</v>
       </c>
@@ -14606,7 +14989,7 @@
         <v>1</v>
       </c>
       <c r="E286" s="8" t="s">
-        <v>22</v>
+        <v>307</v>
       </c>
       <c r="F286" s="10" t="n">
         <v>7</v>
@@ -14621,10 +15004,10 @@
         <v>0</v>
       </c>
       <c r="J286" s="12" t="s">
-        <v>235</v>
+        <v>308</v>
       </c>
       <c r="K286" s="13" t="s">
-        <v>307</v>
+        <v>309</v>
       </c>
       <c r="L286" s="10" t="s">
         <v>17</v>
@@ -14633,44 +15016,41 @@
         <v>62</v>
       </c>
     </row>
-    <row r="287" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="287" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A287" s="0" t="n">
         <v>286</v>
       </c>
       <c r="B287" s="8" t="n">
-        <f aca="false">A$284</f>
-        <v>283</v>
+        <v>285</v>
       </c>
       <c r="C287" s="8" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D287" s="9" t="n">
         <v>1</v>
       </c>
       <c r="E287" s="8" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F287" s="10" t="n">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="G287" s="10" t="n">
-        <v>37</v>
+        <v>14</v>
       </c>
       <c r="H287" s="10" t="s">
-        <v>41</v>
+        <v>310</v>
       </c>
       <c r="I287" s="11" t="n">
         <v>0</v>
       </c>
       <c r="J287" s="12" t="s">
-        <v>308</v>
-      </c>
-      <c r="K287" s="13" t="s">
-        <v>307</v>
-      </c>
-      <c r="L287" s="10" t="s">
-        <v>17</v>
-      </c>
+        <v>133</v>
+      </c>
+      <c r="K287" s="76" t="s">
+        <v>311</v>
+      </c>
+      <c r="L287" s="10"/>
       <c r="M287" s="14" t="s">
         <v>62</v>
       </c>
@@ -14699,7 +15079,7 @@
         <v>9</v>
       </c>
       <c r="H288" s="10" t="s">
-        <v>309</v>
+        <v>312</v>
       </c>
       <c r="I288" s="11" t="n">
         <v>0</v>
@@ -14708,7 +15088,7 @@
         <v>100</v>
       </c>
       <c r="K288" s="13" t="s">
-        <v>310</v>
+        <v>313</v>
       </c>
       <c r="L288" s="10" t="s">
         <v>107</v>
@@ -14741,16 +15121,16 @@
         <v>14</v>
       </c>
       <c r="H289" s="17" t="s">
-        <v>311</v>
+        <v>314</v>
       </c>
       <c r="I289" s="18" t="n">
         <v>0</v>
       </c>
       <c r="J289" s="19" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="K289" s="30" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="L289" s="17" t="s">
         <v>107</v>
@@ -14783,16 +15163,16 @@
         <v>14</v>
       </c>
       <c r="H290" s="17" t="s">
-        <v>314</v>
+        <v>317</v>
       </c>
       <c r="I290" s="18" t="n">
         <v>0</v>
       </c>
       <c r="J290" s="19" t="s">
-        <v>315</v>
+        <v>318</v>
       </c>
       <c r="K290" s="30" t="s">
-        <v>316</v>
+        <v>319</v>
       </c>
       <c r="L290" s="17" t="s">
         <v>107</v>
@@ -14825,16 +15205,16 @@
         <v>17</v>
       </c>
       <c r="H291" s="17" t="s">
-        <v>317</v>
+        <v>320</v>
       </c>
       <c r="I291" s="18" t="n">
         <v>0</v>
       </c>
       <c r="J291" s="19" t="s">
-        <v>318</v>
+        <v>321</v>
       </c>
       <c r="K291" s="30" t="s">
-        <v>319</v>
+        <v>322</v>
       </c>
       <c r="L291" s="17" t="s">
         <v>35</v>
@@ -14867,16 +15247,16 @@
         <v>17</v>
       </c>
       <c r="H292" s="17" t="s">
-        <v>320</v>
+        <v>323</v>
       </c>
       <c r="I292" s="18" t="n">
         <v>0</v>
       </c>
       <c r="J292" s="19" t="s">
-        <v>321</v>
+        <v>324</v>
       </c>
       <c r="K292" s="30" t="s">
-        <v>319</v>
+        <v>322</v>
       </c>
       <c r="L292" s="17" t="s">
         <v>35</v>
@@ -14909,16 +15289,16 @@
         <v>17</v>
       </c>
       <c r="H293" s="17" t="s">
-        <v>322</v>
+        <v>325</v>
       </c>
       <c r="I293" s="18" t="n">
         <v>0</v>
       </c>
       <c r="J293" s="19" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="K293" s="30" t="s">
-        <v>323</v>
+        <v>326</v>
       </c>
       <c r="L293" s="17" t="s">
         <v>35</v>
@@ -14951,16 +15331,16 @@
         <v>17</v>
       </c>
       <c r="H294" s="17" t="s">
-        <v>324</v>
+        <v>327</v>
       </c>
       <c r="I294" s="18" t="n">
         <v>0</v>
       </c>
       <c r="J294" s="19" t="s">
-        <v>325</v>
+        <v>328</v>
       </c>
       <c r="K294" s="30" t="s">
-        <v>326</v>
+        <v>329</v>
       </c>
       <c r="L294" s="17" t="s">
         <v>35</v>
@@ -15002,7 +15382,7 @@
         <v>262</v>
       </c>
       <c r="K295" s="13" t="s">
-        <v>327</v>
+        <v>330</v>
       </c>
       <c r="L295" s="10" t="s">
         <v>17</v>
@@ -15041,10 +15421,10 @@
         <v>0</v>
       </c>
       <c r="J296" s="19" t="s">
-        <v>328</v>
+        <v>331</v>
       </c>
       <c r="K296" s="30" t="s">
-        <v>329</v>
+        <v>332</v>
       </c>
       <c r="L296" s="17" t="s">
         <v>107</v>
@@ -15077,16 +15457,16 @@
         <v>17</v>
       </c>
       <c r="H297" s="17" t="s">
-        <v>330</v>
+        <v>333</v>
       </c>
       <c r="I297" s="18" t="n">
         <v>0</v>
       </c>
       <c r="J297" s="19" t="s">
-        <v>318</v>
+        <v>321</v>
       </c>
       <c r="K297" s="30" t="s">
-        <v>331</v>
+        <v>334</v>
       </c>
       <c r="L297" s="17" t="s">
         <v>44</v>
@@ -15119,16 +15499,16 @@
         <v>17</v>
       </c>
       <c r="H298" s="17" t="s">
-        <v>332</v>
+        <v>335</v>
       </c>
       <c r="I298" s="18" t="n">
         <v>0</v>
       </c>
       <c r="J298" s="19" t="s">
-        <v>321</v>
+        <v>324</v>
       </c>
       <c r="K298" s="30" t="s">
-        <v>331</v>
+        <v>334</v>
       </c>
       <c r="L298" s="17" t="s">
         <v>44</v>
@@ -15161,16 +15541,16 @@
         <v>17</v>
       </c>
       <c r="H299" s="17" t="s">
-        <v>333</v>
+        <v>336</v>
       </c>
       <c r="I299" s="18" t="n">
         <v>0</v>
       </c>
       <c r="J299" s="19" t="s">
-        <v>334</v>
+        <v>337</v>
       </c>
       <c r="K299" s="30" t="s">
-        <v>335</v>
+        <v>338</v>
       </c>
       <c r="L299" s="17" t="s">
         <v>44</v>
@@ -15203,16 +15583,16 @@
         <v>17</v>
       </c>
       <c r="H300" s="17" t="s">
-        <v>336</v>
+        <v>339</v>
       </c>
       <c r="I300" s="18" t="n">
         <v>0</v>
       </c>
       <c r="J300" s="19" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="K300" s="30" t="s">
-        <v>337</v>
+        <v>340</v>
       </c>
       <c r="L300" s="17" t="s">
         <v>44</v>
@@ -15254,7 +15634,7 @@
         <v>112</v>
       </c>
       <c r="K301" s="30" t="s">
-        <v>338</v>
+        <v>341</v>
       </c>
       <c r="L301" s="17" t="s">
         <v>44</v>
@@ -15287,7 +15667,7 @@
         <v>17</v>
       </c>
       <c r="H302" s="17" t="s">
-        <v>339</v>
+        <v>342</v>
       </c>
       <c r="I302" s="18" t="n">
         <v>0</v>
@@ -15296,7 +15676,7 @@
         <v>280</v>
       </c>
       <c r="K302" s="30" t="s">
-        <v>340</v>
+        <v>343</v>
       </c>
       <c r="L302" s="17" t="s">
         <v>44</v>
@@ -15329,7 +15709,7 @@
         <v>17</v>
       </c>
       <c r="H303" s="17" t="s">
-        <v>339</v>
+        <v>342</v>
       </c>
       <c r="I303" s="18" t="n">
         <v>0</v>
@@ -15338,7 +15718,7 @@
         <v>280</v>
       </c>
       <c r="K303" s="30" t="s">
-        <v>340</v>
+        <v>343</v>
       </c>
       <c r="L303" s="17" t="s">
         <v>44</v>
@@ -15371,7 +15751,7 @@
         <v>14</v>
       </c>
       <c r="H304" s="17" t="s">
-        <v>333</v>
+        <v>336</v>
       </c>
       <c r="I304" s="18" t="n">
         <v>0</v>
@@ -15380,7 +15760,7 @@
         <v>167</v>
       </c>
       <c r="K304" s="30" t="s">
-        <v>341</v>
+        <v>344</v>
       </c>
       <c r="L304" s="17" t="s">
         <v>31</v>
@@ -15413,7 +15793,7 @@
         <v>37</v>
       </c>
       <c r="H305" s="10" t="s">
-        <v>342</v>
+        <v>345</v>
       </c>
       <c r="I305" s="11" t="n">
         <v>0</v>
@@ -15422,7 +15802,7 @@
         <v>57</v>
       </c>
       <c r="K305" s="13" t="s">
-        <v>343</v>
+        <v>346</v>
       </c>
       <c r="L305" s="10" t="s">
         <v>44</v>
@@ -15464,7 +15844,7 @@
         <v>114</v>
       </c>
       <c r="K306" s="13" t="s">
-        <v>344</v>
+        <v>347</v>
       </c>
       <c r="L306" s="10" t="s">
         <v>44</v>
@@ -15506,7 +15886,7 @@
         <v>274</v>
       </c>
       <c r="K307" s="13" t="s">
-        <v>344</v>
+        <v>347</v>
       </c>
       <c r="L307" s="10" t="s">
         <v>44</v>
@@ -15539,7 +15919,7 @@
         <v>12</v>
       </c>
       <c r="H308" s="10" t="s">
-        <v>309</v>
+        <v>312</v>
       </c>
       <c r="I308" s="11" t="n">
         <v>0</v>
@@ -15548,7 +15928,7 @@
         <v>119</v>
       </c>
       <c r="K308" s="13" t="s">
-        <v>345</v>
+        <v>348</v>
       </c>
       <c r="L308" s="10" t="s">
         <v>35</v>
@@ -15581,7 +15961,7 @@
         <v>11</v>
       </c>
       <c r="H309" s="10" t="s">
-        <v>346</v>
+        <v>349</v>
       </c>
       <c r="I309" s="11" t="n">
         <v>0</v>
@@ -15590,7 +15970,7 @@
         <v>119</v>
       </c>
       <c r="K309" s="13" t="s">
-        <v>347</v>
+        <v>350</v>
       </c>
       <c r="L309" s="10" t="s">
         <v>35</v>
@@ -15623,19 +16003,19 @@
         <v>9</v>
       </c>
       <c r="H310" s="10" t="s">
-        <v>348</v>
+        <v>351</v>
       </c>
       <c r="I310" s="11" t="n">
         <v>0</v>
       </c>
       <c r="J310" s="12" t="s">
-        <v>349</v>
+        <v>352</v>
       </c>
       <c r="K310" s="13" t="s">
-        <v>350</v>
+        <v>353</v>
       </c>
       <c r="L310" s="10" t="s">
-        <v>351</v>
+        <v>354</v>
       </c>
       <c r="M310" s="14" t="s">
         <v>62</v>
@@ -15665,7 +16045,7 @@
         <v>15</v>
       </c>
       <c r="H311" s="10" t="s">
-        <v>352</v>
+        <v>355</v>
       </c>
       <c r="I311" s="11" t="n">
         <v>0</v>
@@ -15674,7 +16054,7 @@
         <v>280</v>
       </c>
       <c r="K311" s="13" t="s">
-        <v>353</v>
+        <v>356</v>
       </c>
       <c r="L311" s="10" t="s">
         <v>44</v>
@@ -15707,7 +16087,7 @@
         <v>15</v>
       </c>
       <c r="H312" s="10" t="s">
-        <v>352</v>
+        <v>355</v>
       </c>
       <c r="I312" s="11" t="n">
         <v>0</v>
@@ -15716,7 +16096,7 @@
         <v>280</v>
       </c>
       <c r="K312" s="13" t="s">
-        <v>353</v>
+        <v>356</v>
       </c>
       <c r="L312" s="10" t="s">
         <v>44</v>
@@ -15749,7 +16129,7 @@
         <v>16</v>
       </c>
       <c r="H313" s="10" t="s">
-        <v>354</v>
+        <v>357</v>
       </c>
       <c r="I313" s="11" t="n">
         <v>0</v>
@@ -15758,7 +16138,7 @@
         <v>128</v>
       </c>
       <c r="K313" s="13" t="s">
-        <v>355</v>
+        <v>358</v>
       </c>
       <c r="L313" s="10" t="s">
         <v>31</v>
@@ -15791,7 +16171,7 @@
         <v>15</v>
       </c>
       <c r="H314" s="10" t="s">
-        <v>356</v>
+        <v>359</v>
       </c>
       <c r="I314" s="11" t="n">
         <v>0</v>
@@ -15800,7 +16180,7 @@
         <v>280</v>
       </c>
       <c r="K314" s="13" t="s">
-        <v>357</v>
+        <v>360</v>
       </c>
       <c r="L314" s="10" t="s">
         <v>44</v>
@@ -15838,10 +16218,10 @@
         <v>0</v>
       </c>
       <c r="J315" s="5" t="s">
-        <v>358</v>
+        <v>361</v>
       </c>
       <c r="K315" s="6" t="s">
-        <v>359</v>
+        <v>362</v>
       </c>
       <c r="L315" s="3" t="s">
         <v>107</v>
@@ -15879,10 +16259,10 @@
         <v>0</v>
       </c>
       <c r="J316" s="5" t="s">
-        <v>358</v>
+        <v>361</v>
       </c>
       <c r="K316" s="6" t="s">
-        <v>360</v>
+        <v>363</v>
       </c>
       <c r="L316" s="3" t="s">
         <v>107</v>
@@ -15914,16 +16294,16 @@
         <v>17</v>
       </c>
       <c r="H317" s="3" t="s">
-        <v>361</v>
+        <v>364</v>
       </c>
       <c r="I317" s="4" t="n">
         <v>0</v>
       </c>
       <c r="J317" s="5" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="K317" s="6" t="s">
-        <v>363</v>
+        <v>366</v>
       </c>
       <c r="L317" s="3" t="s">
         <v>107</v>
@@ -15955,16 +16335,16 @@
         <v>15</v>
       </c>
       <c r="H318" s="3" t="s">
-        <v>364</v>
+        <v>367</v>
       </c>
       <c r="I318" s="4" t="n">
         <v>0</v>
       </c>
       <c r="J318" s="5" t="s">
-        <v>365</v>
+        <v>368</v>
       </c>
       <c r="K318" s="6" t="s">
-        <v>366</v>
+        <v>369</v>
       </c>
       <c r="L318" s="3" t="s">
         <v>107</v>
@@ -16002,10 +16382,10 @@
         <v>0</v>
       </c>
       <c r="J319" s="5" t="s">
-        <v>367</v>
+        <v>370</v>
       </c>
       <c r="K319" s="6" t="s">
-        <v>368</v>
+        <v>371</v>
       </c>
       <c r="L319" s="3" t="s">
         <v>17</v>
@@ -16037,16 +16417,16 @@
         <v>11</v>
       </c>
       <c r="H320" s="3" t="s">
-        <v>369</v>
+        <v>372</v>
       </c>
       <c r="I320" s="4" t="n">
         <v>0</v>
       </c>
       <c r="J320" s="5" t="s">
-        <v>370</v>
+        <v>373</v>
       </c>
       <c r="K320" s="6" t="s">
-        <v>371</v>
+        <v>374</v>
       </c>
       <c r="L320" s="3" t="s">
         <v>107</v>
@@ -16078,16 +16458,16 @@
         <v>11</v>
       </c>
       <c r="H321" s="3" t="s">
-        <v>372</v>
+        <v>375</v>
       </c>
       <c r="I321" s="4" t="n">
         <v>0</v>
       </c>
       <c r="J321" s="5" t="s">
-        <v>373</v>
+        <v>376</v>
       </c>
       <c r="K321" s="6" t="s">
-        <v>374</v>
+        <v>377</v>
       </c>
       <c r="L321" s="3" t="s">
         <v>107</v>
@@ -16119,16 +16499,16 @@
         <v>11</v>
       </c>
       <c r="H322" s="3" t="s">
-        <v>375</v>
+        <v>378</v>
       </c>
       <c r="I322" s="4" t="n">
         <v>0</v>
       </c>
       <c r="J322" s="5" t="s">
-        <v>376</v>
+        <v>379</v>
       </c>
       <c r="K322" s="6" t="s">
-        <v>377</v>
+        <v>380</v>
       </c>
       <c r="L322" s="3" t="s">
         <v>17</v>
@@ -16160,19 +16540,19 @@
         <v>10</v>
       </c>
       <c r="H323" s="3" t="s">
-        <v>378</v>
+        <v>381</v>
       </c>
       <c r="I323" s="4" t="n">
         <v>0</v>
       </c>
       <c r="J323" s="5" t="s">
-        <v>379</v>
+        <v>382</v>
       </c>
       <c r="K323" s="6" t="s">
-        <v>380</v>
+        <v>383</v>
       </c>
       <c r="L323" s="3" t="s">
-        <v>351</v>
+        <v>354</v>
       </c>
       <c r="M323" s="3" t="s">
         <v>55</v>
@@ -16201,19 +16581,19 @@
         <v>10</v>
       </c>
       <c r="H324" s="3" t="s">
-        <v>378</v>
+        <v>381</v>
       </c>
       <c r="I324" s="4" t="n">
         <v>0</v>
       </c>
       <c r="J324" s="5" t="s">
-        <v>379</v>
+        <v>382</v>
       </c>
       <c r="K324" s="6" t="s">
-        <v>380</v>
+        <v>383</v>
       </c>
       <c r="L324" s="3" t="s">
-        <v>351</v>
+        <v>354</v>
       </c>
       <c r="M324" s="3" t="s">
         <v>55</v>
@@ -16242,19 +16622,19 @@
         <v>10</v>
       </c>
       <c r="H325" s="3" t="s">
-        <v>378</v>
+        <v>381</v>
       </c>
       <c r="I325" s="4" t="n">
         <v>0</v>
       </c>
       <c r="J325" s="5" t="s">
-        <v>379</v>
+        <v>382</v>
       </c>
       <c r="K325" s="6" t="s">
-        <v>380</v>
+        <v>383</v>
       </c>
       <c r="L325" s="3" t="s">
-        <v>351</v>
+        <v>354</v>
       </c>
       <c r="M325" s="3" t="s">
         <v>55</v>
@@ -16283,19 +16663,19 @@
         <v>10</v>
       </c>
       <c r="H326" s="3" t="s">
-        <v>378</v>
+        <v>381</v>
       </c>
       <c r="I326" s="4" t="n">
         <v>0</v>
       </c>
       <c r="J326" s="5" t="s">
-        <v>379</v>
+        <v>382</v>
       </c>
       <c r="K326" s="6" t="s">
-        <v>380</v>
+        <v>383</v>
       </c>
       <c r="L326" s="3" t="s">
-        <v>351</v>
+        <v>354</v>
       </c>
       <c r="M326" s="3" t="s">
         <v>55</v>
@@ -16325,19 +16705,19 @@
         <v>22</v>
       </c>
       <c r="H327" s="3" t="s">
-        <v>381</v>
+        <v>384</v>
       </c>
       <c r="I327" s="4" t="n">
         <v>0</v>
       </c>
       <c r="J327" s="5" t="s">
-        <v>382</v>
+        <v>385</v>
       </c>
       <c r="K327" s="6" t="s">
-        <v>383</v>
+        <v>386</v>
       </c>
       <c r="L327" s="3" t="s">
-        <v>351</v>
+        <v>354</v>
       </c>
       <c r="M327" s="3" t="s">
         <v>55</v>
@@ -16366,19 +16746,19 @@
         <v>10</v>
       </c>
       <c r="H328" s="3" t="s">
-        <v>384</v>
+        <v>387</v>
       </c>
       <c r="I328" s="4" t="n">
         <v>0</v>
       </c>
       <c r="J328" s="5" t="s">
-        <v>385</v>
+        <v>388</v>
       </c>
       <c r="K328" s="6" t="s">
-        <v>386</v>
+        <v>389</v>
       </c>
       <c r="L328" s="3" t="s">
-        <v>351</v>
+        <v>354</v>
       </c>
       <c r="M328" s="3" t="s">
         <v>18</v>
@@ -16407,19 +16787,19 @@
         <v>10</v>
       </c>
       <c r="H329" s="3" t="s">
-        <v>387</v>
+        <v>390</v>
       </c>
       <c r="I329" s="4" t="n">
         <v>0</v>
       </c>
       <c r="J329" s="5" t="s">
-        <v>385</v>
+        <v>388</v>
       </c>
       <c r="K329" s="6" t="s">
-        <v>386</v>
+        <v>389</v>
       </c>
       <c r="L329" s="3" t="s">
-        <v>351</v>
+        <v>354</v>
       </c>
       <c r="M329" s="3" t="s">
         <v>18</v>
@@ -16448,19 +16828,19 @@
         <v>10</v>
       </c>
       <c r="H330" s="3" t="s">
-        <v>388</v>
+        <v>391</v>
       </c>
       <c r="I330" s="4" t="n">
         <v>0</v>
       </c>
       <c r="J330" s="5" t="s">
-        <v>349</v>
+        <v>352</v>
       </c>
       <c r="K330" s="6" t="s">
-        <v>389</v>
+        <v>392</v>
       </c>
       <c r="L330" s="3" t="s">
-        <v>351</v>
+        <v>354</v>
       </c>
       <c r="M330" s="3" t="s">
         <v>62</v>
@@ -16489,19 +16869,19 @@
         <v>10</v>
       </c>
       <c r="H331" s="3" t="s">
-        <v>390</v>
+        <v>393</v>
       </c>
       <c r="I331" s="4" t="n">
         <v>0</v>
       </c>
       <c r="J331" s="5" t="s">
-        <v>349</v>
+        <v>352</v>
       </c>
       <c r="K331" s="6" t="s">
-        <v>389</v>
+        <v>392</v>
       </c>
       <c r="L331" s="3" t="s">
-        <v>351</v>
+        <v>354</v>
       </c>
       <c r="M331" s="3" t="s">
         <v>62</v>
@@ -16536,10 +16916,10 @@
         <v>0</v>
       </c>
       <c r="J332" s="5" t="s">
-        <v>391</v>
+        <v>394</v>
       </c>
       <c r="K332" s="6" t="s">
-        <v>392</v>
+        <v>395</v>
       </c>
       <c r="L332" s="3" t="s">
         <v>17</v>
@@ -16571,19 +16951,19 @@
         <v>10</v>
       </c>
       <c r="H333" s="3" t="s">
-        <v>393</v>
+        <v>396</v>
       </c>
       <c r="I333" s="4" t="n">
         <v>0</v>
       </c>
       <c r="J333" s="5" t="s">
-        <v>349</v>
+        <v>352</v>
       </c>
       <c r="K333" s="6" t="s">
-        <v>394</v>
+        <v>397</v>
       </c>
       <c r="L333" s="3" t="s">
-        <v>351</v>
+        <v>354</v>
       </c>
       <c r="M333" s="3" t="s">
         <v>62</v>
@@ -16612,19 +16992,19 @@
         <v>10</v>
       </c>
       <c r="H334" s="3" t="s">
-        <v>393</v>
+        <v>396</v>
       </c>
       <c r="I334" s="4" t="n">
         <v>0</v>
       </c>
       <c r="J334" s="5" t="s">
-        <v>349</v>
+        <v>352</v>
       </c>
       <c r="K334" s="6" t="s">
-        <v>394</v>
+        <v>397</v>
       </c>
       <c r="L334" s="3" t="s">
-        <v>351</v>
+        <v>354</v>
       </c>
       <c r="M334" s="3" t="s">
         <v>62</v>
@@ -16653,19 +17033,19 @@
         <v>37</v>
       </c>
       <c r="H335" s="3" t="s">
-        <v>378</v>
+        <v>381</v>
       </c>
       <c r="I335" s="4" t="n">
         <v>0</v>
       </c>
       <c r="J335" s="5" t="s">
-        <v>349</v>
+        <v>352</v>
       </c>
       <c r="K335" s="6" t="s">
-        <v>395</v>
+        <v>398</v>
       </c>
       <c r="L335" s="3" t="s">
-        <v>351</v>
+        <v>354</v>
       </c>
       <c r="M335" s="3" t="s">
         <v>62</v>
@@ -16694,19 +17074,19 @@
         <v>37</v>
       </c>
       <c r="H336" s="3" t="s">
-        <v>378</v>
+        <v>381</v>
       </c>
       <c r="I336" s="4" t="n">
         <v>0</v>
       </c>
       <c r="J336" s="5" t="s">
-        <v>349</v>
+        <v>352</v>
       </c>
       <c r="K336" s="6" t="s">
-        <v>395</v>
+        <v>398</v>
       </c>
       <c r="L336" s="3" t="s">
-        <v>351</v>
+        <v>354</v>
       </c>
       <c r="M336" s="3" t="s">
         <v>62</v>
@@ -16736,7 +17116,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -16790,7 +17170,7 @@
       <c r="C2" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="D2" s="76" t="n">
+      <c r="D2" s="77" t="n">
         <v>1</v>
       </c>
       <c r="E2" s="0" t="s">
@@ -16809,15 +17189,15 @@
         <v>0</v>
       </c>
       <c r="J2" s="0" t="s">
-        <v>396</v>
-      </c>
-      <c r="K2" s="77" t="s">
-        <v>397</v>
+        <v>399</v>
+      </c>
+      <c r="K2" s="78" t="s">
+        <v>400</v>
       </c>
       <c r="L2" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="M2" s="78" t="s">
+      <c r="M2" s="79" t="s">
         <v>62</v>
       </c>
     </row>
@@ -16831,7 +17211,7 @@
       <c r="C3" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="D3" s="76" t="n">
+      <c r="D3" s="77" t="n">
         <v>1</v>
       </c>
       <c r="E3" s="0" t="s">
@@ -16851,15 +17231,15 @@
         <v>1</v>
       </c>
       <c r="J3" s="0" t="s">
-        <v>396</v>
-      </c>
-      <c r="K3" s="77" t="s">
-        <v>398</v>
+        <v>399</v>
+      </c>
+      <c r="K3" s="78" t="s">
+        <v>401</v>
       </c>
       <c r="L3" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="M3" s="78" t="s">
+      <c r="M3" s="79" t="s">
         <v>62</v>
       </c>
     </row>
@@ -16873,7 +17253,7 @@
       <c r="C4" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="D4" s="76" t="n">
+      <c r="D4" s="77" t="n">
         <v>1</v>
       </c>
       <c r="E4" s="0" t="s">
@@ -16892,15 +17272,15 @@
         <v>1</v>
       </c>
       <c r="J4" s="0" t="s">
-        <v>396</v>
-      </c>
-      <c r="K4" s="77" t="s">
         <v>399</v>
+      </c>
+      <c r="K4" s="78" t="s">
+        <v>402</v>
       </c>
       <c r="L4" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="M4" s="78" t="s">
+      <c r="M4" s="79" t="s">
         <v>62</v>
       </c>
     </row>
@@ -16914,7 +17294,7 @@
       <c r="C5" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="D5" s="76" t="n">
+      <c r="D5" s="77" t="n">
         <v>1</v>
       </c>
       <c r="E5" s="0" t="s">
@@ -16933,15 +17313,15 @@
         <v>1</v>
       </c>
       <c r="J5" s="0" t="s">
-        <v>396</v>
-      </c>
-      <c r="K5" s="77" t="s">
         <v>399</v>
+      </c>
+      <c r="K5" s="78" t="s">
+        <v>402</v>
       </c>
       <c r="L5" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="M5" s="78" t="s">
+      <c r="M5" s="79" t="s">
         <v>62</v>
       </c>
     </row>
@@ -16969,9 +17349,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="10" min="1" style="0" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="38.7040816326531"/>
-    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="38.2040816326531"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17025,7 +17403,7 @@
       <c r="C2" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="D2" s="76" t="n">
+      <c r="D2" s="77" t="n">
         <v>1</v>
       </c>
       <c r="E2" s="0" t="s">
@@ -17044,15 +17422,15 @@
         <v>0</v>
       </c>
       <c r="J2" s="0" t="s">
-        <v>400</v>
-      </c>
-      <c r="K2" s="77" t="s">
-        <v>401</v>
+        <v>403</v>
+      </c>
+      <c r="K2" s="78" t="s">
+        <v>404</v>
       </c>
       <c r="L2" s="0" t="s">
-        <v>402</v>
-      </c>
-      <c r="M2" s="79"/>
+        <v>405</v>
+      </c>
+      <c r="M2" s="80"/>
     </row>
     <row r="3" customFormat="false" ht="170.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="n">
@@ -17064,7 +17442,7 @@
       <c r="C3" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="D3" s="76" t="n">
+      <c r="D3" s="77" t="n">
         <v>1</v>
       </c>
       <c r="E3" s="0" t="s">
@@ -17085,13 +17463,13 @@
       <c r="J3" s="0" t="s">
         <v>302</v>
       </c>
-      <c r="K3" s="77" t="s">
-        <v>403</v>
+      <c r="K3" s="78" t="s">
+        <v>406</v>
       </c>
       <c r="L3" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="M3" s="79"/>
+      <c r="M3" s="80"/>
     </row>
     <row r="4" customFormat="false" ht="282.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="n">
@@ -17103,7 +17481,7 @@
       <c r="C4" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="D4" s="76" t="n">
+      <c r="D4" s="77" t="n">
         <v>1</v>
       </c>
       <c r="E4" s="0" t="s">
@@ -17122,15 +17500,15 @@
         <v>0</v>
       </c>
       <c r="J4" s="0" t="s">
-        <v>404</v>
-      </c>
-      <c r="K4" s="77" t="s">
-        <v>405</v>
+        <v>407</v>
+      </c>
+      <c r="K4" s="78" t="s">
+        <v>408</v>
       </c>
       <c r="L4" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="M4" s="79"/>
+      <c r="M4" s="80"/>
     </row>
     <row r="5" customFormat="false" ht="129.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="n">
@@ -17142,7 +17520,7 @@
       <c r="C5" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="D5" s="76" t="n">
+      <c r="D5" s="77" t="n">
         <v>1</v>
       </c>
       <c r="E5" s="0" t="s">
@@ -17161,15 +17539,15 @@
         <v>0</v>
       </c>
       <c r="J5" s="0" t="s">
-        <v>406</v>
-      </c>
-      <c r="K5" s="77" t="s">
-        <v>407</v>
+        <v>409</v>
+      </c>
+      <c r="K5" s="78" t="s">
+        <v>410</v>
       </c>
       <c r="L5" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="M5" s="79"/>
+      <c r="M5" s="80"/>
     </row>
     <row r="6" customFormat="false" ht="58.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="n">
@@ -17181,7 +17559,7 @@
       <c r="C6" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="D6" s="76" t="n">
+      <c r="D6" s="77" t="n">
         <v>1</v>
       </c>
       <c r="E6" s="0" t="s">
@@ -17202,13 +17580,13 @@
       <c r="J6" s="0" t="s">
         <v>252</v>
       </c>
-      <c r="K6" s="77" t="s">
-        <v>408</v>
+      <c r="K6" s="78" t="s">
+        <v>411</v>
       </c>
       <c r="L6" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="M6" s="79"/>
+      <c r="M6" s="80"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -17229,22 +17607,22 @@
   <dimension ref="A1:M28"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="525" topLeftCell="A1" activePane="bottomLeft" state="split"/>
+      <pane xSplit="0" ySplit="735" topLeftCell="A1" activePane="bottomLeft" state="split"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="bottomLeft" activeCell="K14" activeCellId="0" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.72959183673469"/>
-    <col collapsed="false" hidden="false" max="7" min="3" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="14.8673469387755"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="16.6683673469388"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="138.107142857143"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="6.11224489795918"/>
-    <col collapsed="false" hidden="false" max="1025" min="13" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="7" min="3" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="14.5816326530612"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="16.469387755102"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="136.612244897959"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="6.0765306122449"/>
+    <col collapsed="false" hidden="false" max="1025" min="13" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17311,16 +17689,16 @@
         <v>21</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>409</v>
+        <v>412</v>
       </c>
       <c r="I2" s="4" t="n">
         <v>0</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>410</v>
+        <v>413</v>
       </c>
       <c r="K2" s="6" t="s">
-        <v>411</v>
+        <v>414</v>
       </c>
       <c r="L2" s="3" t="s">
         <v>17</v>
@@ -17359,10 +17737,10 @@
         <v>0</v>
       </c>
       <c r="J3" s="12" t="s">
-        <v>412</v>
+        <v>415</v>
       </c>
       <c r="K3" s="13" t="s">
-        <v>413</v>
+        <v>416</v>
       </c>
       <c r="L3" s="10" t="s">
         <v>107</v>
@@ -17401,10 +17779,10 @@
         <v>0</v>
       </c>
       <c r="J4" s="12" t="s">
-        <v>414</v>
+        <v>417</v>
       </c>
       <c r="K4" s="13" t="s">
-        <v>415</v>
+        <v>418</v>
       </c>
       <c r="L4" s="10" t="s">
         <v>107</v>
@@ -17443,10 +17821,10 @@
         <v>0</v>
       </c>
       <c r="J5" s="12" t="s">
-        <v>416</v>
+        <v>419</v>
       </c>
       <c r="K5" s="13" t="s">
-        <v>417</v>
+        <v>420</v>
       </c>
       <c r="L5" s="10" t="s">
         <v>107</v>
@@ -17487,7 +17865,7 @@
         <v>100</v>
       </c>
       <c r="K6" s="12" t="s">
-        <v>418</v>
+        <v>421</v>
       </c>
       <c r="L6" s="10" t="s">
         <v>107</v>
@@ -17528,7 +17906,7 @@
         <v>262</v>
       </c>
       <c r="K7" s="12" t="s">
-        <v>419</v>
+        <v>422</v>
       </c>
       <c r="L7" s="10" t="s">
         <v>107</v>
@@ -17638,13 +18016,13 @@
         <v>21</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>409</v>
+        <v>412</v>
       </c>
       <c r="I10" s="4" t="n">
         <v>0</v>
       </c>
       <c r="J10" s="5" t="s">
-        <v>410</v>
+        <v>413</v>
       </c>
       <c r="K10" s="6"/>
       <c r="L10" s="3" t="s">
@@ -17683,7 +18061,7 @@
         <v>0</v>
       </c>
       <c r="J11" s="5" t="s">
-        <v>358</v>
+        <v>361</v>
       </c>
       <c r="K11" s="6"/>
       <c r="L11" s="3" t="s">
@@ -17722,7 +18100,7 @@
         <v>0</v>
       </c>
       <c r="J12" s="5" t="s">
-        <v>358</v>
+        <v>361</v>
       </c>
       <c r="K12" s="6"/>
       <c r="L12" s="3" t="s">
@@ -17761,7 +18139,7 @@
         <v>0</v>
       </c>
       <c r="J13" s="5" t="s">
-        <v>420</v>
+        <v>423</v>
       </c>
       <c r="K13" s="6"/>
       <c r="L13" s="3" t="s">
@@ -17802,7 +18180,7 @@
       </c>
       <c r="K14" s="6"/>
       <c r="L14" s="3" t="s">
-        <v>402</v>
+        <v>405</v>
       </c>
       <c r="M14" s="3" t="s">
         <v>45</v>
@@ -17837,7 +18215,7 @@
         <v>0</v>
       </c>
       <c r="J15" s="5" t="s">
-        <v>349</v>
+        <v>352</v>
       </c>
       <c r="K15" s="5"/>
       <c r="L15" s="3" t="s">
@@ -17876,7 +18254,7 @@
         <v>0</v>
       </c>
       <c r="J16" s="5" t="s">
-        <v>349</v>
+        <v>352</v>
       </c>
       <c r="K16" s="5"/>
       <c r="L16" s="3" t="s">
@@ -17915,7 +18293,7 @@
         <v>0</v>
       </c>
       <c r="J17" s="5" t="s">
-        <v>349</v>
+        <v>352</v>
       </c>
       <c r="K17" s="5"/>
       <c r="L17" s="3" t="s">
@@ -17987,13 +18365,13 @@
         <v>12</v>
       </c>
       <c r="H19" s="3" t="s">
-        <v>378</v>
+        <v>381</v>
       </c>
       <c r="I19" s="4" t="n">
         <v>0</v>
       </c>
       <c r="J19" s="5" t="s">
-        <v>349</v>
+        <v>352</v>
       </c>
       <c r="K19" s="6"/>
       <c r="L19" s="3" t="s">
@@ -18026,13 +18404,13 @@
         <v>12</v>
       </c>
       <c r="H20" s="3" t="s">
-        <v>378</v>
+        <v>381</v>
       </c>
       <c r="I20" s="4" t="n">
         <v>0</v>
       </c>
       <c r="J20" s="5" t="s">
-        <v>349</v>
+        <v>352</v>
       </c>
       <c r="K20" s="6"/>
       <c r="L20" s="3" t="s">
@@ -18065,13 +18443,13 @@
         <v>12</v>
       </c>
       <c r="H21" s="3" t="s">
-        <v>378</v>
+        <v>381</v>
       </c>
       <c r="I21" s="4" t="n">
         <v>0</v>
       </c>
       <c r="J21" s="5" t="s">
-        <v>349</v>
+        <v>352</v>
       </c>
       <c r="K21" s="6"/>
       <c r="L21" s="3" t="s">
@@ -18104,13 +18482,13 @@
         <v>12</v>
       </c>
       <c r="H22" s="3" t="s">
-        <v>378</v>
+        <v>381</v>
       </c>
       <c r="I22" s="4" t="n">
         <v>0</v>
       </c>
       <c r="J22" s="5" t="s">
-        <v>349</v>
+        <v>352</v>
       </c>
       <c r="K22" s="6"/>
       <c r="L22" s="3" t="s">
@@ -18182,13 +18560,13 @@
         <v>12</v>
       </c>
       <c r="H24" s="3" t="s">
-        <v>393</v>
+        <v>396</v>
       </c>
       <c r="I24" s="4" t="n">
         <v>0</v>
       </c>
       <c r="J24" s="5" t="s">
-        <v>349</v>
+        <v>352</v>
       </c>
       <c r="K24" s="6"/>
       <c r="L24" s="3" t="s">
@@ -18221,13 +18599,13 @@
         <v>12</v>
       </c>
       <c r="H25" s="3" t="s">
-        <v>393</v>
+        <v>396</v>
       </c>
       <c r="I25" s="4" t="n">
         <v>0</v>
       </c>
       <c r="J25" s="5" t="s">
-        <v>349</v>
+        <v>352</v>
       </c>
       <c r="K25" s="6"/>
       <c r="L25" s="3" t="s">
@@ -18260,13 +18638,13 @@
         <v>12</v>
       </c>
       <c r="H26" s="3" t="s">
-        <v>393</v>
+        <v>396</v>
       </c>
       <c r="I26" s="4" t="n">
         <v>0</v>
       </c>
       <c r="J26" s="5" t="s">
-        <v>349</v>
+        <v>352</v>
       </c>
       <c r="K26" s="6"/>
       <c r="L26" s="3" t="s">
@@ -18299,13 +18677,13 @@
         <v>12</v>
       </c>
       <c r="H27" s="3" t="s">
-        <v>393</v>
+        <v>396</v>
       </c>
       <c r="I27" s="4" t="n">
         <v>0</v>
       </c>
       <c r="J27" s="5" t="s">
-        <v>349</v>
+        <v>352</v>
       </c>
       <c r="K27" s="6"/>
       <c r="L27" s="3" t="s">

</xml_diff>

<commit_message>
opening 1 diamonds ->  1H (up to 2), try to change suit mark not only in desciption but also in suitLentht (and don't want biding level in table but I dont' know why )!
</commit_message>
<xml_diff>
--- a/bridgeIn.xlsx
+++ b/bridgeIn.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2247" uniqueCount="421">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2335" uniqueCount="449">
   <si>
     <t>bidId</t>
   </si>
@@ -1578,21 +1578,108 @@
     <t>7+ PC,  4 +  kierów/pików ; przy dwóch czwórkach kierowa, przy dwóch piątkach pikowa;  forsuje na jedno okrążenie</t>
   </si>
   <si>
+    <t>4+ karo brak 4 kier</t>
+  </si>
+  <si>
+    <t>kara i piki</t>
+  </si>
+  <si>
+    <t>1pik (tylko po kierze :))- 12-17PC-  4+ karo, 4 piki, brak czterech kierów, [u mnie było forsuje na jedno okrążenie]</t>
+  </si>
+  <si>
+    <t>5-3-3-2</t>
+  </si>
+  <si>
+    <t>1BA  12-14 PC, bez starszej czwórki -  układ -5-3-3-2</t>
+  </si>
+  <si>
+    <t>5+ karo i 4+ trefle</t>
+  </si>
+  <si>
+    <t>kara i trefle</t>
+  </si>
+  <si>
+    <t>2trefl  12-14 PC   5+ karo i  4+  trefli. (w wersji opcjonalnej też z 5 trefli i czwórką karo przy 12-17 PC oraz na dwóch piątkach młodszych 12-14PC)</t>
+  </si>
+  <si>
+    <t>6+ karo, możliwe trefl, bez 4s</t>
+  </si>
+  <si>
+    <t>szóstka karo</t>
+  </si>
+  <si>
+    <t>2karo  12-14 PC, 6+ karo, możliwe trefle, starsza czwórka wykluczona</t>
+  </si>
+  <si>
+    <t>4+ kier, 4+ karo</t>
+  </si>
+  <si>
+    <t>kiery i kara</t>
+  </si>
+  <si>
+    <t>2kier 2pik (licytowany) 12-14 PC  4+ kier pik, 4+ karo;  jeżeli REWERS(po przeciwnym) 15-17 PC,4 drugi starszy i 5 kar</t>
+  </si>
+  <si>
+    <t>4+ pik i 5 karo</t>
+  </si>
+  <si>
+    <t>brak 4s</t>
+  </si>
+  <si>
+    <t>nie BA</t>
+  </si>
+  <si>
+    <t>2BA    15-17 PC, brak starszej  czwórki, karta nie nadająca się do otwarcia 1BA np. ze względu na krótkość lub 6 kar, forsing</t>
+  </si>
+  <si>
+    <t>5-5 na mł</t>
+  </si>
+  <si>
+    <t>5-5 na młodszych</t>
+  </si>
+  <si>
+    <t>3trefl    15-17 PC, układ 5-5 na kolorach młodszych</t>
+  </si>
+  <si>
+    <t>6 karo</t>
+  </si>
+  <si>
+    <t>3karo    15-17 PC, 6 kar z dwiema starszymi figurami, forsing?</t>
+  </si>
+  <si>
+    <t>4+kier, 4+karo</t>
+  </si>
+  <si>
+    <t>3kier 3pik 15-17 PC (licytowany)   4+ kier pik, 4+ karo ;  jeżeli REWERS(po przeciwnym) 4 fit w kolorze odpowiadającego,  5 kar  oraz krótkość w zgłaszanym starszym SPLINTER</t>
+  </si>
+  <si>
+    <t>5 karo  4 kiery i krotkość w pikach</t>
+  </si>
+  <si>
+    <t>pełne kara</t>
+  </si>
+  <si>
+    <t>3BA  kontrakt do gry na pełnych karach (ale lepiej grać bez atu)</t>
+  </si>
+  <si>
+    <t>5+ karo i fit 4 + krótkość trefl</t>
+  </si>
+  <si>
+    <t>4trefl    15-17 PC, 5+ karo - fit 4  w kolorze odpowiadającego (kier pik) + krótkość trefl w  SPLINTER</t>
+  </si>
+  <si>
+    <t>4kier pik  15-17 PC (licytowany kolor) (nie ma REWERSU)- kontrakt  (liczymy że pójdzie na układzie)</t>
+  </si>
+  <si>
     <t>czwórka w pikach</t>
   </si>
   <si>
-    <t>brak 4s</t>
-  </si>
-  <si>
-    <t> 7-9(10) PC, bez starszej czwórki, nie forsuje</t>
+    <t>7-9(10) PC, bez starszej czwórki, nie forsuje</t>
   </si>
   <si>
     <t>5+ kar i 4+ trefl</t>
   </si>
   <si>
-    <t>kara i trefle</t>
-  </si>
-  <si>
     <t>12-14 PC   5+ kar i  4+  trefl .(w wersji opcjonalnej też z 5 trefli i czwórką karo przy 12-17 PC oraz na dwóch piątkach młodszych 12-14PC)</t>
   </si>
   <si>
@@ -1602,7 +1689,7 @@
     <t>kara bez starszej</t>
   </si>
   <si>
-    <t> 12-14 PC, 6+ kar, możliwe trefle, starsza czwórka wykluczona </t>
+    <t>12-14 PC, 6+ kar, możliwe trefle, starsza czwórka wykluczona</t>
   </si>
   <si>
     <t>4 kiery 5+kar</t>
@@ -1617,9 +1704,6 @@
     <t>4 piki 5+kar</t>
   </si>
   <si>
-    <t>kara i piki</t>
-  </si>
-  <si>
     <t>5+, 5+ na młodszych</t>
   </si>
   <si>
@@ -1677,7 +1761,7 @@
     <t>15-17  PC –5+ kar,  4trefle oraz krótkość w kolor  SPLINTER</t>
   </si>
   <si>
-    <t>(RELAY) –12-14 PC  4-4-4-1 </t>
+    <t>(RELAY) –12-14 PC  4-4-4-1</t>
   </si>
   <si>
     <t>3+ kara brak 4s</t>
@@ -1719,7 +1803,7 @@
     <t>bez 4s i 5m</t>
   </si>
   <si>
-    <t> (12)13-16 PC, bez starszej czwórki i młodszej piątki – do gry</t>
+    <t>(12)13-16 PC, bez starszej czwórki i młodszej piątki – do gry</t>
   </si>
   <si>
     <t>4+ kara i singiel terfl</t>
@@ -2209,7 +2293,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="80">
+  <cellXfs count="81">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2514,6 +2598,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2607,12 +2695,12 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M336"/>
+  <dimension ref="A1:M351"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="525" topLeftCell="A278" activePane="bottomLeft" state="split"/>
+      <pane xSplit="0" ySplit="525" topLeftCell="A283" activePane="bottomLeft" state="split"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="L291" activeCellId="0" sqref="L291"/>
+      <selection pane="bottomLeft" activeCell="B301" activeCellId="0" sqref="B301"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -14637,83 +14725,83 @@
       <c r="A287" s="0" t="n">
         <v>286</v>
       </c>
-      <c r="B287" s="8" t="n">
-        <f aca="false">A$284</f>
-        <v>283</v>
-      </c>
-      <c r="C287" s="8" t="n">
+      <c r="B287" s="15" t="n">
+        <f aca="false">A$286</f>
+        <v>285</v>
+      </c>
+      <c r="C287" s="15" t="n">
+        <v>2</v>
+      </c>
+      <c r="D287" s="16" t="n">
         <v>1</v>
       </c>
-      <c r="D287" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="E287" s="8" t="s">
+      <c r="E287" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="F287" s="10" t="n">
-        <v>7</v>
-      </c>
-      <c r="G287" s="10" t="n">
-        <v>37</v>
-      </c>
-      <c r="H287" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="I287" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="J287" s="12" t="s">
+      <c r="F287" s="17" t="n">
+        <v>12</v>
+      </c>
+      <c r="G287" s="17" t="n">
+        <v>17</v>
+      </c>
+      <c r="H287" s="17" t="s">
         <v>308</v>
       </c>
-      <c r="K287" s="13" t="s">
-        <v>307</v>
-      </c>
-      <c r="L287" s="10" t="s">
+      <c r="I287" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="J287" s="19" t="s">
+        <v>309</v>
+      </c>
+      <c r="K287" s="30" t="s">
+        <v>310</v>
+      </c>
+      <c r="L287" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="M287" s="14" t="s">
+      <c r="M287" s="21" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="288" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="288" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A288" s="0" t="n">
         <v>287</v>
       </c>
-      <c r="B288" s="8" t="n">
-        <f aca="false">A$284</f>
-        <v>283</v>
-      </c>
-      <c r="C288" s="8" t="n">
+      <c r="B288" s="15" t="n">
+        <f aca="false">A$286</f>
+        <v>285</v>
+      </c>
+      <c r="C288" s="15" t="n">
+        <v>2</v>
+      </c>
+      <c r="D288" s="16" t="n">
         <v>1</v>
       </c>
-      <c r="D288" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="E288" s="8" t="s">
+      <c r="E288" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="F288" s="10" t="n">
-        <v>7</v>
-      </c>
-      <c r="G288" s="10" t="n">
-        <v>9</v>
-      </c>
-      <c r="H288" s="10" t="s">
-        <v>309</v>
-      </c>
-      <c r="I288" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="J288" s="12" t="s">
-        <v>100</v>
-      </c>
-      <c r="K288" s="13" t="s">
-        <v>310</v>
-      </c>
-      <c r="L288" s="10" t="s">
+      <c r="F288" s="17" t="n">
+        <v>12</v>
+      </c>
+      <c r="G288" s="17" t="n">
+        <v>14</v>
+      </c>
+      <c r="H288" s="17" t="s">
+        <v>311</v>
+      </c>
+      <c r="I288" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="J288" s="19" t="s">
+        <v>133</v>
+      </c>
+      <c r="K288" s="30" t="s">
+        <v>312</v>
+      </c>
+      <c r="L288" s="17" t="s">
         <v>107</v>
       </c>
-      <c r="M288" s="14" t="s">
+      <c r="M288" s="21" t="s">
         <v>62</v>
       </c>
     </row>
@@ -14722,8 +14810,8 @@
         <v>288</v>
       </c>
       <c r="B289" s="15" t="n">
-        <f aca="false">A288</f>
-        <v>287</v>
+        <f aca="false">A$286</f>
+        <v>285</v>
       </c>
       <c r="C289" s="15" t="n">
         <v>2</v>
@@ -14741,16 +14829,16 @@
         <v>14</v>
       </c>
       <c r="H289" s="17" t="s">
-        <v>311</v>
+        <v>313</v>
       </c>
       <c r="I289" s="18" t="n">
         <v>0</v>
       </c>
       <c r="J289" s="19" t="s">
-        <v>312</v>
+        <v>314</v>
       </c>
       <c r="K289" s="30" t="s">
-        <v>313</v>
+        <v>315</v>
       </c>
       <c r="L289" s="17" t="s">
         <v>107</v>
@@ -14764,8 +14852,8 @@
         <v>289</v>
       </c>
       <c r="B290" s="15" t="n">
-        <f aca="false">A288</f>
-        <v>287</v>
+        <f aca="false">A$286</f>
+        <v>285</v>
       </c>
       <c r="C290" s="15" t="n">
         <v>2</v>
@@ -14783,16 +14871,16 @@
         <v>14</v>
       </c>
       <c r="H290" s="17" t="s">
-        <v>314</v>
+        <v>316</v>
       </c>
       <c r="I290" s="18" t="n">
         <v>0</v>
       </c>
       <c r="J290" s="19" t="s">
-        <v>315</v>
+        <v>317</v>
       </c>
       <c r="K290" s="30" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="L290" s="17" t="s">
         <v>107</v>
@@ -14806,8 +14894,8 @@
         <v>290</v>
       </c>
       <c r="B291" s="15" t="n">
-        <f aca="false">A288</f>
-        <v>287</v>
+        <f aca="false">A$286</f>
+        <v>285</v>
       </c>
       <c r="C291" s="15" t="n">
         <v>2</v>
@@ -14819,25 +14907,25 @@
         <v>22</v>
       </c>
       <c r="F291" s="17" t="n">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="G291" s="17" t="n">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="H291" s="17" t="s">
-        <v>317</v>
+        <v>319</v>
       </c>
       <c r="I291" s="18" t="n">
         <v>0</v>
       </c>
       <c r="J291" s="19" t="s">
-        <v>318</v>
+        <v>320</v>
       </c>
       <c r="K291" s="30" t="s">
-        <v>319</v>
+        <v>321</v>
       </c>
       <c r="L291" s="17" t="s">
-        <v>35</v>
+        <v>107</v>
       </c>
       <c r="M291" s="21" t="s">
         <v>62</v>
@@ -14848,8 +14936,8 @@
         <v>291</v>
       </c>
       <c r="B292" s="15" t="n">
-        <f aca="false">A288</f>
-        <v>287</v>
+        <f aca="false">A$286</f>
+        <v>285</v>
       </c>
       <c r="C292" s="15" t="n">
         <v>2</v>
@@ -14861,22 +14949,22 @@
         <v>31</v>
       </c>
       <c r="F292" s="17" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G292" s="17" t="n">
         <v>17</v>
       </c>
       <c r="H292" s="17" t="s">
-        <v>320</v>
+        <v>322</v>
       </c>
       <c r="I292" s="18" t="n">
         <v>0</v>
       </c>
       <c r="J292" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="K292" s="30" t="s">
         <v>321</v>
-      </c>
-      <c r="K292" s="30" t="s">
-        <v>319</v>
       </c>
       <c r="L292" s="17" t="s">
         <v>35</v>
@@ -14890,17 +14978,17 @@
         <v>292</v>
       </c>
       <c r="B293" s="15" t="n">
-        <f aca="false">A288</f>
-        <v>287</v>
+        <f aca="false">A$286</f>
+        <v>285</v>
       </c>
       <c r="C293" s="15" t="n">
         <v>2</v>
       </c>
       <c r="D293" s="16" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E293" s="15" t="s">
-        <v>13</v>
+        <v>32</v>
       </c>
       <c r="F293" s="17" t="n">
         <v>15</v>
@@ -14909,16 +14997,16 @@
         <v>17</v>
       </c>
       <c r="H293" s="17" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="I293" s="18" t="n">
         <v>0</v>
       </c>
       <c r="J293" s="19" t="s">
-        <v>312</v>
+        <v>324</v>
       </c>
       <c r="K293" s="30" t="s">
-        <v>323</v>
+        <v>325</v>
       </c>
       <c r="L293" s="17" t="s">
         <v>35</v>
@@ -14932,8 +15020,8 @@
         <v>293</v>
       </c>
       <c r="B294" s="15" t="n">
-        <f aca="false">A288</f>
-        <v>287</v>
+        <f aca="false">A$286</f>
+        <v>285</v>
       </c>
       <c r="C294" s="15" t="n">
         <v>2</v>
@@ -14942,7 +15030,7 @@
         <v>3</v>
       </c>
       <c r="E294" s="15" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="F294" s="17" t="n">
         <v>15</v>
@@ -14951,16 +15039,16 @@
         <v>17</v>
       </c>
       <c r="H294" s="17" t="s">
-        <v>324</v>
+        <v>326</v>
       </c>
       <c r="I294" s="18" t="n">
         <v>0</v>
       </c>
       <c r="J294" s="19" t="s">
-        <v>325</v>
+        <v>327</v>
       </c>
       <c r="K294" s="30" t="s">
-        <v>326</v>
+        <v>328</v>
       </c>
       <c r="L294" s="17" t="s">
         <v>35</v>
@@ -14973,102 +15061,102 @@
       <c r="A295" s="0" t="n">
         <v>294</v>
       </c>
-      <c r="B295" s="8" t="n">
-        <f aca="false">A$284</f>
-        <v>283</v>
-      </c>
-      <c r="C295" s="8" t="n">
-        <v>1</v>
-      </c>
-      <c r="D295" s="9" t="n">
-        <v>2</v>
-      </c>
-      <c r="E295" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="F295" s="10" t="n">
-        <v>10</v>
-      </c>
-      <c r="G295" s="10" t="n">
-        <v>37</v>
-      </c>
-      <c r="H295" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="I295" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="J295" s="12" t="s">
-        <v>262</v>
-      </c>
-      <c r="K295" s="13" t="s">
-        <v>327</v>
-      </c>
-      <c r="L295" s="10" t="s">
+      <c r="B295" s="15" t="n">
+        <f aca="false">A$286</f>
+        <v>285</v>
+      </c>
+      <c r="C295" s="15" t="n">
+        <v>2</v>
+      </c>
+      <c r="D295" s="16" t="n">
+        <v>3</v>
+      </c>
+      <c r="E295" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="F295" s="17" t="n">
+        <v>15</v>
+      </c>
+      <c r="G295" s="17" t="n">
         <v>17</v>
       </c>
-      <c r="M295" s="14" t="s">
+      <c r="H295" s="17" t="s">
+        <v>329</v>
+      </c>
+      <c r="I295" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="J295" s="19" t="s">
+        <v>317</v>
+      </c>
+      <c r="K295" s="30" t="s">
+        <v>330</v>
+      </c>
+      <c r="L295" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="M295" s="21" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="296" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="296" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A296" s="0" t="n">
         <v>295</v>
       </c>
       <c r="B296" s="15" t="n">
-        <f aca="false">A295</f>
-        <v>294</v>
+        <f aca="false">A$286</f>
+        <v>285</v>
       </c>
       <c r="C296" s="15" t="n">
         <v>2</v>
       </c>
       <c r="D296" s="16" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E296" s="15" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="F296" s="17" t="n">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="G296" s="17" t="n">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="H296" s="17" t="s">
-        <v>36</v>
+        <v>331</v>
       </c>
       <c r="I296" s="18" t="n">
         <v>0</v>
       </c>
       <c r="J296" s="19" t="s">
-        <v>328</v>
-      </c>
-      <c r="K296" s="30" t="s">
-        <v>329</v>
+        <v>320</v>
+      </c>
+      <c r="K296" s="76" t="s">
+        <v>332</v>
       </c>
       <c r="L296" s="17" t="s">
-        <v>107</v>
+        <v>35</v>
       </c>
       <c r="M296" s="21" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="297" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="297" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A297" s="0" t="n">
         <v>296</v>
       </c>
       <c r="B297" s="15" t="n">
-        <f aca="false">A295</f>
-        <v>294</v>
+        <f aca="false">A$286</f>
+        <v>285</v>
       </c>
       <c r="C297" s="15" t="n">
         <v>2</v>
       </c>
       <c r="D297" s="16" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E297" s="15" t="s">
-        <v>22</v>
+        <v>31</v>
       </c>
       <c r="F297" s="17" t="n">
         <v>15</v>
@@ -15077,22 +15165,22 @@
         <v>17</v>
       </c>
       <c r="H297" s="17" t="s">
-        <v>330</v>
+        <v>333</v>
       </c>
       <c r="I297" s="18" t="n">
         <v>0</v>
       </c>
       <c r="J297" s="19" t="s">
-        <v>318</v>
-      </c>
-      <c r="K297" s="30" t="s">
-        <v>331</v>
+        <v>280</v>
+      </c>
+      <c r="K297" s="76" t="s">
+        <v>332</v>
       </c>
       <c r="L297" s="17" t="s">
         <v>44</v>
       </c>
       <c r="M297" s="21" t="s">
-        <v>62</v>
+        <v>18</v>
       </c>
     </row>
     <row r="298" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15100,17 +15188,17 @@
         <v>297</v>
       </c>
       <c r="B298" s="15" t="n">
-        <f aca="false">A295</f>
-        <v>294</v>
+        <f aca="false">A$286</f>
+        <v>285</v>
       </c>
       <c r="C298" s="15" t="n">
         <v>2</v>
       </c>
       <c r="D298" s="16" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E298" s="15" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F298" s="17" t="n">
         <v>15</v>
@@ -15119,19 +15207,19 @@
         <v>17</v>
       </c>
       <c r="H298" s="17" t="s">
-        <v>332</v>
+        <v>334</v>
       </c>
       <c r="I298" s="18" t="n">
         <v>0</v>
       </c>
       <c r="J298" s="19" t="s">
-        <v>321</v>
+        <v>128</v>
       </c>
       <c r="K298" s="30" t="s">
-        <v>331</v>
+        <v>335</v>
       </c>
       <c r="L298" s="17" t="s">
-        <v>44</v>
+        <v>31</v>
       </c>
       <c r="M298" s="21" t="s">
         <v>62</v>
@@ -15142,17 +15230,17 @@
         <v>298</v>
       </c>
       <c r="B299" s="15" t="n">
-        <f aca="false">A295</f>
-        <v>294</v>
+        <f aca="false">A$286</f>
+        <v>285</v>
       </c>
       <c r="C299" s="15" t="n">
         <v>2</v>
       </c>
       <c r="D299" s="16" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E299" s="15" t="s">
-        <v>32</v>
+        <v>13</v>
       </c>
       <c r="F299" s="17" t="n">
         <v>15</v>
@@ -15161,19 +15249,19 @@
         <v>17</v>
       </c>
       <c r="H299" s="17" t="s">
-        <v>333</v>
+        <v>336</v>
       </c>
       <c r="I299" s="18" t="n">
         <v>0</v>
       </c>
       <c r="J299" s="19" t="s">
-        <v>334</v>
+        <v>280</v>
       </c>
       <c r="K299" s="30" t="s">
-        <v>335</v>
+        <v>337</v>
       </c>
       <c r="L299" s="17" t="s">
-        <v>44</v>
+        <v>31</v>
       </c>
       <c r="M299" s="21" t="s">
         <v>18</v>
@@ -15184,17 +15272,17 @@
         <v>299</v>
       </c>
       <c r="B300" s="15" t="n">
-        <f aca="false">A295</f>
-        <v>294</v>
+        <f aca="false">A$286</f>
+        <v>285</v>
       </c>
       <c r="C300" s="15" t="n">
         <v>2</v>
       </c>
       <c r="D300" s="16" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E300" s="15" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="F300" s="17" t="n">
         <v>15</v>
@@ -15202,20 +15290,18 @@
       <c r="G300" s="17" t="n">
         <v>17</v>
       </c>
-      <c r="H300" s="17" t="s">
-        <v>336</v>
-      </c>
+      <c r="H300" s="17"/>
       <c r="I300" s="18" t="n">
         <v>0</v>
       </c>
       <c r="J300" s="19" t="s">
-        <v>312</v>
+        <v>167</v>
       </c>
       <c r="K300" s="30" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="L300" s="17" t="s">
-        <v>44</v>
+        <v>31</v>
       </c>
       <c r="M300" s="21" t="s">
         <v>62</v>
@@ -15226,17 +15312,17 @@
         <v>300</v>
       </c>
       <c r="B301" s="15" t="n">
-        <f aca="false">A295</f>
-        <v>294</v>
+        <f aca="false">A$286</f>
+        <v>285</v>
       </c>
       <c r="C301" s="15" t="n">
         <v>2</v>
       </c>
       <c r="D301" s="16" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E301" s="15" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="F301" s="17" t="n">
         <v>15</v>
@@ -15244,20 +15330,18 @@
       <c r="G301" s="17" t="n">
         <v>17</v>
       </c>
-      <c r="H301" s="17" t="s">
-        <v>95</v>
-      </c>
+      <c r="H301" s="17"/>
       <c r="I301" s="18" t="n">
         <v>0</v>
       </c>
       <c r="J301" s="19" t="s">
-        <v>112</v>
+        <v>167</v>
       </c>
       <c r="K301" s="30" t="s">
         <v>338</v>
       </c>
       <c r="L301" s="17" t="s">
-        <v>44</v>
+        <v>31</v>
       </c>
       <c r="M301" s="21" t="s">
         <v>62</v>
@@ -15267,84 +15351,84 @@
       <c r="A302" s="0" t="n">
         <v>301</v>
       </c>
-      <c r="B302" s="15" t="n">
-        <f aca="false">A295</f>
-        <v>294</v>
-      </c>
-      <c r="C302" s="15" t="n">
-        <v>2</v>
-      </c>
-      <c r="D302" s="16" t="n">
-        <v>3</v>
-      </c>
-      <c r="E302" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="F302" s="17" t="n">
-        <v>15</v>
-      </c>
-      <c r="G302" s="17" t="n">
+      <c r="B302" s="8" t="n">
+        <f aca="false">A$284</f>
+        <v>283</v>
+      </c>
+      <c r="C302" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="D302" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="E302" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="F302" s="10" t="n">
+        <v>7</v>
+      </c>
+      <c r="G302" s="10" t="n">
+        <v>37</v>
+      </c>
+      <c r="H302" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="I302" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="J302" s="12" t="s">
+        <v>339</v>
+      </c>
+      <c r="K302" s="13" t="s">
+        <v>307</v>
+      </c>
+      <c r="L302" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="H302" s="17" t="s">
-        <v>339</v>
-      </c>
-      <c r="I302" s="18" t="n">
-        <v>0</v>
-      </c>
-      <c r="J302" s="19" t="s">
-        <v>280</v>
-      </c>
-      <c r="K302" s="30" t="s">
-        <v>340</v>
-      </c>
-      <c r="L302" s="17" t="s">
-        <v>44</v>
-      </c>
-      <c r="M302" s="21" t="s">
-        <v>18</v>
+      <c r="M302" s="14" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="303" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A303" s="0" t="n">
         <v>302</v>
       </c>
-      <c r="B303" s="15" t="n">
-        <f aca="false">A295</f>
-        <v>294</v>
-      </c>
-      <c r="C303" s="15" t="n">
-        <v>2</v>
-      </c>
-      <c r="D303" s="16" t="n">
-        <v>3</v>
-      </c>
-      <c r="E303" s="15" t="s">
-        <v>31</v>
-      </c>
-      <c r="F303" s="17" t="n">
-        <v>15</v>
-      </c>
-      <c r="G303" s="17" t="n">
-        <v>17</v>
-      </c>
-      <c r="H303" s="17" t="s">
-        <v>339</v>
-      </c>
-      <c r="I303" s="18" t="n">
-        <v>0</v>
-      </c>
-      <c r="J303" s="19" t="s">
-        <v>280</v>
-      </c>
-      <c r="K303" s="30" t="s">
+      <c r="B303" s="8" t="n">
+        <f aca="false">A$284</f>
+        <v>283</v>
+      </c>
+      <c r="C303" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="D303" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="E303" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="F303" s="10" t="n">
+        <v>7</v>
+      </c>
+      <c r="G303" s="10" t="n">
+        <v>9</v>
+      </c>
+      <c r="H303" s="10" t="s">
+        <v>323</v>
+      </c>
+      <c r="I303" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="J303" s="12" t="s">
+        <v>100</v>
+      </c>
+      <c r="K303" s="13" t="s">
         <v>340</v>
       </c>
-      <c r="L303" s="17" t="s">
-        <v>44</v>
-      </c>
-      <c r="M303" s="21" t="s">
-        <v>18</v>
+      <c r="L303" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="M303" s="14" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="304" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15352,17 +15436,17 @@
         <v>303</v>
       </c>
       <c r="B304" s="15" t="n">
-        <f aca="false">A295</f>
-        <v>294</v>
+        <f aca="false">A303</f>
+        <v>302</v>
       </c>
       <c r="C304" s="15" t="n">
         <v>2</v>
       </c>
       <c r="D304" s="16" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E304" s="15" t="s">
-        <v>32</v>
+        <v>13</v>
       </c>
       <c r="F304" s="17" t="n">
         <v>12</v>
@@ -15371,63 +15455,63 @@
         <v>14</v>
       </c>
       <c r="H304" s="17" t="s">
-        <v>333</v>
+        <v>341</v>
       </c>
       <c r="I304" s="18" t="n">
         <v>0</v>
       </c>
       <c r="J304" s="19" t="s">
-        <v>167</v>
+        <v>314</v>
       </c>
       <c r="K304" s="30" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="L304" s="17" t="s">
-        <v>31</v>
+        <v>107</v>
       </c>
       <c r="M304" s="21" t="s">
-        <v>18</v>
+        <v>62</v>
       </c>
     </row>
     <row r="305" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A305" s="0" t="n">
         <v>304</v>
       </c>
-      <c r="B305" s="8" t="n">
-        <f aca="false">A$284</f>
-        <v>283</v>
-      </c>
-      <c r="C305" s="8" t="n">
-        <v>1</v>
-      </c>
-      <c r="D305" s="9" t="n">
-        <v>2</v>
-      </c>
-      <c r="E305" s="8" t="s">
+      <c r="B305" s="15" t="n">
+        <f aca="false">A303</f>
+        <v>302</v>
+      </c>
+      <c r="C305" s="15" t="n">
+        <v>2</v>
+      </c>
+      <c r="D305" s="16" t="n">
+        <v>2</v>
+      </c>
+      <c r="E305" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="F305" s="10" t="n">
+      <c r="F305" s="17" t="n">
         <v>12</v>
       </c>
-      <c r="G305" s="10" t="n">
-        <v>37</v>
-      </c>
-      <c r="H305" s="10" t="s">
-        <v>342</v>
-      </c>
-      <c r="I305" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="J305" s="12" t="s">
-        <v>57</v>
-      </c>
-      <c r="K305" s="13" t="s">
+      <c r="G305" s="17" t="n">
+        <v>14</v>
+      </c>
+      <c r="H305" s="17" t="s">
         <v>343</v>
       </c>
-      <c r="L305" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="M305" s="14" t="s">
+      <c r="I305" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="J305" s="19" t="s">
+        <v>344</v>
+      </c>
+      <c r="K305" s="30" t="s">
+        <v>345</v>
+      </c>
+      <c r="L305" s="17" t="s">
+        <v>107</v>
+      </c>
+      <c r="M305" s="21" t="s">
         <v>62</v>
       </c>
     </row>
@@ -15435,41 +15519,41 @@
       <c r="A306" s="0" t="n">
         <v>305</v>
       </c>
-      <c r="B306" s="8" t="n">
-        <f aca="false">A$284</f>
-        <v>283</v>
-      </c>
-      <c r="C306" s="8" t="n">
-        <v>1</v>
-      </c>
-      <c r="D306" s="9" t="n">
-        <v>2</v>
-      </c>
-      <c r="E306" s="8" t="s">
+      <c r="B306" s="15" t="n">
+        <f aca="false">A303</f>
+        <v>302</v>
+      </c>
+      <c r="C306" s="15" t="n">
+        <v>2</v>
+      </c>
+      <c r="D306" s="16" t="n">
+        <v>2</v>
+      </c>
+      <c r="E306" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="F306" s="10" t="n">
-        <v>12</v>
-      </c>
-      <c r="G306" s="10" t="n">
-        <v>37</v>
-      </c>
-      <c r="H306" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="I306" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="J306" s="12" t="s">
-        <v>114</v>
-      </c>
-      <c r="K306" s="13" t="s">
-        <v>344</v>
-      </c>
-      <c r="L306" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="M306" s="14" t="s">
+      <c r="F306" s="17" t="n">
+        <v>15</v>
+      </c>
+      <c r="G306" s="17" t="n">
+        <v>17</v>
+      </c>
+      <c r="H306" s="17" t="s">
+        <v>346</v>
+      </c>
+      <c r="I306" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="J306" s="19" t="s">
+        <v>347</v>
+      </c>
+      <c r="K306" s="30" t="s">
+        <v>348</v>
+      </c>
+      <c r="L306" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="M306" s="21" t="s">
         <v>62</v>
       </c>
     </row>
@@ -15477,41 +15561,41 @@
       <c r="A307" s="0" t="n">
         <v>306</v>
       </c>
-      <c r="B307" s="8" t="n">
-        <f aca="false">A$284</f>
-        <v>283</v>
-      </c>
-      <c r="C307" s="8" t="n">
-        <v>1</v>
-      </c>
-      <c r="D307" s="9" t="n">
-        <v>2</v>
-      </c>
-      <c r="E307" s="8" t="s">
+      <c r="B307" s="15" t="n">
+        <f aca="false">A303</f>
+        <v>302</v>
+      </c>
+      <c r="C307" s="15" t="n">
+        <v>2</v>
+      </c>
+      <c r="D307" s="16" t="n">
+        <v>2</v>
+      </c>
+      <c r="E307" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="F307" s="10" t="n">
-        <v>12</v>
-      </c>
-      <c r="G307" s="10" t="n">
-        <v>37</v>
-      </c>
-      <c r="H307" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="I307" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="J307" s="12" t="s">
-        <v>274</v>
-      </c>
-      <c r="K307" s="13" t="s">
-        <v>344</v>
-      </c>
-      <c r="L307" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="M307" s="14" t="s">
+      <c r="F307" s="17" t="n">
+        <v>15</v>
+      </c>
+      <c r="G307" s="17" t="n">
+        <v>17</v>
+      </c>
+      <c r="H307" s="17" t="s">
+        <v>349</v>
+      </c>
+      <c r="I307" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="J307" s="19" t="s">
+        <v>309</v>
+      </c>
+      <c r="K307" s="30" t="s">
+        <v>348</v>
+      </c>
+      <c r="L307" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="M307" s="21" t="s">
         <v>62</v>
       </c>
     </row>
@@ -15519,41 +15603,41 @@
       <c r="A308" s="0" t="n">
         <v>307</v>
       </c>
-      <c r="B308" s="8" t="n">
-        <f aca="false">A$284</f>
-        <v>283</v>
-      </c>
-      <c r="C308" s="8" t="n">
-        <v>1</v>
-      </c>
-      <c r="D308" s="9" t="n">
-        <v>2</v>
-      </c>
-      <c r="E308" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="F308" s="10" t="n">
-        <v>11</v>
-      </c>
-      <c r="G308" s="10" t="n">
-        <v>12</v>
-      </c>
-      <c r="H308" s="10" t="s">
-        <v>309</v>
-      </c>
-      <c r="I308" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="J308" s="12" t="s">
-        <v>119</v>
-      </c>
-      <c r="K308" s="13" t="s">
-        <v>345</v>
-      </c>
-      <c r="L308" s="10" t="s">
+      <c r="B308" s="15" t="n">
+        <f aca="false">A303</f>
+        <v>302</v>
+      </c>
+      <c r="C308" s="15" t="n">
+        <v>2</v>
+      </c>
+      <c r="D308" s="16" t="n">
+        <v>3</v>
+      </c>
+      <c r="E308" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="F308" s="17" t="n">
+        <v>15</v>
+      </c>
+      <c r="G308" s="17" t="n">
+        <v>17</v>
+      </c>
+      <c r="H308" s="17" t="s">
+        <v>350</v>
+      </c>
+      <c r="I308" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="J308" s="19" t="s">
+        <v>314</v>
+      </c>
+      <c r="K308" s="30" t="s">
+        <v>351</v>
+      </c>
+      <c r="L308" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="M308" s="14" t="s">
+      <c r="M308" s="21" t="s">
         <v>62</v>
       </c>
     </row>
@@ -15561,41 +15645,41 @@
       <c r="A309" s="0" t="n">
         <v>308</v>
       </c>
-      <c r="B309" s="8" t="n">
-        <f aca="false">A$284</f>
-        <v>283</v>
-      </c>
-      <c r="C309" s="8" t="n">
-        <v>1</v>
-      </c>
-      <c r="D309" s="9" t="n">
-        <v>3</v>
-      </c>
-      <c r="E309" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="F309" s="10" t="n">
-        <v>9</v>
-      </c>
-      <c r="G309" s="10" t="n">
-        <v>11</v>
-      </c>
-      <c r="H309" s="10" t="s">
-        <v>346</v>
-      </c>
-      <c r="I309" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="J309" s="12" t="s">
-        <v>119</v>
-      </c>
-      <c r="K309" s="13" t="s">
-        <v>347</v>
-      </c>
-      <c r="L309" s="10" t="s">
+      <c r="B309" s="15" t="n">
+        <f aca="false">A303</f>
+        <v>302</v>
+      </c>
+      <c r="C309" s="15" t="n">
+        <v>2</v>
+      </c>
+      <c r="D309" s="16" t="n">
+        <v>3</v>
+      </c>
+      <c r="E309" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="F309" s="17" t="n">
+        <v>15</v>
+      </c>
+      <c r="G309" s="17" t="n">
+        <v>17</v>
+      </c>
+      <c r="H309" s="17" t="s">
+        <v>352</v>
+      </c>
+      <c r="I309" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="J309" s="19" t="s">
+        <v>353</v>
+      </c>
+      <c r="K309" s="30" t="s">
+        <v>354</v>
+      </c>
+      <c r="L309" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="M309" s="14" t="s">
+      <c r="M309" s="21" t="s">
         <v>62</v>
       </c>
     </row>
@@ -15611,31 +15695,31 @@
         <v>1</v>
       </c>
       <c r="D310" s="9" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E310" s="8" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="F310" s="10" t="n">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="G310" s="10" t="n">
-        <v>9</v>
+        <v>37</v>
       </c>
       <c r="H310" s="10" t="s">
-        <v>348</v>
+        <v>36</v>
       </c>
       <c r="I310" s="11" t="n">
         <v>0</v>
       </c>
       <c r="J310" s="12" t="s">
-        <v>349</v>
+        <v>262</v>
       </c>
       <c r="K310" s="13" t="s">
-        <v>350</v>
+        <v>355</v>
       </c>
       <c r="L310" s="10" t="s">
-        <v>351</v>
+        <v>17</v>
       </c>
       <c r="M310" s="14" t="s">
         <v>62</v>
@@ -15645,125 +15729,125 @@
       <c r="A311" s="0" t="n">
         <v>310</v>
       </c>
-      <c r="B311" s="8" t="n">
-        <f aca="false">A$284</f>
-        <v>283</v>
-      </c>
-      <c r="C311" s="8" t="n">
-        <v>1</v>
-      </c>
-      <c r="D311" s="9" t="n">
-        <v>3</v>
-      </c>
-      <c r="E311" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="F311" s="10" t="n">
+      <c r="B311" s="15" t="n">
+        <f aca="false">A310</f>
+        <v>309</v>
+      </c>
+      <c r="C311" s="15" t="n">
+        <v>2</v>
+      </c>
+      <c r="D311" s="16" t="n">
+        <v>2</v>
+      </c>
+      <c r="E311" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="F311" s="17" t="n">
         <v>12</v>
       </c>
-      <c r="G311" s="10" t="n">
-        <v>15</v>
-      </c>
-      <c r="H311" s="10" t="s">
-        <v>352</v>
-      </c>
-      <c r="I311" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="J311" s="12" t="s">
-        <v>280</v>
-      </c>
-      <c r="K311" s="13" t="s">
-        <v>353</v>
-      </c>
-      <c r="L311" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="M311" s="14" t="s">
-        <v>18</v>
+      <c r="G311" s="17" t="n">
+        <v>14</v>
+      </c>
+      <c r="H311" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="I311" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="J311" s="19" t="s">
+        <v>356</v>
+      </c>
+      <c r="K311" s="30" t="s">
+        <v>357</v>
+      </c>
+      <c r="L311" s="17" t="s">
+        <v>107</v>
+      </c>
+      <c r="M311" s="21" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="312" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A312" s="0" t="n">
         <v>311</v>
       </c>
-      <c r="B312" s="8" t="n">
-        <f aca="false">A$284</f>
-        <v>283</v>
-      </c>
-      <c r="C312" s="8" t="n">
-        <v>1</v>
-      </c>
-      <c r="D312" s="9" t="n">
-        <v>3</v>
-      </c>
-      <c r="E312" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="F312" s="10" t="n">
-        <v>12</v>
-      </c>
-      <c r="G312" s="10" t="n">
+      <c r="B312" s="15" t="n">
+        <f aca="false">A310</f>
+        <v>309</v>
+      </c>
+      <c r="C312" s="15" t="n">
+        <v>2</v>
+      </c>
+      <c r="D312" s="16" t="n">
+        <v>2</v>
+      </c>
+      <c r="E312" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="F312" s="17" t="n">
         <v>15</v>
       </c>
-      <c r="H312" s="10" t="s">
-        <v>352</v>
-      </c>
-      <c r="I312" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="J312" s="12" t="s">
-        <v>280</v>
-      </c>
-      <c r="K312" s="13" t="s">
-        <v>353</v>
-      </c>
-      <c r="L312" s="10" t="s">
+      <c r="G312" s="17" t="n">
+        <v>17</v>
+      </c>
+      <c r="H312" s="17" t="s">
+        <v>358</v>
+      </c>
+      <c r="I312" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="J312" s="19" t="s">
+        <v>347</v>
+      </c>
+      <c r="K312" s="30" t="s">
+        <v>359</v>
+      </c>
+      <c r="L312" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="M312" s="14" t="s">
-        <v>18</v>
+      <c r="M312" s="21" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="313" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A313" s="0" t="n">
         <v>312</v>
       </c>
-      <c r="B313" s="8" t="n">
-        <f aca="false">A$284</f>
-        <v>283</v>
-      </c>
-      <c r="C313" s="8" t="n">
-        <v>1</v>
-      </c>
-      <c r="D313" s="9" t="n">
-        <v>3</v>
-      </c>
-      <c r="E313" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="F313" s="10" t="n">
-        <v>13</v>
-      </c>
-      <c r="G313" s="10" t="n">
-        <v>16</v>
-      </c>
-      <c r="H313" s="10" t="s">
-        <v>354</v>
-      </c>
-      <c r="I313" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="J313" s="12" t="s">
-        <v>128</v>
-      </c>
-      <c r="K313" s="13" t="s">
-        <v>355</v>
-      </c>
-      <c r="L313" s="10" t="s">
+      <c r="B313" s="15" t="n">
+        <f aca="false">A310</f>
+        <v>309</v>
+      </c>
+      <c r="C313" s="15" t="n">
+        <v>2</v>
+      </c>
+      <c r="D313" s="16" t="n">
+        <v>2</v>
+      </c>
+      <c r="E313" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="M313" s="14" t="s">
+      <c r="F313" s="17" t="n">
+        <v>15</v>
+      </c>
+      <c r="G313" s="17" t="n">
+        <v>17</v>
+      </c>
+      <c r="H313" s="17" t="s">
+        <v>360</v>
+      </c>
+      <c r="I313" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="J313" s="19" t="s">
+        <v>309</v>
+      </c>
+      <c r="K313" s="30" t="s">
+        <v>359</v>
+      </c>
+      <c r="L313" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="M313" s="21" t="s">
         <v>62</v>
       </c>
     </row>
@@ -15771,41 +15855,41 @@
       <c r="A314" s="0" t="n">
         <v>313</v>
       </c>
-      <c r="B314" s="8" t="n">
-        <f aca="false">A$284</f>
-        <v>283</v>
-      </c>
-      <c r="C314" s="8" t="n">
-        <v>1</v>
-      </c>
-      <c r="D314" s="9" t="n">
-        <v>4</v>
-      </c>
-      <c r="E314" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="F314" s="10" t="n">
-        <v>12</v>
-      </c>
-      <c r="G314" s="10" t="n">
+      <c r="B314" s="15" t="n">
+        <f aca="false">A310</f>
+        <v>309</v>
+      </c>
+      <c r="C314" s="15" t="n">
+        <v>2</v>
+      </c>
+      <c r="D314" s="16" t="n">
+        <v>2</v>
+      </c>
+      <c r="E314" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="F314" s="17" t="n">
         <v>15</v>
       </c>
-      <c r="H314" s="10" t="s">
-        <v>356</v>
-      </c>
-      <c r="I314" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="J314" s="12" t="s">
-        <v>280</v>
-      </c>
-      <c r="K314" s="13" t="s">
-        <v>357</v>
-      </c>
-      <c r="L314" s="10" t="s">
+      <c r="G314" s="17" t="n">
+        <v>17</v>
+      </c>
+      <c r="H314" s="17" t="s">
+        <v>361</v>
+      </c>
+      <c r="I314" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="J314" s="19" t="s">
+        <v>362</v>
+      </c>
+      <c r="K314" s="30" t="s">
+        <v>363</v>
+      </c>
+      <c r="L314" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="M314" s="14" t="s">
+      <c r="M314" s="21" t="s">
         <v>18</v>
       </c>
     </row>
@@ -15813,40 +15897,41 @@
       <c r="A315" s="0" t="n">
         <v>314</v>
       </c>
-      <c r="B315" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="C315" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="D315" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="E315" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F315" s="3" t="n">
-        <v>12</v>
-      </c>
-      <c r="G315" s="3" t="n">
+      <c r="B315" s="15" t="n">
+        <f aca="false">A310</f>
+        <v>309</v>
+      </c>
+      <c r="C315" s="15" t="n">
+        <v>2</v>
+      </c>
+      <c r="D315" s="16" t="n">
+        <v>3</v>
+      </c>
+      <c r="E315" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="F315" s="17" t="n">
+        <v>15</v>
+      </c>
+      <c r="G315" s="17" t="n">
         <v>17</v>
       </c>
-      <c r="H315" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="I315" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="J315" s="5" t="s">
-        <v>358</v>
-      </c>
-      <c r="K315" s="6" t="s">
-        <v>359</v>
-      </c>
-      <c r="L315" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="M315" s="3" t="s">
+      <c r="H315" s="17" t="s">
+        <v>364</v>
+      </c>
+      <c r="I315" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="J315" s="19" t="s">
+        <v>314</v>
+      </c>
+      <c r="K315" s="30" t="s">
+        <v>365</v>
+      </c>
+      <c r="L315" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="M315" s="21" t="s">
         <v>62</v>
       </c>
     </row>
@@ -15854,578 +15939,591 @@
       <c r="A316" s="0" t="n">
         <v>315</v>
       </c>
-      <c r="B316" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="C316" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="D316" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="E316" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="F316" s="3" t="n">
-        <v>12</v>
-      </c>
-      <c r="G316" s="3" t="n">
+      <c r="B316" s="15" t="n">
+        <f aca="false">A310</f>
+        <v>309</v>
+      </c>
+      <c r="C316" s="15" t="n">
+        <v>2</v>
+      </c>
+      <c r="D316" s="16" t="n">
+        <v>3</v>
+      </c>
+      <c r="E316" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="F316" s="17" t="n">
+        <v>15</v>
+      </c>
+      <c r="G316" s="17" t="n">
         <v>17</v>
       </c>
-      <c r="H316" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="I316" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="J316" s="5" t="s">
-        <v>358</v>
-      </c>
-      <c r="K316" s="6" t="s">
-        <v>360</v>
-      </c>
-      <c r="L316" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="M316" s="3" t="s">
+      <c r="H316" s="17" t="s">
+        <v>95</v>
+      </c>
+      <c r="I316" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="J316" s="19" t="s">
+        <v>112</v>
+      </c>
+      <c r="K316" s="30" t="s">
+        <v>366</v>
+      </c>
+      <c r="L316" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="M316" s="21" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="317" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="317" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A317" s="0" t="n">
         <v>316</v>
       </c>
-      <c r="B317" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="C317" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="D317" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="E317" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="F317" s="3" t="n">
+      <c r="B317" s="15" t="n">
+        <f aca="false">A310</f>
+        <v>309</v>
+      </c>
+      <c r="C317" s="15" t="n">
+        <v>2</v>
+      </c>
+      <c r="D317" s="16" t="n">
+        <v>3</v>
+      </c>
+      <c r="E317" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="F317" s="17" t="n">
         <v>15</v>
       </c>
-      <c r="G317" s="3" t="n">
+      <c r="G317" s="17" t="n">
         <v>17</v>
       </c>
-      <c r="H317" s="3" t="s">
-        <v>361</v>
-      </c>
-      <c r="I317" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="J317" s="5" t="s">
-        <v>362</v>
-      </c>
-      <c r="K317" s="6" t="s">
-        <v>363</v>
-      </c>
-      <c r="L317" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="M317" s="3" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="318" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H317" s="17" t="s">
+        <v>367</v>
+      </c>
+      <c r="I317" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="J317" s="19" t="s">
+        <v>280</v>
+      </c>
+      <c r="K317" s="30" t="s">
+        <v>368</v>
+      </c>
+      <c r="L317" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="M317" s="21" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="318" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A318" s="0" t="n">
         <v>317</v>
       </c>
-      <c r="B318" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="C318" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="D318" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="E318" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F318" s="3" t="n">
-        <v>11</v>
-      </c>
-      <c r="G318" s="3" t="n">
+      <c r="B318" s="15" t="n">
+        <f aca="false">A310</f>
+        <v>309</v>
+      </c>
+      <c r="C318" s="15" t="n">
+        <v>2</v>
+      </c>
+      <c r="D318" s="16" t="n">
+        <v>3</v>
+      </c>
+      <c r="E318" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="F318" s="17" t="n">
         <v>15</v>
       </c>
-      <c r="H318" s="3" t="s">
-        <v>364</v>
-      </c>
-      <c r="I318" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="J318" s="5" t="s">
-        <v>365</v>
-      </c>
-      <c r="K318" s="6" t="s">
-        <v>366</v>
-      </c>
-      <c r="L318" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="M318" s="3" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="319" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G318" s="17" t="n">
+        <v>17</v>
+      </c>
+      <c r="H318" s="17" t="s">
+        <v>367</v>
+      </c>
+      <c r="I318" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="J318" s="19" t="s">
+        <v>280</v>
+      </c>
+      <c r="K318" s="30" t="s">
+        <v>368</v>
+      </c>
+      <c r="L318" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="M318" s="21" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="319" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A319" s="0" t="n">
         <v>318</v>
       </c>
-      <c r="B319" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="C319" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="D319" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="E319" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F319" s="3" t="n">
-        <v>7</v>
-      </c>
-      <c r="G319" s="3" t="n">
-        <v>11</v>
-      </c>
-      <c r="H319" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="I319" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="J319" s="5" t="s">
-        <v>367</v>
-      </c>
-      <c r="K319" s="6" t="s">
-        <v>368</v>
-      </c>
-      <c r="L319" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="M319" s="3" t="s">
+      <c r="B319" s="15" t="n">
+        <f aca="false">A310</f>
+        <v>309</v>
+      </c>
+      <c r="C319" s="15" t="n">
+        <v>2</v>
+      </c>
+      <c r="D319" s="16" t="n">
+        <v>3</v>
+      </c>
+      <c r="E319" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="F319" s="17" t="n">
+        <v>12</v>
+      </c>
+      <c r="G319" s="17" t="n">
+        <v>14</v>
+      </c>
+      <c r="H319" s="17" t="s">
+        <v>361</v>
+      </c>
+      <c r="I319" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="J319" s="19" t="s">
+        <v>167</v>
+      </c>
+      <c r="K319" s="30" t="s">
+        <v>369</v>
+      </c>
+      <c r="L319" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="M319" s="21" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="320" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="320" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A320" s="0" t="n">
         <v>319</v>
       </c>
-      <c r="B320" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="C320" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="D320" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="E320" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F320" s="3" t="n">
-        <v>7</v>
-      </c>
-      <c r="G320" s="3" t="n">
-        <v>11</v>
-      </c>
-      <c r="H320" s="3" t="s">
-        <v>369</v>
-      </c>
-      <c r="I320" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="J320" s="5" t="s">
+      <c r="B320" s="8" t="n">
+        <f aca="false">A$284</f>
+        <v>283</v>
+      </c>
+      <c r="C320" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="D320" s="9" t="n">
+        <v>2</v>
+      </c>
+      <c r="E320" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="F320" s="10" t="n">
+        <v>12</v>
+      </c>
+      <c r="G320" s="10" t="n">
+        <v>37</v>
+      </c>
+      <c r="H320" s="10" t="s">
         <v>370</v>
       </c>
-      <c r="K320" s="6" t="s">
+      <c r="I320" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="J320" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="K320" s="13" t="s">
         <v>371</v>
       </c>
-      <c r="L320" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="M320" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="321" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L320" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="M320" s="14" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="321" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A321" s="0" t="n">
         <v>320</v>
       </c>
-      <c r="B321" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="C321" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="D321" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="E321" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="F321" s="3" t="n">
-        <v>7</v>
-      </c>
-      <c r="G321" s="3" t="n">
-        <v>11</v>
-      </c>
-      <c r="H321" s="3" t="s">
+      <c r="B321" s="8" t="n">
+        <f aca="false">A$284</f>
+        <v>283</v>
+      </c>
+      <c r="C321" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="D321" s="9" t="n">
+        <v>2</v>
+      </c>
+      <c r="E321" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="F321" s="10" t="n">
+        <v>12</v>
+      </c>
+      <c r="G321" s="10" t="n">
+        <v>37</v>
+      </c>
+      <c r="H321" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="I321" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="J321" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="K321" s="13" t="s">
         <v>372</v>
       </c>
-      <c r="I321" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="J321" s="5" t="s">
-        <v>373</v>
-      </c>
-      <c r="K321" s="6" t="s">
-        <v>374</v>
-      </c>
-      <c r="L321" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="M321" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="322" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L321" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="M321" s="14" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="322" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A322" s="0" t="n">
         <v>321</v>
       </c>
-      <c r="B322" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="C322" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="D322" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="E322" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="F322" s="3" t="n">
-        <v>7</v>
-      </c>
-      <c r="G322" s="3" t="n">
-        <v>11</v>
-      </c>
-      <c r="H322" s="3" t="s">
-        <v>375</v>
-      </c>
-      <c r="I322" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="J322" s="5" t="s">
-        <v>376</v>
-      </c>
-      <c r="K322" s="6" t="s">
-        <v>377</v>
-      </c>
-      <c r="L322" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="M322" s="3" t="s">
-        <v>18</v>
+      <c r="B322" s="8" t="n">
+        <f aca="false">A$284</f>
+        <v>283</v>
+      </c>
+      <c r="C322" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="D322" s="9" t="n">
+        <v>2</v>
+      </c>
+      <c r="E322" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="F322" s="10" t="n">
+        <v>12</v>
+      </c>
+      <c r="G322" s="10" t="n">
+        <v>37</v>
+      </c>
+      <c r="H322" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="I322" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="J322" s="12" t="s">
+        <v>274</v>
+      </c>
+      <c r="K322" s="13" t="s">
+        <v>372</v>
+      </c>
+      <c r="L322" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="M322" s="14" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="323" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A323" s="0" t="n">
         <v>322</v>
       </c>
-      <c r="B323" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="C323" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="D323" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="E323" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F323" s="3" t="n">
-        <v>6</v>
-      </c>
-      <c r="G323" s="3" t="n">
-        <v>10</v>
-      </c>
-      <c r="H323" s="3" t="s">
-        <v>378</v>
-      </c>
-      <c r="I323" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="J323" s="5" t="s">
-        <v>379</v>
-      </c>
-      <c r="K323" s="6" t="s">
-        <v>380</v>
-      </c>
-      <c r="L323" s="3" t="s">
-        <v>351</v>
-      </c>
-      <c r="M323" s="3" t="s">
-        <v>55</v>
+      <c r="B323" s="8" t="n">
+        <f aca="false">A$284</f>
+        <v>283</v>
+      </c>
+      <c r="C323" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="D323" s="9" t="n">
+        <v>2</v>
+      </c>
+      <c r="E323" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="F323" s="10" t="n">
+        <v>11</v>
+      </c>
+      <c r="G323" s="10" t="n">
+        <v>12</v>
+      </c>
+      <c r="H323" s="10" t="s">
+        <v>323</v>
+      </c>
+      <c r="I323" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="J323" s="12" t="s">
+        <v>119</v>
+      </c>
+      <c r="K323" s="13" t="s">
+        <v>373</v>
+      </c>
+      <c r="L323" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="M323" s="14" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="324" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A324" s="0" t="n">
         <v>323</v>
       </c>
-      <c r="B324" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="C324" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="D324" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="E324" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F324" s="3" t="n">
-        <v>6</v>
-      </c>
-      <c r="G324" s="3" t="n">
-        <v>10</v>
-      </c>
-      <c r="H324" s="3" t="s">
-        <v>378</v>
-      </c>
-      <c r="I324" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="J324" s="5" t="s">
-        <v>379</v>
-      </c>
-      <c r="K324" s="6" t="s">
-        <v>380</v>
-      </c>
-      <c r="L324" s="3" t="s">
-        <v>351</v>
-      </c>
-      <c r="M324" s="3" t="s">
-        <v>55</v>
+      <c r="B324" s="8" t="n">
+        <f aca="false">A$284</f>
+        <v>283</v>
+      </c>
+      <c r="C324" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="D324" s="9" t="n">
+        <v>3</v>
+      </c>
+      <c r="E324" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="F324" s="10" t="n">
+        <v>9</v>
+      </c>
+      <c r="G324" s="10" t="n">
+        <v>11</v>
+      </c>
+      <c r="H324" s="10" t="s">
+        <v>374</v>
+      </c>
+      <c r="I324" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="J324" s="12" t="s">
+        <v>119</v>
+      </c>
+      <c r="K324" s="13" t="s">
+        <v>375</v>
+      </c>
+      <c r="L324" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="M324" s="14" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="325" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A325" s="0" t="n">
         <v>324</v>
       </c>
-      <c r="B325" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="C325" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="D325" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="E325" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F325" s="3" t="n">
-        <v>6</v>
-      </c>
-      <c r="G325" s="3" t="n">
-        <v>10</v>
-      </c>
-      <c r="H325" s="3" t="s">
+      <c r="B325" s="8" t="n">
+        <f aca="false">A$284</f>
+        <v>283</v>
+      </c>
+      <c r="C325" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="D325" s="9" t="n">
+        <v>3</v>
+      </c>
+      <c r="E325" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="F325" s="10" t="n">
+        <v>7</v>
+      </c>
+      <c r="G325" s="10" t="n">
+        <v>9</v>
+      </c>
+      <c r="H325" s="10" t="s">
+        <v>376</v>
+      </c>
+      <c r="I325" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="J325" s="12" t="s">
+        <v>377</v>
+      </c>
+      <c r="K325" s="13" t="s">
         <v>378</v>
       </c>
-      <c r="I325" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="J325" s="5" t="s">
+      <c r="L325" s="10" t="s">
         <v>379</v>
       </c>
-      <c r="K325" s="6" t="s">
-        <v>380</v>
-      </c>
-      <c r="L325" s="3" t="s">
-        <v>351</v>
-      </c>
-      <c r="M325" s="3" t="s">
-        <v>55</v>
+      <c r="M325" s="14" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="326" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A326" s="0" t="n">
         <v>325</v>
       </c>
-      <c r="B326" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="C326" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="D326" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="E326" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="F326" s="3" t="n">
-        <v>6</v>
-      </c>
-      <c r="G326" s="3" t="n">
-        <v>10</v>
-      </c>
-      <c r="H326" s="3" t="s">
-        <v>378</v>
-      </c>
-      <c r="I326" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="J326" s="5" t="s">
-        <v>379</v>
-      </c>
-      <c r="K326" s="6" t="s">
+      <c r="B326" s="8" t="n">
+        <f aca="false">A$284</f>
+        <v>283</v>
+      </c>
+      <c r="C326" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="D326" s="9" t="n">
+        <v>3</v>
+      </c>
+      <c r="E326" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="F326" s="10" t="n">
+        <v>12</v>
+      </c>
+      <c r="G326" s="10" t="n">
+        <v>15</v>
+      </c>
+      <c r="H326" s="10" t="s">
         <v>380</v>
       </c>
-      <c r="L326" s="3" t="s">
-        <v>351</v>
-      </c>
-      <c r="M326" s="3" t="s">
-        <v>55</v>
+      <c r="I326" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="J326" s="12" t="s">
+        <v>280</v>
+      </c>
+      <c r="K326" s="13" t="s">
+        <v>381</v>
+      </c>
+      <c r="L326" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="M326" s="14" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="327" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A327" s="0" t="n">
         <v>326</v>
       </c>
-      <c r="B327" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="C327" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="D327" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="E327" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="F327" s="3" t="n">
-        <v>9</v>
-      </c>
-      <c r="G327" s="3" t="n">
-        <f aca="false">F327+13</f>
-        <v>22</v>
-      </c>
-      <c r="H327" s="3" t="s">
+      <c r="B327" s="8" t="n">
+        <f aca="false">A$284</f>
+        <v>283</v>
+      </c>
+      <c r="C327" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="D327" s="9" t="n">
+        <v>3</v>
+      </c>
+      <c r="E327" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="F327" s="10" t="n">
+        <v>12</v>
+      </c>
+      <c r="G327" s="10" t="n">
+        <v>15</v>
+      </c>
+      <c r="H327" s="10" t="s">
+        <v>380</v>
+      </c>
+      <c r="I327" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="J327" s="12" t="s">
+        <v>280</v>
+      </c>
+      <c r="K327" s="13" t="s">
         <v>381</v>
       </c>
-      <c r="I327" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="J327" s="5" t="s">
-        <v>382</v>
-      </c>
-      <c r="K327" s="6" t="s">
-        <v>383</v>
-      </c>
-      <c r="L327" s="3" t="s">
-        <v>351</v>
-      </c>
-      <c r="M327" s="3" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="328" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L327" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="M327" s="14" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="328" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A328" s="0" t="n">
         <v>327</v>
       </c>
-      <c r="B328" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="C328" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="D328" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="E328" s="1" t="s">
+      <c r="B328" s="8" t="n">
+        <f aca="false">A$284</f>
+        <v>283</v>
+      </c>
+      <c r="C328" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="D328" s="9" t="n">
+        <v>3</v>
+      </c>
+      <c r="E328" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="F328" s="10" t="n">
         <v>13</v>
       </c>
-      <c r="F328" s="3" t="n">
-        <v>8</v>
-      </c>
-      <c r="G328" s="3" t="n">
-        <v>10</v>
-      </c>
-      <c r="H328" s="3" t="s">
-        <v>384</v>
-      </c>
-      <c r="I328" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="J328" s="5" t="s">
-        <v>385</v>
-      </c>
-      <c r="K328" s="6" t="s">
-        <v>386</v>
-      </c>
-      <c r="L328" s="3" t="s">
-        <v>351</v>
-      </c>
-      <c r="M328" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="329" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G328" s="10" t="n">
+        <v>16</v>
+      </c>
+      <c r="H328" s="10" t="s">
+        <v>382</v>
+      </c>
+      <c r="I328" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="J328" s="12" t="s">
+        <v>128</v>
+      </c>
+      <c r="K328" s="13" t="s">
+        <v>383</v>
+      </c>
+      <c r="L328" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="M328" s="14" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="329" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A329" s="0" t="n">
         <v>328</v>
       </c>
-      <c r="B329" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="C329" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="D329" s="1" t="n">
+      <c r="B329" s="8" t="n">
+        <f aca="false">A$284</f>
+        <v>283</v>
+      </c>
+      <c r="C329" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="D329" s="9" t="n">
         <v>4</v>
       </c>
-      <c r="E329" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F329" s="3" t="n">
-        <v>8</v>
-      </c>
-      <c r="G329" s="3" t="n">
-        <v>10</v>
-      </c>
-      <c r="H329" s="3" t="s">
-        <v>387</v>
-      </c>
-      <c r="I329" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="J329" s="5" t="s">
+      <c r="E329" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="F329" s="10" t="n">
+        <v>12</v>
+      </c>
+      <c r="G329" s="10" t="n">
+        <v>15</v>
+      </c>
+      <c r="H329" s="10" t="s">
+        <v>384</v>
+      </c>
+      <c r="I329" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="J329" s="12" t="s">
+        <v>280</v>
+      </c>
+      <c r="K329" s="13" t="s">
         <v>385</v>
       </c>
-      <c r="K329" s="6" t="s">
-        <v>386</v>
-      </c>
-      <c r="L329" s="3" t="s">
-        <v>351</v>
-      </c>
-      <c r="M329" s="3" t="s">
+      <c r="L329" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="M329" s="14" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="330" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="330" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A330" s="0" t="n">
         <v>329</v>
       </c>
@@ -16436,37 +16534,37 @@
         <v>0</v>
       </c>
       <c r="D330" s="1" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E330" s="1" t="s">
         <v>22</v>
       </c>
       <c r="F330" s="3" t="n">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="G330" s="3" t="n">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="H330" s="3" t="s">
-        <v>388</v>
+        <v>36</v>
       </c>
       <c r="I330" s="4" t="n">
         <v>0</v>
       </c>
       <c r="J330" s="5" t="s">
-        <v>349</v>
+        <v>386</v>
       </c>
       <c r="K330" s="6" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="L330" s="3" t="s">
-        <v>351</v>
+        <v>107</v>
       </c>
       <c r="M330" s="3" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="331" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="331" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A331" s="0" t="n">
         <v>330</v>
       </c>
@@ -16477,37 +16575,37 @@
         <v>0</v>
       </c>
       <c r="D331" s="1" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E331" s="1" t="s">
         <v>31</v>
       </c>
       <c r="F331" s="3" t="n">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="G331" s="3" t="n">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="H331" s="3" t="s">
-        <v>390</v>
+        <v>36</v>
       </c>
       <c r="I331" s="4" t="n">
         <v>0</v>
       </c>
       <c r="J331" s="5" t="s">
-        <v>349</v>
+        <v>386</v>
       </c>
       <c r="K331" s="6" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="L331" s="3" t="s">
-        <v>351</v>
+        <v>107</v>
       </c>
       <c r="M331" s="3" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="332" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="332" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A332" s="0" t="n">
         <v>331</v>
       </c>
@@ -16518,37 +16616,37 @@
         <v>0</v>
       </c>
       <c r="D332" s="1" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E332" s="1" t="s">
         <v>32</v>
       </c>
       <c r="F332" s="3" t="n">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G332" s="3" t="n">
-        <v>32</v>
+        <v>17</v>
       </c>
       <c r="H332" s="3" t="s">
-        <v>73</v>
+        <v>389</v>
       </c>
       <c r="I332" s="4" t="n">
         <v>0</v>
       </c>
       <c r="J332" s="5" t="s">
+        <v>390</v>
+      </c>
+      <c r="K332" s="6" t="s">
         <v>391</v>
       </c>
-      <c r="K332" s="6" t="s">
-        <v>392</v>
-      </c>
       <c r="L332" s="3" t="s">
-        <v>17</v>
+        <v>107</v>
       </c>
       <c r="M332" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="333" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="333" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A333" s="0" t="n">
         <v>332</v>
       </c>
@@ -16559,37 +16657,37 @@
         <v>0</v>
       </c>
       <c r="D333" s="1" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E333" s="1" t="s">
         <v>13</v>
       </c>
       <c r="F333" s="3" t="n">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="G333" s="3" t="n">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="H333" s="3" t="s">
+        <v>392</v>
+      </c>
+      <c r="I333" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="J333" s="5" t="s">
         <v>393</v>
-      </c>
-      <c r="I333" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="J333" s="5" t="s">
-        <v>349</v>
       </c>
       <c r="K333" s="6" t="s">
         <v>394</v>
       </c>
       <c r="L333" s="3" t="s">
-        <v>351</v>
+        <v>107</v>
       </c>
       <c r="M333" s="3" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="334" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="334" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A334" s="0" t="n">
         <v>333</v>
       </c>
@@ -16600,37 +16698,37 @@
         <v>0</v>
       </c>
       <c r="D334" s="1" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E334" s="1" t="s">
         <v>19</v>
       </c>
       <c r="F334" s="3" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G334" s="3" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H334" s="3" t="s">
-        <v>393</v>
+        <v>95</v>
       </c>
       <c r="I334" s="4" t="n">
         <v>0</v>
       </c>
       <c r="J334" s="5" t="s">
-        <v>349</v>
+        <v>395</v>
       </c>
       <c r="K334" s="6" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="L334" s="3" t="s">
-        <v>351</v>
+        <v>17</v>
       </c>
       <c r="M334" s="3" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="335" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="335" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A335" s="0" t="n">
         <v>334</v>
       </c>
@@ -16641,37 +16739,37 @@
         <v>0</v>
       </c>
       <c r="D335" s="1" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E335" s="1" t="s">
         <v>22</v>
       </c>
       <c r="F335" s="3" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="G335" s="3" t="n">
-        <v>37</v>
+        <v>11</v>
       </c>
       <c r="H335" s="3" t="s">
-        <v>378</v>
+        <v>397</v>
       </c>
       <c r="I335" s="4" t="n">
         <v>0</v>
       </c>
       <c r="J335" s="5" t="s">
-        <v>349</v>
+        <v>398</v>
       </c>
       <c r="K335" s="6" t="s">
-        <v>395</v>
+        <v>399</v>
       </c>
       <c r="L335" s="3" t="s">
-        <v>351</v>
+        <v>107</v>
       </c>
       <c r="M335" s="3" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="336" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="336" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A336" s="0" t="n">
         <v>335</v>
       </c>
@@ -16682,33 +16780,649 @@
         <v>0</v>
       </c>
       <c r="D336" s="1" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E336" s="1" t="s">
         <v>31</v>
       </c>
       <c r="F336" s="3" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="G336" s="3" t="n">
+        <v>11</v>
+      </c>
+      <c r="H336" s="3" t="s">
+        <v>400</v>
+      </c>
+      <c r="I336" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="J336" s="5" t="s">
+        <v>401</v>
+      </c>
+      <c r="K336" s="6" t="s">
+        <v>402</v>
+      </c>
+      <c r="L336" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="M336" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="337" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A337" s="0" t="n">
+        <v>336</v>
+      </c>
+      <c r="B337" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C337" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D337" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="E337" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F337" s="3" t="n">
+        <v>7</v>
+      </c>
+      <c r="G337" s="3" t="n">
+        <v>11</v>
+      </c>
+      <c r="H337" s="3" t="s">
+        <v>403</v>
+      </c>
+      <c r="I337" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="J337" s="5" t="s">
+        <v>404</v>
+      </c>
+      <c r="K337" s="6" t="s">
+        <v>405</v>
+      </c>
+      <c r="L337" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="M337" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="338" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A338" s="0" t="n">
+        <v>337</v>
+      </c>
+      <c r="B338" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C338" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D338" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="E338" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F338" s="3" t="n">
+        <v>6</v>
+      </c>
+      <c r="G338" s="3" t="n">
+        <v>10</v>
+      </c>
+      <c r="H338" s="3" t="s">
+        <v>406</v>
+      </c>
+      <c r="I338" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="J338" s="5" t="s">
+        <v>407</v>
+      </c>
+      <c r="K338" s="6" t="s">
+        <v>408</v>
+      </c>
+      <c r="L338" s="3" t="s">
+        <v>379</v>
+      </c>
+      <c r="M338" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="339" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A339" s="0" t="n">
+        <v>338</v>
+      </c>
+      <c r="B339" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C339" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D339" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="E339" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F339" s="3" t="n">
+        <v>6</v>
+      </c>
+      <c r="G339" s="3" t="n">
+        <v>10</v>
+      </c>
+      <c r="H339" s="3" t="s">
+        <v>406</v>
+      </c>
+      <c r="I339" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="J339" s="5" t="s">
+        <v>407</v>
+      </c>
+      <c r="K339" s="6" t="s">
+        <v>408</v>
+      </c>
+      <c r="L339" s="3" t="s">
+        <v>379</v>
+      </c>
+      <c r="M339" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="340" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A340" s="0" t="n">
+        <v>339</v>
+      </c>
+      <c r="B340" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C340" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D340" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="E340" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F340" s="3" t="n">
+        <v>6</v>
+      </c>
+      <c r="G340" s="3" t="n">
+        <v>10</v>
+      </c>
+      <c r="H340" s="3" t="s">
+        <v>406</v>
+      </c>
+      <c r="I340" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="J340" s="5" t="s">
+        <v>407</v>
+      </c>
+      <c r="K340" s="6" t="s">
+        <v>408</v>
+      </c>
+      <c r="L340" s="3" t="s">
+        <v>379</v>
+      </c>
+      <c r="M340" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="341" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A341" s="0" t="n">
+        <v>340</v>
+      </c>
+      <c r="B341" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C341" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D341" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="E341" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F341" s="3" t="n">
+        <v>6</v>
+      </c>
+      <c r="G341" s="3" t="n">
+        <v>10</v>
+      </c>
+      <c r="H341" s="3" t="s">
+        <v>406</v>
+      </c>
+      <c r="I341" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="J341" s="5" t="s">
+        <v>407</v>
+      </c>
+      <c r="K341" s="6" t="s">
+        <v>408</v>
+      </c>
+      <c r="L341" s="3" t="s">
+        <v>379</v>
+      </c>
+      <c r="M341" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="342" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A342" s="0" t="n">
+        <v>341</v>
+      </c>
+      <c r="B342" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C342" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D342" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="E342" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F342" s="3" t="n">
+        <v>9</v>
+      </c>
+      <c r="G342" s="3" t="n">
+        <f aca="false">F342+13</f>
+        <v>22</v>
+      </c>
+      <c r="H342" s="3" t="s">
+        <v>409</v>
+      </c>
+      <c r="I342" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="J342" s="5" t="s">
+        <v>410</v>
+      </c>
+      <c r="K342" s="6" t="s">
+        <v>411</v>
+      </c>
+      <c r="L342" s="3" t="s">
+        <v>379</v>
+      </c>
+      <c r="M342" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="343" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A343" s="0" t="n">
+        <v>342</v>
+      </c>
+      <c r="B343" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C343" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D343" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="E343" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F343" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="G343" s="3" t="n">
+        <v>10</v>
+      </c>
+      <c r="H343" s="3" t="s">
+        <v>412</v>
+      </c>
+      <c r="I343" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="J343" s="5" t="s">
+        <v>413</v>
+      </c>
+      <c r="K343" s="6" t="s">
+        <v>414</v>
+      </c>
+      <c r="L343" s="3" t="s">
+        <v>379</v>
+      </c>
+      <c r="M343" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="344" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A344" s="0" t="n">
+        <v>343</v>
+      </c>
+      <c r="B344" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C344" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D344" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="E344" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F344" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="G344" s="3" t="n">
+        <v>10</v>
+      </c>
+      <c r="H344" s="3" t="s">
+        <v>415</v>
+      </c>
+      <c r="I344" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="J344" s="5" t="s">
+        <v>413</v>
+      </c>
+      <c r="K344" s="6" t="s">
+        <v>414</v>
+      </c>
+      <c r="L344" s="3" t="s">
+        <v>379</v>
+      </c>
+      <c r="M344" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="345" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A345" s="0" t="n">
+        <v>344</v>
+      </c>
+      <c r="B345" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C345" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D345" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="E345" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F345" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="G345" s="3" t="n">
+        <v>10</v>
+      </c>
+      <c r="H345" s="3" t="s">
+        <v>416</v>
+      </c>
+      <c r="I345" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="J345" s="5" t="s">
+        <v>377</v>
+      </c>
+      <c r="K345" s="6" t="s">
+        <v>417</v>
+      </c>
+      <c r="L345" s="3" t="s">
+        <v>379</v>
+      </c>
+      <c r="M345" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="346" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A346" s="0" t="n">
+        <v>345</v>
+      </c>
+      <c r="B346" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C346" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D346" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="E346" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F346" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="G346" s="3" t="n">
+        <v>10</v>
+      </c>
+      <c r="H346" s="3" t="s">
+        <v>418</v>
+      </c>
+      <c r="I346" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="J346" s="5" t="s">
+        <v>377</v>
+      </c>
+      <c r="K346" s="6" t="s">
+        <v>417</v>
+      </c>
+      <c r="L346" s="3" t="s">
+        <v>379</v>
+      </c>
+      <c r="M346" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="347" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A347" s="0" t="n">
+        <v>346</v>
+      </c>
+      <c r="B347" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C347" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D347" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="E347" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F347" s="3" t="n">
+        <v>16</v>
+      </c>
+      <c r="G347" s="3" t="n">
+        <v>32</v>
+      </c>
+      <c r="H347" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="I347" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="J347" s="5" t="s">
+        <v>419</v>
+      </c>
+      <c r="K347" s="6" t="s">
+        <v>420</v>
+      </c>
+      <c r="L347" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="M347" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="348" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A348" s="0" t="n">
+        <v>347</v>
+      </c>
+      <c r="B348" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C348" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D348" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="E348" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F348" s="3" t="n">
+        <v>6</v>
+      </c>
+      <c r="G348" s="3" t="n">
+        <v>10</v>
+      </c>
+      <c r="H348" s="3" t="s">
+        <v>421</v>
+      </c>
+      <c r="I348" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="J348" s="5" t="s">
+        <v>377</v>
+      </c>
+      <c r="K348" s="6" t="s">
+        <v>422</v>
+      </c>
+      <c r="L348" s="3" t="s">
+        <v>379</v>
+      </c>
+      <c r="M348" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="349" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A349" s="0" t="n">
+        <v>348</v>
+      </c>
+      <c r="B349" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C349" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D349" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="E349" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F349" s="3" t="n">
+        <v>6</v>
+      </c>
+      <c r="G349" s="3" t="n">
+        <v>10</v>
+      </c>
+      <c r="H349" s="3" t="s">
+        <v>421</v>
+      </c>
+      <c r="I349" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="J349" s="5" t="s">
+        <v>377</v>
+      </c>
+      <c r="K349" s="6" t="s">
+        <v>422</v>
+      </c>
+      <c r="L349" s="3" t="s">
+        <v>379</v>
+      </c>
+      <c r="M349" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="350" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A350" s="0" t="n">
+        <v>349</v>
+      </c>
+      <c r="B350" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C350" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D350" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="E350" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F350" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G350" s="3" t="n">
         <v>37</v>
       </c>
-      <c r="H336" s="3" t="s">
-        <v>378</v>
-      </c>
-      <c r="I336" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="J336" s="5" t="s">
-        <v>349</v>
-      </c>
-      <c r="K336" s="6" t="s">
-        <v>395</v>
-      </c>
-      <c r="L336" s="3" t="s">
-        <v>351</v>
-      </c>
-      <c r="M336" s="3" t="s">
+      <c r="H350" s="3" t="s">
+        <v>406</v>
+      </c>
+      <c r="I350" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="J350" s="5" t="s">
+        <v>377</v>
+      </c>
+      <c r="K350" s="6" t="s">
+        <v>423</v>
+      </c>
+      <c r="L350" s="3" t="s">
+        <v>379</v>
+      </c>
+      <c r="M350" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="351" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A351" s="0" t="n">
+        <v>350</v>
+      </c>
+      <c r="B351" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C351" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D351" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="E351" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F351" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G351" s="3" t="n">
+        <v>37</v>
+      </c>
+      <c r="H351" s="3" t="s">
+        <v>406</v>
+      </c>
+      <c r="I351" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="J351" s="5" t="s">
+        <v>377</v>
+      </c>
+      <c r="K351" s="6" t="s">
+        <v>423</v>
+      </c>
+      <c r="L351" s="3" t="s">
+        <v>379</v>
+      </c>
+      <c r="M351" s="3" t="s">
         <v>62</v>
       </c>
     </row>
@@ -16790,7 +17504,7 @@
       <c r="C2" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="D2" s="76" t="n">
+      <c r="D2" s="77" t="n">
         <v>1</v>
       </c>
       <c r="E2" s="0" t="s">
@@ -16809,15 +17523,15 @@
         <v>0</v>
       </c>
       <c r="J2" s="0" t="s">
-        <v>396</v>
-      </c>
-      <c r="K2" s="77" t="s">
-        <v>397</v>
+        <v>424</v>
+      </c>
+      <c r="K2" s="78" t="s">
+        <v>425</v>
       </c>
       <c r="L2" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="M2" s="78" t="s">
+      <c r="M2" s="79" t="s">
         <v>62</v>
       </c>
     </row>
@@ -16831,7 +17545,7 @@
       <c r="C3" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="D3" s="76" t="n">
+      <c r="D3" s="77" t="n">
         <v>1</v>
       </c>
       <c r="E3" s="0" t="s">
@@ -16851,15 +17565,15 @@
         <v>1</v>
       </c>
       <c r="J3" s="0" t="s">
-        <v>396</v>
-      </c>
-      <c r="K3" s="77" t="s">
-        <v>398</v>
+        <v>424</v>
+      </c>
+      <c r="K3" s="78" t="s">
+        <v>426</v>
       </c>
       <c r="L3" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="M3" s="78" t="s">
+      <c r="M3" s="79" t="s">
         <v>62</v>
       </c>
     </row>
@@ -16873,7 +17587,7 @@
       <c r="C4" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="D4" s="76" t="n">
+      <c r="D4" s="77" t="n">
         <v>1</v>
       </c>
       <c r="E4" s="0" t="s">
@@ -16892,15 +17606,15 @@
         <v>1</v>
       </c>
       <c r="J4" s="0" t="s">
-        <v>396</v>
-      </c>
-      <c r="K4" s="77" t="s">
-        <v>399</v>
+        <v>424</v>
+      </c>
+      <c r="K4" s="78" t="s">
+        <v>427</v>
       </c>
       <c r="L4" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="M4" s="78" t="s">
+      <c r="M4" s="79" t="s">
         <v>62</v>
       </c>
     </row>
@@ -16914,7 +17628,7 @@
       <c r="C5" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="D5" s="76" t="n">
+      <c r="D5" s="77" t="n">
         <v>1</v>
       </c>
       <c r="E5" s="0" t="s">
@@ -16933,15 +17647,15 @@
         <v>1</v>
       </c>
       <c r="J5" s="0" t="s">
-        <v>396</v>
-      </c>
-      <c r="K5" s="77" t="s">
-        <v>399</v>
+        <v>424</v>
+      </c>
+      <c r="K5" s="78" t="s">
+        <v>427</v>
       </c>
       <c r="L5" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="M5" s="78" t="s">
+      <c r="M5" s="79" t="s">
         <v>62</v>
       </c>
     </row>
@@ -17025,7 +17739,7 @@
       <c r="C2" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="D2" s="76" t="n">
+      <c r="D2" s="77" t="n">
         <v>1</v>
       </c>
       <c r="E2" s="0" t="s">
@@ -17044,15 +17758,15 @@
         <v>0</v>
       </c>
       <c r="J2" s="0" t="s">
-        <v>400</v>
-      </c>
-      <c r="K2" s="77" t="s">
-        <v>401</v>
+        <v>428</v>
+      </c>
+      <c r="K2" s="78" t="s">
+        <v>429</v>
       </c>
       <c r="L2" s="0" t="s">
-        <v>402</v>
-      </c>
-      <c r="M2" s="79"/>
+        <v>430</v>
+      </c>
+      <c r="M2" s="80"/>
     </row>
     <row r="3" customFormat="false" ht="170.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="n">
@@ -17064,7 +17778,7 @@
       <c r="C3" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="D3" s="76" t="n">
+      <c r="D3" s="77" t="n">
         <v>1</v>
       </c>
       <c r="E3" s="0" t="s">
@@ -17085,13 +17799,13 @@
       <c r="J3" s="0" t="s">
         <v>302</v>
       </c>
-      <c r="K3" s="77" t="s">
-        <v>403</v>
+      <c r="K3" s="78" t="s">
+        <v>431</v>
       </c>
       <c r="L3" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="M3" s="79"/>
+      <c r="M3" s="80"/>
     </row>
     <row r="4" customFormat="false" ht="282.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="n">
@@ -17103,7 +17817,7 @@
       <c r="C4" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="D4" s="76" t="n">
+      <c r="D4" s="77" t="n">
         <v>1</v>
       </c>
       <c r="E4" s="0" t="s">
@@ -17122,15 +17836,15 @@
         <v>0</v>
       </c>
       <c r="J4" s="0" t="s">
-        <v>404</v>
-      </c>
-      <c r="K4" s="77" t="s">
-        <v>405</v>
+        <v>432</v>
+      </c>
+      <c r="K4" s="78" t="s">
+        <v>433</v>
       </c>
       <c r="L4" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="M4" s="79"/>
+      <c r="M4" s="80"/>
     </row>
     <row r="5" customFormat="false" ht="129.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="n">
@@ -17142,7 +17856,7 @@
       <c r="C5" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="D5" s="76" t="n">
+      <c r="D5" s="77" t="n">
         <v>1</v>
       </c>
       <c r="E5" s="0" t="s">
@@ -17161,15 +17875,15 @@
         <v>0</v>
       </c>
       <c r="J5" s="0" t="s">
-        <v>406</v>
-      </c>
-      <c r="K5" s="77" t="s">
-        <v>407</v>
+        <v>434</v>
+      </c>
+      <c r="K5" s="78" t="s">
+        <v>435</v>
       </c>
       <c r="L5" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="M5" s="79"/>
+      <c r="M5" s="80"/>
     </row>
     <row r="6" customFormat="false" ht="58.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="n">
@@ -17181,7 +17895,7 @@
       <c r="C6" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="D6" s="76" t="n">
+      <c r="D6" s="77" t="n">
         <v>1</v>
       </c>
       <c r="E6" s="0" t="s">
@@ -17202,13 +17916,13 @@
       <c r="J6" s="0" t="s">
         <v>252</v>
       </c>
-      <c r="K6" s="77" t="s">
-        <v>408</v>
+      <c r="K6" s="78" t="s">
+        <v>436</v>
       </c>
       <c r="L6" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="M6" s="79"/>
+      <c r="M6" s="80"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -17311,16 +18025,16 @@
         <v>21</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>409</v>
+        <v>437</v>
       </c>
       <c r="I2" s="4" t="n">
         <v>0</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>410</v>
+        <v>438</v>
       </c>
       <c r="K2" s="6" t="s">
-        <v>411</v>
+        <v>439</v>
       </c>
       <c r="L2" s="3" t="s">
         <v>17</v>
@@ -17359,10 +18073,10 @@
         <v>0</v>
       </c>
       <c r="J3" s="12" t="s">
-        <v>412</v>
+        <v>440</v>
       </c>
       <c r="K3" s="13" t="s">
-        <v>413</v>
+        <v>441</v>
       </c>
       <c r="L3" s="10" t="s">
         <v>107</v>
@@ -17401,10 +18115,10 @@
         <v>0</v>
       </c>
       <c r="J4" s="12" t="s">
-        <v>414</v>
+        <v>442</v>
       </c>
       <c r="K4" s="13" t="s">
-        <v>415</v>
+        <v>443</v>
       </c>
       <c r="L4" s="10" t="s">
         <v>107</v>
@@ -17443,10 +18157,10 @@
         <v>0</v>
       </c>
       <c r="J5" s="12" t="s">
-        <v>416</v>
+        <v>444</v>
       </c>
       <c r="K5" s="13" t="s">
-        <v>417</v>
+        <v>445</v>
       </c>
       <c r="L5" s="10" t="s">
         <v>107</v>
@@ -17487,7 +18201,7 @@
         <v>100</v>
       </c>
       <c r="K6" s="12" t="s">
-        <v>418</v>
+        <v>446</v>
       </c>
       <c r="L6" s="10" t="s">
         <v>107</v>
@@ -17528,7 +18242,7 @@
         <v>262</v>
       </c>
       <c r="K7" s="12" t="s">
-        <v>419</v>
+        <v>447</v>
       </c>
       <c r="L7" s="10" t="s">
         <v>107</v>
@@ -17638,13 +18352,13 @@
         <v>21</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>409</v>
+        <v>437</v>
       </c>
       <c r="I10" s="4" t="n">
         <v>0</v>
       </c>
       <c r="J10" s="5" t="s">
-        <v>410</v>
+        <v>438</v>
       </c>
       <c r="K10" s="6"/>
       <c r="L10" s="3" t="s">
@@ -17683,7 +18397,7 @@
         <v>0</v>
       </c>
       <c r="J11" s="5" t="s">
-        <v>358</v>
+        <v>386</v>
       </c>
       <c r="K11" s="6"/>
       <c r="L11" s="3" t="s">
@@ -17722,7 +18436,7 @@
         <v>0</v>
       </c>
       <c r="J12" s="5" t="s">
-        <v>358</v>
+        <v>386</v>
       </c>
       <c r="K12" s="6"/>
       <c r="L12" s="3" t="s">
@@ -17761,7 +18475,7 @@
         <v>0</v>
       </c>
       <c r="J13" s="5" t="s">
-        <v>420</v>
+        <v>448</v>
       </c>
       <c r="K13" s="6"/>
       <c r="L13" s="3" t="s">
@@ -17802,7 +18516,7 @@
       </c>
       <c r="K14" s="6"/>
       <c r="L14" s="3" t="s">
-        <v>402</v>
+        <v>430</v>
       </c>
       <c r="M14" s="3" t="s">
         <v>45</v>
@@ -17837,7 +18551,7 @@
         <v>0</v>
       </c>
       <c r="J15" s="5" t="s">
-        <v>349</v>
+        <v>377</v>
       </c>
       <c r="K15" s="5"/>
       <c r="L15" s="3" t="s">
@@ -17876,7 +18590,7 @@
         <v>0</v>
       </c>
       <c r="J16" s="5" t="s">
-        <v>349</v>
+        <v>377</v>
       </c>
       <c r="K16" s="5"/>
       <c r="L16" s="3" t="s">
@@ -17915,7 +18629,7 @@
         <v>0</v>
       </c>
       <c r="J17" s="5" t="s">
-        <v>349</v>
+        <v>377</v>
       </c>
       <c r="K17" s="5"/>
       <c r="L17" s="3" t="s">
@@ -17987,13 +18701,13 @@
         <v>12</v>
       </c>
       <c r="H19" s="3" t="s">
-        <v>378</v>
+        <v>406</v>
       </c>
       <c r="I19" s="4" t="n">
         <v>0</v>
       </c>
       <c r="J19" s="5" t="s">
-        <v>349</v>
+        <v>377</v>
       </c>
       <c r="K19" s="6"/>
       <c r="L19" s="3" t="s">
@@ -18026,13 +18740,13 @@
         <v>12</v>
       </c>
       <c r="H20" s="3" t="s">
-        <v>378</v>
+        <v>406</v>
       </c>
       <c r="I20" s="4" t="n">
         <v>0</v>
       </c>
       <c r="J20" s="5" t="s">
-        <v>349</v>
+        <v>377</v>
       </c>
       <c r="K20" s="6"/>
       <c r="L20" s="3" t="s">
@@ -18065,13 +18779,13 @@
         <v>12</v>
       </c>
       <c r="H21" s="3" t="s">
-        <v>378</v>
+        <v>406</v>
       </c>
       <c r="I21" s="4" t="n">
         <v>0</v>
       </c>
       <c r="J21" s="5" t="s">
-        <v>349</v>
+        <v>377</v>
       </c>
       <c r="K21" s="6"/>
       <c r="L21" s="3" t="s">
@@ -18104,13 +18818,13 @@
         <v>12</v>
       </c>
       <c r="H22" s="3" t="s">
-        <v>378</v>
+        <v>406</v>
       </c>
       <c r="I22" s="4" t="n">
         <v>0</v>
       </c>
       <c r="J22" s="5" t="s">
-        <v>349</v>
+        <v>377</v>
       </c>
       <c r="K22" s="6"/>
       <c r="L22" s="3" t="s">
@@ -18182,13 +18896,13 @@
         <v>12</v>
       </c>
       <c r="H24" s="3" t="s">
-        <v>393</v>
+        <v>421</v>
       </c>
       <c r="I24" s="4" t="n">
         <v>0</v>
       </c>
       <c r="J24" s="5" t="s">
-        <v>349</v>
+        <v>377</v>
       </c>
       <c r="K24" s="6"/>
       <c r="L24" s="3" t="s">
@@ -18221,13 +18935,13 @@
         <v>12</v>
       </c>
       <c r="H25" s="3" t="s">
-        <v>393</v>
+        <v>421</v>
       </c>
       <c r="I25" s="4" t="n">
         <v>0</v>
       </c>
       <c r="J25" s="5" t="s">
-        <v>349</v>
+        <v>377</v>
       </c>
       <c r="K25" s="6"/>
       <c r="L25" s="3" t="s">
@@ -18260,13 +18974,13 @@
         <v>12</v>
       </c>
       <c r="H26" s="3" t="s">
-        <v>393</v>
+        <v>421</v>
       </c>
       <c r="I26" s="4" t="n">
         <v>0</v>
       </c>
       <c r="J26" s="5" t="s">
-        <v>349</v>
+        <v>377</v>
       </c>
       <c r="K26" s="6"/>
       <c r="L26" s="3" t="s">
@@ -18299,13 +19013,13 @@
         <v>12</v>
       </c>
       <c r="H27" s="3" t="s">
-        <v>393</v>
+        <v>421</v>
       </c>
       <c r="I27" s="4" t="n">
         <v>0</v>
       </c>
       <c r="J27" s="5" t="s">
-        <v>349</v>
+        <v>377</v>
       </c>
       <c r="K27" s="6"/>
       <c r="L27" s="3" t="s">

</xml_diff>

<commit_message>
all opening 3 and more  - second (~ 449 bids...)
</commit_message>
<xml_diff>
--- a/bridgeIn.xlsx
+++ b/bridgeIn.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2922" uniqueCount="550">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2922" uniqueCount="551">
   <si>
     <t>bidId</t>
   </si>
@@ -336,7 +336,7 @@
     <t>4-6 PC zrównoważony (nie wyklucza czwórki) – dalej 3 jest Staymanem</t>
   </si>
   <si>
-    <t>Splinter</t>
+    <t>SPLINTER</t>
   </si>
   <si>
     <r>
@@ -522,7 +522,7 @@
     </r>
   </si>
   <si>
-    <t>inwit do 3 NT</t>
+    <t>inwit do 3 BA</t>
   </si>
   <si>
     <r>
@@ -582,7 +582,7 @@
     <t>inwit do 4 pik</t>
   </si>
   <si>
-    <t>kontakt 3NT</t>
+    <t>kontrakt 3BA</t>
   </si>
   <si>
     <r>
@@ -599,7 +599,7 @@
     </r>
   </si>
   <si>
-    <t>Kontrakt 4 kier</t>
+    <t>kontrakt 4 kier</t>
   </si>
   <si>
     <r>
@@ -616,7 +616,7 @@
     </r>
   </si>
   <si>
-    <t>Kontrakt 4 pik</t>
+    <t>kontrakt 4 pik</t>
   </si>
   <si>
     <t>bez starszej czwórki</t>
@@ -793,7 +793,7 @@
     <t>5+ trefli</t>
   </si>
   <si>
-    <t>inwit do 3 NT/ Magister INŻYNIER</t>
+    <t>inwit do 3 BA/ Magister INŻYNIER</t>
   </si>
   <si>
     <t>2BA 11-12 PC skład zrównoważony inwit do 3BA – ??????? albo  (AUTORELAY) - gadżet  MAGISTER INŻYNIER (jak MAGISTER.  oraz 5+ trefli!)</t>
@@ -1386,6 +1386,9 @@
     <t>2BA  22-24 PC, układ zrównoważony inwit do szlemika ??? coś było inaczej ale bez sensu</t>
   </si>
   <si>
+    <t>kontakt 3NT</t>
+  </si>
+  <si>
     <t>3BA  18-21 PC  układ zrównoważony - kontrakt</t>
   </si>
   <si>
@@ -1424,9 +1427,6 @@
     <t>4 kara + splinter</t>
   </si>
   <si>
-    <t>SPLINTER</t>
-  </si>
-  <si>
     <t>15+  PC, 4 kart w kolorze partnera – SPLINTER wskazanie krótkości</t>
   </si>
   <si>
@@ -1508,7 +1508,7 @@
     </r>
   </si>
   <si>
-    <t>Blok albo autosplintere</t>
+    <t>Blok albo autoSPLINTERe</t>
   </si>
   <si>
     <r>
@@ -1569,34 +1569,34 @@
     <t>Brak 4 kar</t>
   </si>
   <si>
+    <t>nic ciekawego – patrz 3 kara...</t>
+  </si>
+  <si>
+    <t>7+ PC,  4 +  kierów/pików ; przy dwóch czwórkach kierowa, przy dwóch piątkach pikowa;  forsuje na jedno okrążenie</t>
+  </si>
+  <si>
+    <t>4+ karo brak 4 kier</t>
+  </si>
+  <si>
+    <t>kara i piki</t>
+  </si>
+  <si>
+    <t>1pik (tylko po kierze :))- 12-17PC-  4+ karo, 4 piki, brak czterech kierów, [u mnie było forsuje na jedno okrążenie]</t>
+  </si>
+  <si>
+    <t>5-3-3-2</t>
+  </si>
+  <si>
+    <t>1BA  12-14 PC, bez starszej czwórki -  układ -5-3-3-2</t>
+  </si>
+  <si>
     <t>pas</t>
   </si>
   <si>
-    <t>nic ciekawego – patrz 3 kara...</t>
-  </si>
-  <si>
-    <t>7+ PC,  4 +  kierów/pików ; przy dwóch czwórkach kierowa, przy dwóch piątkach pikowa;  forsuje na jedno okrążenie</t>
-  </si>
-  <si>
-    <t>4+ karo brak 4 kier</t>
-  </si>
-  <si>
-    <t>kara i piki</t>
-  </si>
-  <si>
-    <t>1pik (tylko po kierze :))- 12-17PC-  4+ karo, 4 piki, brak czterech kierów, [u mnie było forsuje na jedno okrążenie]</t>
-  </si>
-  <si>
-    <t>5-3-3-2</t>
-  </si>
-  <si>
-    <t>1BA  12-14 PC, bez starszej czwórki -  układ -5-3-3-2</t>
-  </si>
-  <si>
     <t>Pas – 7-10 PC układ zrównoważony</t>
   </si>
   <si>
-    <t>5+ kier </t>
+    <t>5+ kier</t>
   </si>
   <si>
     <t>trójznaczne trefl</t>
@@ -1614,13 +1614,10 @@
     <t>2karo 7-9 PC – 4 kolor i 3 +kara</t>
   </si>
   <si>
-    <t>5+ kier</t>
-  </si>
-  <si>
     <t>kiery</t>
   </si>
   <si>
-    <t>2kier   7-9  PC  kolor licytowany -   5+ w kolor </t>
+    <t>2kier   7-9  PC  kolor licytowany -   5+ w kolor</t>
   </si>
   <si>
     <t>5+ pik i 4 + kier</t>
@@ -1629,7 +1626,7 @@
     <t>piki i kiery</t>
   </si>
   <si>
-    <t>2pik  REWERS(chyba tylko po pikach bo kiery wykluczają piki):   5+ w  kolor (pik) oraz  i 4+ drugi starszy (kier) </t>
+    <t>2pik  REWERS(chyba tylko po pikach bo kiery wykluczają piki):   5+ w  kolor (pik) oraz  i 4+ drugi starszy (kier)</t>
   </si>
   <si>
     <t>2BA  11-12 PC zrówn -(po kierach bez  4 pik) iinwit do 3BA</t>
@@ -1647,7 +1644,7 @@
     <t>3karo 9-11 PC – 4  w kolor i 3 +kara inwit do 3BA</t>
   </si>
   <si>
-    <t>6+ kier </t>
+    <t>6+ kier</t>
   </si>
   <si>
     <t>3kier  po licytowanym: 10-12 PC 6+kier :inwit do 4 w kolor</t>
@@ -1665,9 +1662,6 @@
     <t>3BA 13-16 PC skład zrównoważony</t>
   </si>
   <si>
-    <t>6+ kier</t>
-  </si>
-  <si>
     <t>4kier  12-16 PC, 6+ w kolor.</t>
   </si>
   <si>
@@ -1716,7 +1710,7 @@
     <t>4-5 kier i 4+ karo</t>
   </si>
   <si>
-    <t>3karo 8-11 PC 4-5 w kolor  i 4 +kara inwit </t>
+    <t>3karo 8-11 PC 4-5 w kolor  i 4 +kara inwit</t>
   </si>
   <si>
     <t>3kier po licytowanym: 10-12 PC 6+kier :inwit do 4 w kolor</t>
@@ -1731,13 +1725,13 @@
     <t>3BA 13-16 PC wartości w pikach i kierach</t>
   </si>
   <si>
-    <t>4kier </t>
+    <t>4kier</t>
   </si>
   <si>
     <t>6+ pik</t>
   </si>
   <si>
-    <t>4pik  12-16  PC 6+ w kolor </t>
+    <t>4pik  12-16  PC 6+ w kolor</t>
   </si>
   <si>
     <t>6+ karo, możliwe trefl, bez 4s</t>
@@ -1761,7 +1755,7 @@
     <t>4+ pik i 5 karo</t>
   </si>
   <si>
-    <t>3kier/3pik - powtórzenie swojego koloru - </t>
+    <t>3kier/3pik - powtórzenie swojego koloru -</t>
   </si>
   <si>
     <t>4 kier i 5 pik lub 5-5</t>
@@ -1821,7 +1815,7 @@
     <t>czwórka w pikach</t>
   </si>
   <si>
-    <t>5+ pik </t>
+    <t>5+ pik</t>
   </si>
   <si>
     <t>4 pik i 3+ karo</t>
@@ -1831,9 +1825,6 @@
   </si>
   <si>
     <t>4+ pik i 4 + kier</t>
-  </si>
-  <si>
-    <t>5+ pik</t>
   </si>
   <si>
     <t>piki</t>
@@ -2081,7 +2072,7 @@
     <t>x-5-X-X</t>
   </si>
   <si>
-    <t>DWUKOLORÓWKA  5+ kier i 5+ młodszy</t>
+    <t>DWUKOLORÓWKA  5+ kier i 5+ mł.</t>
   </si>
   <si>
     <t>(6)7-10(11) PC, (przed partią nawet 4-9) dwie piątki: kierowa i dowolna  Licytacja po interwencji przeciwnika Po interwencji przeciwnika kontry są karne, a nowy kolor pełni rolę „pa­suj lub popraw".</t>
@@ -2090,7 +2081,7 @@
     <t>5-x-X-X</t>
   </si>
   <si>
-    <t>DWUKOLORÓWKA 5+ pik i 5+ dowolny</t>
+    <t>DWUKOLORÓWKA 5+ pik i 5+</t>
   </si>
   <si>
     <t>(6)7-10(11) PC, (przed partią nawet 4-9) dwie piątki: pikowa i młodsza Licytacja po interwencji przeciwnika Po interwencji przeciwnika kontry są karne, a nowy kolor pełni rolę „pa­suj lub popraw".</t>
@@ -2108,13 +2099,16 @@
     <t>7+</t>
   </si>
   <si>
-    <t>BLOK słaby</t>
+    <t>Dobry 7(8) kart</t>
   </si>
   <si>
     <t>(blokujące) (5)6-10 PC,  dobry licytowany kolor   7+ (przed partią może być dobre 6); w młodszym chętnie 8+ (lub dobry) Otwarcia są naturalne. Po partii ozna­czają kolor siedmiokartowy, a przed partią 3 w kolor młodszy może być oparte na  kolorze sześciokartowym. Siła otwar­cia  zależy od stylu gracza i ustaleń w pa­rze. W przypadku braku takowych pro­ponuję stosować metodę 4-3-2-2. (**) Ozna­cza ona, że do zapowiedzianego kon­traktu brakuje nam „na ręku": czterech lew, jeśli jesteśmy w założeniach ko­rzystnych, trzech lew w założeniach przedpartyjnych, dwóch lew jeśli jeste­śmy po partii.</t>
   </si>
   <si>
     <t>(blokujące) (5)6-10 PC,  dobry licytowany kolor   7+ (przed partią może być dobre 6); w młodszym chętnie 8+ (lub dobry)Otwarcia są naturalne. Po partii ozna­czają kolor siedmiokartowy, a przed partią 3 w kolor młodszy może być oparte na  kolorze sześciokartowym. Siła otwar­cia  zależy od stylu gracza i ustaleń w pa­rze. W przypadku braku takowych pro­ponuję stosować metodę 4-3-2-2. (**) Ozna­cza ona, że do zapowiedzianego kon­traktu brakuje nam „na ręku": czterech lew, jeśli jesteśmy w założeniach ko­rzystnych, trzech lew w założeniach przedpartyjnych, dwóch lew jeśli jeste­śmy po partii.</t>
+  </si>
+  <si>
+    <t>Dobry 7-kart</t>
   </si>
   <si>
     <t>GAMBLING</t>
@@ -2128,6 +2122,7 @@
         <sz val="7"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Otwarcia 3BA  raczej nie stosowane przez początkujących brydżystów.</t>
     </r>
@@ -2166,7 +2161,7 @@
     <t>krótkość w drugim młodszym</t>
   </si>
   <si>
-    <t> krótkość w kolorze młodszym licytuje poprzez 4BA. </t>
+    <t>krótkość w kolorze młodszym licytuje poprzez 4BA.</t>
   </si>
   <si>
     <t>5trefl, 5karo oznaczają brak krótkości</t>
@@ -2233,6 +2228,9 @@
   </si>
   <si>
     <t>8+</t>
+  </si>
+  <si>
+    <t>Dobry 8-kart</t>
   </si>
   <si>
     <r>
@@ -2244,6 +2242,7 @@
         <color rgb="FFFF0000"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">karo</t>
     </r>
@@ -2252,13 +2251,16 @@
         <sz val="7"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">  raczej nie stosowane przez początkujących brydżystów.</t>
     </r>
   </si>
   <si>
-    <t>kompletna ręka w kolorze licytowanym BEZ Asa i Króla &lt;font color=red&gt; [chyba to znaczy wszystkie zatrzymania i 7+ kartowy kolor (11 lew) -Otwarcia 5kier, 5pik raczej nie stosowane przez początkujących brydżystów.
-</t>
+    <t>Kompletna ręka bez A i K</t>
+  </si>
+  <si>
+    <t>kompletna ręka w kolorze licytowanym BEZ Asa i Króla &lt;font color=red&gt; [chyba to znaczy wszystkie zatrzymania i 7+ kartowy kolor (11 lew) -Otwarcia 5kier, 5pik raczej nie stosowane przez początkujących brydżystów.</t>
   </si>
   <si>
     <t>układowe</t>
@@ -2282,8 +2284,7 @@
     <t>7kier/pik– jest  As i Król w kolorze</t>
   </si>
   <si>
-    <t>kompletna ręka w kolorze licytowanym BEZ Asa i Króla &lt;font color=red&gt; [chyba to znaczy wszystkie zatrzymania i 7+ kartowy kolor (11 lew) Otwarcia 5kier, 5pik raczej nie stosowane przez początkujących brydżystów.
-</t>
+    <t>kompletna ręka w kolorze licytowanym BEZ Asa i Króla &lt;font color=red&gt; [chyba to znaczy wszystkie zatrzymania i 7+ kartowy kolor (11 lew) Otwarcia 5kier, 5pik raczej nie stosowane przez początkujących brydżystów.</t>
   </si>
   <si>
     <t>brak odzywki na otwarcie na pierwszym ręku na poziomie 1 (0-11PC) lub 2 (0-5 PC i długi kolor (6+) lub układ na dwóch piątkach) lub 3 itp. ...</t>
@@ -2417,6 +2418,9 @@
     <t>6+ PC, 5+ trefli, wyklucza 4 kara, 4 kiery, 4 piki;</t>
   </si>
   <si>
+    <t>inwit do 3 NT</t>
+  </si>
+  <si>
     <t>Naturalne bez Atu</t>
   </si>
 </sst>
@@ -2429,7 +2433,7 @@
     <numFmt numFmtId="165" formatCode="0"/>
     <numFmt numFmtId="166" formatCode="@"/>
   </numFmts>
-  <fonts count="17">
+  <fonts count="16">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -2522,14 +2526,10 @@
     </font>
     <font>
       <sz val="7"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-    </font>
-    <font>
-      <sz val="7"/>
       <color rgb="FFFF0000"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="8">
@@ -3047,9 +3047,9 @@
   <dimension ref="A1:M450"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="525" topLeftCell="A421" activePane="bottomLeft" state="split"/>
+      <pane xSplit="0" ySplit="525" topLeftCell="A246" activePane="bottomLeft" state="split"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="K409" activeCellId="0" sqref="K409"/>
+      <selection pane="bottomLeft" activeCell="G252" activeCellId="0" sqref="G252"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -3525,7 +3525,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="n">
         <v>11</v>
       </c>
@@ -3567,7 +3567,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="n">
         <v>12</v>
       </c>
@@ -3987,7 +3987,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="n">
         <v>22</v>
       </c>
@@ -4071,7 +4071,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="n">
         <v>24</v>
       </c>
@@ -4492,7 +4492,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="n">
         <v>34</v>
       </c>
@@ -4534,7 +4534,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="n">
         <v>35</v>
       </c>
@@ -4576,7 +4576,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="n">
         <v>36</v>
       </c>
@@ -4744,7 +4744,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="41" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="n">
         <v>40</v>
       </c>
@@ -4786,7 +4786,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="n">
         <v>41</v>
       </c>
@@ -4828,7 +4828,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="n">
         <v>42</v>
       </c>
@@ -4870,7 +4870,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="44" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="n">
         <v>43</v>
       </c>
@@ -5290,7 +5290,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="54" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="54" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="n">
         <v>53</v>
       </c>
@@ -5332,7 +5332,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="55" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="55" customFormat="false" ht="17.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="n">
         <v>54</v>
       </c>
@@ -5374,7 +5374,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="56" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="56" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="n">
         <v>55</v>
       </c>
@@ -5500,7 +5500,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="59" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="59" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="n">
         <v>58</v>
       </c>
@@ -5542,7 +5542,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="60" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="60" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="n">
         <v>59</v>
       </c>
@@ -5584,7 +5584,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="61" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="61" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="n">
         <v>60</v>
       </c>
@@ -5626,7 +5626,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="62" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="62" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="n">
         <v>61</v>
       </c>
@@ -5668,7 +5668,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="63" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="63" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="n">
         <v>62</v>
       </c>
@@ -5710,7 +5710,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="64" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="64" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="n">
         <v>63</v>
       </c>
@@ -5836,7 +5836,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="67" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="n">
         <v>66</v>
       </c>
@@ -5920,7 +5920,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="69" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="n">
         <v>68</v>
       </c>
@@ -5962,7 +5962,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="70" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="70" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="n">
         <v>69</v>
       </c>
@@ -6046,7 +6046,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="72" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="n">
         <v>71</v>
       </c>
@@ -6088,7 +6088,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="73" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="0" t="n">
         <v>72</v>
       </c>
@@ -6214,7 +6214,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="76" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="0" t="n">
         <v>75</v>
       </c>
@@ -6256,7 +6256,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="77" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="0" t="n">
         <v>76</v>
       </c>
@@ -6340,7 +6340,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="79" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="0" t="n">
         <v>78</v>
       </c>
@@ -6382,7 +6382,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="80" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="0" t="n">
         <v>79</v>
       </c>
@@ -6466,7 +6466,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="82" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="82" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="0" t="n">
         <v>81</v>
       </c>
@@ -6550,7 +6550,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="84" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="84" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="0" t="n">
         <v>83</v>
       </c>
@@ -6592,7 +6592,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="85" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="0" t="n">
         <v>84</v>
       </c>
@@ -6760,7 +6760,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="89" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="0" t="n">
         <v>88</v>
       </c>
@@ -6802,7 +6802,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="90" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="90" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="0" t="n">
         <v>89</v>
       </c>
@@ -6844,7 +6844,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="91" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="91" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="0" t="n">
         <v>90</v>
       </c>
@@ -6928,7 +6928,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="93" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="93" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="0" t="n">
         <v>92</v>
       </c>
@@ -6970,7 +6970,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="94" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="94" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="0" t="n">
         <v>93</v>
       </c>
@@ -7054,7 +7054,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="96" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="96" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="0" t="n">
         <v>95</v>
       </c>
@@ -7264,7 +7264,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="101" customFormat="false" ht="17.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="101" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="0" t="n">
         <v>100</v>
       </c>
@@ -7390,7 +7390,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="104" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="104" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="0" t="n">
         <v>103</v>
       </c>
@@ -7432,7 +7432,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="105" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="105" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="0" t="n">
         <v>104</v>
       </c>
@@ -7771,7 +7771,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="113" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="0" t="n">
         <v>112</v>
       </c>
@@ -7813,7 +7813,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="114" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="0" t="n">
         <v>113</v>
       </c>
@@ -7897,7 +7897,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="116" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="116" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="0" t="n">
         <v>115</v>
       </c>
@@ -7939,7 +7939,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="117" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="117" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="0" t="n">
         <v>116</v>
       </c>
@@ -7981,7 +7981,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="118" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="0" t="n">
         <v>117</v>
       </c>
@@ -8023,7 +8023,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="119" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="119" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="0" t="n">
         <v>118</v>
       </c>
@@ -8107,7 +8107,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="121" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="121" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="0" t="n">
         <v>120</v>
       </c>
@@ -8149,7 +8149,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="122" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="122" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="0" t="n">
         <v>121</v>
       </c>
@@ -8191,7 +8191,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="123" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="123" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="0" t="n">
         <v>122</v>
       </c>
@@ -8233,7 +8233,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="124" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="124" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="0" t="n">
         <v>123</v>
       </c>
@@ -8275,7 +8275,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="125" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="125" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="0" t="n">
         <v>124</v>
       </c>
@@ -8317,7 +8317,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="126" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="126" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="0" t="n">
         <v>125</v>
       </c>
@@ -8359,7 +8359,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="127" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="127" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="0" t="n">
         <v>126</v>
       </c>
@@ -8401,7 +8401,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="128" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="128" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="0" t="n">
         <v>127</v>
       </c>
@@ -8443,7 +8443,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="129" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="129" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="0" t="n">
         <v>128</v>
       </c>
@@ -8653,7 +8653,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="134" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="134" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="0" t="n">
         <v>133</v>
       </c>
@@ -8779,7 +8779,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="137" customFormat="false" ht="70.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="137" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A137" s="0" t="n">
         <v>136</v>
       </c>
@@ -9409,7 +9409,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="152" customFormat="false" ht="17.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="152" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A152" s="0" t="n">
         <v>151</v>
       </c>
@@ -11383,7 +11383,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="199" customFormat="false" ht="17.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="199" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A199" s="0" t="n">
         <v>198</v>
       </c>
@@ -11890,7 +11890,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="211" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="211" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A211" s="0" t="n">
         <v>210</v>
       </c>
@@ -11932,7 +11932,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="212" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="212" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A212" s="0" t="n">
         <v>211</v>
       </c>
@@ -12016,7 +12016,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="214" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="214" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A214" s="0" t="n">
         <v>213</v>
       </c>
@@ -12058,7 +12058,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="215" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="215" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A215" s="0" t="n">
         <v>214</v>
       </c>
@@ -12100,7 +12100,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="216" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="216" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A216" s="0" t="n">
         <v>215</v>
       </c>
@@ -12142,7 +12142,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="217" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="217" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A217" s="0" t="n">
         <v>216</v>
       </c>
@@ -12184,7 +12184,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="218" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="218" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A218" s="0" t="n">
         <v>217</v>
       </c>
@@ -12226,7 +12226,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="219" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="219" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A219" s="0" t="n">
         <v>218</v>
       </c>
@@ -12268,7 +12268,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="220" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="220" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A220" s="0" t="n">
         <v>219</v>
       </c>
@@ -12310,7 +12310,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="221" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="221" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A221" s="0" t="n">
         <v>220</v>
       </c>
@@ -12352,7 +12352,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="222" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="222" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A222" s="0" t="n">
         <v>221</v>
       </c>
@@ -12394,7 +12394,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="223" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="223" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A223" s="0" t="n">
         <v>222</v>
       </c>
@@ -12436,7 +12436,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="224" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="224" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A224" s="0" t="n">
         <v>223</v>
       </c>
@@ -12478,7 +12478,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="225" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="225" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A225" s="0" t="n">
         <v>224</v>
       </c>
@@ -12520,7 +12520,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="226" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="226" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A226" s="0" t="n">
         <v>225</v>
       </c>
@@ -12562,7 +12562,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="227" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="227" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A227" s="0" t="n">
         <v>226</v>
       </c>
@@ -12772,7 +12772,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="232" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="232" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A232" s="0" t="n">
         <v>231</v>
       </c>
@@ -12898,7 +12898,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="235" customFormat="false" ht="70.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="235" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A235" s="0" t="n">
         <v>234</v>
       </c>
@@ -13150,7 +13150,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="241" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="241" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A241" s="0" t="n">
         <v>240</v>
       </c>
@@ -13640,11 +13640,11 @@
       <c r="I252" s="18" t="n">
         <v>0</v>
       </c>
-      <c r="J252" s="19" t="s">
-        <v>128</v>
+      <c r="J252" s="17" t="s">
+        <v>271</v>
       </c>
       <c r="K252" s="67" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="L252" s="17" t="s">
         <v>31</v>
@@ -13685,7 +13685,7 @@
         <v>262</v>
       </c>
       <c r="K253" s="68" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="L253" s="10" t="s">
         <v>44</v>
@@ -13727,7 +13727,7 @@
         <v>112</v>
       </c>
       <c r="K254" s="69" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="L254" s="17" t="s">
         <v>17</v>
@@ -13736,7 +13736,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="255" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="255" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A255" s="0" t="n">
         <v>254</v>
       </c>
@@ -13769,7 +13769,7 @@
         <v>114</v>
       </c>
       <c r="K255" s="69" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="L255" s="17" t="s">
         <v>17</v>
@@ -13778,7 +13778,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="256" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="256" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A256" s="0" t="n">
         <v>255</v>
       </c>
@@ -13808,10 +13808,10 @@
         <v>0</v>
       </c>
       <c r="J256" s="19" t="s">
+        <v>275</v>
+      </c>
+      <c r="K256" s="69" t="s">
         <v>274</v>
-      </c>
-      <c r="K256" s="69" t="s">
-        <v>273</v>
       </c>
       <c r="L256" s="17" t="s">
         <v>17</v>
@@ -13853,7 +13853,7 @@
         <v>85</v>
       </c>
       <c r="K257" s="70" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="L257" s="17" t="s">
         <v>107</v>
@@ -13886,16 +13886,16 @@
         <v>14</v>
       </c>
       <c r="H258" s="17" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="I258" s="18" t="n">
         <v>0</v>
       </c>
       <c r="J258" s="19" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="K258" s="67" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="L258" s="17" t="s">
         <v>17</v>
@@ -13928,13 +13928,13 @@
         <v>37</v>
       </c>
       <c r="H259" s="17" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="I259" s="18" t="n">
         <v>0</v>
       </c>
       <c r="J259" s="19" t="s">
-        <v>280</v>
+        <v>87</v>
       </c>
       <c r="K259" s="67" t="s">
         <v>281</v>
@@ -13970,13 +13970,13 @@
         <v>37</v>
       </c>
       <c r="H260" s="17" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="I260" s="18" t="n">
         <v>0</v>
       </c>
       <c r="J260" s="19" t="s">
-        <v>280</v>
+        <v>87</v>
       </c>
       <c r="K260" s="67" t="s">
         <v>282</v>
@@ -14012,13 +14012,13 @@
         <v>37</v>
       </c>
       <c r="H261" s="17" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="I261" s="18" t="n">
         <v>0</v>
       </c>
       <c r="J261" s="19" t="s">
-        <v>280</v>
+        <v>87</v>
       </c>
       <c r="K261" s="67" t="s">
         <v>283</v>
@@ -14054,13 +14054,13 @@
         <v>37</v>
       </c>
       <c r="H262" s="17" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="I262" s="18" t="n">
         <v>0</v>
       </c>
       <c r="J262" s="19" t="s">
-        <v>280</v>
+        <v>87</v>
       </c>
       <c r="K262" s="67" t="s">
         <v>284</v>
@@ -14104,7 +14104,7 @@
         <v>112</v>
       </c>
       <c r="K263" s="68" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="L263" s="10" t="s">
         <v>44</v>
@@ -14113,7 +14113,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="264" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="264" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A264" s="0" t="n">
         <v>263</v>
       </c>
@@ -14146,7 +14146,7 @@
         <v>114</v>
       </c>
       <c r="K264" s="69" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="L264" s="17" t="s">
         <v>17</v>
@@ -14155,7 +14155,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="265" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="265" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A265" s="0" t="n">
         <v>264</v>
       </c>
@@ -14185,10 +14185,10 @@
         <v>0</v>
       </c>
       <c r="J265" s="19" t="s">
+        <v>275</v>
+      </c>
+      <c r="K265" s="69" t="s">
         <v>274</v>
-      </c>
-      <c r="K265" s="69" t="s">
-        <v>273</v>
       </c>
       <c r="L265" s="17" t="s">
         <v>17</v>
@@ -14230,7 +14230,7 @@
         <v>85</v>
       </c>
       <c r="K266" s="70" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="L266" s="17" t="s">
         <v>107</v>
@@ -14263,16 +14263,16 @@
         <v>14</v>
       </c>
       <c r="H267" s="17" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="I267" s="18" t="n">
         <v>0</v>
       </c>
       <c r="J267" s="19" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="K267" s="67" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="L267" s="17" t="s">
         <v>17</v>
@@ -14305,13 +14305,13 @@
         <v>37</v>
       </c>
       <c r="H268" s="17" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="I268" s="18" t="n">
         <v>0</v>
       </c>
       <c r="J268" s="19" t="s">
-        <v>280</v>
+        <v>87</v>
       </c>
       <c r="K268" s="67" t="s">
         <v>281</v>
@@ -14347,13 +14347,13 @@
         <v>37</v>
       </c>
       <c r="H269" s="17" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="I269" s="18" t="n">
         <v>0</v>
       </c>
       <c r="J269" s="19" t="s">
-        <v>280</v>
+        <v>87</v>
       </c>
       <c r="K269" s="67" t="s">
         <v>281</v>
@@ -14389,13 +14389,13 @@
         <v>37</v>
       </c>
       <c r="H270" s="17" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="I270" s="18" t="n">
         <v>0</v>
       </c>
       <c r="J270" s="19" t="s">
-        <v>280</v>
+        <v>87</v>
       </c>
       <c r="K270" s="67" t="s">
         <v>281</v>
@@ -14477,7 +14477,7 @@
         <v>0</v>
       </c>
       <c r="J272" s="12" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="K272" s="72" t="s">
         <v>287</v>
@@ -15016,10 +15016,10 @@
         <v>0</v>
       </c>
       <c r="J285" s="12" t="s">
+        <v>167</v>
+      </c>
+      <c r="K285" s="13" t="s">
         <v>305</v>
-      </c>
-      <c r="K285" s="13" t="s">
-        <v>306</v>
       </c>
       <c r="L285" s="10" t="s">
         <v>31</v>
@@ -15061,7 +15061,7 @@
         <v>235</v>
       </c>
       <c r="K286" s="13" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="L286" s="10" t="s">
         <v>17</v>
@@ -15094,16 +15094,16 @@
         <v>17</v>
       </c>
       <c r="H287" s="17" t="s">
+        <v>307</v>
+      </c>
+      <c r="I287" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="J287" s="19" t="s">
         <v>308</v>
       </c>
-      <c r="I287" s="18" t="n">
-        <v>0</v>
-      </c>
-      <c r="J287" s="19" t="s">
+      <c r="K287" s="30" t="s">
         <v>309</v>
-      </c>
-      <c r="K287" s="30" t="s">
-        <v>310</v>
       </c>
       <c r="L287" s="17" t="s">
         <v>17</v>
@@ -15136,7 +15136,7 @@
         <v>14</v>
       </c>
       <c r="H288" s="17" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="I288" s="18" t="n">
         <v>0</v>
@@ -15145,7 +15145,7 @@
         <v>133</v>
       </c>
       <c r="K288" s="30" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="L288" s="17" t="s">
         <v>107</v>
@@ -15184,7 +15184,7 @@
         <v>0</v>
       </c>
       <c r="J289" s="26" t="s">
-        <v>305</v>
+        <v>312</v>
       </c>
       <c r="K289" s="27" t="s">
         <v>313</v>
@@ -15304,16 +15304,16 @@
         <v>9</v>
       </c>
       <c r="H292" s="24" t="s">
+        <v>314</v>
+      </c>
+      <c r="I292" s="25" t="n">
+        <v>0</v>
+      </c>
+      <c r="J292" s="26" t="s">
         <v>320</v>
       </c>
-      <c r="I292" s="25" t="n">
-        <v>0</v>
-      </c>
-      <c r="J292" s="26" t="s">
+      <c r="K292" s="27" t="s">
         <v>321</v>
-      </c>
-      <c r="K292" s="27" t="s">
-        <v>322</v>
       </c>
       <c r="L292" s="24" t="s">
         <v>31</v>
@@ -15346,16 +15346,16 @@
         <v>9</v>
       </c>
       <c r="H293" s="24" t="s">
+        <v>322</v>
+      </c>
+      <c r="I293" s="25" t="n">
+        <v>0</v>
+      </c>
+      <c r="J293" s="26" t="s">
         <v>323</v>
       </c>
-      <c r="I293" s="25" t="n">
-        <v>0</v>
-      </c>
-      <c r="J293" s="26" t="s">
+      <c r="K293" s="27" t="s">
         <v>324</v>
-      </c>
-      <c r="K293" s="27" t="s">
-        <v>325</v>
       </c>
       <c r="L293" s="24" t="s">
         <v>31</v>
@@ -15397,7 +15397,7 @@
         <v>119</v>
       </c>
       <c r="K294" s="27" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="L294" s="24" t="s">
         <v>35</v>
@@ -15430,16 +15430,16 @@
         <v>37</v>
       </c>
       <c r="H295" s="24" t="s">
+        <v>326</v>
+      </c>
+      <c r="I295" s="25" t="n">
+        <v>0</v>
+      </c>
+      <c r="J295" s="26" t="s">
         <v>327</v>
       </c>
-      <c r="I295" s="25" t="n">
-        <v>0</v>
-      </c>
-      <c r="J295" s="26" t="s">
+      <c r="K295" s="27" t="s">
         <v>328</v>
-      </c>
-      <c r="K295" s="27" t="s">
-        <v>329</v>
       </c>
       <c r="L295" s="24" t="s">
         <v>44</v>
@@ -15481,7 +15481,7 @@
         <v>119</v>
       </c>
       <c r="K296" s="27" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="L296" s="24" t="s">
         <v>35</v>
@@ -15514,7 +15514,7 @@
         <v>12</v>
       </c>
       <c r="H297" s="24" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="I297" s="25" t="n">
         <v>0</v>
@@ -15523,7 +15523,7 @@
         <v>125</v>
       </c>
       <c r="K297" s="27" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="L297" s="24" t="s">
         <v>35</v>
@@ -15556,16 +15556,16 @@
         <v>37</v>
       </c>
       <c r="H298" s="24" t="s">
+        <v>332</v>
+      </c>
+      <c r="I298" s="25" t="n">
+        <v>0</v>
+      </c>
+      <c r="J298" s="26" t="s">
         <v>333</v>
       </c>
-      <c r="I298" s="25" t="n">
-        <v>0</v>
-      </c>
-      <c r="J298" s="26" t="s">
+      <c r="K298" s="27" t="s">
         <v>334</v>
-      </c>
-      <c r="K298" s="27" t="s">
-        <v>335</v>
       </c>
       <c r="L298" s="24" t="s">
         <v>44</v>
@@ -15607,7 +15607,7 @@
         <v>167</v>
       </c>
       <c r="K299" s="27" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="L299" s="24" t="s">
         <v>31</v>
@@ -15640,16 +15640,16 @@
         <v>16</v>
       </c>
       <c r="H300" s="24" t="s">
-        <v>337</v>
+        <v>330</v>
       </c>
       <c r="I300" s="25" t="n">
         <v>0</v>
       </c>
       <c r="J300" s="26" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="K300" s="27" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="L300" s="24" t="s">
         <v>31</v>
@@ -15682,16 +15682,16 @@
         <v>14</v>
       </c>
       <c r="H301" s="17" t="s">
+        <v>337</v>
+      </c>
+      <c r="I301" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="J301" s="19" t="s">
+        <v>338</v>
+      </c>
+      <c r="K301" s="30" t="s">
         <v>339</v>
-      </c>
-      <c r="I301" s="18" t="n">
-        <v>0</v>
-      </c>
-      <c r="J301" s="19" t="s">
-        <v>340</v>
-      </c>
-      <c r="K301" s="30" t="s">
-        <v>341</v>
       </c>
       <c r="L301" s="17" t="s">
         <v>107</v>
@@ -15724,7 +15724,7 @@
         <v>9</v>
       </c>
       <c r="H302" s="24" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="I302" s="25" t="n">
         <v>0</v>
@@ -15733,7 +15733,7 @@
         <v>318</v>
       </c>
       <c r="K302" s="27" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="L302" s="24" t="s">
         <v>31</v>
@@ -15766,16 +15766,16 @@
         <v>9</v>
       </c>
       <c r="H303" s="24" t="s">
-        <v>337</v>
+        <v>330</v>
       </c>
       <c r="I303" s="25" t="n">
         <v>0</v>
       </c>
       <c r="J303" s="26" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="K303" s="27" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="L303" s="24" t="s">
         <v>31</v>
@@ -15808,7 +15808,7 @@
         <v>9</v>
       </c>
       <c r="H304" s="24" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="I304" s="25" t="n">
         <v>0</v>
@@ -15817,7 +15817,7 @@
         <v>46</v>
       </c>
       <c r="K304" s="76" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="L304" s="24" t="s">
         <v>17</v>
@@ -15850,7 +15850,7 @@
         <v>12</v>
       </c>
       <c r="H305" s="24" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="I305" s="25" t="n">
         <v>0</v>
@@ -15859,7 +15859,7 @@
         <v>119</v>
       </c>
       <c r="K305" s="27" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="L305" s="24" t="s">
         <v>35</v>
@@ -15892,16 +15892,16 @@
         <v>11</v>
       </c>
       <c r="H306" s="24" t="s">
+        <v>348</v>
+      </c>
+      <c r="I306" s="25" t="n">
+        <v>0</v>
+      </c>
+      <c r="J306" s="26" t="s">
+        <v>349</v>
+      </c>
+      <c r="K306" s="27" t="s">
         <v>350</v>
-      </c>
-      <c r="I306" s="25" t="n">
-        <v>0</v>
-      </c>
-      <c r="J306" s="26" t="s">
-        <v>351</v>
-      </c>
-      <c r="K306" s="27" t="s">
-        <v>352</v>
       </c>
       <c r="L306" s="24" t="s">
         <v>35</v>
@@ -15934,7 +15934,7 @@
         <v>11</v>
       </c>
       <c r="H307" s="24" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="I307" s="25" t="n">
         <v>0</v>
@@ -15943,7 +15943,7 @@
         <v>318</v>
       </c>
       <c r="K307" s="27" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="L307" s="24" t="s">
         <v>35</v>
@@ -15976,7 +15976,7 @@
         <v>12</v>
       </c>
       <c r="H308" s="24" t="s">
-        <v>337</v>
+        <v>330</v>
       </c>
       <c r="I308" s="25" t="n">
         <v>0</v>
@@ -15985,7 +15985,7 @@
         <v>125</v>
       </c>
       <c r="K308" s="27" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="L308" s="24" t="s">
         <v>35</v>
@@ -16018,7 +16018,7 @@
         <v>37</v>
       </c>
       <c r="H309" s="24" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="I309" s="25" t="n">
         <v>0</v>
@@ -16027,7 +16027,7 @@
         <v>46</v>
       </c>
       <c r="K309" s="27" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="L309" s="24" t="s">
         <v>44</v>
@@ -16060,16 +16060,16 @@
         <v>16</v>
       </c>
       <c r="H310" s="24" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="I310" s="25" t="n">
         <v>0</v>
       </c>
       <c r="J310" s="26" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="K310" s="27" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="L310" s="24" t="s">
         <v>107</v>
@@ -16102,7 +16102,7 @@
         <v>16</v>
       </c>
       <c r="H311" s="24" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="I311" s="25" t="n">
         <v>0</v>
@@ -16111,7 +16111,7 @@
         <v>167</v>
       </c>
       <c r="K311" s="27" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="L311" s="24" t="s">
         <v>107</v>
@@ -16144,16 +16144,16 @@
         <v>16</v>
       </c>
       <c r="H312" s="24" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="I312" s="25" t="n">
         <v>0</v>
       </c>
       <c r="J312" s="26" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="K312" s="27" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="L312" s="24" t="s">
         <v>107</v>
@@ -16186,16 +16186,16 @@
         <v>14</v>
       </c>
       <c r="H313" s="17" t="s">
+        <v>360</v>
+      </c>
+      <c r="I313" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="J313" s="19" t="s">
+        <v>361</v>
+      </c>
+      <c r="K313" s="30" t="s">
         <v>362</v>
-      </c>
-      <c r="I313" s="18" t="n">
-        <v>0</v>
-      </c>
-      <c r="J313" s="19" t="s">
-        <v>363</v>
-      </c>
-      <c r="K313" s="30" t="s">
-        <v>364</v>
       </c>
       <c r="L313" s="17" t="s">
         <v>107</v>
@@ -16228,16 +16228,16 @@
         <v>37</v>
       </c>
       <c r="H314" s="24" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="I314" s="25" t="n">
         <v>0</v>
       </c>
       <c r="J314" s="26" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="K314" s="27" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="L314" s="24" t="s">
         <v>44</v>
@@ -16270,7 +16270,7 @@
         <v>14</v>
       </c>
       <c r="H315" s="17" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="I315" s="18" t="n">
         <v>0</v>
@@ -16279,7 +16279,7 @@
         <v>318</v>
       </c>
       <c r="K315" s="30" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="L315" s="17" t="s">
         <v>107</v>
@@ -16312,7 +16312,7 @@
         <v>17</v>
       </c>
       <c r="H316" s="17" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="I316" s="18" t="n">
         <v>0</v>
@@ -16321,7 +16321,7 @@
         <v>46</v>
       </c>
       <c r="K316" s="30" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="L316" s="17" t="s">
         <v>35</v>
@@ -16363,7 +16363,7 @@
         <v>119</v>
       </c>
       <c r="K317" s="27" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="L317" s="24" t="s">
         <v>35</v>
@@ -16396,7 +16396,7 @@
         <v>37</v>
       </c>
       <c r="H318" s="24" t="s">
-        <v>320</v>
+        <v>314</v>
       </c>
       <c r="I318" s="25" t="n">
         <v>0</v>
@@ -16405,7 +16405,7 @@
         <v>114</v>
       </c>
       <c r="K318" s="27" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="L318" s="24" t="s">
         <v>17</v>
@@ -16438,16 +16438,16 @@
         <v>37</v>
       </c>
       <c r="H319" s="24" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="I319" s="25" t="n">
         <v>0</v>
       </c>
       <c r="J319" s="26" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="K319" s="27" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="L319" s="24" t="s">
         <v>44</v>
@@ -16480,16 +16480,16 @@
         <v>17</v>
       </c>
       <c r="H320" s="17" t="s">
+        <v>370</v>
+      </c>
+      <c r="I320" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="J320" s="19" t="s">
+        <v>371</v>
+      </c>
+      <c r="K320" s="30" t="s">
         <v>372</v>
-      </c>
-      <c r="I320" s="18" t="n">
-        <v>0</v>
-      </c>
-      <c r="J320" s="19" t="s">
-        <v>373</v>
-      </c>
-      <c r="K320" s="30" t="s">
-        <v>374</v>
       </c>
       <c r="L320" s="17" t="s">
         <v>35</v>
@@ -16522,16 +16522,16 @@
         <v>17</v>
       </c>
       <c r="H321" s="17" t="s">
+        <v>373</v>
+      </c>
+      <c r="I321" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="J321" s="19" t="s">
+        <v>374</v>
+      </c>
+      <c r="K321" s="30" t="s">
         <v>375</v>
-      </c>
-      <c r="I321" s="18" t="n">
-        <v>0</v>
-      </c>
-      <c r="J321" s="19" t="s">
-        <v>376</v>
-      </c>
-      <c r="K321" s="30" t="s">
-        <v>377</v>
       </c>
       <c r="L321" s="17" t="s">
         <v>35</v>
@@ -16564,16 +16564,16 @@
         <v>17</v>
       </c>
       <c r="H322" s="17" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="I322" s="18" t="n">
         <v>0</v>
       </c>
       <c r="J322" s="19" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="K322" s="30" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="L322" s="17" t="s">
         <v>35</v>
@@ -16606,7 +16606,7 @@
         <v>17</v>
       </c>
       <c r="H323" s="17" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="I323" s="18" t="n">
         <v>0</v>
@@ -16615,7 +16615,7 @@
         <v>318</v>
       </c>
       <c r="K323" s="77" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="L323" s="17" t="s">
         <v>35</v>
@@ -16648,16 +16648,16 @@
         <v>17</v>
       </c>
       <c r="H324" s="17" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="I324" s="18" t="n">
         <v>0</v>
       </c>
       <c r="J324" s="19" t="s">
-        <v>280</v>
+        <v>87</v>
       </c>
       <c r="K324" s="77" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="L324" s="17" t="s">
         <v>44</v>
@@ -16690,7 +16690,7 @@
         <v>17</v>
       </c>
       <c r="H325" s="17" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="I325" s="18" t="n">
         <v>0</v>
@@ -16699,7 +16699,7 @@
         <v>128</v>
       </c>
       <c r="K325" s="30" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="L325" s="17" t="s">
         <v>31</v>
@@ -16732,16 +16732,16 @@
         <v>17</v>
       </c>
       <c r="H326" s="17" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="I326" s="18" t="n">
         <v>0</v>
       </c>
       <c r="J326" s="19" t="s">
-        <v>280</v>
+        <v>87</v>
       </c>
       <c r="K326" s="30" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="L326" s="17" t="s">
         <v>31</v>
@@ -16781,7 +16781,7 @@
         <v>167</v>
       </c>
       <c r="K327" s="30" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="L327" s="17" t="s">
         <v>31</v>
@@ -16821,7 +16821,7 @@
         <v>167</v>
       </c>
       <c r="K328" s="30" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="L328" s="17" t="s">
         <v>31</v>
@@ -16860,10 +16860,10 @@
         <v>0</v>
       </c>
       <c r="J329" s="12" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="K329" s="13" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="L329" s="10" t="s">
         <v>17</v>
@@ -16896,7 +16896,7 @@
         <v>14</v>
       </c>
       <c r="H330" s="17" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="I330" s="18" t="n">
         <v>0</v>
@@ -16905,7 +16905,7 @@
         <v>133</v>
       </c>
       <c r="K330" s="30" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="L330" s="17" t="s">
         <v>107</v>
@@ -16944,7 +16944,7 @@
         <v>0</v>
       </c>
       <c r="J331" s="26" t="s">
-        <v>305</v>
+        <v>167</v>
       </c>
       <c r="K331" s="27" t="s">
         <v>313</v>
@@ -16980,7 +16980,7 @@
         <v>37</v>
       </c>
       <c r="H332" s="24" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="I332" s="25" t="n">
         <v>0</v>
@@ -17022,13 +17022,13 @@
         <v>9</v>
       </c>
       <c r="H333" s="24" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="I333" s="25" t="n">
         <v>0</v>
       </c>
       <c r="J333" s="26" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="K333" s="27" t="s">
         <v>319</v>
@@ -17064,16 +17064,16 @@
         <v>9</v>
       </c>
       <c r="H334" s="24" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="I334" s="25" t="n">
         <v>0</v>
       </c>
       <c r="J334" s="26" t="s">
+        <v>323</v>
+      </c>
+      <c r="K334" s="27" t="s">
         <v>324</v>
-      </c>
-      <c r="K334" s="27" t="s">
-        <v>325</v>
       </c>
       <c r="L334" s="24" t="s">
         <v>31</v>
@@ -17106,16 +17106,16 @@
         <v>9</v>
       </c>
       <c r="H335" s="24" t="s">
-        <v>393</v>
+        <v>387</v>
       </c>
       <c r="I335" s="25" t="n">
         <v>0</v>
       </c>
       <c r="J335" s="26" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="K335" s="27" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="L335" s="24" t="s">
         <v>31</v>
@@ -17157,7 +17157,7 @@
         <v>119</v>
       </c>
       <c r="K336" s="27" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
       <c r="L336" s="24" t="s">
         <v>35</v>
@@ -17190,16 +17190,16 @@
         <v>37</v>
       </c>
       <c r="H337" s="24" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
       <c r="I337" s="25" t="n">
         <v>0</v>
       </c>
       <c r="J337" s="26" t="s">
-        <v>397</v>
+        <v>394</v>
       </c>
       <c r="K337" s="27" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="L337" s="24" t="s">
         <v>44</v>
@@ -17232,7 +17232,7 @@
         <v>11</v>
       </c>
       <c r="H338" s="24" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="I338" s="25" t="n">
         <v>0</v>
@@ -17241,7 +17241,7 @@
         <v>119</v>
       </c>
       <c r="K338" s="27" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="L338" s="24" t="s">
         <v>35</v>
@@ -17274,7 +17274,7 @@
         <v>12</v>
       </c>
       <c r="H339" s="24" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="I339" s="25" t="n">
         <v>0</v>
@@ -17283,7 +17283,7 @@
         <v>127</v>
       </c>
       <c r="K339" s="27" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="L339" s="24" t="s">
         <v>35</v>
@@ -17316,16 +17316,16 @@
         <v>37</v>
       </c>
       <c r="H340" s="24" t="s">
+        <v>332</v>
+      </c>
+      <c r="I340" s="25" t="n">
+        <v>0</v>
+      </c>
+      <c r="J340" s="26" t="s">
         <v>333</v>
       </c>
-      <c r="I340" s="25" t="n">
-        <v>0</v>
-      </c>
-      <c r="J340" s="26" t="s">
-        <v>334</v>
-      </c>
       <c r="K340" s="27" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="L340" s="24" t="s">
         <v>44</v>
@@ -17367,7 +17367,7 @@
         <v>167</v>
       </c>
       <c r="K341" s="27" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="L341" s="24" t="s">
         <v>31</v>
@@ -17400,16 +17400,16 @@
         <v>16</v>
       </c>
       <c r="H342" s="24" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="I342" s="25" t="n">
         <v>0</v>
       </c>
       <c r="J342" s="26" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="K342" s="27" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="L342" s="24" t="s">
         <v>31</v>
@@ -17442,16 +17442,16 @@
         <v>14</v>
       </c>
       <c r="H343" s="17" t="s">
+        <v>337</v>
+      </c>
+      <c r="I343" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="J343" s="19" t="s">
+        <v>338</v>
+      </c>
+      <c r="K343" s="30" t="s">
         <v>339</v>
-      </c>
-      <c r="I343" s="18" t="n">
-        <v>0</v>
-      </c>
-      <c r="J343" s="19" t="s">
-        <v>340</v>
-      </c>
-      <c r="K343" s="30" t="s">
-        <v>341</v>
       </c>
       <c r="L343" s="17" t="s">
         <v>107</v>
@@ -17484,16 +17484,16 @@
         <v>9</v>
       </c>
       <c r="H344" s="24" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
       <c r="I344" s="25" t="n">
         <v>0</v>
       </c>
       <c r="J344" s="26" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
       <c r="K344" s="27" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="L344" s="24" t="s">
         <v>31</v>
@@ -17526,16 +17526,16 @@
         <v>9</v>
       </c>
       <c r="H345" s="24" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="I345" s="25" t="n">
         <v>0</v>
       </c>
       <c r="J345" s="26" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
       <c r="K345" s="27" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="L345" s="24" t="s">
         <v>31</v>
@@ -17568,7 +17568,7 @@
         <v>9</v>
       </c>
       <c r="H346" s="24" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="I346" s="25" t="n">
         <v>0</v>
@@ -17577,7 +17577,7 @@
         <v>46</v>
       </c>
       <c r="K346" s="76" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="L346" s="24" t="s">
         <v>17</v>
@@ -17610,7 +17610,7 @@
         <v>12</v>
       </c>
       <c r="H347" s="24" t="s">
-        <v>401</v>
+        <v>398</v>
       </c>
       <c r="I347" s="25" t="n">
         <v>0</v>
@@ -17619,7 +17619,7 @@
         <v>119</v>
       </c>
       <c r="K347" s="27" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="L347" s="24" t="s">
         <v>35</v>
@@ -17652,16 +17652,16 @@
         <v>11</v>
       </c>
       <c r="H348" s="24" t="s">
-        <v>402</v>
+        <v>399</v>
       </c>
       <c r="I348" s="25" t="n">
         <v>0</v>
       </c>
       <c r="J348" s="26" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="K348" s="27" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="L348" s="24" t="s">
         <v>35</v>
@@ -17694,16 +17694,16 @@
         <v>11</v>
       </c>
       <c r="H349" s="24" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
       <c r="I349" s="25" t="n">
         <v>0</v>
       </c>
       <c r="J349" s="26" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
       <c r="K349" s="27" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="L349" s="24" t="s">
         <v>35</v>
@@ -17736,7 +17736,7 @@
         <v>12</v>
       </c>
       <c r="H350" s="24" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="I350" s="25" t="n">
         <v>0</v>
@@ -17745,7 +17745,7 @@
         <v>127</v>
       </c>
       <c r="K350" s="27" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="L350" s="24" t="s">
         <v>35</v>
@@ -17778,7 +17778,7 @@
         <v>37</v>
       </c>
       <c r="H351" s="24" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="I351" s="25" t="n">
         <v>0</v>
@@ -17787,7 +17787,7 @@
         <v>46</v>
       </c>
       <c r="K351" s="27" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="L351" s="24" t="s">
         <v>44</v>
@@ -17820,16 +17820,16 @@
         <v>16</v>
       </c>
       <c r="H352" s="24" t="s">
-        <v>405</v>
+        <v>402</v>
       </c>
       <c r="I352" s="25" t="n">
         <v>0</v>
       </c>
       <c r="J352" s="26" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="K352" s="27" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="L352" s="24" t="s">
         <v>107</v>
@@ -17862,7 +17862,7 @@
         <v>16</v>
       </c>
       <c r="H353" s="24" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="I353" s="25" t="n">
         <v>0</v>
@@ -17871,7 +17871,7 @@
         <v>167</v>
       </c>
       <c r="K353" s="27" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="L353" s="24" t="s">
         <v>107</v>
@@ -17904,16 +17904,16 @@
         <v>16</v>
       </c>
       <c r="H354" s="24" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="I354" s="25" t="n">
         <v>0</v>
       </c>
       <c r="J354" s="26" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="K354" s="27" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="L354" s="24" t="s">
         <v>107</v>
@@ -17946,16 +17946,16 @@
         <v>14</v>
       </c>
       <c r="H355" s="17" t="s">
+        <v>360</v>
+      </c>
+      <c r="I355" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="J355" s="19" t="s">
+        <v>361</v>
+      </c>
+      <c r="K355" s="30" t="s">
         <v>362</v>
-      </c>
-      <c r="I355" s="18" t="n">
-        <v>0</v>
-      </c>
-      <c r="J355" s="19" t="s">
-        <v>363</v>
-      </c>
-      <c r="K355" s="30" t="s">
-        <v>364</v>
       </c>
       <c r="L355" s="17" t="s">
         <v>107</v>
@@ -17988,16 +17988,16 @@
         <v>37</v>
       </c>
       <c r="H356" s="24" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="I356" s="25" t="n">
         <v>0</v>
       </c>
       <c r="J356" s="26" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="K356" s="27" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="L356" s="24" t="s">
         <v>44</v>
@@ -18030,16 +18030,16 @@
         <v>14</v>
       </c>
       <c r="H357" s="17" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
       <c r="I357" s="18" t="n">
         <v>0</v>
       </c>
       <c r="J357" s="19" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
       <c r="K357" s="30" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="L357" s="17" t="s">
         <v>107</v>
@@ -18072,7 +18072,7 @@
         <v>17</v>
       </c>
       <c r="H358" s="17" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="I358" s="18" t="n">
         <v>0</v>
@@ -18081,7 +18081,7 @@
         <v>46</v>
       </c>
       <c r="K358" s="30" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="L358" s="17" t="s">
         <v>35</v>
@@ -18114,7 +18114,7 @@
         <v>11</v>
       </c>
       <c r="H359" s="24" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="I359" s="25" t="n">
         <v>0</v>
@@ -18123,7 +18123,7 @@
         <v>119</v>
       </c>
       <c r="K359" s="27" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="L359" s="24" t="s">
         <v>35</v>
@@ -18156,16 +18156,16 @@
         <v>37</v>
       </c>
       <c r="H360" s="24" t="s">
-        <v>393</v>
+        <v>387</v>
       </c>
       <c r="I360" s="25" t="n">
         <v>0</v>
       </c>
       <c r="J360" s="26" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="K360" s="27" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="L360" s="24" t="s">
         <v>17</v>
@@ -18198,16 +18198,16 @@
         <v>37</v>
       </c>
       <c r="H361" s="24" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
       <c r="I361" s="25" t="n">
         <v>0</v>
       </c>
       <c r="J361" s="26" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="K361" s="27" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="L361" s="24" t="s">
         <v>44</v>
@@ -18240,16 +18240,16 @@
         <v>17</v>
       </c>
       <c r="H362" s="17" t="s">
+        <v>370</v>
+      </c>
+      <c r="I362" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="J362" s="19" t="s">
+        <v>371</v>
+      </c>
+      <c r="K362" s="30" t="s">
         <v>372</v>
-      </c>
-      <c r="I362" s="18" t="n">
-        <v>0</v>
-      </c>
-      <c r="J362" s="19" t="s">
-        <v>373</v>
-      </c>
-      <c r="K362" s="30" t="s">
-        <v>374</v>
       </c>
       <c r="L362" s="17" t="s">
         <v>35</v>
@@ -18282,16 +18282,16 @@
         <v>17</v>
       </c>
       <c r="H363" s="17" t="s">
+        <v>373</v>
+      </c>
+      <c r="I363" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="J363" s="19" t="s">
+        <v>374</v>
+      </c>
+      <c r="K363" s="30" t="s">
         <v>375</v>
-      </c>
-      <c r="I363" s="18" t="n">
-        <v>0</v>
-      </c>
-      <c r="J363" s="19" t="s">
-        <v>376</v>
-      </c>
-      <c r="K363" s="30" t="s">
-        <v>377</v>
       </c>
       <c r="L363" s="17" t="s">
         <v>35</v>
@@ -18324,16 +18324,16 @@
         <v>17</v>
       </c>
       <c r="H364" s="17" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="I364" s="18" t="n">
         <v>0</v>
       </c>
       <c r="J364" s="19" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="K364" s="30" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="L364" s="17" t="s">
         <v>35</v>
@@ -18366,16 +18366,16 @@
         <v>17</v>
       </c>
       <c r="H365" s="17" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="I365" s="18" t="n">
         <v>0</v>
       </c>
       <c r="J365" s="19" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
       <c r="K365" s="77" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="L365" s="17" t="s">
         <v>35</v>
@@ -18408,16 +18408,16 @@
         <v>17</v>
       </c>
       <c r="H366" s="17" t="s">
-        <v>409</v>
+        <v>406</v>
       </c>
       <c r="I366" s="18" t="n">
         <v>0</v>
       </c>
       <c r="J366" s="19" t="s">
-        <v>280</v>
+        <v>87</v>
       </c>
       <c r="K366" s="77" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="L366" s="17" t="s">
         <v>44</v>
@@ -18450,7 +18450,7 @@
         <v>17</v>
       </c>
       <c r="H367" s="17" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="I367" s="18" t="n">
         <v>0</v>
@@ -18459,7 +18459,7 @@
         <v>128</v>
       </c>
       <c r="K367" s="30" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="L367" s="17" t="s">
         <v>31</v>
@@ -18492,16 +18492,16 @@
         <v>17</v>
       </c>
       <c r="H368" s="17" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="I368" s="18" t="n">
         <v>0</v>
       </c>
       <c r="J368" s="19" t="s">
-        <v>280</v>
+        <v>87</v>
       </c>
       <c r="K368" s="30" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="L368" s="17" t="s">
         <v>31</v>
@@ -18541,7 +18541,7 @@
         <v>167</v>
       </c>
       <c r="K369" s="30" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="L369" s="17" t="s">
         <v>31</v>
@@ -18581,7 +18581,7 @@
         <v>167</v>
       </c>
       <c r="K370" s="30" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="L370" s="17" t="s">
         <v>31</v>
@@ -18614,7 +18614,7 @@
         <v>9</v>
       </c>
       <c r="H371" s="10" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="I371" s="11" t="n">
         <v>0</v>
@@ -18623,7 +18623,7 @@
         <v>100</v>
       </c>
       <c r="K371" s="13" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
       <c r="L371" s="10" t="s">
         <v>107</v>
@@ -18656,16 +18656,16 @@
         <v>14</v>
       </c>
       <c r="H372" s="17" t="s">
-        <v>411</v>
+        <v>408</v>
       </c>
       <c r="I372" s="18" t="n">
         <v>0</v>
       </c>
       <c r="J372" s="19" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="K372" s="30" t="s">
-        <v>412</v>
+        <v>409</v>
       </c>
       <c r="L372" s="17" t="s">
         <v>107</v>
@@ -18698,16 +18698,16 @@
         <v>14</v>
       </c>
       <c r="H373" s="17" t="s">
-        <v>413</v>
+        <v>410</v>
       </c>
       <c r="I373" s="18" t="n">
         <v>0</v>
       </c>
       <c r="J373" s="19" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="K373" s="30" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
       <c r="L373" s="17" t="s">
         <v>107</v>
@@ -18740,16 +18740,16 @@
         <v>17</v>
       </c>
       <c r="H374" s="17" t="s">
-        <v>416</v>
+        <v>413</v>
       </c>
       <c r="I374" s="18" t="n">
         <v>0</v>
       </c>
       <c r="J374" s="19" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
       <c r="K374" s="30" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
       <c r="L374" s="17" t="s">
         <v>35</v>
@@ -18782,16 +18782,16 @@
         <v>17</v>
       </c>
       <c r="H375" s="17" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
       <c r="I375" s="18" t="n">
         <v>0</v>
       </c>
       <c r="J375" s="19" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="K375" s="30" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
       <c r="L375" s="17" t="s">
         <v>35</v>
@@ -18824,16 +18824,16 @@
         <v>17</v>
       </c>
       <c r="H376" s="17" t="s">
-        <v>420</v>
+        <v>417</v>
       </c>
       <c r="I376" s="18" t="n">
         <v>0</v>
       </c>
       <c r="J376" s="19" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="K376" s="30" t="s">
-        <v>421</v>
+        <v>418</v>
       </c>
       <c r="L376" s="17" t="s">
         <v>35</v>
@@ -18866,16 +18866,16 @@
         <v>17</v>
       </c>
       <c r="H377" s="17" t="s">
-        <v>422</v>
+        <v>419</v>
       </c>
       <c r="I377" s="18" t="n">
         <v>0</v>
       </c>
       <c r="J377" s="19" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="K377" s="30" t="s">
-        <v>424</v>
+        <v>421</v>
       </c>
       <c r="L377" s="17" t="s">
         <v>35</v>
@@ -18917,7 +18917,7 @@
         <v>262</v>
       </c>
       <c r="K378" s="13" t="s">
-        <v>425</v>
+        <v>422</v>
       </c>
       <c r="L378" s="10" t="s">
         <v>17</v>
@@ -18956,10 +18956,10 @@
         <v>0</v>
       </c>
       <c r="J379" s="19" t="s">
-        <v>426</v>
+        <v>423</v>
       </c>
       <c r="K379" s="30" t="s">
-        <v>427</v>
+        <v>424</v>
       </c>
       <c r="L379" s="17" t="s">
         <v>107</v>
@@ -18992,16 +18992,16 @@
         <v>17</v>
       </c>
       <c r="H380" s="17" t="s">
-        <v>428</v>
+        <v>425</v>
       </c>
       <c r="I380" s="18" t="n">
         <v>0</v>
       </c>
       <c r="J380" s="19" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
       <c r="K380" s="30" t="s">
-        <v>429</v>
+        <v>426</v>
       </c>
       <c r="L380" s="17" t="s">
         <v>44</v>
@@ -19034,16 +19034,16 @@
         <v>17</v>
       </c>
       <c r="H381" s="17" t="s">
-        <v>430</v>
+        <v>427</v>
       </c>
       <c r="I381" s="18" t="n">
         <v>0</v>
       </c>
       <c r="J381" s="19" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="K381" s="30" t="s">
-        <v>429</v>
+        <v>426</v>
       </c>
       <c r="L381" s="17" t="s">
         <v>44</v>
@@ -19076,16 +19076,16 @@
         <v>17</v>
       </c>
       <c r="H382" s="17" t="s">
-        <v>431</v>
+        <v>428</v>
       </c>
       <c r="I382" s="18" t="n">
         <v>0</v>
       </c>
       <c r="J382" s="19" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="K382" s="30" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="L382" s="17" t="s">
         <v>44</v>
@@ -19118,16 +19118,16 @@
         <v>17</v>
       </c>
       <c r="H383" s="17" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
       <c r="I383" s="18" t="n">
         <v>0</v>
       </c>
       <c r="J383" s="19" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="K383" s="30" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
       <c r="L383" s="17" t="s">
         <v>44</v>
@@ -19169,7 +19169,7 @@
         <v>112</v>
       </c>
       <c r="K384" s="30" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="L384" s="17" t="s">
         <v>44</v>
@@ -19202,16 +19202,16 @@
         <v>17</v>
       </c>
       <c r="H385" s="17" t="s">
-        <v>437</v>
+        <v>434</v>
       </c>
       <c r="I385" s="18" t="n">
         <v>0</v>
       </c>
       <c r="J385" s="19" t="s">
-        <v>280</v>
+        <v>87</v>
       </c>
       <c r="K385" s="30" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
       <c r="L385" s="17" t="s">
         <v>44</v>
@@ -19244,16 +19244,16 @@
         <v>17</v>
       </c>
       <c r="H386" s="17" t="s">
-        <v>437</v>
+        <v>434</v>
       </c>
       <c r="I386" s="18" t="n">
         <v>0</v>
       </c>
       <c r="J386" s="19" t="s">
-        <v>280</v>
+        <v>87</v>
       </c>
       <c r="K386" s="30" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
       <c r="L386" s="17" t="s">
         <v>44</v>
@@ -19286,7 +19286,7 @@
         <v>14</v>
       </c>
       <c r="H387" s="17" t="s">
-        <v>431</v>
+        <v>428</v>
       </c>
       <c r="I387" s="18" t="n">
         <v>0</v>
@@ -19295,7 +19295,7 @@
         <v>167</v>
       </c>
       <c r="K387" s="30" t="s">
-        <v>439</v>
+        <v>436</v>
       </c>
       <c r="L387" s="17" t="s">
         <v>31</v>
@@ -19328,7 +19328,7 @@
         <v>37</v>
       </c>
       <c r="H388" s="10" t="s">
-        <v>440</v>
+        <v>437</v>
       </c>
       <c r="I388" s="11" t="n">
         <v>0</v>
@@ -19337,7 +19337,7 @@
         <v>57</v>
       </c>
       <c r="K388" s="13" t="s">
-        <v>441</v>
+        <v>438</v>
       </c>
       <c r="L388" s="10" t="s">
         <v>44</v>
@@ -19379,7 +19379,7 @@
         <v>114</v>
       </c>
       <c r="K389" s="13" t="s">
-        <v>442</v>
+        <v>439</v>
       </c>
       <c r="L389" s="10" t="s">
         <v>44</v>
@@ -19418,10 +19418,10 @@
         <v>0</v>
       </c>
       <c r="J390" s="12" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="K390" s="13" t="s">
-        <v>442</v>
+        <v>439</v>
       </c>
       <c r="L390" s="10" t="s">
         <v>44</v>
@@ -19454,7 +19454,7 @@
         <v>12</v>
       </c>
       <c r="H391" s="10" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="I391" s="11" t="n">
         <v>0</v>
@@ -19463,7 +19463,7 @@
         <v>119</v>
       </c>
       <c r="K391" s="13" t="s">
-        <v>443</v>
+        <v>440</v>
       </c>
       <c r="L391" s="10" t="s">
         <v>35</v>
@@ -19496,7 +19496,7 @@
         <v>11</v>
       </c>
       <c r="H392" s="10" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="I392" s="11" t="n">
         <v>0</v>
@@ -19505,7 +19505,7 @@
         <v>119</v>
       </c>
       <c r="K392" s="13" t="s">
-        <v>445</v>
+        <v>442</v>
       </c>
       <c r="L392" s="10" t="s">
         <v>35</v>
@@ -19538,19 +19538,19 @@
         <v>9</v>
       </c>
       <c r="H393" s="10" t="s">
+        <v>443</v>
+      </c>
+      <c r="I393" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="J393" s="12" t="s">
+        <v>444</v>
+      </c>
+      <c r="K393" s="13" t="s">
+        <v>445</v>
+      </c>
+      <c r="L393" s="10" t="s">
         <v>446</v>
-      </c>
-      <c r="I393" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="J393" s="12" t="s">
-        <v>447</v>
-      </c>
-      <c r="K393" s="13" t="s">
-        <v>448</v>
-      </c>
-      <c r="L393" s="10" t="s">
-        <v>449</v>
       </c>
       <c r="M393" s="14" t="s">
         <v>62</v>
@@ -19580,16 +19580,16 @@
         <v>15</v>
       </c>
       <c r="H394" s="10" t="s">
-        <v>450</v>
+        <v>447</v>
       </c>
       <c r="I394" s="11" t="n">
         <v>0</v>
       </c>
       <c r="J394" s="12" t="s">
-        <v>280</v>
+        <v>87</v>
       </c>
       <c r="K394" s="13" t="s">
-        <v>451</v>
+        <v>448</v>
       </c>
       <c r="L394" s="10" t="s">
         <v>44</v>
@@ -19622,16 +19622,16 @@
         <v>15</v>
       </c>
       <c r="H395" s="10" t="s">
-        <v>450</v>
+        <v>447</v>
       </c>
       <c r="I395" s="11" t="n">
         <v>0</v>
       </c>
       <c r="J395" s="12" t="s">
-        <v>280</v>
+        <v>87</v>
       </c>
       <c r="K395" s="13" t="s">
-        <v>451</v>
+        <v>448</v>
       </c>
       <c r="L395" s="10" t="s">
         <v>44</v>
@@ -19664,7 +19664,7 @@
         <v>16</v>
       </c>
       <c r="H396" s="10" t="s">
-        <v>452</v>
+        <v>449</v>
       </c>
       <c r="I396" s="11" t="n">
         <v>0</v>
@@ -19673,7 +19673,7 @@
         <v>128</v>
       </c>
       <c r="K396" s="13" t="s">
-        <v>453</v>
+        <v>450</v>
       </c>
       <c r="L396" s="10" t="s">
         <v>31</v>
@@ -19706,16 +19706,16 @@
         <v>15</v>
       </c>
       <c r="H397" s="10" t="s">
-        <v>454</v>
+        <v>451</v>
       </c>
       <c r="I397" s="11" t="n">
         <v>0</v>
       </c>
       <c r="J397" s="12" t="s">
-        <v>280</v>
+        <v>87</v>
       </c>
       <c r="K397" s="13" t="s">
-        <v>455</v>
+        <v>452</v>
       </c>
       <c r="L397" s="10" t="s">
         <v>44</v>
@@ -19753,10 +19753,10 @@
         <v>0</v>
       </c>
       <c r="J398" s="5" t="s">
-        <v>456</v>
+        <v>453</v>
       </c>
       <c r="K398" s="6" t="s">
-        <v>457</v>
+        <v>454</v>
       </c>
       <c r="L398" s="3" t="s">
         <v>107</v>
@@ -19794,10 +19794,10 @@
         <v>0</v>
       </c>
       <c r="J399" s="5" t="s">
-        <v>456</v>
+        <v>453</v>
       </c>
       <c r="K399" s="6" t="s">
-        <v>458</v>
+        <v>455</v>
       </c>
       <c r="L399" s="3" t="s">
         <v>107</v>
@@ -19829,16 +19829,16 @@
         <v>17</v>
       </c>
       <c r="H400" s="3" t="s">
-        <v>459</v>
+        <v>456</v>
       </c>
       <c r="I400" s="4" t="n">
         <v>0</v>
       </c>
       <c r="J400" s="5" t="s">
-        <v>460</v>
+        <v>457</v>
       </c>
       <c r="K400" s="6" t="s">
-        <v>461</v>
+        <v>458</v>
       </c>
       <c r="L400" s="3" t="s">
         <v>107</v>
@@ -19870,16 +19870,16 @@
         <v>15</v>
       </c>
       <c r="H401" s="3" t="s">
-        <v>462</v>
+        <v>459</v>
       </c>
       <c r="I401" s="4" t="n">
         <v>0</v>
       </c>
       <c r="J401" s="5" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="K401" s="6" t="s">
-        <v>464</v>
+        <v>461</v>
       </c>
       <c r="L401" s="3" t="s">
         <v>107</v>
@@ -19917,10 +19917,10 @@
         <v>0</v>
       </c>
       <c r="J402" s="5" t="s">
-        <v>465</v>
+        <v>462</v>
       </c>
       <c r="K402" s="6" t="s">
-        <v>466</v>
+        <v>463</v>
       </c>
       <c r="L402" s="3" t="s">
         <v>17</v>
@@ -19929,7 +19929,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="403" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="403" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A403" s="0" t="n">
         <v>402</v>
       </c>
@@ -19952,16 +19952,16 @@
         <v>11</v>
       </c>
       <c r="H403" s="3" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
       <c r="I403" s="4" t="n">
         <v>0</v>
       </c>
       <c r="J403" s="5" t="s">
-        <v>468</v>
+        <v>465</v>
       </c>
       <c r="K403" s="6" t="s">
-        <v>469</v>
+        <v>466</v>
       </c>
       <c r="L403" s="3" t="s">
         <v>107</v>
@@ -19993,16 +19993,16 @@
         <v>11</v>
       </c>
       <c r="H404" s="3" t="s">
-        <v>470</v>
+        <v>467</v>
       </c>
       <c r="I404" s="4" t="n">
         <v>0</v>
       </c>
       <c r="J404" s="5" t="s">
-        <v>471</v>
+        <v>468</v>
       </c>
       <c r="K404" s="6" t="s">
-        <v>472</v>
+        <v>469</v>
       </c>
       <c r="L404" s="3" t="s">
         <v>107</v>
@@ -20034,16 +20034,16 @@
         <v>11</v>
       </c>
       <c r="H405" s="3" t="s">
-        <v>473</v>
+        <v>470</v>
       </c>
       <c r="I405" s="4" t="n">
         <v>0</v>
       </c>
       <c r="J405" s="5" t="s">
-        <v>474</v>
+        <v>471</v>
       </c>
       <c r="K405" s="6" t="s">
-        <v>475</v>
+        <v>472</v>
       </c>
       <c r="L405" s="3" t="s">
         <v>17</v>
@@ -20075,19 +20075,19 @@
         <v>10</v>
       </c>
       <c r="H406" s="3" t="s">
-        <v>476</v>
+        <v>473</v>
       </c>
       <c r="I406" s="4" t="n">
         <v>0</v>
       </c>
       <c r="J406" s="5" t="s">
-        <v>477</v>
+        <v>474</v>
       </c>
       <c r="K406" s="6" t="s">
-        <v>478</v>
+        <v>475</v>
       </c>
       <c r="L406" s="3" t="s">
-        <v>449</v>
+        <v>446</v>
       </c>
       <c r="M406" s="3" t="s">
         <v>55</v>
@@ -20116,19 +20116,19 @@
         <v>10</v>
       </c>
       <c r="H407" s="3" t="s">
+        <v>473</v>
+      </c>
+      <c r="I407" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="J407" s="5" t="s">
+        <v>474</v>
+      </c>
+      <c r="K407" s="6" t="s">
         <v>476</v>
       </c>
-      <c r="I407" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="J407" s="5" t="s">
-        <v>477</v>
-      </c>
-      <c r="K407" s="6" t="s">
-        <v>479</v>
-      </c>
       <c r="L407" s="3" t="s">
-        <v>449</v>
+        <v>446</v>
       </c>
       <c r="M407" s="3" t="s">
         <v>55</v>
@@ -20157,7 +20157,7 @@
         <v>10</v>
       </c>
       <c r="H408" s="3" t="s">
-        <v>476</v>
+        <v>473</v>
       </c>
       <c r="I408" s="4" t="n">
         <v>0</v>
@@ -20166,10 +20166,10 @@
         <v>477</v>
       </c>
       <c r="K408" s="6" t="s">
-        <v>478</v>
+        <v>475</v>
       </c>
       <c r="L408" s="3" t="s">
-        <v>449</v>
+        <v>446</v>
       </c>
       <c r="M408" s="3" t="s">
         <v>55</v>
@@ -20198,7 +20198,7 @@
         <v>10</v>
       </c>
       <c r="H409" s="3" t="s">
-        <v>476</v>
+        <v>473</v>
       </c>
       <c r="I409" s="4" t="n">
         <v>0</v>
@@ -20207,10 +20207,10 @@
         <v>477</v>
       </c>
       <c r="K409" s="6" t="s">
-        <v>478</v>
+        <v>475</v>
       </c>
       <c r="L409" s="3" t="s">
-        <v>449</v>
+        <v>446</v>
       </c>
       <c r="M409" s="3" t="s">
         <v>55</v>
@@ -20239,19 +20239,19 @@
         <v>17</v>
       </c>
       <c r="H410" s="3" t="s">
-        <v>476</v>
+        <v>473</v>
       </c>
       <c r="I410" s="4" t="n">
         <v>0</v>
       </c>
       <c r="J410" s="5" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="K410" s="6" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="L410" s="3" t="s">
-        <v>449</v>
+        <v>446</v>
       </c>
       <c r="M410" s="3" t="s">
         <v>55</v>
@@ -20281,7 +20281,7 @@
         <v>37</v>
       </c>
       <c r="H411" s="10" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="I411" s="11" t="n">
         <v>0</v>
@@ -20290,7 +20290,7 @@
         <v>167</v>
       </c>
       <c r="K411" s="13" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="L411" s="10" t="s">
         <v>31</v>
@@ -20323,16 +20323,16 @@
         <v>37</v>
       </c>
       <c r="H412" s="10" t="s">
+        <v>482</v>
+      </c>
+      <c r="I412" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="J412" s="12" t="s">
+        <v>483</v>
+      </c>
+      <c r="K412" s="13" t="s">
         <v>484</v>
-      </c>
-      <c r="I412" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="J412" s="12" t="s">
-        <v>485</v>
-      </c>
-      <c r="K412" s="13" t="s">
-        <v>486</v>
       </c>
       <c r="L412" s="10" t="s">
         <v>31</v>
@@ -20365,16 +20365,16 @@
         <v>37</v>
       </c>
       <c r="H413" s="10" t="s">
+        <v>485</v>
+      </c>
+      <c r="I413" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="J413" s="12" t="s">
+        <v>486</v>
+      </c>
+      <c r="K413" s="13" t="s">
         <v>487</v>
-      </c>
-      <c r="I413" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="J413" s="12" t="s">
-        <v>488</v>
-      </c>
-      <c r="K413" s="13" t="s">
-        <v>489</v>
       </c>
       <c r="L413" s="10" t="s">
         <v>17</v>
@@ -20416,10 +20416,10 @@
         <v>0</v>
       </c>
       <c r="J414" s="19" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="K414" s="30" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="L414" s="17" t="s">
         <v>17</v>
@@ -20461,10 +20461,10 @@
         <v>0</v>
       </c>
       <c r="J415" s="19" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="K415" s="30" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="L415" s="17" t="s">
         <v>17</v>
@@ -20506,10 +20506,10 @@
         <v>0</v>
       </c>
       <c r="J416" s="19" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="K416" s="30" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="L416" s="17" t="s">
         <v>17</v>
@@ -20554,7 +20554,7 @@
         <v>262</v>
       </c>
       <c r="K417" s="30" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="L417" s="17" t="s">
         <v>31</v>
@@ -20599,7 +20599,7 @@
         <v>112</v>
       </c>
       <c r="K418" s="30" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="L418" s="17" t="s">
         <v>31</v>
@@ -20632,7 +20632,7 @@
         <v>37</v>
       </c>
       <c r="H419" s="10" t="s">
-        <v>476</v>
+        <v>473</v>
       </c>
       <c r="I419" s="11" t="n">
         <v>0</v>
@@ -20641,7 +20641,7 @@
         <v>114</v>
       </c>
       <c r="K419" s="13" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="L419" s="10" t="s">
         <v>31</v>
@@ -20674,16 +20674,16 @@
         <v>37</v>
       </c>
       <c r="H420" s="10" t="s">
-        <v>476</v>
+        <v>473</v>
       </c>
       <c r="I420" s="11" t="n">
         <v>0</v>
       </c>
       <c r="J420" s="12" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="K420" s="13" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="L420" s="10" t="s">
         <v>31</v>
@@ -20716,16 +20716,16 @@
         <v>37</v>
       </c>
       <c r="H421" s="10" t="s">
+        <v>482</v>
+      </c>
+      <c r="I421" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="J421" s="12" t="s">
+        <v>483</v>
+      </c>
+      <c r="K421" s="13" t="s">
         <v>484</v>
-      </c>
-      <c r="I421" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="J421" s="12" t="s">
-        <v>485</v>
-      </c>
-      <c r="K421" s="13" t="s">
-        <v>486</v>
       </c>
       <c r="L421" s="10" t="s">
         <v>31</v>
@@ -20757,19 +20757,19 @@
         <v>10</v>
       </c>
       <c r="H422" s="3" t="s">
+        <v>494</v>
+      </c>
+      <c r="I422" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="J422" s="5" t="s">
+        <v>495</v>
+      </c>
+      <c r="K422" s="6" t="s">
         <v>496</v>
       </c>
-      <c r="I422" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="J422" s="5" t="s">
-        <v>497</v>
-      </c>
-      <c r="K422" s="6" t="s">
-        <v>498</v>
-      </c>
       <c r="L422" s="3" t="s">
-        <v>449</v>
+        <v>446</v>
       </c>
       <c r="M422" s="3" t="s">
         <v>18</v>
@@ -20800,14 +20800,14 @@
         <v>29</v>
       </c>
       <c r="H423" s="10" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="I423" s="11"/>
       <c r="J423" s="12" t="s">
         <v>167</v>
       </c>
       <c r="K423" s="13" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="L423" s="10" t="s">
         <v>44</v>
@@ -20845,10 +20845,10 @@
       </c>
       <c r="I424" s="11"/>
       <c r="J424" s="12" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="K424" s="13" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="L424" s="10" t="s">
         <v>44</v>
@@ -20882,16 +20882,16 @@
         <v>22</v>
       </c>
       <c r="H425" s="10" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="I425" s="11" t="n">
         <v>0</v>
       </c>
       <c r="J425" s="12" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="K425" s="13" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="L425" s="10" t="s">
         <v>31</v>
@@ -20925,16 +20925,16 @@
         <v>22</v>
       </c>
       <c r="H426" s="10" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="I426" s="11" t="n">
         <v>0</v>
       </c>
       <c r="J426" s="10" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="K426" s="13" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
       <c r="L426" s="10" t="s">
         <v>17</v>
@@ -20966,19 +20966,19 @@
         <v>10</v>
       </c>
       <c r="H427" s="3" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="I427" s="4" t="n">
         <v>0</v>
       </c>
       <c r="J427" s="5" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="K427" s="6" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="L427" s="3" t="s">
-        <v>449</v>
+        <v>446</v>
       </c>
       <c r="M427" s="3" t="s">
         <v>18</v>
@@ -21009,14 +21009,14 @@
         <v>29</v>
       </c>
       <c r="H428" s="10" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="I428" s="11"/>
       <c r="J428" s="12" t="s">
         <v>167</v>
       </c>
       <c r="K428" s="13" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="L428" s="10" t="s">
         <v>44</v>
@@ -21054,10 +21054,10 @@
       </c>
       <c r="I429" s="11"/>
       <c r="J429" s="12" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="K429" s="13" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="L429" s="10" t="s">
         <v>44</v>
@@ -21091,16 +21091,16 @@
         <v>22</v>
       </c>
       <c r="H430" s="10" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="I430" s="11" t="n">
         <v>0</v>
       </c>
       <c r="J430" s="12" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="K430" s="13" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="L430" s="10" t="s">
         <v>31</v>
@@ -21134,16 +21134,16 @@
         <v>22</v>
       </c>
       <c r="H431" s="10" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="I431" s="11" t="n">
         <v>0</v>
       </c>
       <c r="J431" s="10" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="K431" s="13" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
       <c r="L431" s="10" t="s">
         <v>17</v>
@@ -21175,19 +21175,19 @@
         <v>10</v>
       </c>
       <c r="H432" s="3" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="I432" s="4" t="n">
         <v>0</v>
       </c>
       <c r="J432" s="5" t="s">
-        <v>447</v>
+        <v>477</v>
       </c>
       <c r="K432" s="6" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="L432" s="3" t="s">
-        <v>449</v>
+        <v>446</v>
       </c>
       <c r="M432" s="3" t="s">
         <v>62</v>
@@ -21224,10 +21224,10 @@
         <v>0</v>
       </c>
       <c r="J433" s="12" t="s">
-        <v>502</v>
+        <v>167</v>
       </c>
       <c r="K433" s="13" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="L433" s="10" t="s">
         <v>31</v>
@@ -21261,16 +21261,16 @@
         <v>29</v>
       </c>
       <c r="H434" s="10" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="I434" s="11" t="n">
         <v>0</v>
       </c>
       <c r="J434" s="10" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="K434" s="13" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
       <c r="L434" s="10" t="s">
         <v>17</v>
@@ -21302,19 +21302,19 @@
         <v>10</v>
       </c>
       <c r="H435" s="3" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="I435" s="4" t="n">
         <v>0</v>
       </c>
       <c r="J435" s="5" t="s">
-        <v>447</v>
+        <v>477</v>
       </c>
       <c r="K435" s="6" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="L435" s="3" t="s">
-        <v>449</v>
+        <v>446</v>
       </c>
       <c r="M435" s="3" t="s">
         <v>62</v>
@@ -21351,10 +21351,10 @@
         <v>0</v>
       </c>
       <c r="J436" s="12" t="s">
-        <v>502</v>
+        <v>167</v>
       </c>
       <c r="K436" s="13" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="L436" s="10" t="s">
         <v>31</v>
@@ -21388,16 +21388,16 @@
         <v>29</v>
       </c>
       <c r="H437" s="10" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="I437" s="11" t="n">
         <v>0</v>
       </c>
       <c r="J437" s="10" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="K437" s="13" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
       <c r="L437" s="10" t="s">
         <v>17</v>
@@ -21429,16 +21429,16 @@
         <v>32</v>
       </c>
       <c r="H438" s="3" t="s">
-        <v>73</v>
+        <v>14</v>
       </c>
       <c r="I438" s="4" t="n">
         <v>0</v>
       </c>
       <c r="J438" s="5" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="K438" s="6" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
       <c r="L438" s="3" t="s">
         <v>44</v>
@@ -21470,19 +21470,19 @@
         <v>10</v>
       </c>
       <c r="H439" s="3" t="s">
+        <v>513</v>
+      </c>
+      <c r="I439" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="J439" s="5" t="s">
+        <v>514</v>
+      </c>
+      <c r="K439" s="6" t="s">
         <v>515</v>
       </c>
-      <c r="I439" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="J439" s="5" t="s">
-        <v>447</v>
-      </c>
-      <c r="K439" s="6" t="s">
-        <v>516</v>
-      </c>
       <c r="L439" s="3" t="s">
-        <v>449</v>
+        <v>446</v>
       </c>
       <c r="M439" s="3" t="s">
         <v>62</v>
@@ -21519,10 +21519,10 @@
         <v>0</v>
       </c>
       <c r="J440" s="12" t="s">
-        <v>502</v>
+        <v>167</v>
       </c>
       <c r="K440" s="13" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="L440" s="10" t="s">
         <v>31</v>
@@ -21554,19 +21554,19 @@
         <v>10</v>
       </c>
       <c r="H441" s="3" t="s">
+        <v>513</v>
+      </c>
+      <c r="I441" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="J441" s="5" t="s">
+        <v>514</v>
+      </c>
+      <c r="K441" s="6" t="s">
         <v>515</v>
       </c>
-      <c r="I441" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="J441" s="5" t="s">
-        <v>447</v>
-      </c>
-      <c r="K441" s="6" t="s">
-        <v>516</v>
-      </c>
       <c r="L441" s="3" t="s">
-        <v>449</v>
+        <v>446</v>
       </c>
       <c r="M441" s="3" t="s">
         <v>62</v>
@@ -21603,10 +21603,10 @@
         <v>0</v>
       </c>
       <c r="J442" s="12" t="s">
-        <v>502</v>
+        <v>167</v>
       </c>
       <c r="K442" s="13" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="L442" s="10" t="s">
         <v>31</v>
@@ -21615,7 +21615,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="443" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="443" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A443" s="0" t="n">
         <v>442</v>
       </c>
@@ -21632,19 +21632,19 @@
         <v>22</v>
       </c>
       <c r="F443" s="3" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="G443" s="3" t="n">
         <v>37</v>
       </c>
       <c r="H443" s="3" t="s">
-        <v>476</v>
+        <v>473</v>
       </c>
       <c r="I443" s="4" t="n">
         <v>0</v>
       </c>
       <c r="J443" s="5" t="s">
-        <v>447</v>
+        <v>516</v>
       </c>
       <c r="K443" s="6" t="s">
         <v>517</v>
@@ -21782,7 +21782,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="447" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="447" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A447" s="0" t="n">
         <v>446</v>
       </c>
@@ -21799,19 +21799,19 @@
         <v>31</v>
       </c>
       <c r="F447" s="3" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="G447" s="3" t="n">
         <v>37</v>
       </c>
       <c r="H447" s="3" t="s">
-        <v>476</v>
+        <v>473</v>
       </c>
       <c r="I447" s="4" t="n">
         <v>0</v>
       </c>
       <c r="J447" s="5" t="s">
-        <v>447</v>
+        <v>516</v>
       </c>
       <c r="K447" s="6" t="s">
         <v>525</v>
@@ -22046,7 +22046,7 @@
         <v>0</v>
       </c>
       <c r="J2" s="0" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="K2" s="79" t="s">
         <v>526</v>
@@ -22088,7 +22088,7 @@
         <v>1</v>
       </c>
       <c r="J3" s="0" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="K3" s="79" t="s">
         <v>527</v>
@@ -22129,7 +22129,7 @@
         <v>1</v>
       </c>
       <c r="J4" s="0" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="K4" s="79" t="s">
         <v>528</v>
@@ -22170,7 +22170,7 @@
         <v>1</v>
       </c>
       <c r="J5" s="0" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="K5" s="79" t="s">
         <v>528</v>
@@ -22803,7 +22803,7 @@
         <v>0</v>
       </c>
       <c r="J8" s="12" t="s">
-        <v>119</v>
+        <v>549</v>
       </c>
       <c r="K8" s="12"/>
       <c r="L8" s="10" t="s">
@@ -22920,7 +22920,7 @@
         <v>0</v>
       </c>
       <c r="J11" s="5" t="s">
-        <v>456</v>
+        <v>453</v>
       </c>
       <c r="K11" s="6"/>
       <c r="L11" s="3" t="s">
@@ -22959,7 +22959,7 @@
         <v>0</v>
       </c>
       <c r="J12" s="5" t="s">
-        <v>456</v>
+        <v>453</v>
       </c>
       <c r="K12" s="6"/>
       <c r="L12" s="3" t="s">
@@ -22998,7 +22998,7 @@
         <v>0</v>
       </c>
       <c r="J13" s="5" t="s">
-        <v>549</v>
+        <v>550</v>
       </c>
       <c r="K13" s="6"/>
       <c r="L13" s="3" t="s">
@@ -23074,7 +23074,7 @@
         <v>0</v>
       </c>
       <c r="J15" s="5" t="s">
-        <v>447</v>
+        <v>444</v>
       </c>
       <c r="K15" s="5"/>
       <c r="L15" s="3" t="s">
@@ -23113,7 +23113,7 @@
         <v>0</v>
       </c>
       <c r="J16" s="5" t="s">
-        <v>447</v>
+        <v>444</v>
       </c>
       <c r="K16" s="5"/>
       <c r="L16" s="3" t="s">
@@ -23152,7 +23152,7 @@
         <v>0</v>
       </c>
       <c r="J17" s="5" t="s">
-        <v>447</v>
+        <v>444</v>
       </c>
       <c r="K17" s="5"/>
       <c r="L17" s="3" t="s">
@@ -23224,13 +23224,13 @@
         <v>12</v>
       </c>
       <c r="H19" s="3" t="s">
-        <v>476</v>
+        <v>473</v>
       </c>
       <c r="I19" s="4" t="n">
         <v>0</v>
       </c>
       <c r="J19" s="5" t="s">
-        <v>447</v>
+        <v>444</v>
       </c>
       <c r="K19" s="6"/>
       <c r="L19" s="3" t="s">
@@ -23263,13 +23263,13 @@
         <v>12</v>
       </c>
       <c r="H20" s="3" t="s">
-        <v>476</v>
+        <v>473</v>
       </c>
       <c r="I20" s="4" t="n">
         <v>0</v>
       </c>
       <c r="J20" s="5" t="s">
-        <v>447</v>
+        <v>444</v>
       </c>
       <c r="K20" s="6"/>
       <c r="L20" s="3" t="s">
@@ -23302,13 +23302,13 @@
         <v>12</v>
       </c>
       <c r="H21" s="3" t="s">
-        <v>476</v>
+        <v>473</v>
       </c>
       <c r="I21" s="4" t="n">
         <v>0</v>
       </c>
       <c r="J21" s="5" t="s">
-        <v>447</v>
+        <v>444</v>
       </c>
       <c r="K21" s="6"/>
       <c r="L21" s="3" t="s">
@@ -23341,13 +23341,13 @@
         <v>12</v>
       </c>
       <c r="H22" s="3" t="s">
-        <v>476</v>
+        <v>473</v>
       </c>
       <c r="I22" s="4" t="n">
         <v>0</v>
       </c>
       <c r="J22" s="5" t="s">
-        <v>447</v>
+        <v>444</v>
       </c>
       <c r="K22" s="6"/>
       <c r="L22" s="3" t="s">
@@ -23419,13 +23419,13 @@
         <v>12</v>
       </c>
       <c r="H24" s="3" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="I24" s="4" t="n">
         <v>0</v>
       </c>
       <c r="J24" s="5" t="s">
-        <v>447</v>
+        <v>444</v>
       </c>
       <c r="K24" s="6"/>
       <c r="L24" s="3" t="s">
@@ -23458,13 +23458,13 @@
         <v>12</v>
       </c>
       <c r="H25" s="3" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="I25" s="4" t="n">
         <v>0</v>
       </c>
       <c r="J25" s="5" t="s">
-        <v>447</v>
+        <v>444</v>
       </c>
       <c r="K25" s="6"/>
       <c r="L25" s="3" t="s">
@@ -23497,13 +23497,13 @@
         <v>12</v>
       </c>
       <c r="H26" s="3" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="I26" s="4" t="n">
         <v>0</v>
       </c>
       <c r="J26" s="5" t="s">
-        <v>447</v>
+        <v>444</v>
       </c>
       <c r="K26" s="6"/>
       <c r="L26" s="3" t="s">
@@ -23536,13 +23536,13 @@
         <v>12</v>
       </c>
       <c r="H27" s="3" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="I27" s="4" t="n">
         <v>0</v>
       </c>
       <c r="J27" s="5" t="s">
-        <v>447</v>
+        <v>444</v>
       </c>
       <c r="K27" s="6"/>
       <c r="L27" s="3" t="s">

</xml_diff>

<commit_message>
bidds (natural) and my version of runM. but oslo probably wrong
</commit_message>
<xml_diff>
--- a/bridgeIn.xlsx
+++ b/bridgeIn.xlsx
@@ -5,19 +5,20 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="544" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="544" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="W-J 2017" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="poInterwencji" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="SA_z_piatek" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="NaturalnaKM" sheetId="4" state="visible" r:id="rId5"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4449" uniqueCount="979">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4813" uniqueCount="1034">
   <si>
     <t>bidId</t>
   </si>
@@ -3732,33 +3733,102 @@
     <t>brak odzywki na otwarcie po pasie partnera  na poziomie 1 (0-11PC) lub 2 (0-5 PC i długi kolor (6+) lub układ na dwóch piątkach) lub 3 itp. ...</t>
   </si>
   <si>
+    <t>3+ trefl</t>
+  </si>
+  <si>
+    <t>Otwarcie 1 młodszy</t>
+  </si>
+  <si>
+    <t>otwarcie bez starszej piątki – w dłuższy młodszy oraz 3-3 na karach i treflach</t>
+  </si>
+  <si>
+    <t>One – over one</t>
+  </si>
+  <si>
+    <t>czwórka karowa nie wyklucza fitu trefl ani starszej czwórki...</t>
+  </si>
+  <si>
+    <t>czwórka kierowa, wyklucza czwórkę karo, nie wyklucza pikowej, ani fitu trefl</t>
+  </si>
+  <si>
+    <t>czwórka pikowa, wyklucza czwórki karo i kier, nie wyklucza fitu trefl</t>
+  </si>
+  <si>
+    <t>6-10 PC, wyklucza (raczej 4  karo),  4 kier, 4 pik i 5 trefl;</t>
+  </si>
+  <si>
+    <t>Two – over – one</t>
+  </si>
+  <si>
+    <t>6+ PC, 5+ w kolor, wyklucza starsze czwórki;</t>
+  </si>
+  <si>
+    <t>6+ PC, 5+(ewentualnie 4 kara) , wyklucza starsze czwórki;</t>
+  </si>
+  <si>
+    <t>inwit do 3 NT</t>
+  </si>
+  <si>
+    <t>końcówka</t>
+  </si>
+  <si>
+    <t>raczej bez starszej czwórki</t>
+  </si>
+  <si>
     <t>3+</t>
   </si>
   <si>
-    <t>Otwarcie 1 młodszy</t>
-  </si>
-  <si>
-    <t>otwarcie bez starszej piątki – w dłuższy młodszy oraz 3-3 na karach i treflach</t>
+    <t>Otwarcie bez starszej piątki, w dłuższy młodszy (min 3 kara)  lub na układzie 4-4 w młodszym</t>
+  </si>
+  <si>
+    <t>Zawsze dłuższy kolor, przy dwóch piątkach (lub dwóch szóstkach) w starszą)</t>
+  </si>
+  <si>
+    <t>6-10 PC, wyklucza fit w kolor otwarcia</t>
+  </si>
+  <si>
+    <t>3+ fit + zrównoważony</t>
+  </si>
+  <si>
+    <t>inwit</t>
+  </si>
+  <si>
+    <t>inwit do końcówki w BA lub kolor</t>
+  </si>
+  <si>
+    <t>Naturalne bez Atu</t>
+  </si>
+  <si>
+    <t>dobra szóstka karo, wykluczona starsza czwórka</t>
+  </si>
+  <si>
+    <t>słaba</t>
+  </si>
+  <si>
+    <t>dobra szóstka kier, wykluczona czwórka pik</t>
+  </si>
+  <si>
+    <t>dobra szóstka pik, wyklucza czwórkę kier</t>
+  </si>
+  <si>
+    <t>8+</t>
+  </si>
+  <si>
+    <t>??</t>
+  </si>
+  <si>
+    <t>dobry ośmiokart, silniejsze niż otwarcie 3 w kolor</t>
   </si>
   <si>
     <t>poparcie na 4 karo</t>
   </si>
   <si>
-    <t>czwórka karowa nie wyklucza fitu trefl ani starszej czwórki...</t>
-  </si>
-  <si>
     <t>poparcie na 4 kier</t>
   </si>
   <si>
-    <t>czwórka kierowa, wyklucza czwórkę karo, nie wyklucza pikowej, ani fitu trefl</t>
-  </si>
-  <si>
     <t>poparcie na 4 pik</t>
   </si>
   <si>
-    <t>czwórka pikowa, wyklucza czwórki karo i kier, nie wyklucza fitu trefl</t>
-  </si>
-  <si>
     <t>6-10 PC, wyklucza 4 kara, 4 kiery, 4 piki i 5 trefli;</t>
   </si>
   <si>
@@ -3768,19 +3838,115 @@
     <t>6+ PC, 5+ trefli, wyklucza 4 kara, 4 kiery, 4 piki;</t>
   </si>
   <si>
-    <t>inwit do 3 NT</t>
-  </si>
-  <si>
-    <t>Naturalne bez Atu</t>
+    <t>Wyjątkowo od 11 (dobry układ) zwykle od 12PC. Najdłuższy kolor, czyli układ z 5kier  nie wyklucza młodszej piątki, wyklucza dowolną szóstkę. Jeżeli kierów jest 6 to może być dowlona inna piątka (nawet pikowa)   </t>
+  </si>
+  <si>
+    <t>brak poparcia</t>
+  </si>
+  <si>
+    <t>Brak punktów, poparcia i układu</t>
+  </si>
+  <si>
+    <t>One – over – one</t>
+  </si>
+  <si>
+    <t>One – over – one własna słaba starsza czwórka Słabe zgłoszenie czwórki pików, możliwy fit kier</t>
+  </si>
+  <si>
+    <t>Two – over – one </t>
+  </si>
+  <si>
+    <t>Two – over – one własna piątka, możliwy fit </t>
+  </si>
+  <si>
+    <t>słabe poparcie kier</t>
+  </si>
+  <si>
+    <t>Poparcie kierowe czyli jest fit 3+ kier – co prawda końcówka prawdopodobnie nie idzie, ale może … jeżeli masz maksimu, przeciwnicy pewnie też mają fit skoro my mamy to nie należy im ułatwiać... </t>
+  </si>
+  <si>
+    <t>silne poparcie kier aspiracje szlemikowe</t>
+  </si>
+  <si>
+    <t>silna karta (z fitem kier) – skoro na pewno mamy końcówkę to postarajmy się dogadać szczegółowo (w niektórych systemach naturalnych może to być inwit do kierowej końcówki, ale jak wtedy zgłaszać silną kartę)</t>
+  </si>
+  <si>
+    <t>Końcówka 4 kier</t>
+  </si>
+  <si>
+    <t>Poparcie na końcówkę limitowane z góry – jeżeli punktów honorowych jest 10 (albo nawet mniej)  ale dobry układ np. singiel (albo singiel i dubel a punkty w innych kolorach oczywiście) to należy zalicytować końcówkę … Najczęściej próba uzgodnienia czegoś innego daje obrońcom informacje o korzystnej obronie  </t>
+  </si>
+  <si>
+    <t>2 kier, zrównoważony</t>
+  </si>
+  <si>
+    <t>Układ zrównoważony (4-3-3-2, 5-4-2-2 itp.) brak singla, brak fitu (3+ kier) </t>
+  </si>
+  <si>
+    <t>Końcówka 4 pik</t>
+  </si>
+  <si>
+    <t>Wyjątkowo od 11 (dobry układ) zwykle od 12PC.  Najdłuższy kolor, czyli układ z 5 pik wyklucza inną piątkę, która jest możliwa tylko jeżeli pików jest 6 (lub więcej)</t>
+  </si>
+  <si>
+    <t>Two – over – one własna piątka, możliwy fit  ( w drodze wyjątku możliwa czwórka kier!)</t>
+  </si>
+  <si>
+    <t>słabe poparcie pik</t>
+  </si>
+  <si>
+    <t>Poparcie kierowe czyli jest fit 3+ pik – co prawda końcówka prawdopodobnie nie idzie, ale może … jeżeli masz maksimu, przeciwnicy pewnie też mają fit skoro my mamy to nie należy im ułatwiać... </t>
+  </si>
+  <si>
+    <t>silne poparcie pik aspiracje szlemikowe</t>
+  </si>
+  <si>
+    <t>silna karta (z fitem pik) – skoro na pewno mamy końcówkę to postarajmy się dogadać szczegółowo (w niektórych systemach naturalnych może to być inwit do kierowej końcówki, ale jak wtedy zgłaszać silną kartę)</t>
+  </si>
+  <si>
+    <t>2 pik, zrównoważony</t>
+  </si>
+  <si>
+    <t>Układ zrównoważony (4-3-3-2, 5-4-2-2 itp.) brak singla, brak fitu (3+ pik) </t>
+  </si>
+  <si>
+    <t>Układ zrównoważony (4-3-3-3, lub 4-4-3-2) : brak singla, tylko jeden  dubel, nie liczą się punkty układowe. Dopuszczalny układ 5-4-2-2 jeżeli  5 jest w trefl / karo i dubel zawiera minimum damę. </t>
+  </si>
+  <si>
+    <t>Razem jest maksymalnie 18-25 PC (dokładnie możesz policzyć dodając swoje PC do 18) co jest za mało na 3BA (potrzebne 26 PC) a granie 2BA nic nie daje </t>
+  </si>
+  <si>
+    <t>Razem jest na pewno 24 -25PC (dokładnie możesz policzyć dodając swoje punkty do 16) i być może o 2PC więcej więc to otwierającemu zostawiamy decyzję co do kontraktu</t>
+  </si>
+  <si>
+    <t>kontrakt firmowy</t>
+  </si>
+  <si>
+    <t>przy minimum otwierającego jest 26, czyli na pewno powinien iść firmowy (oczywiście może akurat nie pójść, ale trzeba grać) , za to na pewno nie ma na więcej bo maksimum obu rąk jest 31&lt; 32PC potrzebne na szlemika w BA</t>
   </si>
   <si>
     <t>F</t>
   </si>
   <si>
-    <t>słaba</t>
-  </si>
-  <si>
-    <t>8+</t>
+    <t>7+ C</t>
+  </si>
+  <si>
+    <t>Blok na dobrym siedmiokartowym (lub dłuższym kolorze)  - maksymalnie 5 lew oddających  </t>
+  </si>
+  <si>
+    <t>7+ D</t>
+  </si>
+  <si>
+    <t>7+ H</t>
+  </si>
+  <si>
+    <t>7+ S</t>
+  </si>
+  <si>
+    <t>samodzielny kontrakt firmowy</t>
+  </si>
+  <si>
+    <t>Niezależnie co ma partner idzie 3 BA – zatrzymania we wszystkich kolorach, dobry układ </t>
   </si>
 </sst>
 </file>
@@ -4460,10 +4626,10 @@
   </sheetPr>
   <dimension ref="A1:N711"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A634" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A634" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="525" topLeftCell="A688" activePane="bottomLeft" state="split"/>
       <selection pane="topLeft" activeCell="A634" activeCellId="0" sqref="A634"/>
-      <selection pane="bottomLeft" activeCell="A226" activeCellId="0" sqref="A226:A711"/>
+      <selection pane="bottomLeft" activeCell="A226" activeCellId="1" sqref="A4:A41 A226"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -36565,7 +36731,7 @@
   <dimension ref="A1:N5"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I2" activeCellId="1" sqref="A226:A711 I2"/>
+      <selection pane="topLeft" activeCell="I2" activeCellId="1" sqref="A4:A41 I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -36810,12 +36976,12 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:N28"/>
+  <dimension ref="A1:N41"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="525" topLeftCell="A1" activePane="bottomLeft" state="split"/>
-      <selection pane="topLeft" activeCell="G1" activeCellId="0" sqref="G1"/>
-      <selection pane="bottomLeft" activeCell="I2" activeCellId="1" sqref="A226:A711 I2"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="525" topLeftCell="A16" activePane="bottomLeft" state="split"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="A4" activeCellId="0" sqref="A4:A41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -36943,7 +37109,7 @@
         <v>37</v>
       </c>
       <c r="H3" s="12" t="s">
-        <v>263</v>
+        <v>518</v>
       </c>
       <c r="I3" s="13" t="n">
         <v>0</v>
@@ -36955,7 +37121,7 @@
         <v>966</v>
       </c>
       <c r="L3" s="12" t="s">
-        <v>81</v>
+        <v>18</v>
       </c>
       <c r="M3" s="16" t="s">
         <v>31</v>
@@ -36988,19 +37154,19 @@
         <v>37</v>
       </c>
       <c r="H4" s="12" t="s">
-        <v>263</v>
+        <v>24</v>
       </c>
       <c r="I4" s="13" t="n">
         <v>0</v>
       </c>
       <c r="J4" s="14" t="s">
+        <v>965</v>
+      </c>
+      <c r="K4" s="15" t="s">
         <v>967</v>
       </c>
-      <c r="K4" s="15" t="s">
-        <v>968</v>
-      </c>
       <c r="L4" s="12" t="s">
-        <v>81</v>
+        <v>18</v>
       </c>
       <c r="M4" s="16" t="s">
         <v>31</v>
@@ -37033,19 +37199,19 @@
         <v>37</v>
       </c>
       <c r="H5" s="12" t="s">
-        <v>263</v>
+        <v>59</v>
       </c>
       <c r="I5" s="13" t="n">
         <v>0</v>
       </c>
       <c r="J5" s="14" t="s">
-        <v>969</v>
+        <v>965</v>
       </c>
       <c r="K5" s="15" t="s">
-        <v>970</v>
+        <v>968</v>
       </c>
       <c r="L5" s="12" t="s">
-        <v>81</v>
+        <v>18</v>
       </c>
       <c r="M5" s="16" t="s">
         <v>31</v>
@@ -37077,7 +37243,7 @@
         <v>10</v>
       </c>
       <c r="H6" s="12" t="s">
-        <v>145</v>
+        <v>57</v>
       </c>
       <c r="I6" s="13" t="n">
         <v>0</v>
@@ -37086,7 +37252,7 @@
         <v>111</v>
       </c>
       <c r="K6" s="14" t="s">
-        <v>971</v>
+        <v>969</v>
       </c>
       <c r="L6" s="12" t="s">
         <v>81</v>
@@ -37118,19 +37284,19 @@
         <v>6</v>
       </c>
       <c r="G7" s="12" t="n">
-        <v>37</v>
+        <v>9</v>
       </c>
       <c r="H7" s="12" t="s">
-        <v>124</v>
+        <v>36</v>
       </c>
       <c r="I7" s="13" t="n">
         <v>0</v>
       </c>
       <c r="J7" s="14" t="s">
-        <v>972</v>
+        <v>970</v>
       </c>
       <c r="K7" s="14" t="s">
-        <v>973</v>
+        <v>971</v>
       </c>
       <c r="L7" s="12" t="s">
         <v>81</v>
@@ -37156,6 +37322,1836 @@
         <v>2</v>
       </c>
       <c r="E8" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="F8" s="12" t="n">
+        <v>6</v>
+      </c>
+      <c r="G8" s="12" t="n">
+        <v>9</v>
+      </c>
+      <c r="H8" s="12" t="s">
+        <v>518</v>
+      </c>
+      <c r="I8" s="13" t="n">
+        <v>0</v>
+      </c>
+      <c r="J8" s="14" t="s">
+        <v>970</v>
+      </c>
+      <c r="K8" s="14" t="s">
+        <v>972</v>
+      </c>
+      <c r="L8" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="M8" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="N8" s="13" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="C9" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="D9" s="11" t="n">
+        <v>2</v>
+      </c>
+      <c r="E9" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="F9" s="12" t="n">
+        <v>6</v>
+      </c>
+      <c r="G9" s="12" t="n">
+        <v>9</v>
+      </c>
+      <c r="H9" s="12" t="s">
+        <v>148</v>
+      </c>
+      <c r="I9" s="13" t="n">
+        <v>0</v>
+      </c>
+      <c r="J9" s="14" t="s">
+        <v>970</v>
+      </c>
+      <c r="K9" s="14" t="s">
+        <v>971</v>
+      </c>
+      <c r="L9" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="M9" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="N9" s="13" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="C10" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="D10" s="11" t="n">
+        <v>2</v>
+      </c>
+      <c r="E10" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="F10" s="12" t="n">
+        <v>6</v>
+      </c>
+      <c r="G10" s="12" t="n">
+        <v>9</v>
+      </c>
+      <c r="H10" s="12" t="s">
+        <v>332</v>
+      </c>
+      <c r="I10" s="13" t="n">
+        <v>0</v>
+      </c>
+      <c r="J10" s="14" t="s">
+        <v>970</v>
+      </c>
+      <c r="K10" s="14" t="s">
+        <v>971</v>
+      </c>
+      <c r="L10" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="M10" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="N10" s="13" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="C11" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="D11" s="11" t="n">
+        <v>2</v>
+      </c>
+      <c r="E11" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="F11" s="12" t="n">
+        <v>13</v>
+      </c>
+      <c r="G11" s="12" t="n">
+        <v>14</v>
+      </c>
+      <c r="H11" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="I11" s="13" t="n">
+        <v>0</v>
+      </c>
+      <c r="J11" s="14" t="s">
+        <v>973</v>
+      </c>
+      <c r="K11" s="14"/>
+      <c r="L11" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="M11" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="N11" s="13" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="B12" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="C12" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="D12" s="11" t="n">
+        <v>3</v>
+      </c>
+      <c r="E12" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="F12" s="12" t="n">
+        <v>15</v>
+      </c>
+      <c r="G12" s="12" t="n">
+        <v>17</v>
+      </c>
+      <c r="H12" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="I12" s="13" t="n">
+        <v>0</v>
+      </c>
+      <c r="J12" s="14" t="s">
+        <v>974</v>
+      </c>
+      <c r="K12" s="14" t="s">
+        <v>975</v>
+      </c>
+      <c r="L12" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="M12" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="N12" s="13" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="B13" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C13" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D13" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F13" s="5" t="n">
+        <v>13</v>
+      </c>
+      <c r="G13" s="5" t="n">
+        <v>21</v>
+      </c>
+      <c r="H13" s="5" t="s">
+        <v>976</v>
+      </c>
+      <c r="I13" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="J13" s="7" t="s">
+        <v>963</v>
+      </c>
+      <c r="K13" s="8" t="s">
+        <v>977</v>
+      </c>
+      <c r="L13" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="M13" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="N13" s="6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="B14" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C14" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D14" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F14" s="5" t="n">
+        <v>13</v>
+      </c>
+      <c r="G14" s="5" t="n">
+        <v>21</v>
+      </c>
+      <c r="H14" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="I14" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="J14" s="7" t="s">
+        <v>529</v>
+      </c>
+      <c r="K14" s="8" t="s">
+        <v>978</v>
+      </c>
+      <c r="L14" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="M14" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="N14" s="6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="B15" s="10" t="n">
+        <f aca="false">A14</f>
+        <v>13</v>
+      </c>
+      <c r="C15" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="D15" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="E15" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="F15" s="12" t="n">
+        <v>6</v>
+      </c>
+      <c r="G15" s="12" t="n">
+        <v>37</v>
+      </c>
+      <c r="H15" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="I15" s="13" t="n">
+        <v>0</v>
+      </c>
+      <c r="J15" s="14" t="s">
+        <v>965</v>
+      </c>
+      <c r="K15" s="15" t="s">
+        <v>968</v>
+      </c>
+      <c r="L15" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="M15" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="N15" s="13" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="B16" s="10" t="n">
+        <f aca="false">B15</f>
+        <v>13</v>
+      </c>
+      <c r="C16" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="D16" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="E16" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="F16" s="12" t="n">
+        <v>6</v>
+      </c>
+      <c r="G16" s="12" t="n">
+        <v>10</v>
+      </c>
+      <c r="H16" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="I16" s="13" t="n">
+        <v>0</v>
+      </c>
+      <c r="J16" s="14" t="s">
+        <v>111</v>
+      </c>
+      <c r="K16" s="14" t="s">
+        <v>979</v>
+      </c>
+      <c r="L16" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="M16" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="N16" s="13" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="B17" s="10" t="n">
+        <f aca="false">B16</f>
+        <v>13</v>
+      </c>
+      <c r="C17" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="D17" s="11" t="n">
+        <v>2</v>
+      </c>
+      <c r="E17" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="F17" s="12" t="n">
+        <v>11</v>
+      </c>
+      <c r="G17" s="12" t="n">
+        <v>37</v>
+      </c>
+      <c r="H17" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="I17" s="13" t="n">
+        <v>0</v>
+      </c>
+      <c r="J17" s="14" t="s">
+        <v>970</v>
+      </c>
+      <c r="K17" s="14" t="s">
+        <v>971</v>
+      </c>
+      <c r="L17" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="M17" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="N17" s="13" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="B18" s="10" t="n">
+        <f aca="false">B17</f>
+        <v>13</v>
+      </c>
+      <c r="C18" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="D18" s="11" t="n">
+        <v>2</v>
+      </c>
+      <c r="E18" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="F18" s="12" t="n">
+        <v>11</v>
+      </c>
+      <c r="G18" s="12" t="n">
+        <v>37</v>
+      </c>
+      <c r="H18" s="12" t="s">
+        <v>518</v>
+      </c>
+      <c r="I18" s="13" t="n">
+        <v>0</v>
+      </c>
+      <c r="J18" s="14" t="s">
+        <v>970</v>
+      </c>
+      <c r="K18" s="14" t="s">
+        <v>972</v>
+      </c>
+      <c r="L18" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="M18" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="N18" s="13" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="B19" s="10" t="n">
+        <f aca="false">B18</f>
+        <v>13</v>
+      </c>
+      <c r="C19" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="D19" s="11" t="n">
+        <v>2</v>
+      </c>
+      <c r="E19" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="F19" s="12" t="n">
+        <v>11</v>
+      </c>
+      <c r="G19" s="12" t="n">
+        <v>37</v>
+      </c>
+      <c r="H19" s="12" t="s">
+        <v>148</v>
+      </c>
+      <c r="I19" s="13" t="n">
+        <v>0</v>
+      </c>
+      <c r="J19" s="14" t="s">
+        <v>970</v>
+      </c>
+      <c r="K19" s="14" t="s">
+        <v>971</v>
+      </c>
+      <c r="L19" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="M19" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="N19" s="13" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="n">
+        <v>19</v>
+      </c>
+      <c r="B20" s="10" t="n">
+        <f aca="false">B19</f>
+        <v>13</v>
+      </c>
+      <c r="C20" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="D20" s="11" t="n">
+        <v>2</v>
+      </c>
+      <c r="E20" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="F20" s="12" t="n">
+        <v>11</v>
+      </c>
+      <c r="G20" s="12" t="n">
+        <v>37</v>
+      </c>
+      <c r="H20" s="12" t="s">
+        <v>332</v>
+      </c>
+      <c r="I20" s="13" t="n">
+        <v>0</v>
+      </c>
+      <c r="J20" s="14" t="s">
+        <v>970</v>
+      </c>
+      <c r="K20" s="14" t="s">
+        <v>971</v>
+      </c>
+      <c r="L20" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="M20" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="N20" s="13" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="B21" s="10" t="n">
+        <f aca="false">B20</f>
+        <v>13</v>
+      </c>
+      <c r="C21" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="D21" s="11" t="n">
+        <v>2</v>
+      </c>
+      <c r="E21" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="F21" s="12" t="n">
+        <v>13</v>
+      </c>
+      <c r="G21" s="12" t="n">
+        <v>37</v>
+      </c>
+      <c r="H21" s="12" t="s">
+        <v>980</v>
+      </c>
+      <c r="I21" s="13" t="n">
+        <v>0</v>
+      </c>
+      <c r="J21" s="14" t="s">
+        <v>981</v>
+      </c>
+      <c r="K21" s="14" t="s">
+        <v>982</v>
+      </c>
+      <c r="L21" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="M21" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="N21" s="13" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="B22" s="10" t="n">
+        <f aca="false">B21</f>
+        <v>13</v>
+      </c>
+      <c r="C22" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="D22" s="11" t="n">
+        <v>3</v>
+      </c>
+      <c r="E22" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="F22" s="12" t="n">
+        <v>15</v>
+      </c>
+      <c r="G22" s="12" t="n">
+        <v>17</v>
+      </c>
+      <c r="H22" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="I22" s="13" t="n">
+        <v>0</v>
+      </c>
+      <c r="J22" s="14" t="s">
+        <v>974</v>
+      </c>
+      <c r="K22" s="14" t="s">
+        <v>975</v>
+      </c>
+      <c r="L22" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="M22" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="N22" s="13" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="n">
+        <v>22</v>
+      </c>
+      <c r="B23" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C23" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D23" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="F23" s="5" t="n">
+        <v>13</v>
+      </c>
+      <c r="G23" s="5" t="n">
+        <v>21</v>
+      </c>
+      <c r="H23" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="I23" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="J23" s="7" t="s">
+        <v>529</v>
+      </c>
+      <c r="K23" s="8" t="s">
+        <v>978</v>
+      </c>
+      <c r="L23" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="M23" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="N23" s="6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="n">
+        <v>23</v>
+      </c>
+      <c r="B24" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C24" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D24" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F24" s="5" t="n">
+        <v>15</v>
+      </c>
+      <c r="G24" s="5" t="n">
+        <v>17</v>
+      </c>
+      <c r="H24" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="I24" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="J24" s="7" t="s">
+        <v>983</v>
+      </c>
+      <c r="K24" s="8"/>
+      <c r="L24" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="M24" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="N24" s="6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="B25" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C25" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D25" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F25" s="5" t="n">
+        <v>22</v>
+      </c>
+      <c r="G25" s="5" t="n">
+        <v>37</v>
+      </c>
+      <c r="H25" s="5"/>
+      <c r="I25" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="J25" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="K25" s="8"/>
+      <c r="L25" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="M25" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="N25" s="6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="B26" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C26" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D26" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F26" s="5" t="n">
+        <v>6</v>
+      </c>
+      <c r="G26" s="5" t="n">
+        <v>12</v>
+      </c>
+      <c r="H26" s="5" t="s">
+        <v>201</v>
+      </c>
+      <c r="I26" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="J26" s="7" t="s">
+        <v>519</v>
+      </c>
+      <c r="K26" s="7" t="s">
+        <v>984</v>
+      </c>
+      <c r="L26" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="M26" s="5" t="s">
+        <v>985</v>
+      </c>
+      <c r="N26" s="6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="n">
+        <v>26</v>
+      </c>
+      <c r="B27" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C27" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D27" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F27" s="5" t="n">
+        <v>6</v>
+      </c>
+      <c r="G27" s="5" t="n">
+        <v>12</v>
+      </c>
+      <c r="H27" s="5" t="s">
+        <v>201</v>
+      </c>
+      <c r="I27" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="J27" s="7" t="s">
+        <v>519</v>
+      </c>
+      <c r="K27" s="7" t="s">
+        <v>986</v>
+      </c>
+      <c r="L27" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="M27" s="5" t="s">
+        <v>985</v>
+      </c>
+      <c r="N27" s="6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="n">
+        <v>27</v>
+      </c>
+      <c r="B28" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C28" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D28" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="F28" s="5" t="n">
+        <v>6</v>
+      </c>
+      <c r="G28" s="5" t="n">
+        <v>12</v>
+      </c>
+      <c r="H28" s="5" t="s">
+        <v>201</v>
+      </c>
+      <c r="I28" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="J28" s="7" t="s">
+        <v>519</v>
+      </c>
+      <c r="K28" s="7" t="s">
+        <v>987</v>
+      </c>
+      <c r="L28" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="M28" s="5" t="s">
+        <v>985</v>
+      </c>
+      <c r="N28" s="6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="B29" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C29" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D29" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F29" s="5" t="n">
+        <v>20</v>
+      </c>
+      <c r="G29" s="5" t="n">
+        <v>21</v>
+      </c>
+      <c r="H29" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="I29" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="J29" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="K29" s="8"/>
+      <c r="L29" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="M29" s="5" t="s">
+        <v>985</v>
+      </c>
+      <c r="N29" s="6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0" t="n">
+        <v>29</v>
+      </c>
+      <c r="B30" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C30" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D30" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="E30" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F30" s="5" t="n">
+        <v>7</v>
+      </c>
+      <c r="G30" s="5" t="n">
+        <v>12</v>
+      </c>
+      <c r="H30" s="5" t="s">
+        <v>579</v>
+      </c>
+      <c r="I30" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="J30" s="7" t="s">
+        <v>519</v>
+      </c>
+      <c r="K30" s="8"/>
+      <c r="L30" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="M30" s="5" t="s">
+        <v>985</v>
+      </c>
+      <c r="N30" s="6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="B31" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C31" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D31" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="E31" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F31" s="5" t="n">
+        <v>7</v>
+      </c>
+      <c r="G31" s="5" t="n">
+        <v>12</v>
+      </c>
+      <c r="H31" s="5" t="s">
+        <v>579</v>
+      </c>
+      <c r="I31" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="J31" s="7" t="s">
+        <v>519</v>
+      </c>
+      <c r="K31" s="8"/>
+      <c r="L31" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="M31" s="5" t="s">
+        <v>985</v>
+      </c>
+      <c r="N31" s="6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="0" t="n">
+        <v>31</v>
+      </c>
+      <c r="B32" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C32" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D32" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="E32" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F32" s="5" t="n">
+        <v>7</v>
+      </c>
+      <c r="G32" s="5" t="n">
+        <v>12</v>
+      </c>
+      <c r="H32" s="5" t="s">
+        <v>579</v>
+      </c>
+      <c r="I32" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="J32" s="7" t="s">
+        <v>519</v>
+      </c>
+      <c r="K32" s="8"/>
+      <c r="L32" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="M32" s="5" t="s">
+        <v>985</v>
+      </c>
+      <c r="N32" s="6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="0" t="n">
+        <v>32</v>
+      </c>
+      <c r="B33" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C33" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D33" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="E33" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="F33" s="5" t="n">
+        <v>7</v>
+      </c>
+      <c r="G33" s="5" t="n">
+        <v>12</v>
+      </c>
+      <c r="H33" s="5" t="s">
+        <v>579</v>
+      </c>
+      <c r="I33" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="J33" s="7" t="s">
+        <v>519</v>
+      </c>
+      <c r="K33" s="8"/>
+      <c r="L33" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="M33" s="5" t="s">
+        <v>985</v>
+      </c>
+      <c r="N33" s="6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="0" t="n">
+        <v>33</v>
+      </c>
+      <c r="B34" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C34" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D34" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="E34" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F34" s="5" t="n">
+        <v>25</v>
+      </c>
+      <c r="G34" s="5" t="n">
+        <v>27</v>
+      </c>
+      <c r="H34" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="I34" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="J34" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="K34" s="8"/>
+      <c r="L34" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="M34" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="N34" s="6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="0" t="n">
+        <v>34</v>
+      </c>
+      <c r="B35" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C35" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D35" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="E35" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F35" s="5" t="n">
+        <v>7</v>
+      </c>
+      <c r="G35" s="5" t="n">
+        <v>15</v>
+      </c>
+      <c r="H35" s="5" t="s">
+        <v>988</v>
+      </c>
+      <c r="I35" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="J35" s="7" t="s">
+        <v>519</v>
+      </c>
+      <c r="K35" s="8" t="s">
+        <v>989</v>
+      </c>
+      <c r="L35" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="M35" s="5" t="s">
+        <v>985</v>
+      </c>
+      <c r="N35" s="6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="0" t="n">
+        <v>35</v>
+      </c>
+      <c r="B36" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C36" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D36" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="E36" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F36" s="5" t="n">
+        <v>7</v>
+      </c>
+      <c r="G36" s="5" t="n">
+        <v>15</v>
+      </c>
+      <c r="H36" s="5" t="s">
+        <v>988</v>
+      </c>
+      <c r="I36" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="J36" s="7" t="s">
+        <v>519</v>
+      </c>
+      <c r="K36" s="8" t="s">
+        <v>989</v>
+      </c>
+      <c r="L36" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="M36" s="5" t="s">
+        <v>985</v>
+      </c>
+      <c r="N36" s="6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="0" t="n">
+        <v>36</v>
+      </c>
+      <c r="B37" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C37" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D37" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="E37" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F37" s="5" t="n">
+        <v>7</v>
+      </c>
+      <c r="G37" s="5" t="n">
+        <v>15</v>
+      </c>
+      <c r="H37" s="5" t="s">
+        <v>988</v>
+      </c>
+      <c r="I37" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="J37" s="7" t="s">
+        <v>974</v>
+      </c>
+      <c r="K37" s="8" t="s">
+        <v>990</v>
+      </c>
+      <c r="L37" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="M37" s="5" t="s">
+        <v>985</v>
+      </c>
+      <c r="N37" s="6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="0" t="n">
+        <v>37</v>
+      </c>
+      <c r="B38" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C38" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D38" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="E38" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="F38" s="5" t="n">
+        <v>7</v>
+      </c>
+      <c r="G38" s="5" t="n">
+        <v>15</v>
+      </c>
+      <c r="H38" s="5" t="s">
+        <v>988</v>
+      </c>
+      <c r="I38" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="J38" s="7" t="s">
+        <v>974</v>
+      </c>
+      <c r="K38" s="8" t="s">
+        <v>990</v>
+      </c>
+      <c r="L38" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="M38" s="5" t="s">
+        <v>985</v>
+      </c>
+      <c r="N38" s="6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="0" t="n">
+        <v>38</v>
+      </c>
+      <c r="B39" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C39" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D39" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="E39" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F39" s="5" t="n">
+        <v>25</v>
+      </c>
+      <c r="G39" s="5" t="n">
+        <v>27</v>
+      </c>
+      <c r="H39" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="I39" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="J39" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="K39" s="8"/>
+      <c r="L39" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="M39" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="N39" s="6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="0" t="n">
+        <v>39</v>
+      </c>
+      <c r="B40" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C40" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D40" s="3" t="n">
+        <v>5</v>
+      </c>
+      <c r="E40" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F40" s="5" t="n">
+        <v>7</v>
+      </c>
+      <c r="G40" s="5" t="n">
+        <v>15</v>
+      </c>
+      <c r="H40" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="I40" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="J40" s="7" t="s">
+        <v>974</v>
+      </c>
+      <c r="K40" s="8" t="s">
+        <v>990</v>
+      </c>
+      <c r="L40" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="M40" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="N40" s="6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="0" t="n">
+        <v>40</v>
+      </c>
+      <c r="B41" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C41" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D41" s="3" t="n">
+        <v>5</v>
+      </c>
+      <c r="E41" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F41" s="5" t="n">
+        <v>7</v>
+      </c>
+      <c r="G41" s="5" t="n">
+        <v>15</v>
+      </c>
+      <c r="H41" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="I41" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="J41" s="7" t="s">
+        <v>974</v>
+      </c>
+      <c r="K41" s="8" t="s">
+        <v>990</v>
+      </c>
+      <c r="L41" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="M41" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="N41" s="6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:N46"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="525" topLeftCell="A26" activePane="bottomLeft" state="split"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="A5" activeCellId="0" sqref="A4:A41"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.72959183673469"/>
+    <col collapsed="false" hidden="false" max="7" min="3" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="14.8673469387755"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="16.6683673469388"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="124.913265306122"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="6.11224489795918"/>
+    <col collapsed="false" hidden="false" max="1025" min="13" style="0" width="8.50510204081633"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="0" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="80.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C2" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D2" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" s="5" t="n">
+        <v>12</v>
+      </c>
+      <c r="G2" s="5" t="n">
+        <v>21</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>976</v>
+      </c>
+      <c r="I2" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="J2" s="7" t="s">
+        <v>963</v>
+      </c>
+      <c r="K2" s="8" t="s">
+        <v>964</v>
+      </c>
+      <c r="L2" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="M2" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="N2" s="6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" s="10" t="n">
+        <f aca="false">A2</f>
+        <v>1</v>
+      </c>
+      <c r="C3" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="D3" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="E3" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="F3" s="12" t="n">
+        <v>6</v>
+      </c>
+      <c r="G3" s="12" t="n">
+        <v>37</v>
+      </c>
+      <c r="H3" s="12" t="s">
+        <v>263</v>
+      </c>
+      <c r="I3" s="13" t="n">
+        <v>0</v>
+      </c>
+      <c r="J3" s="14" t="s">
+        <v>991</v>
+      </c>
+      <c r="K3" s="15" t="s">
+        <v>966</v>
+      </c>
+      <c r="L3" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="M3" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="N3" s="13" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" s="10" t="n">
+        <f aca="false">A2</f>
+        <v>1</v>
+      </c>
+      <c r="C4" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="D4" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="E4" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="F4" s="12" t="n">
+        <v>6</v>
+      </c>
+      <c r="G4" s="12" t="n">
+        <v>37</v>
+      </c>
+      <c r="H4" s="12" t="s">
+        <v>263</v>
+      </c>
+      <c r="I4" s="13" t="n">
+        <v>0</v>
+      </c>
+      <c r="J4" s="14" t="s">
+        <v>992</v>
+      </c>
+      <c r="K4" s="15" t="s">
+        <v>967</v>
+      </c>
+      <c r="L4" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="M4" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="N4" s="13" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" s="10" t="n">
+        <f aca="false">A2</f>
+        <v>1</v>
+      </c>
+      <c r="C5" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="D5" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="E5" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="F5" s="12" t="n">
+        <v>6</v>
+      </c>
+      <c r="G5" s="12" t="n">
+        <v>37</v>
+      </c>
+      <c r="H5" s="12" t="s">
+        <v>263</v>
+      </c>
+      <c r="I5" s="13" t="n">
+        <v>0</v>
+      </c>
+      <c r="J5" s="14" t="s">
+        <v>993</v>
+      </c>
+      <c r="K5" s="15" t="s">
+        <v>968</v>
+      </c>
+      <c r="L5" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="M5" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="N5" s="13" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="C6" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="D6" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="E6" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="F6" s="12" t="n">
+        <v>6</v>
+      </c>
+      <c r="G6" s="12" t="n">
+        <v>10</v>
+      </c>
+      <c r="H6" s="12" t="s">
+        <v>145</v>
+      </c>
+      <c r="I6" s="13" t="n">
+        <v>0</v>
+      </c>
+      <c r="J6" s="14" t="s">
+        <v>111</v>
+      </c>
+      <c r="K6" s="14" t="s">
+        <v>994</v>
+      </c>
+      <c r="L6" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="M6" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="N6" s="13" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="C7" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="D7" s="11" t="n">
+        <v>2</v>
+      </c>
+      <c r="E7" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="F7" s="12" t="n">
+        <v>6</v>
+      </c>
+      <c r="G7" s="12" t="n">
+        <v>37</v>
+      </c>
+      <c r="H7" s="12" t="s">
+        <v>124</v>
+      </c>
+      <c r="I7" s="13" t="n">
+        <v>0</v>
+      </c>
+      <c r="J7" s="14" t="s">
+        <v>995</v>
+      </c>
+      <c r="K7" s="14" t="s">
+        <v>996</v>
+      </c>
+      <c r="L7" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="M7" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="N7" s="13" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="C8" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="D8" s="11" t="n">
+        <v>2</v>
+      </c>
+      <c r="E8" s="10" t="s">
         <v>32</v>
       </c>
       <c r="F8" s="12" t="n">
@@ -37171,7 +39167,7 @@
         <v>0</v>
       </c>
       <c r="J8" s="14" t="s">
-        <v>974</v>
+        <v>130</v>
       </c>
       <c r="K8" s="14"/>
       <c r="L8" s="12" t="s">
@@ -37226,7 +39222,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="n">
         <v>9</v>
       </c>
@@ -37243,13 +39239,13 @@
         <v>20</v>
       </c>
       <c r="F10" s="5" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G10" s="5" t="n">
         <v>21</v>
       </c>
       <c r="H10" s="5" t="s">
-        <v>962</v>
+        <v>976</v>
       </c>
       <c r="I10" s="6" t="n">
         <v>0</v>
@@ -37268,7 +39264,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="n">
         <v>10</v>
       </c>
@@ -37285,13 +39281,13 @@
         <v>23</v>
       </c>
       <c r="F11" s="5" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G11" s="5" t="n">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="H11" s="5" t="s">
-        <v>124</v>
+        <v>148</v>
       </c>
       <c r="I11" s="6" t="n">
         <v>0</v>
@@ -37299,7 +39295,9 @@
       <c r="J11" s="7" t="s">
         <v>529</v>
       </c>
-      <c r="K11" s="8"/>
+      <c r="K11" s="8" t="s">
+        <v>997</v>
+      </c>
       <c r="L11" s="5" t="s">
         <v>81</v>
       </c>
@@ -37310,425 +39308,458 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="n">
         <v>11</v>
       </c>
-      <c r="B12" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="C12" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="D12" s="3" t="n">
+      <c r="B12" s="10" t="n">
+        <f aca="false">A11</f>
+        <v>10</v>
+      </c>
+      <c r="C12" s="10" t="n">
         <v>1</v>
       </c>
-      <c r="E12" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="F12" s="5" t="n">
-        <v>13</v>
-      </c>
-      <c r="G12" s="5" t="n">
-        <v>21</v>
-      </c>
-      <c r="H12" s="5" t="s">
-        <v>124</v>
-      </c>
-      <c r="I12" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="J12" s="7" t="s">
-        <v>529</v>
-      </c>
-      <c r="K12" s="8"/>
-      <c r="L12" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="M12" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="N12" s="6" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D12" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="E12" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="F12" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="G12" s="12" t="n">
+        <v>6</v>
+      </c>
+      <c r="H12" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="I12" s="13" t="n">
+        <v>0</v>
+      </c>
+      <c r="J12" s="14" t="s">
+        <v>998</v>
+      </c>
+      <c r="K12" s="15" t="s">
+        <v>999</v>
+      </c>
+      <c r="L12" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="M12" s="12" t="s">
+        <v>985</v>
+      </c>
+      <c r="N12" s="13" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="n">
         <v>12</v>
       </c>
-      <c r="B13" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="C13" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="D13" s="3" t="n">
+      <c r="B13" s="10" t="n">
+        <f aca="false">B12</f>
+        <v>10</v>
+      </c>
+      <c r="C13" s="10" t="n">
         <v>1</v>
       </c>
-      <c r="E13" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="F13" s="5" t="n">
-        <v>15</v>
-      </c>
-      <c r="G13" s="5" t="n">
-        <v>17</v>
-      </c>
-      <c r="H13" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="I13" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="J13" s="7" t="s">
-        <v>975</v>
-      </c>
-      <c r="K13" s="8"/>
-      <c r="L13" s="5" t="s">
+      <c r="D13" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="E13" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="F13" s="12" t="n">
+        <v>7</v>
+      </c>
+      <c r="G13" s="12" t="n">
+        <v>11</v>
+      </c>
+      <c r="H13" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="I13" s="13" t="n">
+        <v>0</v>
+      </c>
+      <c r="J13" s="14" t="s">
+        <v>1000</v>
+      </c>
+      <c r="K13" s="15" t="s">
+        <v>1001</v>
+      </c>
+      <c r="L13" s="12" t="s">
         <v>81</v>
       </c>
-      <c r="M13" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="N13" s="6" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M13" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="N13" s="13" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="n">
         <v>13</v>
       </c>
-      <c r="B14" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="C14" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="D14" s="3" t="n">
-        <v>2</v>
-      </c>
-      <c r="E14" s="3" t="s">
+      <c r="B14" s="10" t="n">
+        <f aca="false">B13</f>
+        <v>10</v>
+      </c>
+      <c r="C14" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="D14" s="10" t="n">
+        <v>2</v>
+      </c>
+      <c r="E14" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="F14" s="5" t="n">
-        <v>21</v>
-      </c>
-      <c r="G14" s="5" t="n">
-        <v>37</v>
-      </c>
-      <c r="H14" s="5"/>
-      <c r="I14" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="J14" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="K14" s="8"/>
-      <c r="L14" s="5" t="s">
-        <v>976</v>
-      </c>
-      <c r="M14" s="5" t="s">
+      <c r="F14" s="12" t="n">
+        <v>9</v>
+      </c>
+      <c r="G14" s="12" t="n">
+        <v>12</v>
+      </c>
+      <c r="H14" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="I14" s="13" t="n">
+        <v>0</v>
+      </c>
+      <c r="J14" s="14" t="s">
+        <v>1002</v>
+      </c>
+      <c r="K14" s="15" t="s">
+        <v>1003</v>
+      </c>
+      <c r="L14" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="M14" s="12" t="s">
         <v>71</v>
       </c>
-      <c r="N14" s="6" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="N14" s="13" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="n">
         <v>14</v>
       </c>
-      <c r="B15" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="C15" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="D15" s="3" t="n">
-        <v>2</v>
-      </c>
-      <c r="E15" s="3" t="s">
+      <c r="B15" s="10" t="n">
+        <f aca="false">B14</f>
+        <v>10</v>
+      </c>
+      <c r="C15" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="D15" s="10" t="n">
+        <v>2</v>
+      </c>
+      <c r="E15" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="F15" s="5" t="n">
-        <v>6</v>
-      </c>
-      <c r="G15" s="5" t="n">
+      <c r="F15" s="12" t="n">
+        <v>9</v>
+      </c>
+      <c r="G15" s="12" t="n">
         <v>12</v>
       </c>
-      <c r="H15" s="5" t="s">
-        <v>201</v>
-      </c>
-      <c r="I15" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="J15" s="7" t="s">
-        <v>519</v>
-      </c>
-      <c r="K15" s="7"/>
-      <c r="L15" s="5" t="s">
+      <c r="H15" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="I15" s="13" t="n">
+        <v>0</v>
+      </c>
+      <c r="J15" s="14" t="s">
+        <v>1002</v>
+      </c>
+      <c r="K15" s="15" t="s">
+        <v>1003</v>
+      </c>
+      <c r="L15" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="M15" s="5" t="s">
-        <v>977</v>
-      </c>
-      <c r="N15" s="6" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M15" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="N15" s="13" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="n">
         <v>15</v>
       </c>
-      <c r="B16" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="C16" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="D16" s="3" t="n">
-        <v>2</v>
-      </c>
-      <c r="E16" s="3" t="s">
+      <c r="B16" s="10" t="n">
+        <f aca="false">B15</f>
+        <v>10</v>
+      </c>
+      <c r="C16" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="D16" s="10" t="n">
+        <v>2</v>
+      </c>
+      <c r="E16" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="F16" s="5" t="n">
-        <v>6</v>
-      </c>
-      <c r="G16" s="5" t="n">
-        <v>12</v>
-      </c>
-      <c r="H16" s="5" t="s">
-        <v>201</v>
-      </c>
-      <c r="I16" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="J16" s="7" t="s">
-        <v>519</v>
-      </c>
-      <c r="K16" s="7"/>
-      <c r="L16" s="5" t="s">
+      <c r="F16" s="12" t="n">
+        <v>7</v>
+      </c>
+      <c r="G16" s="12" t="n">
+        <v>11</v>
+      </c>
+      <c r="H16" s="12" t="s">
+        <v>586</v>
+      </c>
+      <c r="I16" s="13" t="n">
+        <v>0</v>
+      </c>
+      <c r="J16" s="14" t="s">
+        <v>1004</v>
+      </c>
+      <c r="K16" s="15" t="s">
+        <v>1005</v>
+      </c>
+      <c r="L16" s="12" t="s">
         <v>81</v>
       </c>
-      <c r="M16" s="5" t="s">
-        <v>977</v>
-      </c>
-      <c r="N16" s="6" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M16" s="12" t="s">
+        <v>985</v>
+      </c>
+      <c r="N16" s="13" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="n">
         <v>16</v>
       </c>
-      <c r="B17" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="C17" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="D17" s="3" t="n">
-        <v>2</v>
-      </c>
-      <c r="E17" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="F17" s="5" t="n">
-        <v>6</v>
-      </c>
-      <c r="G17" s="5" t="n">
-        <v>12</v>
-      </c>
-      <c r="H17" s="5" t="s">
-        <v>201</v>
-      </c>
-      <c r="I17" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="J17" s="7" t="s">
-        <v>519</v>
-      </c>
-      <c r="K17" s="7"/>
-      <c r="L17" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="M17" s="5" t="s">
-        <v>977</v>
-      </c>
-      <c r="N17" s="6" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B17" s="10" t="n">
+        <f aca="false">B16</f>
+        <v>10</v>
+      </c>
+      <c r="C17" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="D17" s="10" t="n">
+        <v>3</v>
+      </c>
+      <c r="E17" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="F17" s="12" t="n">
+        <v>15</v>
+      </c>
+      <c r="G17" s="12" t="n">
+        <f aca="false">40-F11</f>
+        <v>28</v>
+      </c>
+      <c r="H17" s="12" t="s">
+        <v>586</v>
+      </c>
+      <c r="I17" s="13" t="n">
+        <v>0</v>
+      </c>
+      <c r="J17" s="14" t="s">
+        <v>1006</v>
+      </c>
+      <c r="K17" s="15" t="s">
+        <v>1007</v>
+      </c>
+      <c r="L17" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="M17" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="N17" s="13" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="n">
         <v>17</v>
       </c>
-      <c r="B18" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="C18" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="D18" s="3" t="n">
-        <v>2</v>
-      </c>
-      <c r="E18" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="F18" s="5" t="n">
-        <v>20</v>
-      </c>
-      <c r="G18" s="5" t="n">
-        <v>21</v>
-      </c>
-      <c r="H18" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="I18" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="J18" s="7" t="s">
-        <v>90</v>
-      </c>
-      <c r="K18" s="8"/>
-      <c r="L18" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="M18" s="5" t="s">
-        <v>977</v>
-      </c>
-      <c r="N18" s="6" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B18" s="10" t="n">
+        <f aca="false">B17</f>
+        <v>10</v>
+      </c>
+      <c r="C18" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="D18" s="10" t="n">
+        <v>4</v>
+      </c>
+      <c r="E18" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="F18" s="12" t="n">
+        <v>12</v>
+      </c>
+      <c r="G18" s="12" t="n">
+        <v>14</v>
+      </c>
+      <c r="H18" s="12" t="s">
+        <v>586</v>
+      </c>
+      <c r="I18" s="13" t="n">
+        <v>0</v>
+      </c>
+      <c r="J18" s="14" t="s">
+        <v>1008</v>
+      </c>
+      <c r="K18" s="15" t="s">
+        <v>1009</v>
+      </c>
+      <c r="L18" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="M18" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="N18" s="13" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="n">
         <v>18</v>
       </c>
-      <c r="B19" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="C19" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="D19" s="3" t="n">
-        <v>3</v>
-      </c>
-      <c r="E19" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="F19" s="5" t="n">
+      <c r="B19" s="10" t="n">
+        <f aca="false">B18</f>
+        <v>10</v>
+      </c>
+      <c r="C19" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="D19" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="E19" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="F19" s="12" t="n">
         <v>7</v>
       </c>
-      <c r="G19" s="5" t="n">
-        <v>12</v>
-      </c>
-      <c r="H19" s="5" t="s">
-        <v>579</v>
-      </c>
-      <c r="I19" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="J19" s="7" t="s">
-        <v>519</v>
-      </c>
-      <c r="K19" s="8"/>
-      <c r="L19" s="5" t="s">
+      <c r="G19" s="12" t="n">
+        <v>11</v>
+      </c>
+      <c r="H19" s="14" t="s">
+        <v>1010</v>
+      </c>
+      <c r="I19" s="13" t="n">
+        <v>0</v>
+      </c>
+      <c r="J19" s="14" t="s">
+        <v>111</v>
+      </c>
+      <c r="K19" s="15" t="s">
+        <v>1011</v>
+      </c>
+      <c r="L19" s="12" t="s">
         <v>81</v>
       </c>
-      <c r="M19" s="5" t="s">
-        <v>977</v>
-      </c>
-      <c r="N19" s="6" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M19" s="12" t="s">
+        <v>985</v>
+      </c>
+      <c r="N19" s="13" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="n">
         <v>19</v>
       </c>
-      <c r="B20" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="C20" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="D20" s="3" t="n">
-        <v>3</v>
-      </c>
-      <c r="E20" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="F20" s="5" t="n">
-        <v>7</v>
-      </c>
-      <c r="G20" s="5" t="n">
+      <c r="B20" s="10" t="n">
+        <f aca="false">B19</f>
+        <v>10</v>
+      </c>
+      <c r="C20" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="D20" s="10" t="n">
+        <v>2</v>
+      </c>
+      <c r="E20" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="F20" s="12" t="n">
         <v>12</v>
       </c>
-      <c r="H20" s="5" t="s">
-        <v>579</v>
-      </c>
-      <c r="I20" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="J20" s="7" t="s">
-        <v>519</v>
-      </c>
-      <c r="K20" s="8"/>
-      <c r="L20" s="5" t="s">
+      <c r="G20" s="12" t="n">
+        <v>15</v>
+      </c>
+      <c r="H20" s="14" t="s">
+        <v>1010</v>
+      </c>
+      <c r="I20" s="13" t="n">
+        <v>0</v>
+      </c>
+      <c r="J20" s="14" t="s">
+        <v>1012</v>
+      </c>
+      <c r="K20" s="15" t="s">
+        <v>1011</v>
+      </c>
+      <c r="L20" s="12" t="s">
         <v>81</v>
       </c>
-      <c r="M20" s="5" t="s">
-        <v>977</v>
-      </c>
-      <c r="N20" s="6" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M20" s="12" t="s">
+        <v>985</v>
+      </c>
+      <c r="N20" s="13" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="n">
         <v>20</v>
       </c>
-      <c r="B21" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="C21" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="D21" s="3" t="n">
-        <v>3</v>
-      </c>
-      <c r="E21" s="3" t="s">
+      <c r="B21" s="10" t="n">
+        <f aca="false">B20</f>
+        <v>10</v>
+      </c>
+      <c r="C21" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="D21" s="10" t="n">
+        <v>4</v>
+      </c>
+      <c r="E21" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="F21" s="5" t="n">
-        <v>7</v>
-      </c>
-      <c r="G21" s="5" t="n">
+      <c r="F21" s="12" t="n">
         <v>12</v>
       </c>
-      <c r="H21" s="5" t="s">
-        <v>579</v>
-      </c>
-      <c r="I21" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="J21" s="7" t="s">
-        <v>519</v>
-      </c>
-      <c r="K21" s="8"/>
-      <c r="L21" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="M21" s="5" t="s">
-        <v>977</v>
-      </c>
-      <c r="N21" s="6" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G21" s="12" t="n">
+        <v>13</v>
+      </c>
+      <c r="H21" s="12" t="s">
+        <v>586</v>
+      </c>
+      <c r="I21" s="13" t="n">
+        <v>0</v>
+      </c>
+      <c r="J21" s="14" t="s">
+        <v>1008</v>
+      </c>
+      <c r="K21" s="15" t="s">
+        <v>1009</v>
+      </c>
+      <c r="L21" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="M21" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="N21" s="13" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="n">
         <v>21</v>
       </c>
@@ -37739,286 +39770,1094 @@
         <v>0</v>
       </c>
       <c r="D22" s="3" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E22" s="3" t="s">
         <v>45</v>
       </c>
       <c r="F22" s="5" t="n">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="G22" s="5" t="n">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="H22" s="5" t="s">
-        <v>579</v>
+        <v>332</v>
       </c>
       <c r="I22" s="6" t="n">
         <v>0</v>
       </c>
       <c r="J22" s="7" t="s">
-        <v>519</v>
-      </c>
-      <c r="K22" s="8"/>
+        <v>594</v>
+      </c>
+      <c r="K22" s="8" t="s">
+        <v>1013</v>
+      </c>
       <c r="L22" s="5" t="s">
         <v>81</v>
       </c>
       <c r="M22" s="5" t="s">
-        <v>977</v>
+        <v>31</v>
       </c>
       <c r="N22" s="6" t="n">
         <v>0</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="n">
         <v>22</v>
       </c>
-      <c r="B23" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="C23" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="D23" s="3" t="n">
-        <v>3</v>
-      </c>
-      <c r="E23" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="F23" s="5" t="n">
-        <v>25</v>
-      </c>
-      <c r="G23" s="5" t="n">
+      <c r="B23" s="10" t="n">
+        <f aca="false">A22</f>
+        <v>21</v>
+      </c>
+      <c r="C23" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="D23" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="E23" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="H23" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="I23" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="J23" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="K23" s="8"/>
-      <c r="L23" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="M23" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="N23" s="6" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F23" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="G23" s="12" t="n">
+        <v>6</v>
+      </c>
+      <c r="H23" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="I23" s="13" t="n">
+        <v>0</v>
+      </c>
+      <c r="J23" s="14" t="s">
+        <v>998</v>
+      </c>
+      <c r="K23" s="15" t="s">
+        <v>999</v>
+      </c>
+      <c r="L23" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="M23" s="12" t="s">
+        <v>985</v>
+      </c>
+      <c r="N23" s="13" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="n">
         <v>23</v>
       </c>
-      <c r="B24" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="C24" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="D24" s="3" t="n">
-        <v>4</v>
-      </c>
-      <c r="E24" s="3" t="s">
+      <c r="B24" s="10" t="n">
+        <f aca="false">B23</f>
+        <v>21</v>
+      </c>
+      <c r="C24" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="D24" s="10" t="n">
+        <v>2</v>
+      </c>
+      <c r="E24" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="F24" s="5" t="n">
-        <v>7</v>
-      </c>
-      <c r="G24" s="5" t="n">
+      <c r="F24" s="12" t="n">
+        <v>9</v>
+      </c>
+      <c r="G24" s="12" t="n">
         <v>12</v>
       </c>
-      <c r="H24" s="5" t="s">
-        <v>978</v>
-      </c>
-      <c r="I24" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="J24" s="7" t="s">
-        <v>519</v>
-      </c>
-      <c r="K24" s="8"/>
-      <c r="L24" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="M24" s="5" t="s">
-        <v>977</v>
-      </c>
-      <c r="N24" s="6" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H24" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="I24" s="13" t="n">
+        <v>0</v>
+      </c>
+      <c r="J24" s="14" t="s">
+        <v>1002</v>
+      </c>
+      <c r="K24" s="15" t="s">
+        <v>1003</v>
+      </c>
+      <c r="L24" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="M24" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="N24" s="13" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="n">
         <v>24</v>
       </c>
-      <c r="B25" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="C25" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="D25" s="3" t="n">
-        <v>4</v>
-      </c>
-      <c r="E25" s="3" t="s">
+      <c r="B25" s="10" t="n">
+        <f aca="false">B24</f>
+        <v>21</v>
+      </c>
+      <c r="C25" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="D25" s="10" t="n">
+        <v>2</v>
+      </c>
+      <c r="E25" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="F25" s="5" t="n">
-        <v>7</v>
-      </c>
-      <c r="G25" s="5" t="n">
+      <c r="F25" s="12" t="n">
+        <v>9</v>
+      </c>
+      <c r="G25" s="12" t="n">
         <v>12</v>
       </c>
-      <c r="H25" s="5" t="s">
-        <v>978</v>
-      </c>
-      <c r="I25" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="J25" s="7" t="s">
-        <v>519</v>
-      </c>
-      <c r="K25" s="8"/>
-      <c r="L25" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="M25" s="5" t="s">
-        <v>977</v>
-      </c>
-      <c r="N25" s="6" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H25" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="I25" s="13" t="n">
+        <v>0</v>
+      </c>
+      <c r="J25" s="14" t="s">
+        <v>1002</v>
+      </c>
+      <c r="K25" s="15" t="s">
+        <v>1003</v>
+      </c>
+      <c r="L25" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="M25" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="N25" s="13" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="n">
         <v>25</v>
       </c>
-      <c r="B26" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="C26" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="D26" s="3" t="n">
-        <v>4</v>
-      </c>
-      <c r="E26" s="3" t="s">
+      <c r="B26" s="10" t="n">
+        <f aca="false">B25</f>
+        <v>21</v>
+      </c>
+      <c r="C26" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="D26" s="10" t="n">
+        <v>2</v>
+      </c>
+      <c r="E26" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="F26" s="5" t="n">
-        <v>7</v>
-      </c>
-      <c r="G26" s="5" t="n">
+      <c r="F26" s="12" t="n">
+        <v>9</v>
+      </c>
+      <c r="G26" s="12" t="n">
         <v>12</v>
       </c>
-      <c r="H26" s="5" t="s">
-        <v>978</v>
-      </c>
-      <c r="I26" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="J26" s="7" t="s">
-        <v>519</v>
-      </c>
-      <c r="K26" s="8"/>
-      <c r="L26" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="M26" s="5" t="s">
-        <v>977</v>
-      </c>
-      <c r="N26" s="6" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H26" s="14" t="s">
+        <v>148</v>
+      </c>
+      <c r="I26" s="13" t="n">
+        <v>0</v>
+      </c>
+      <c r="J26" s="14" t="s">
+        <v>1002</v>
+      </c>
+      <c r="K26" s="15" t="s">
+        <v>1014</v>
+      </c>
+      <c r="L26" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="M26" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="N26" s="13" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="n">
         <v>26</v>
       </c>
-      <c r="B27" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="C27" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="D27" s="3" t="n">
-        <v>4</v>
-      </c>
-      <c r="E27" s="3" t="s">
+      <c r="B27" s="10" t="n">
+        <f aca="false">A22</f>
+        <v>21</v>
+      </c>
+      <c r="C27" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="D27" s="10" t="n">
+        <v>2</v>
+      </c>
+      <c r="E27" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="F27" s="5" t="n">
+      <c r="F27" s="12" t="n">
         <v>7</v>
       </c>
-      <c r="G27" s="5" t="n">
-        <v>12</v>
-      </c>
-      <c r="H27" s="5" t="s">
-        <v>978</v>
-      </c>
-      <c r="I27" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="J27" s="7" t="s">
-        <v>519</v>
-      </c>
-      <c r="K27" s="8"/>
-      <c r="L27" s="5" t="s">
+      <c r="G27" s="12" t="n">
+        <v>11</v>
+      </c>
+      <c r="H27" s="12" t="s">
+        <v>598</v>
+      </c>
+      <c r="I27" s="13" t="n">
+        <v>0</v>
+      </c>
+      <c r="J27" s="14" t="s">
+        <v>1015</v>
+      </c>
+      <c r="K27" s="15" t="s">
+        <v>1016</v>
+      </c>
+      <c r="L27" s="12" t="s">
         <v>81</v>
       </c>
-      <c r="M27" s="5" t="s">
-        <v>977</v>
-      </c>
-      <c r="N27" s="6" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M27" s="12" t="s">
+        <v>985</v>
+      </c>
+      <c r="N27" s="13" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="n">
         <v>27</v>
       </c>
-      <c r="B28" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="C28" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="D28" s="3" t="n">
+      <c r="B28" s="10" t="n">
+        <f aca="false">B27</f>
+        <v>21</v>
+      </c>
+      <c r="C28" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="D28" s="10" t="n">
+        <v>3</v>
+      </c>
+      <c r="E28" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="F28" s="12" t="n">
+        <v>15</v>
+      </c>
+      <c r="G28" s="12" t="n">
+        <f aca="false">40-F22</f>
+        <v>28</v>
+      </c>
+      <c r="H28" s="12" t="s">
+        <v>598</v>
+      </c>
+      <c r="I28" s="13" t="n">
+        <v>0</v>
+      </c>
+      <c r="J28" s="14" t="s">
+        <v>1017</v>
+      </c>
+      <c r="K28" s="15" t="s">
+        <v>1018</v>
+      </c>
+      <c r="L28" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="M28" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="N28" s="13" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="B29" s="10" t="n">
+        <f aca="false">B28</f>
+        <v>21</v>
+      </c>
+      <c r="C29" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="D29" s="10" t="n">
         <v>4</v>
       </c>
-      <c r="E28" s="3" t="s">
+      <c r="E29" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="F29" s="12" t="n">
+        <v>12</v>
+      </c>
+      <c r="G29" s="12" t="n">
+        <v>14</v>
+      </c>
+      <c r="H29" s="12" t="s">
+        <v>598</v>
+      </c>
+      <c r="I29" s="13" t="n">
+        <v>0</v>
+      </c>
+      <c r="J29" s="14" t="s">
+        <v>1012</v>
+      </c>
+      <c r="K29" s="15" t="s">
+        <v>1009</v>
+      </c>
+      <c r="L29" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="M29" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="N29" s="13" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0" t="n">
+        <v>29</v>
+      </c>
+      <c r="B30" s="10" t="n">
+        <f aca="false">B29</f>
+        <v>21</v>
+      </c>
+      <c r="C30" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="D30" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="E30" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="F28" s="5" t="n">
-        <v>25</v>
-      </c>
-      <c r="G28" s="5" t="n">
+      <c r="F30" s="12" t="n">
+        <v>7</v>
+      </c>
+      <c r="G30" s="12" t="n">
+        <v>11</v>
+      </c>
+      <c r="H30" s="14" t="s">
+        <v>1019</v>
+      </c>
+      <c r="I30" s="13" t="n">
+        <v>0</v>
+      </c>
+      <c r="J30" s="14" t="s">
+        <v>1012</v>
+      </c>
+      <c r="K30" s="15" t="s">
+        <v>1020</v>
+      </c>
+      <c r="L30" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="M30" s="12" t="s">
+        <v>985</v>
+      </c>
+      <c r="N30" s="13" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="B31" s="10" t="n">
+        <f aca="false">B29</f>
+        <v>21</v>
+      </c>
+      <c r="C31" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="D31" s="10" t="n">
+        <v>2</v>
+      </c>
+      <c r="E31" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="F31" s="12" t="n">
+        <v>12</v>
+      </c>
+      <c r="G31" s="12" t="n">
+        <v>15</v>
+      </c>
+      <c r="H31" s="14" t="s">
+        <v>1019</v>
+      </c>
+      <c r="I31" s="13" t="n">
+        <v>0</v>
+      </c>
+      <c r="J31" s="14" t="s">
+        <v>1012</v>
+      </c>
+      <c r="K31" s="15" t="s">
+        <v>1020</v>
+      </c>
+      <c r="L31" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="M31" s="12" t="s">
+        <v>985</v>
+      </c>
+      <c r="N31" s="13" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="0" t="n">
+        <v>31</v>
+      </c>
+      <c r="B32" s="10" t="n">
+        <f aca="false">B29</f>
+        <v>21</v>
+      </c>
+      <c r="C32" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="D32" s="10" t="n">
+        <v>4</v>
+      </c>
+      <c r="E32" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="F32" s="12" t="n">
+        <v>12</v>
+      </c>
+      <c r="G32" s="12" t="n">
+        <v>13</v>
+      </c>
+      <c r="H32" s="12" t="s">
+        <v>598</v>
+      </c>
+      <c r="I32" s="13" t="n">
+        <v>0</v>
+      </c>
+      <c r="J32" s="14" t="s">
+        <v>1012</v>
+      </c>
+      <c r="K32" s="15" t="s">
+        <v>1009</v>
+      </c>
+      <c r="L32" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="M32" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="N32" s="13" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="0" t="n">
+        <v>32</v>
+      </c>
+      <c r="B33" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C33" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D33" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="E33" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F33" s="5" t="n">
+        <v>16</v>
+      </c>
+      <c r="G33" s="5" t="n">
+        <v>18</v>
+      </c>
+      <c r="H33" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="I33" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="J33" s="7" t="s">
+        <v>983</v>
+      </c>
+      <c r="K33" s="8" t="s">
+        <v>1021</v>
+      </c>
+      <c r="L33" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="M33" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="N33" s="6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="0" t="n">
+        <v>33</v>
+      </c>
+      <c r="B34" s="10" t="n">
+        <f aca="false">A33</f>
+        <v>32</v>
+      </c>
+      <c r="C34" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="D34" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="E34" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="H28" s="5" t="s">
+      <c r="F34" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="G34" s="12" t="n">
+        <v>7</v>
+      </c>
+      <c r="H34" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="I28" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="J28" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="K28" s="8"/>
-      <c r="L28" s="5" t="s">
+      <c r="I34" s="13" t="n">
+        <v>0</v>
+      </c>
+      <c r="J34" s="14" t="s">
+        <v>810</v>
+      </c>
+      <c r="K34" s="15" t="s">
+        <v>1022</v>
+      </c>
+      <c r="L34" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="M34" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="N34" s="13" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="0" t="n">
+        <v>34</v>
+      </c>
+      <c r="B35" s="10" t="n">
+        <f aca="false">B34</f>
+        <v>32</v>
+      </c>
+      <c r="C35" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="D35" s="10" t="n">
+        <v>2</v>
+      </c>
+      <c r="E35" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="F35" s="12" t="n">
+        <v>8</v>
+      </c>
+      <c r="G35" s="12" t="n">
+        <v>9</v>
+      </c>
+      <c r="H35" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="I35" s="13" t="n">
+        <v>0</v>
+      </c>
+      <c r="J35" s="14" t="s">
+        <v>130</v>
+      </c>
+      <c r="K35" s="15" t="s">
+        <v>1023</v>
+      </c>
+      <c r="L35" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="M35" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="N35" s="13" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="0" t="n">
+        <v>35</v>
+      </c>
+      <c r="B36" s="10" t="n">
+        <f aca="false">B35</f>
+        <v>32</v>
+      </c>
+      <c r="C36" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="D36" s="10" t="n">
+        <v>3</v>
+      </c>
+      <c r="E36" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="F36" s="12" t="n">
+        <v>10</v>
+      </c>
+      <c r="G36" s="12" t="n">
+        <v>13</v>
+      </c>
+      <c r="H36" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="I36" s="13" t="n">
+        <v>0</v>
+      </c>
+      <c r="J36" s="14" t="s">
+        <v>1024</v>
+      </c>
+      <c r="K36" s="15" t="s">
+        <v>1025</v>
+      </c>
+      <c r="L36" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="M36" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="N36" s="13" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="0" t="n">
+        <v>36</v>
+      </c>
+      <c r="B37" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C37" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D37" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="E37" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F37" s="5" t="n">
+        <v>19</v>
+      </c>
+      <c r="G37" s="5" t="n">
+        <v>37</v>
+      </c>
+      <c r="H37" s="5"/>
+      <c r="I37" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="J37" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="K37" s="8"/>
+      <c r="L37" s="5" t="s">
+        <v>1026</v>
+      </c>
+      <c r="M37" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="N37" s="6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="0" t="n">
+        <v>37</v>
+      </c>
+      <c r="B38" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C38" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D38" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="E38" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F38" s="5" t="n">
+        <v>6</v>
+      </c>
+      <c r="G38" s="5" t="n">
+        <v>12</v>
+      </c>
+      <c r="H38" s="5" t="s">
+        <v>201</v>
+      </c>
+      <c r="I38" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="J38" s="7" t="s">
+        <v>519</v>
+      </c>
+      <c r="K38" s="7"/>
+      <c r="L38" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="M38" s="5" t="s">
+        <v>985</v>
+      </c>
+      <c r="N38" s="6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="0" t="n">
+        <v>38</v>
+      </c>
+      <c r="B39" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C39" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D39" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="E39" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F39" s="5" t="n">
+        <v>6</v>
+      </c>
+      <c r="G39" s="5" t="n">
+        <v>12</v>
+      </c>
+      <c r="H39" s="5" t="s">
+        <v>201</v>
+      </c>
+      <c r="I39" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="J39" s="7" t="s">
+        <v>519</v>
+      </c>
+      <c r="K39" s="7"/>
+      <c r="L39" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="M28" s="5" t="s">
+      <c r="M39" s="5" t="s">
+        <v>985</v>
+      </c>
+      <c r="N39" s="6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="0" t="n">
+        <v>39</v>
+      </c>
+      <c r="B40" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C40" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D40" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="E40" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="F40" s="5" t="n">
+        <v>6</v>
+      </c>
+      <c r="G40" s="5" t="n">
+        <v>12</v>
+      </c>
+      <c r="H40" s="5" t="s">
+        <v>201</v>
+      </c>
+      <c r="I40" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="J40" s="7" t="s">
+        <v>519</v>
+      </c>
+      <c r="K40" s="7"/>
+      <c r="L40" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="M40" s="5" t="s">
+        <v>985</v>
+      </c>
+      <c r="N40" s="6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="0" t="n">
+        <v>40</v>
+      </c>
+      <c r="B41" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C41" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D41" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="E41" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F41" s="5" t="n">
+        <v>19</v>
+      </c>
+      <c r="G41" s="5" t="n">
+        <v>23</v>
+      </c>
+      <c r="H41" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="I41" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="J41" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="K41" s="8"/>
+      <c r="L41" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="M41" s="5" t="s">
+        <v>985</v>
+      </c>
+      <c r="N41" s="6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="0" t="n">
+        <v>41</v>
+      </c>
+      <c r="B42" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C42" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D42" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="E42" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F42" s="5" t="n">
+        <v>7</v>
+      </c>
+      <c r="G42" s="5" t="n">
+        <v>12</v>
+      </c>
+      <c r="H42" s="5" t="s">
+        <v>1027</v>
+      </c>
+      <c r="I42" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="J42" s="7" t="s">
+        <v>519</v>
+      </c>
+      <c r="K42" s="8" t="s">
+        <v>1028</v>
+      </c>
+      <c r="L42" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="M42" s="5" t="s">
+        <v>985</v>
+      </c>
+      <c r="N42" s="6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="0" t="n">
+        <v>42</v>
+      </c>
+      <c r="B43" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C43" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D43" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="E43" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F43" s="5" t="n">
+        <v>7</v>
+      </c>
+      <c r="G43" s="5" t="n">
+        <v>12</v>
+      </c>
+      <c r="H43" s="5" t="s">
+        <v>1029</v>
+      </c>
+      <c r="I43" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="J43" s="7" t="s">
+        <v>519</v>
+      </c>
+      <c r="K43" s="8" t="s">
+        <v>1028</v>
+      </c>
+      <c r="L43" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="M43" s="5" t="s">
+        <v>985</v>
+      </c>
+      <c r="N43" s="6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="0" t="n">
+        <v>43</v>
+      </c>
+      <c r="B44" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C44" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D44" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="E44" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F44" s="5" t="n">
+        <v>7</v>
+      </c>
+      <c r="G44" s="5" t="n">
+        <v>12</v>
+      </c>
+      <c r="H44" s="5" t="s">
+        <v>1030</v>
+      </c>
+      <c r="I44" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="J44" s="7" t="s">
+        <v>519</v>
+      </c>
+      <c r="K44" s="8" t="s">
+        <v>1028</v>
+      </c>
+      <c r="L44" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="M44" s="5" t="s">
+        <v>985</v>
+      </c>
+      <c r="N44" s="6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="0" t="n">
+        <v>44</v>
+      </c>
+      <c r="B45" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C45" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D45" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="E45" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="F45" s="5" t="n">
+        <v>7</v>
+      </c>
+      <c r="G45" s="5" t="n">
+        <v>12</v>
+      </c>
+      <c r="H45" s="5" t="s">
+        <v>1031</v>
+      </c>
+      <c r="I45" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="J45" s="7" t="s">
+        <v>519</v>
+      </c>
+      <c r="K45" s="8" t="s">
+        <v>1028</v>
+      </c>
+      <c r="L45" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="M45" s="5" t="s">
+        <v>985</v>
+      </c>
+      <c r="N45" s="6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="0" t="n">
+        <v>45</v>
+      </c>
+      <c r="B46" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C46" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D46" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="E46" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F46" s="5" t="n">
+        <v>24</v>
+      </c>
+      <c r="G46" s="5" t="n">
+        <v>27</v>
+      </c>
+      <c r="H46" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="I46" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="J46" s="7" t="s">
+        <v>1032</v>
+      </c>
+      <c r="K46" s="8" t="s">
+        <v>1033</v>
+      </c>
+      <c r="L46" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="M46" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="N28" s="6" t="n">
+      <c r="N46" s="6" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Uproszczony SYSTEM ZIELONY dla początkujących (zarys). Znakomity starter zarówno dla STREFY jak i WJ. System jest zmodyfikowaną wersją SAYC i Systemu Zielonego W. Izdebskiego. Znacznie jednak łatwiejszy i poza otwarciami na wys. 2-ch, spójny zarówno ze STREFĄ i WJ. System-kręgosłup, który z czasem obrośnie ciałem czyli kompatybilnymi konwencjami i gadżetami.
</commit_message>
<xml_diff>
--- a/bridgeIn.xlsx
+++ b/bridgeIn.xlsx
@@ -5,20 +5,21 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="544" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="544" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="W-J 2017" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="poInterwencji" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="SA_z_piatek" sheetId="3" state="visible" r:id="rId4"/>
     <sheet name="NaturalnaKM" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="NaturalnaZielony" sheetId="5" state="visible" r:id="rId6"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4813" uniqueCount="1046">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5187" uniqueCount="1087">
   <si>
     <t>bidId</t>
   </si>
@@ -3983,6 +3984,129 @@
   </si>
   <si>
     <t>Niezależnie co ma partner idzie 3 BA – zatrzymania we wszystkich kolorach, dobry układ</t>
+  </si>
+  <si>
+    <t>wieloznaczny trefl</t>
+  </si>
+  <si>
+    <t>1) 11 + PC 5+ trefli , 2) 12-14 równy rozkład (słabe bez atu), 18-20 równy rozkład (silne bez atu) – zawsze przynajmniej 3 trefle</t>
+  </si>
+  <si>
+    <t>6-10 PC, wyklucza 4 kara, 4 kiery, 4 piki i 5 trefli; bilansowe</t>
+  </si>
+  <si>
+    <t>'5+ trefl</t>
+  </si>
+  <si>
+    <t>poparcie treflowe (bilansowe)</t>
+  </si>
+  <si>
+    <t>'5+ karo</t>
+  </si>
+  <si>
+    <t>kolor karowy</t>
+  </si>
+  <si>
+    <t>własne otwarcie karowe</t>
+  </si>
+  <si>
+    <t>'5+ kier</t>
+  </si>
+  <si>
+    <t>kolor kierowy</t>
+  </si>
+  <si>
+    <t>własne otwarcie kierowe</t>
+  </si>
+  <si>
+    <t>'5+ pik</t>
+  </si>
+  <si>
+    <t>kolor pikowy</t>
+  </si>
+  <si>
+    <t>własne otwarcie pikowe</t>
+  </si>
+  <si>
+    <t>z bilansu</t>
+  </si>
+  <si>
+    <t>końcówka z bilansu</t>
+  </si>
+  <si>
+    <t>1) 11-18(20) PC 5+ kar, 2) układy na czwórkach: 4441 lub 4432 (min 3 kara)</t>
+  </si>
+  <si>
+    <t>Układ zrównoważony (4-3-3-3) : brak singla, tylko jeden  dubel, nie liczą się punkty układowe.  Możliwa młodsza piątka lub bardzo słaba starsza</t>
+  </si>
+  <si>
+    <t>słabe trefl</t>
+  </si>
+  <si>
+    <t>5+ kart w kolorze, mało punktów do 8PC (ewentualnie mniej punktów ale niemożnośc spasowania- np. niezrównoważony układ)</t>
+  </si>
+  <si>
+    <t>słabe karo</t>
+  </si>
+  <si>
+    <t>słabe kier</t>
+  </si>
+  <si>
+    <t>słabe pik</t>
+  </si>
+  <si>
+    <t>silny trefl</t>
+  </si>
+  <si>
+    <t>5+ kart w kolorze, od (9) 10 PC – nielimitowane  mocny kolor do gry</t>
+  </si>
+  <si>
+    <t>silny karo</t>
+  </si>
+  <si>
+    <t>silny kier</t>
+  </si>
+  <si>
+    <t>silny pik</t>
+  </si>
+  <si>
+    <t>(5)6+ C</t>
+  </si>
+  <si>
+    <t>SILNE</t>
+  </si>
+  <si>
+    <t>Przy mniejszej sile DOBRY KOLOR i maksimum 5 lew przegrywających</t>
+  </si>
+  <si>
+    <t>(5)6+ D</t>
+  </si>
+  <si>
+    <t>(5)6+ H</t>
+  </si>
+  <si>
+    <t>(5)6+ S</t>
+  </si>
+  <si>
+    <t> – możliwa jest młodsza piątka albo bardzo słaba starsza</t>
+  </si>
+  <si>
+    <t>Niezależnie co ma partner idzie 3 BA – zatrzymania we wszystkich kolorach, dobry układ – możliwa jest młodsza piątka albo bardzo słaba starsza</t>
+  </si>
+  <si>
+    <t>8+ C</t>
+  </si>
+  <si>
+    <t>blokujące na dobrym 8+ kartowym kolorze – punkty w tym kolorze, brak 2 asów</t>
+  </si>
+  <si>
+    <t>8+ D</t>
+  </si>
+  <si>
+    <t>8+ H</t>
+  </si>
+  <si>
+    <t>8+ S</t>
   </si>
 </sst>
 </file>
@@ -4218,7 +4342,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="91">
+  <cellXfs count="92">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -4583,6 +4707,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
@@ -4662,10 +4790,10 @@
   </sheetPr>
   <dimension ref="A1:N711"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A634" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A634" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="525" topLeftCell="A430" activePane="bottomLeft" state="split"/>
       <selection pane="topLeft" activeCell="A634" activeCellId="0" sqref="A634"/>
-      <selection pane="bottomLeft" activeCell="K444" activeCellId="0" sqref="K444"/>
+      <selection pane="bottomLeft" activeCell="K444" activeCellId="1" sqref="H43:H46 K444"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -36767,7 +36895,7 @@
   <dimension ref="A1:N5"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I2" activeCellId="0" sqref="I2"/>
+      <selection pane="topLeft" activeCell="I2" activeCellId="1" sqref="H43:H46 I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -37017,7 +37145,7 @@
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="525" topLeftCell="A16" activePane="bottomLeft" state="split"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+      <selection pane="bottomLeft" activeCell="A4" activeCellId="1" sqref="H43:H46 A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -38847,7 +38975,7 @@
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="525" topLeftCell="A26" activePane="bottomLeft" state="split"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
+      <selection pane="bottomLeft" activeCell="A5" activeCellId="1" sqref="H43:H46 A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -40906,4 +41034,2755 @@
     <oddFooter/>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:N61"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H43" activeCellId="0" sqref="H43:H46"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.72959183673469"/>
+    <col collapsed="false" hidden="false" max="7" min="3" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="14.8673469387755"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="16.6683673469388"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="124.913265306122"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="6.11224489795918"/>
+    <col collapsed="false" hidden="false" max="1025" min="13" style="0" width="8.50510204081633"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="0" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="80.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C2" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D2" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" s="5" t="n">
+        <v>11</v>
+      </c>
+      <c r="G2" s="5" t="n">
+        <v>20</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>989</v>
+      </c>
+      <c r="I2" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="J2" s="7" t="s">
+        <v>1046</v>
+      </c>
+      <c r="K2" s="91" t="s">
+        <v>1047</v>
+      </c>
+      <c r="L2" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="M2" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="N2" s="6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" s="10" t="n">
+        <f aca="false">A2</f>
+        <v>1</v>
+      </c>
+      <c r="C3" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="D3" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="E3" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="F3" s="12" t="n">
+        <v>7</v>
+      </c>
+      <c r="G3" s="12" t="n">
+        <v>37</v>
+      </c>
+      <c r="H3" s="12" t="s">
+        <v>263</v>
+      </c>
+      <c r="I3" s="13" t="n">
+        <v>0</v>
+      </c>
+      <c r="J3" s="14" t="s">
+        <v>1004</v>
+      </c>
+      <c r="K3" s="15" t="s">
+        <v>979</v>
+      </c>
+      <c r="L3" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="M3" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="N3" s="13" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" s="10" t="n">
+        <f aca="false">A2</f>
+        <v>1</v>
+      </c>
+      <c r="C4" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="D4" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="E4" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="F4" s="12" t="n">
+        <v>7</v>
+      </c>
+      <c r="G4" s="12" t="n">
+        <v>37</v>
+      </c>
+      <c r="H4" s="12" t="s">
+        <v>263</v>
+      </c>
+      <c r="I4" s="13" t="n">
+        <v>0</v>
+      </c>
+      <c r="J4" s="14" t="s">
+        <v>1005</v>
+      </c>
+      <c r="K4" s="15" t="s">
+        <v>980</v>
+      </c>
+      <c r="L4" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="M4" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="N4" s="13" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" s="10" t="n">
+        <f aca="false">A2</f>
+        <v>1</v>
+      </c>
+      <c r="C5" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="D5" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="E5" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="F5" s="12" t="n">
+        <v>7</v>
+      </c>
+      <c r="G5" s="12" t="n">
+        <v>37</v>
+      </c>
+      <c r="H5" s="12" t="s">
+        <v>263</v>
+      </c>
+      <c r="I5" s="13" t="n">
+        <v>0</v>
+      </c>
+      <c r="J5" s="14" t="s">
+        <v>1006</v>
+      </c>
+      <c r="K5" s="15" t="s">
+        <v>981</v>
+      </c>
+      <c r="L5" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="M5" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="N5" s="13" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="C6" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="D6" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="E6" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="F6" s="12" t="n">
+        <v>7</v>
+      </c>
+      <c r="G6" s="12" t="n">
+        <v>10</v>
+      </c>
+      <c r="H6" s="12" t="s">
+        <v>145</v>
+      </c>
+      <c r="I6" s="13" t="n">
+        <v>0</v>
+      </c>
+      <c r="J6" s="14" t="s">
+        <v>111</v>
+      </c>
+      <c r="K6" s="14" t="s">
+        <v>1048</v>
+      </c>
+      <c r="L6" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="M6" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="N6" s="13" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="C7" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="D7" s="11" t="n">
+        <v>2</v>
+      </c>
+      <c r="E7" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="F7" s="12" t="n">
+        <v>7</v>
+      </c>
+      <c r="G7" s="12" t="n">
+        <v>10</v>
+      </c>
+      <c r="H7" s="12" t="s">
+        <v>1049</v>
+      </c>
+      <c r="I7" s="13" t="n">
+        <v>0</v>
+      </c>
+      <c r="J7" s="14" t="s">
+        <v>1008</v>
+      </c>
+      <c r="K7" s="14" t="s">
+        <v>1050</v>
+      </c>
+      <c r="L7" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="M7" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="N7" s="13" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="C8" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="D8" s="11" t="n">
+        <v>2</v>
+      </c>
+      <c r="E8" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="F8" s="12" t="n">
+        <v>13</v>
+      </c>
+      <c r="G8" s="12" t="n">
+        <v>37</v>
+      </c>
+      <c r="H8" s="12" t="s">
+        <v>1051</v>
+      </c>
+      <c r="I8" s="13" t="n">
+        <v>0</v>
+      </c>
+      <c r="J8" s="14" t="s">
+        <v>1052</v>
+      </c>
+      <c r="K8" s="14" t="s">
+        <v>1053</v>
+      </c>
+      <c r="L8" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="M8" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="N8" s="13" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="C9" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="D9" s="11" t="n">
+        <v>2</v>
+      </c>
+      <c r="E9" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="F9" s="12" t="n">
+        <v>13</v>
+      </c>
+      <c r="G9" s="12" t="n">
+        <v>37</v>
+      </c>
+      <c r="H9" s="12" t="s">
+        <v>1054</v>
+      </c>
+      <c r="I9" s="13" t="n">
+        <v>0</v>
+      </c>
+      <c r="J9" s="14" t="s">
+        <v>1055</v>
+      </c>
+      <c r="K9" s="14" t="s">
+        <v>1056</v>
+      </c>
+      <c r="L9" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="M9" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="N9" s="13" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="C10" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="D10" s="11" t="n">
+        <v>2</v>
+      </c>
+      <c r="E10" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="F10" s="12" t="n">
+        <v>13</v>
+      </c>
+      <c r="G10" s="12" t="n">
+        <v>37</v>
+      </c>
+      <c r="H10" s="12" t="s">
+        <v>1057</v>
+      </c>
+      <c r="I10" s="13" t="n">
+        <v>0</v>
+      </c>
+      <c r="J10" s="14" t="s">
+        <v>1058</v>
+      </c>
+      <c r="K10" s="14" t="s">
+        <v>1059</v>
+      </c>
+      <c r="L10" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="M10" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="N10" s="13" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="C11" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="D11" s="11" t="n">
+        <v>2</v>
+      </c>
+      <c r="E11" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="F11" s="12" t="n">
+        <v>10</v>
+      </c>
+      <c r="G11" s="12" t="n">
+        <v>14</v>
+      </c>
+      <c r="H11" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="I11" s="13" t="n">
+        <v>0</v>
+      </c>
+      <c r="J11" s="14" t="s">
+        <v>130</v>
+      </c>
+      <c r="K11" s="14" t="s">
+        <v>1060</v>
+      </c>
+      <c r="L11" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="M11" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="N11" s="13" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="B12" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="C12" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="D12" s="11" t="n">
+        <v>3</v>
+      </c>
+      <c r="E12" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="F12" s="12" t="n">
+        <v>15</v>
+      </c>
+      <c r="G12" s="12" t="n">
+        <v>17</v>
+      </c>
+      <c r="H12" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="I12" s="13" t="n">
+        <v>0</v>
+      </c>
+      <c r="J12" s="14" t="s">
+        <v>1036</v>
+      </c>
+      <c r="K12" s="14" t="s">
+        <v>1061</v>
+      </c>
+      <c r="L12" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="M12" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="N12" s="13" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="B13" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C13" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D13" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F13" s="5" t="n">
+        <v>11</v>
+      </c>
+      <c r="G13" s="5" t="n">
+        <v>18</v>
+      </c>
+      <c r="H13" s="5" t="s">
+        <v>989</v>
+      </c>
+      <c r="I13" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="J13" s="7" t="s">
+        <v>976</v>
+      </c>
+      <c r="K13" s="8" t="s">
+        <v>1062</v>
+      </c>
+      <c r="L13" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="M13" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="N13" s="6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="B14" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C14" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D14" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F14" s="5" t="n">
+        <v>11</v>
+      </c>
+      <c r="G14" s="5" t="n">
+        <v>18</v>
+      </c>
+      <c r="H14" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="I14" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="J14" s="7" t="s">
+        <v>529</v>
+      </c>
+      <c r="K14" s="8" t="s">
+        <v>1010</v>
+      </c>
+      <c r="L14" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="M14" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="N14" s="6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="B15" s="10" t="n">
+        <f aca="false">A14</f>
+        <v>13</v>
+      </c>
+      <c r="C15" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="D15" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="E15" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="F15" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="G15" s="12" t="n">
+        <v>6</v>
+      </c>
+      <c r="H15" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="I15" s="13" t="n">
+        <v>0</v>
+      </c>
+      <c r="J15" s="14" t="s">
+        <v>1011</v>
+      </c>
+      <c r="K15" s="15" t="s">
+        <v>1012</v>
+      </c>
+      <c r="L15" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="M15" s="12" t="s">
+        <v>998</v>
+      </c>
+      <c r="N15" s="13" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="B16" s="10" t="n">
+        <f aca="false">B15</f>
+        <v>13</v>
+      </c>
+      <c r="C16" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="D16" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="E16" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="F16" s="12" t="n">
+        <v>7</v>
+      </c>
+      <c r="G16" s="12" t="n">
+        <v>11</v>
+      </c>
+      <c r="H16" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="I16" s="13" t="n">
+        <v>0</v>
+      </c>
+      <c r="J16" s="14" t="s">
+        <v>1013</v>
+      </c>
+      <c r="K16" s="15" t="s">
+        <v>1014</v>
+      </c>
+      <c r="L16" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="M16" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="N16" s="13" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="B17" s="10" t="n">
+        <f aca="false">B16</f>
+        <v>13</v>
+      </c>
+      <c r="C17" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="D17" s="10" t="n">
+        <v>2</v>
+      </c>
+      <c r="E17" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="F17" s="12" t="n">
+        <v>9</v>
+      </c>
+      <c r="G17" s="12" t="n">
+        <v>12</v>
+      </c>
+      <c r="H17" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="I17" s="13" t="n">
+        <v>0</v>
+      </c>
+      <c r="J17" s="14" t="s">
+        <v>983</v>
+      </c>
+      <c r="K17" s="15" t="s">
+        <v>1015</v>
+      </c>
+      <c r="L17" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="M17" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="N17" s="13" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="B18" s="10" t="n">
+        <f aca="false">B17</f>
+        <v>13</v>
+      </c>
+      <c r="C18" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="D18" s="10" t="n">
+        <v>2</v>
+      </c>
+      <c r="E18" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="F18" s="12" t="n">
+        <v>9</v>
+      </c>
+      <c r="G18" s="12" t="n">
+        <v>12</v>
+      </c>
+      <c r="H18" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="I18" s="13" t="n">
+        <v>0</v>
+      </c>
+      <c r="J18" s="14" t="s">
+        <v>983</v>
+      </c>
+      <c r="K18" s="15" t="s">
+        <v>1015</v>
+      </c>
+      <c r="L18" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="M18" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="N18" s="13" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="B19" s="10" t="n">
+        <f aca="false">B18</f>
+        <v>13</v>
+      </c>
+      <c r="C19" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="D19" s="10" t="n">
+        <v>2</v>
+      </c>
+      <c r="E19" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="F19" s="12" t="n">
+        <v>7</v>
+      </c>
+      <c r="G19" s="12" t="n">
+        <v>11</v>
+      </c>
+      <c r="H19" s="12" t="s">
+        <v>597</v>
+      </c>
+      <c r="I19" s="13" t="n">
+        <v>0</v>
+      </c>
+      <c r="J19" s="14" t="s">
+        <v>1016</v>
+      </c>
+      <c r="K19" s="15" t="s">
+        <v>1017</v>
+      </c>
+      <c r="L19" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="M19" s="12" t="s">
+        <v>998</v>
+      </c>
+      <c r="N19" s="13" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="n">
+        <v>19</v>
+      </c>
+      <c r="B20" s="10" t="n">
+        <f aca="false">B19</f>
+        <v>13</v>
+      </c>
+      <c r="C20" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="D20" s="10" t="n">
+        <v>3</v>
+      </c>
+      <c r="E20" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="F20" s="12" t="n">
+        <v>15</v>
+      </c>
+      <c r="G20" s="12" t="n">
+        <f aca="false">40-F14</f>
+        <v>29</v>
+      </c>
+      <c r="H20" s="12" t="s">
+        <v>597</v>
+      </c>
+      <c r="I20" s="13" t="n">
+        <v>0</v>
+      </c>
+      <c r="J20" s="14" t="s">
+        <v>1018</v>
+      </c>
+      <c r="K20" s="15" t="s">
+        <v>1019</v>
+      </c>
+      <c r="L20" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="M20" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="N20" s="13" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="B21" s="10" t="n">
+        <f aca="false">B20</f>
+        <v>13</v>
+      </c>
+      <c r="C21" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="D21" s="10" t="n">
+        <v>4</v>
+      </c>
+      <c r="E21" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="F21" s="12" t="n">
+        <v>12</v>
+      </c>
+      <c r="G21" s="12" t="n">
+        <v>14</v>
+      </c>
+      <c r="H21" s="12" t="s">
+        <v>597</v>
+      </c>
+      <c r="I21" s="13" t="n">
+        <v>0</v>
+      </c>
+      <c r="J21" s="14" t="s">
+        <v>1020</v>
+      </c>
+      <c r="K21" s="15" t="s">
+        <v>1021</v>
+      </c>
+      <c r="L21" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="M21" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="N21" s="13" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="B22" s="10" t="n">
+        <f aca="false">B21</f>
+        <v>13</v>
+      </c>
+      <c r="C22" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="D22" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="E22" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="F22" s="12" t="n">
+        <v>7</v>
+      </c>
+      <c r="G22" s="12" t="n">
+        <v>11</v>
+      </c>
+      <c r="H22" s="14" t="s">
+        <v>1022</v>
+      </c>
+      <c r="I22" s="13" t="n">
+        <v>0</v>
+      </c>
+      <c r="J22" s="14" t="s">
+        <v>111</v>
+      </c>
+      <c r="K22" s="15" t="s">
+        <v>1023</v>
+      </c>
+      <c r="L22" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="M22" s="12" t="s">
+        <v>998</v>
+      </c>
+      <c r="N22" s="13" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="n">
+        <v>22</v>
+      </c>
+      <c r="B23" s="10" t="n">
+        <f aca="false">B22</f>
+        <v>13</v>
+      </c>
+      <c r="C23" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="D23" s="10" t="n">
+        <v>2</v>
+      </c>
+      <c r="E23" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="F23" s="12" t="n">
+        <v>12</v>
+      </c>
+      <c r="G23" s="12" t="n">
+        <v>15</v>
+      </c>
+      <c r="H23" s="14" t="s">
+        <v>1022</v>
+      </c>
+      <c r="I23" s="13" t="n">
+        <v>0</v>
+      </c>
+      <c r="J23" s="14" t="s">
+        <v>1024</v>
+      </c>
+      <c r="K23" s="15" t="s">
+        <v>1023</v>
+      </c>
+      <c r="L23" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="M23" s="12" t="s">
+        <v>998</v>
+      </c>
+      <c r="N23" s="13" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="n">
+        <v>23</v>
+      </c>
+      <c r="B24" s="10" t="n">
+        <f aca="false">B23</f>
+        <v>13</v>
+      </c>
+      <c r="C24" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="D24" s="10" t="n">
+        <v>4</v>
+      </c>
+      <c r="E24" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="F24" s="12" t="n">
+        <v>12</v>
+      </c>
+      <c r="G24" s="12" t="n">
+        <v>13</v>
+      </c>
+      <c r="H24" s="12" t="s">
+        <v>597</v>
+      </c>
+      <c r="I24" s="13" t="n">
+        <v>0</v>
+      </c>
+      <c r="J24" s="14" t="s">
+        <v>1020</v>
+      </c>
+      <c r="K24" s="15" t="s">
+        <v>1021</v>
+      </c>
+      <c r="L24" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="M24" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="N24" s="13" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="B25" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C25" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D25" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="F25" s="5" t="n">
+        <v>12</v>
+      </c>
+      <c r="G25" s="5" t="n">
+        <v>18</v>
+      </c>
+      <c r="H25" s="5" t="s">
+        <v>332</v>
+      </c>
+      <c r="I25" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="J25" s="7" t="s">
+        <v>605</v>
+      </c>
+      <c r="K25" s="8" t="s">
+        <v>1025</v>
+      </c>
+      <c r="L25" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="M25" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="N25" s="6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="B26" s="10" t="n">
+        <f aca="false">A25</f>
+        <v>24</v>
+      </c>
+      <c r="C26" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="D26" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="E26" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="F26" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="G26" s="12" t="n">
+        <v>6</v>
+      </c>
+      <c r="H26" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="I26" s="13" t="n">
+        <v>0</v>
+      </c>
+      <c r="J26" s="14" t="s">
+        <v>1011</v>
+      </c>
+      <c r="K26" s="15" t="s">
+        <v>1012</v>
+      </c>
+      <c r="L26" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="M26" s="12" t="s">
+        <v>998</v>
+      </c>
+      <c r="N26" s="13" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="n">
+        <v>26</v>
+      </c>
+      <c r="B27" s="10" t="n">
+        <f aca="false">B26</f>
+        <v>24</v>
+      </c>
+      <c r="C27" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="D27" s="10" t="n">
+        <v>2</v>
+      </c>
+      <c r="E27" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="F27" s="12" t="n">
+        <v>9</v>
+      </c>
+      <c r="G27" s="12" t="n">
+        <v>12</v>
+      </c>
+      <c r="H27" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="I27" s="13" t="n">
+        <v>0</v>
+      </c>
+      <c r="J27" s="14" t="s">
+        <v>983</v>
+      </c>
+      <c r="K27" s="15" t="s">
+        <v>1015</v>
+      </c>
+      <c r="L27" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="M27" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="N27" s="13" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="n">
+        <v>27</v>
+      </c>
+      <c r="B28" s="10" t="n">
+        <f aca="false">B27</f>
+        <v>24</v>
+      </c>
+      <c r="C28" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="D28" s="10" t="n">
+        <v>2</v>
+      </c>
+      <c r="E28" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="F28" s="12" t="n">
+        <v>9</v>
+      </c>
+      <c r="G28" s="12" t="n">
+        <v>12</v>
+      </c>
+      <c r="H28" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="I28" s="13" t="n">
+        <v>0</v>
+      </c>
+      <c r="J28" s="14" t="s">
+        <v>983</v>
+      </c>
+      <c r="K28" s="15" t="s">
+        <v>1015</v>
+      </c>
+      <c r="L28" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="M28" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="N28" s="13" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="B29" s="10" t="n">
+        <f aca="false">B28</f>
+        <v>24</v>
+      </c>
+      <c r="C29" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="D29" s="10" t="n">
+        <v>2</v>
+      </c>
+      <c r="E29" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="F29" s="12" t="n">
+        <v>9</v>
+      </c>
+      <c r="G29" s="12" t="n">
+        <v>12</v>
+      </c>
+      <c r="H29" s="14" t="s">
+        <v>148</v>
+      </c>
+      <c r="I29" s="13" t="n">
+        <v>0</v>
+      </c>
+      <c r="J29" s="14" t="s">
+        <v>983</v>
+      </c>
+      <c r="K29" s="15" t="s">
+        <v>1026</v>
+      </c>
+      <c r="L29" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="M29" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="N29" s="13" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0" t="n">
+        <v>29</v>
+      </c>
+      <c r="B30" s="10" t="n">
+        <f aca="false">A25</f>
+        <v>24</v>
+      </c>
+      <c r="C30" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="D30" s="10" t="n">
+        <v>2</v>
+      </c>
+      <c r="E30" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="F30" s="12" t="n">
+        <v>7</v>
+      </c>
+      <c r="G30" s="12" t="n">
+        <v>11</v>
+      </c>
+      <c r="H30" s="12" t="s">
+        <v>612</v>
+      </c>
+      <c r="I30" s="13" t="n">
+        <v>0</v>
+      </c>
+      <c r="J30" s="14" t="s">
+        <v>1027</v>
+      </c>
+      <c r="K30" s="15" t="s">
+        <v>1028</v>
+      </c>
+      <c r="L30" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="M30" s="12" t="s">
+        <v>998</v>
+      </c>
+      <c r="N30" s="13" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="B31" s="10" t="n">
+        <f aca="false">B30</f>
+        <v>24</v>
+      </c>
+      <c r="C31" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="D31" s="10" t="n">
+        <v>3</v>
+      </c>
+      <c r="E31" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="F31" s="12" t="n">
+        <v>15</v>
+      </c>
+      <c r="G31" s="12" t="n">
+        <f aca="false">40-F25</f>
+        <v>28</v>
+      </c>
+      <c r="H31" s="12" t="s">
+        <v>612</v>
+      </c>
+      <c r="I31" s="13" t="n">
+        <v>0</v>
+      </c>
+      <c r="J31" s="14" t="s">
+        <v>1029</v>
+      </c>
+      <c r="K31" s="15" t="s">
+        <v>1030</v>
+      </c>
+      <c r="L31" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="M31" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="N31" s="13" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="0" t="n">
+        <v>31</v>
+      </c>
+      <c r="B32" s="10" t="n">
+        <f aca="false">B31</f>
+        <v>24</v>
+      </c>
+      <c r="C32" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="D32" s="10" t="n">
+        <v>4</v>
+      </c>
+      <c r="E32" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="F32" s="12" t="n">
+        <v>12</v>
+      </c>
+      <c r="G32" s="12" t="n">
+        <v>14</v>
+      </c>
+      <c r="H32" s="12" t="s">
+        <v>612</v>
+      </c>
+      <c r="I32" s="13" t="n">
+        <v>0</v>
+      </c>
+      <c r="J32" s="14" t="s">
+        <v>1024</v>
+      </c>
+      <c r="K32" s="15" t="s">
+        <v>1021</v>
+      </c>
+      <c r="L32" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="M32" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="N32" s="13" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="0" t="n">
+        <v>32</v>
+      </c>
+      <c r="B33" s="10" t="n">
+        <f aca="false">B32</f>
+        <v>24</v>
+      </c>
+      <c r="C33" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="D33" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="E33" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="F33" s="12" t="n">
+        <v>7</v>
+      </c>
+      <c r="G33" s="12" t="n">
+        <v>11</v>
+      </c>
+      <c r="H33" s="14" t="s">
+        <v>1031</v>
+      </c>
+      <c r="I33" s="13" t="n">
+        <v>0</v>
+      </c>
+      <c r="J33" s="14" t="s">
+        <v>1024</v>
+      </c>
+      <c r="K33" s="15" t="s">
+        <v>1032</v>
+      </c>
+      <c r="L33" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="M33" s="12" t="s">
+        <v>998</v>
+      </c>
+      <c r="N33" s="13" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="0" t="n">
+        <v>33</v>
+      </c>
+      <c r="B34" s="10" t="n">
+        <f aca="false">B32</f>
+        <v>24</v>
+      </c>
+      <c r="C34" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="D34" s="10" t="n">
+        <v>2</v>
+      </c>
+      <c r="E34" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="F34" s="12" t="n">
+        <v>12</v>
+      </c>
+      <c r="G34" s="12" t="n">
+        <v>15</v>
+      </c>
+      <c r="H34" s="14" t="s">
+        <v>1031</v>
+      </c>
+      <c r="I34" s="13" t="n">
+        <v>0</v>
+      </c>
+      <c r="J34" s="14" t="s">
+        <v>1024</v>
+      </c>
+      <c r="K34" s="15" t="s">
+        <v>1032</v>
+      </c>
+      <c r="L34" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="M34" s="12" t="s">
+        <v>998</v>
+      </c>
+      <c r="N34" s="13" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="0" t="n">
+        <v>34</v>
+      </c>
+      <c r="B35" s="10" t="n">
+        <f aca="false">B32</f>
+        <v>24</v>
+      </c>
+      <c r="C35" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="D35" s="10" t="n">
+        <v>4</v>
+      </c>
+      <c r="E35" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="F35" s="12" t="n">
+        <v>12</v>
+      </c>
+      <c r="G35" s="12" t="n">
+        <v>13</v>
+      </c>
+      <c r="H35" s="12" t="s">
+        <v>612</v>
+      </c>
+      <c r="I35" s="13" t="n">
+        <v>0</v>
+      </c>
+      <c r="J35" s="14" t="s">
+        <v>1024</v>
+      </c>
+      <c r="K35" s="15" t="s">
+        <v>1021</v>
+      </c>
+      <c r="L35" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="M35" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="N35" s="13" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="0" t="n">
+        <v>35</v>
+      </c>
+      <c r="B36" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C36" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D36" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="E36" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F36" s="5" t="n">
+        <v>15</v>
+      </c>
+      <c r="G36" s="5" t="n">
+        <v>17</v>
+      </c>
+      <c r="H36" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="I36" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="J36" s="7" t="s">
+        <v>996</v>
+      </c>
+      <c r="K36" s="8" t="s">
+        <v>1063</v>
+      </c>
+      <c r="L36" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="M36" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="N36" s="6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="0" t="n">
+        <v>36</v>
+      </c>
+      <c r="B37" s="10" t="n">
+        <f aca="false">A36</f>
+        <v>35</v>
+      </c>
+      <c r="C37" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="D37" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="E37" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="F37" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="G37" s="12" t="n">
+        <v>7</v>
+      </c>
+      <c r="H37" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="I37" s="13" t="n">
+        <v>0</v>
+      </c>
+      <c r="J37" s="14" t="s">
+        <v>823</v>
+      </c>
+      <c r="K37" s="15" t="s">
+        <v>1034</v>
+      </c>
+      <c r="L37" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="M37" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="N37" s="13" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="0" t="n">
+        <v>37</v>
+      </c>
+      <c r="B38" s="10" t="n">
+        <v>35</v>
+      </c>
+      <c r="C38" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="D38" s="10" t="n">
+        <v>2</v>
+      </c>
+      <c r="E38" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="F38" s="12" t="n">
+        <v>5</v>
+      </c>
+      <c r="G38" s="12" t="n">
+        <v>9</v>
+      </c>
+      <c r="H38" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="I38" s="13" t="n">
+        <v>0</v>
+      </c>
+      <c r="J38" s="12" t="s">
+        <v>1064</v>
+      </c>
+      <c r="K38" s="15" t="s">
+        <v>1065</v>
+      </c>
+      <c r="L38" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="M38" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="N38" s="13" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="0" t="n">
+        <v>38</v>
+      </c>
+      <c r="B39" s="10" t="n">
+        <v>35</v>
+      </c>
+      <c r="C39" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="D39" s="10" t="n">
+        <v>2</v>
+      </c>
+      <c r="E39" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="F39" s="12" t="n">
+        <v>5</v>
+      </c>
+      <c r="G39" s="12" t="n">
+        <v>9</v>
+      </c>
+      <c r="H39" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="I39" s="13" t="n">
+        <v>0</v>
+      </c>
+      <c r="J39" s="12" t="s">
+        <v>1066</v>
+      </c>
+      <c r="K39" s="15" t="s">
+        <v>1065</v>
+      </c>
+      <c r="L39" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="M39" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="N39" s="13" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="0" t="n">
+        <v>39</v>
+      </c>
+      <c r="B40" s="10" t="n">
+        <v>35</v>
+      </c>
+      <c r="C40" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="D40" s="10" t="n">
+        <v>2</v>
+      </c>
+      <c r="E40" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="F40" s="12" t="n">
+        <v>5</v>
+      </c>
+      <c r="G40" s="12" t="n">
+        <v>9</v>
+      </c>
+      <c r="H40" s="14" t="s">
+        <v>148</v>
+      </c>
+      <c r="I40" s="13" t="n">
+        <v>0</v>
+      </c>
+      <c r="J40" s="12" t="s">
+        <v>1067</v>
+      </c>
+      <c r="K40" s="15" t="s">
+        <v>1065</v>
+      </c>
+      <c r="L40" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="M40" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="N40" s="13" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="0" t="n">
+        <v>40</v>
+      </c>
+      <c r="B41" s="10" t="n">
+        <v>35</v>
+      </c>
+      <c r="C41" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="D41" s="10" t="n">
+        <v>2</v>
+      </c>
+      <c r="E41" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="F41" s="12" t="n">
+        <v>5</v>
+      </c>
+      <c r="G41" s="12" t="n">
+        <v>9</v>
+      </c>
+      <c r="H41" s="12" t="s">
+        <v>332</v>
+      </c>
+      <c r="I41" s="13" t="n">
+        <v>0</v>
+      </c>
+      <c r="J41" s="12" t="s">
+        <v>1068</v>
+      </c>
+      <c r="K41" s="15" t="s">
+        <v>1065</v>
+      </c>
+      <c r="L41" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="M41" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="N41" s="13" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="0" t="n">
+        <v>41</v>
+      </c>
+      <c r="B42" s="10" t="n">
+        <f aca="false">B37</f>
+        <v>35</v>
+      </c>
+      <c r="C42" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="D42" s="10" t="n">
+        <v>2</v>
+      </c>
+      <c r="E42" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="F42" s="12" t="n">
+        <v>8</v>
+      </c>
+      <c r="G42" s="12" t="n">
+        <v>9</v>
+      </c>
+      <c r="H42" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="I42" s="13" t="n">
+        <v>0</v>
+      </c>
+      <c r="J42" s="14" t="s">
+        <v>130</v>
+      </c>
+      <c r="K42" s="15" t="s">
+        <v>1035</v>
+      </c>
+      <c r="L42" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="M42" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="N42" s="13" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="0" t="n">
+        <v>42</v>
+      </c>
+      <c r="B43" s="10" t="n">
+        <v>35</v>
+      </c>
+      <c r="C43" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="D43" s="10" t="n">
+        <v>3</v>
+      </c>
+      <c r="E43" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="F43" s="12" t="n">
+        <v>10</v>
+      </c>
+      <c r="G43" s="12" t="n">
+        <f aca="false">40-F36</f>
+        <v>25</v>
+      </c>
+      <c r="H43" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="I43" s="13" t="n">
+        <v>0</v>
+      </c>
+      <c r="J43" s="12" t="s">
+        <v>1069</v>
+      </c>
+      <c r="K43" s="15" t="s">
+        <v>1070</v>
+      </c>
+      <c r="L43" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="M43" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="N43" s="13" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="0" t="n">
+        <v>43</v>
+      </c>
+      <c r="B44" s="10" t="n">
+        <v>35</v>
+      </c>
+      <c r="C44" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="D44" s="10" t="n">
+        <v>3</v>
+      </c>
+      <c r="E44" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="F44" s="12" t="n">
+        <v>10</v>
+      </c>
+      <c r="G44" s="12" t="n">
+        <f aca="false">G43</f>
+        <v>25</v>
+      </c>
+      <c r="H44" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="I44" s="13" t="n">
+        <v>0</v>
+      </c>
+      <c r="J44" s="12" t="s">
+        <v>1071</v>
+      </c>
+      <c r="K44" s="15" t="s">
+        <v>1070</v>
+      </c>
+      <c r="L44" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="M44" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="N44" s="13" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="0" t="n">
+        <v>44</v>
+      </c>
+      <c r="B45" s="10" t="n">
+        <v>35</v>
+      </c>
+      <c r="C45" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="D45" s="10" t="n">
+        <v>3</v>
+      </c>
+      <c r="E45" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="F45" s="12" t="n">
+        <v>10</v>
+      </c>
+      <c r="G45" s="12" t="n">
+        <f aca="false">G44</f>
+        <v>25</v>
+      </c>
+      <c r="H45" s="14" t="s">
+        <v>148</v>
+      </c>
+      <c r="I45" s="13" t="n">
+        <v>0</v>
+      </c>
+      <c r="J45" s="12" t="s">
+        <v>1072</v>
+      </c>
+      <c r="K45" s="15" t="s">
+        <v>1070</v>
+      </c>
+      <c r="L45" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="M45" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="N45" s="13" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="0" t="n">
+        <v>45</v>
+      </c>
+      <c r="B46" s="10" t="n">
+        <v>35</v>
+      </c>
+      <c r="C46" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="D46" s="10" t="n">
+        <v>3</v>
+      </c>
+      <c r="E46" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="F46" s="12" t="n">
+        <v>10</v>
+      </c>
+      <c r="G46" s="12" t="n">
+        <f aca="false">G45</f>
+        <v>25</v>
+      </c>
+      <c r="H46" s="12" t="s">
+        <v>332</v>
+      </c>
+      <c r="I46" s="13" t="n">
+        <v>0</v>
+      </c>
+      <c r="J46" s="12" t="s">
+        <v>1073</v>
+      </c>
+      <c r="K46" s="15" t="s">
+        <v>1070</v>
+      </c>
+      <c r="L46" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="M46" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="N46" s="13" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="0" t="n">
+        <v>46</v>
+      </c>
+      <c r="B47" s="10" t="n">
+        <f aca="false">B42</f>
+        <v>35</v>
+      </c>
+      <c r="C47" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="D47" s="10" t="n">
+        <v>3</v>
+      </c>
+      <c r="E47" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="F47" s="12" t="n">
+        <v>10</v>
+      </c>
+      <c r="G47" s="12" t="n">
+        <v>13</v>
+      </c>
+      <c r="H47" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="I47" s="13" t="n">
+        <v>0</v>
+      </c>
+      <c r="J47" s="14" t="s">
+        <v>1036</v>
+      </c>
+      <c r="K47" s="15" t="s">
+        <v>1037</v>
+      </c>
+      <c r="L47" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="M47" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="N47" s="13" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="0" t="n">
+        <v>47</v>
+      </c>
+      <c r="B48" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C48" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D48" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="E48" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F48" s="5" t="n">
+        <v>18</v>
+      </c>
+      <c r="G48" s="5" t="n">
+        <v>37</v>
+      </c>
+      <c r="H48" s="5" t="s">
+        <v>1074</v>
+      </c>
+      <c r="I48" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="J48" s="7" t="s">
+        <v>1075</v>
+      </c>
+      <c r="K48" s="8" t="s">
+        <v>1076</v>
+      </c>
+      <c r="L48" s="5" t="s">
+        <v>1038</v>
+      </c>
+      <c r="M48" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="N48" s="6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="0" t="n">
+        <v>48</v>
+      </c>
+      <c r="B49" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C49" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D49" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="E49" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F49" s="5" t="n">
+        <v>18</v>
+      </c>
+      <c r="G49" s="5" t="n">
+        <v>37</v>
+      </c>
+      <c r="H49" s="5" t="s">
+        <v>1077</v>
+      </c>
+      <c r="I49" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="J49" s="7" t="s">
+        <v>1075</v>
+      </c>
+      <c r="K49" s="8" t="s">
+        <v>1076</v>
+      </c>
+      <c r="L49" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="M49" s="5" t="s">
+        <v>998</v>
+      </c>
+      <c r="N49" s="6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="0" t="n">
+        <v>49</v>
+      </c>
+      <c r="B50" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C50" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D50" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="E50" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F50" s="5" t="n">
+        <v>18</v>
+      </c>
+      <c r="G50" s="5" t="n">
+        <v>37</v>
+      </c>
+      <c r="H50" s="5" t="s">
+        <v>1078</v>
+      </c>
+      <c r="I50" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="J50" s="7" t="s">
+        <v>1075</v>
+      </c>
+      <c r="K50" s="8" t="s">
+        <v>1076</v>
+      </c>
+      <c r="L50" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="M50" s="5" t="s">
+        <v>998</v>
+      </c>
+      <c r="N50" s="6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="B51" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C51" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D51" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="E51" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="F51" s="5" t="n">
+        <v>18</v>
+      </c>
+      <c r="G51" s="5" t="n">
+        <v>37</v>
+      </c>
+      <c r="H51" s="5" t="s">
+        <v>1079</v>
+      </c>
+      <c r="I51" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="J51" s="7" t="s">
+        <v>1075</v>
+      </c>
+      <c r="K51" s="8" t="s">
+        <v>1076</v>
+      </c>
+      <c r="L51" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="M51" s="5" t="s">
+        <v>998</v>
+      </c>
+      <c r="N51" s="6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="0" t="n">
+        <v>51</v>
+      </c>
+      <c r="B52" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C52" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D52" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="E52" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F52" s="5" t="n">
+        <v>21</v>
+      </c>
+      <c r="G52" s="5" t="n">
+        <v>23</v>
+      </c>
+      <c r="H52" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="I52" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="J52" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="K52" s="8" t="s">
+        <v>1080</v>
+      </c>
+      <c r="L52" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="M52" s="5" t="s">
+        <v>998</v>
+      </c>
+      <c r="N52" s="6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="0" t="n">
+        <v>52</v>
+      </c>
+      <c r="B53" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C53" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D53" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="E53" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F53" s="5" t="n">
+        <v>7</v>
+      </c>
+      <c r="G53" s="5" t="n">
+        <v>12</v>
+      </c>
+      <c r="H53" s="5" t="s">
+        <v>1039</v>
+      </c>
+      <c r="I53" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="J53" s="7" t="s">
+        <v>519</v>
+      </c>
+      <c r="K53" s="8" t="s">
+        <v>1040</v>
+      </c>
+      <c r="L53" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="M53" s="5" t="s">
+        <v>998</v>
+      </c>
+      <c r="N53" s="6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="0" t="n">
+        <v>53</v>
+      </c>
+      <c r="B54" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C54" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D54" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="E54" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F54" s="5" t="n">
+        <v>7</v>
+      </c>
+      <c r="G54" s="5" t="n">
+        <v>12</v>
+      </c>
+      <c r="H54" s="5" t="s">
+        <v>1041</v>
+      </c>
+      <c r="I54" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="J54" s="7" t="s">
+        <v>519</v>
+      </c>
+      <c r="K54" s="8" t="s">
+        <v>1040</v>
+      </c>
+      <c r="L54" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="M54" s="5" t="s">
+        <v>998</v>
+      </c>
+      <c r="N54" s="6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="0" t="n">
+        <v>54</v>
+      </c>
+      <c r="B55" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C55" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D55" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="E55" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F55" s="5" t="n">
+        <v>7</v>
+      </c>
+      <c r="G55" s="5" t="n">
+        <v>12</v>
+      </c>
+      <c r="H55" s="5" t="s">
+        <v>1042</v>
+      </c>
+      <c r="I55" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="J55" s="7" t="s">
+        <v>519</v>
+      </c>
+      <c r="K55" s="8" t="s">
+        <v>1040</v>
+      </c>
+      <c r="L55" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="M55" s="5" t="s">
+        <v>998</v>
+      </c>
+      <c r="N55" s="6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="0" t="n">
+        <v>55</v>
+      </c>
+      <c r="B56" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C56" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D56" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="E56" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="F56" s="5" t="n">
+        <v>7</v>
+      </c>
+      <c r="G56" s="5" t="n">
+        <v>12</v>
+      </c>
+      <c r="H56" s="5" t="s">
+        <v>1043</v>
+      </c>
+      <c r="I56" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="J56" s="7" t="s">
+        <v>519</v>
+      </c>
+      <c r="K56" s="8" t="s">
+        <v>1040</v>
+      </c>
+      <c r="L56" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="M56" s="5" t="s">
+        <v>998</v>
+      </c>
+      <c r="N56" s="6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="0" t="n">
+        <v>56</v>
+      </c>
+      <c r="B57" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C57" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D57" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="E57" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F57" s="5" t="n">
+        <v>24</v>
+      </c>
+      <c r="G57" s="5" t="n">
+        <v>27</v>
+      </c>
+      <c r="H57" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="I57" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="J57" s="7" t="s">
+        <v>1044</v>
+      </c>
+      <c r="K57" s="8" t="s">
+        <v>1081</v>
+      </c>
+      <c r="L57" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="M57" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="N57" s="6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="0" t="n">
+        <v>57</v>
+      </c>
+      <c r="B58" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C58" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D58" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="E58" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F58" s="5" t="n">
+        <v>7</v>
+      </c>
+      <c r="G58" s="5" t="n">
+        <v>12</v>
+      </c>
+      <c r="H58" s="5" t="s">
+        <v>1082</v>
+      </c>
+      <c r="I58" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="J58" s="7" t="s">
+        <v>519</v>
+      </c>
+      <c r="K58" s="8" t="s">
+        <v>1083</v>
+      </c>
+      <c r="L58" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="M58" s="5" t="s">
+        <v>998</v>
+      </c>
+      <c r="N58" s="6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="0" t="n">
+        <v>58</v>
+      </c>
+      <c r="B59" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C59" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D59" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="E59" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F59" s="5" t="n">
+        <v>7</v>
+      </c>
+      <c r="G59" s="5" t="n">
+        <v>12</v>
+      </c>
+      <c r="H59" s="5" t="s">
+        <v>1084</v>
+      </c>
+      <c r="I59" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="J59" s="7" t="s">
+        <v>519</v>
+      </c>
+      <c r="K59" s="8" t="s">
+        <v>1083</v>
+      </c>
+      <c r="L59" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="M59" s="5" t="s">
+        <v>998</v>
+      </c>
+      <c r="N59" s="6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="0" t="n">
+        <v>59</v>
+      </c>
+      <c r="B60" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C60" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D60" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="E60" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F60" s="5" t="n">
+        <v>7</v>
+      </c>
+      <c r="G60" s="5" t="n">
+        <v>12</v>
+      </c>
+      <c r="H60" s="5" t="s">
+        <v>1085</v>
+      </c>
+      <c r="I60" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="J60" s="7" t="s">
+        <v>519</v>
+      </c>
+      <c r="K60" s="8" t="s">
+        <v>1083</v>
+      </c>
+      <c r="L60" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="M60" s="5" t="s">
+        <v>998</v>
+      </c>
+      <c r="N60" s="6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="0" t="n">
+        <v>60</v>
+      </c>
+      <c r="B61" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C61" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D61" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="E61" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="F61" s="5" t="n">
+        <v>7</v>
+      </c>
+      <c r="G61" s="5" t="n">
+        <v>12</v>
+      </c>
+      <c r="H61" s="5" t="s">
+        <v>1086</v>
+      </c>
+      <c r="I61" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="J61" s="7" t="s">
+        <v>519</v>
+      </c>
+      <c r="K61" s="8" t="s">
+        <v>1083</v>
+      </c>
+      <c r="L61" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="M61" s="5" t="s">
+        <v>998</v>
+      </c>
+      <c r="N61" s="6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Normalny"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normalny"&amp;12Strona &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>